<commit_message>
Merged PR 7526: PRI-22082 Flow Chart Tab - Update Template to support 5 week month 1, 2 or 3 in a Quarter
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\plan-excel-generation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0D3E9CC2-EFB1-4D34-BEE4-ABC703384B5A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{77FFFB5B-80E2-47F3-B61E-E13D6193EABF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="27360" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="27360" windowHeight="15240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Proposal (By Plan)" sheetId="1" state="hidden" r:id="rId4"/>
     <sheet name="Terms &amp; Conditions" sheetId="7" r:id="rId5"/>
     <sheet name="Proposal" sheetId="5" r:id="rId6"/>
+    <sheet name="Flow Chart template tables" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="91">
   <si>
     <t>Broadcast Proposal Gorilla Glue Q4 '19 - Q1 '20</t>
   </si>
@@ -677,15 +678,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="#,##0.000"/>
-    <numFmt numFmtId="169" formatCode="d/m;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -743,13 +743,6 @@
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFECF0F3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1150,11 +1143,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1336,17 +1329,8 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
@@ -1459,10 +1443,10 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1531,8 +1515,8 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
@@ -1578,35 +1562,11 @@
     <xf numFmtId="10" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1614,27 +1574,15 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="169" fontId="13" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1657,6 +1605,39 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1671,18 +1652,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1692,7 +1673,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2457,13 +2438,13 @@
   </sheetPr>
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.25" style="88" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="3.25" style="85" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="3" style="3" customWidth="1"/>
     <col min="3" max="4" width="24.875" style="3" customWidth="1"/>
     <col min="5" max="5" width="9.875" style="3" customWidth="1"/>
@@ -2517,40 +2498,40 @@
       </c>
     </row>
     <row r="5" spans="3:20" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="65">
+      <c r="C5" s="62">
         <f>Proposal!C5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="159">
+      <c r="D5" s="144">
         <f>Proposal!E5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="172">
+      <c r="E5" s="168">
         <f>Proposal!I5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="172"/>
-      <c r="G5" s="65">
+      <c r="F5" s="168"/>
+      <c r="G5" s="62">
         <f>Proposal!K5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="65">
+      <c r="H5" s="62">
         <f>Proposal!M5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="65">
+      <c r="I5" s="62">
         <f>Proposal!O5</f>
         <v>0</v>
       </c>
-      <c r="J5" s="65">
+      <c r="J5" s="62">
         <f>Proposal!P5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="65">
+      <c r="K5" s="62">
         <f>Proposal!R5</f>
         <v>0</v>
       </c>
-      <c r="L5" s="65">
+      <c r="L5" s="62">
         <f>Proposal!U5</f>
         <v>0</v>
       </c>
@@ -2587,31 +2568,31 @@
       <c r="T7" s="54"/>
     </row>
     <row r="8" spans="3:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="76" t="s">
+      <c r="D8" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="76" t="s">
+      <c r="E8" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="76" t="s">
+      <c r="F8" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="76" t="s">
+      <c r="G8" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="76" t="s">
+      <c r="H8" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="J8" s="81" t="s">
+      <c r="J8" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="K8" s="77" t="s">
+      <c r="K8" s="74" t="s">
         <v>26</v>
       </c>
       <c r="M8" s="54"/>
@@ -2624,32 +2605,32 @@
       <c r="T8" s="54"/>
     </row>
     <row r="9" spans="3:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="70"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="82"/>
-      <c r="K9" s="84"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="81"/>
     </row>
     <row r="10" spans="3:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="35"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="79" t="s">
+      <c r="D10" s="77"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="85" t="s">
+      <c r="G10" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="78"/>
-      <c r="I10" s="79" t="s">
+      <c r="H10" s="75"/>
+      <c r="I10" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="83"/>
-      <c r="K10" s="87"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="84"/>
     </row>
     <row r="12" spans="3:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="49" t="s">
@@ -2658,266 +2639,266 @@
       <c r="I12" s="54"/>
     </row>
     <row r="13" spans="3:20" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="89" t="s">
+      <c r="C13" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="90" t="s">
+      <c r="D13" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90" t="s">
+      <c r="E13" s="87"/>
+      <c r="F13" s="87" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="90"/>
-      <c r="H13" s="90" t="s">
+      <c r="G13" s="87"/>
+      <c r="H13" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="91"/>
-    </row>
-    <row r="14" spans="3:20" s="88" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="92"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="93"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="95"/>
+      <c r="I13" s="88"/>
+    </row>
+    <row r="14" spans="3:20" s="85" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="89"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="93"/>
+      <c r="I14" s="92"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="117"/>
-      <c r="M14" s="117"/>
-      <c r="N14" s="117"/>
-      <c r="O14" s="117"/>
-      <c r="P14" s="117"/>
-      <c r="Q14" s="117"/>
-      <c r="R14" s="117"/>
-    </row>
-    <row r="15" spans="3:20" s="88" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="99"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="100"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="101"/>
-      <c r="H15" s="97"/>
-      <c r="I15" s="97"/>
+      <c r="L14" s="114"/>
+      <c r="M14" s="114"/>
+      <c r="N14" s="114"/>
+      <c r="O14" s="114"/>
+      <c r="P14" s="114"/>
+      <c r="Q14" s="114"/>
+      <c r="R14" s="114"/>
+    </row>
+    <row r="15" spans="3:20" s="85" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="96"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="94"/>
+      <c r="I15" s="94"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="65"/>
-      <c r="M15" s="65"/>
-      <c r="N15" s="65"/>
-      <c r="O15" s="65"/>
-      <c r="P15" s="65"/>
-      <c r="Q15" s="65"/>
-      <c r="R15" s="65"/>
-    </row>
-    <row r="16" spans="3:20" s="108" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="102" t="s">
+      <c r="L15" s="62"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="62"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="62"/>
+      <c r="R15" s="62"/>
+    </row>
+    <row r="16" spans="3:20" s="105" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="99" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="98"/>
-      <c r="E16" s="98"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="103" t="s">
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="H16" s="98"/>
-      <c r="I16" s="104"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="101"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="117"/>
-      <c r="M16" s="117"/>
-      <c r="N16" s="117"/>
-      <c r="O16" s="117"/>
-      <c r="P16" s="117"/>
-      <c r="Q16" s="117"/>
-      <c r="R16" s="117"/>
-    </row>
-    <row r="17" spans="3:18" s="88" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="99"/>
-      <c r="D17" s="100"/>
-      <c r="E17" s="100"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="101"/>
-      <c r="H17" s="97"/>
-      <c r="I17" s="97"/>
+      <c r="L16" s="114"/>
+      <c r="M16" s="114"/>
+      <c r="N16" s="114"/>
+      <c r="O16" s="114"/>
+      <c r="P16" s="114"/>
+      <c r="Q16" s="114"/>
+      <c r="R16" s="114"/>
+    </row>
+    <row r="17" spans="3:18" s="85" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="96"/>
+      <c r="D17" s="97"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="98"/>
+      <c r="H17" s="94"/>
+      <c r="I17" s="94"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="109"/>
-      <c r="M17" s="109"/>
-      <c r="N17" s="109"/>
-      <c r="O17" s="109"/>
-      <c r="P17" s="109"/>
-      <c r="Q17" s="109"/>
-      <c r="R17" s="109"/>
-    </row>
-    <row r="18" spans="3:18" s="88" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L17" s="106"/>
+      <c r="M17" s="106"/>
+      <c r="N17" s="106"/>
+      <c r="O17" s="106"/>
+      <c r="P17" s="106"/>
+      <c r="Q17" s="106"/>
+      <c r="R17" s="106"/>
+    </row>
+    <row r="18" spans="3:18" s="85" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="175">
+      <c r="D18" s="171">
         <f>Proposal!F20</f>
         <v>0</v>
       </c>
-      <c r="E18" s="175"/>
-      <c r="F18" s="175"/>
-      <c r="G18" s="175"/>
-      <c r="H18" s="175"/>
-      <c r="I18" s="175"/>
-      <c r="J18" s="175"/>
-      <c r="K18" s="175"/>
-      <c r="L18" s="117"/>
-      <c r="M18" s="117"/>
-      <c r="N18" s="117"/>
-      <c r="O18" s="117"/>
-      <c r="P18" s="117"/>
-      <c r="Q18" s="117"/>
-      <c r="R18" s="117"/>
-    </row>
-    <row r="19" spans="3:18" s="88" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="171"/>
+      <c r="F18" s="171"/>
+      <c r="G18" s="171"/>
+      <c r="H18" s="171"/>
+      <c r="I18" s="171"/>
+      <c r="J18" s="171"/>
+      <c r="K18" s="171"/>
+      <c r="L18" s="114"/>
+      <c r="M18" s="114"/>
+      <c r="N18" s="114"/>
+      <c r="O18" s="114"/>
+      <c r="P18" s="114"/>
+      <c r="Q18" s="114"/>
+      <c r="R18" s="114"/>
+    </row>
+    <row r="19" spans="3:18" s="85" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
-      <c r="K19" s="65"/>
-      <c r="L19" s="109"/>
-      <c r="M19" s="109"/>
-      <c r="N19" s="109"/>
-      <c r="O19" s="109"/>
-      <c r="P19" s="109"/>
-      <c r="Q19" s="109"/>
-      <c r="R19" s="109"/>
-    </row>
-    <row r="20" spans="3:18" s="108" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="106"/>
+      <c r="M19" s="106"/>
+      <c r="N19" s="106"/>
+      <c r="O19" s="106"/>
+      <c r="P19" s="106"/>
+      <c r="Q19" s="106"/>
+      <c r="R19" s="106"/>
+    </row>
+    <row r="20" spans="3:18" s="105" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="175">
+      <c r="D20" s="171">
         <f>Proposal!F22</f>
         <v>0</v>
       </c>
-      <c r="E20" s="175"/>
-      <c r="F20" s="175"/>
-      <c r="G20" s="175"/>
-      <c r="H20" s="175"/>
-      <c r="I20" s="175"/>
-      <c r="J20" s="175"/>
-      <c r="K20" s="175"/>
-      <c r="L20" s="117"/>
-      <c r="M20" s="117"/>
-      <c r="N20" s="117"/>
-      <c r="O20" s="117"/>
-      <c r="P20" s="117"/>
-      <c r="Q20" s="117"/>
-      <c r="R20" s="117"/>
-    </row>
-    <row r="21" spans="3:18" s="88" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="171"/>
+      <c r="F20" s="171"/>
+      <c r="G20" s="171"/>
+      <c r="H20" s="171"/>
+      <c r="I20" s="171"/>
+      <c r="J20" s="171"/>
+      <c r="K20" s="171"/>
+      <c r="L20" s="114"/>
+      <c r="M20" s="114"/>
+      <c r="N20" s="114"/>
+      <c r="O20" s="114"/>
+      <c r="P20" s="114"/>
+      <c r="Q20" s="114"/>
+      <c r="R20" s="114"/>
+    </row>
+    <row r="21" spans="3:18" s="85" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
-      <c r="D21" s="109"/>
-      <c r="E21" s="109"/>
-      <c r="F21" s="109"/>
-      <c r="G21" s="109"/>
-      <c r="H21" s="109"/>
-      <c r="I21" s="109"/>
-      <c r="J21" s="109"/>
-      <c r="K21" s="109"/>
-      <c r="L21" s="109"/>
-      <c r="M21" s="109"/>
-      <c r="N21" s="109"/>
-      <c r="O21" s="109"/>
-      <c r="P21" s="109"/>
-      <c r="Q21" s="109"/>
-      <c r="R21" s="109"/>
-    </row>
-    <row r="22" spans="3:18" s="88" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="106"/>
+      <c r="E21" s="106"/>
+      <c r="F21" s="106"/>
+      <c r="G21" s="106"/>
+      <c r="H21" s="106"/>
+      <c r="I21" s="106"/>
+      <c r="J21" s="106"/>
+      <c r="K21" s="106"/>
+      <c r="L21" s="106"/>
+      <c r="M21" s="106"/>
+      <c r="N21" s="106"/>
+      <c r="O21" s="106"/>
+      <c r="P21" s="106"/>
+      <c r="Q21" s="106"/>
+      <c r="R21" s="106"/>
+    </row>
+    <row r="22" spans="3:18" s="85" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="175">
+      <c r="D22" s="171">
         <f>Proposal!F24</f>
         <v>0</v>
       </c>
-      <c r="E22" s="175"/>
-      <c r="F22" s="175"/>
-      <c r="G22" s="175"/>
-      <c r="H22" s="175"/>
-      <c r="I22" s="175"/>
-      <c r="J22" s="175"/>
-      <c r="K22" s="175"/>
-      <c r="L22" s="66"/>
-      <c r="M22" s="66"/>
-      <c r="N22" s="66"/>
-      <c r="O22" s="66"/>
-      <c r="P22" s="66"/>
-      <c r="Q22" s="66"/>
-      <c r="R22" s="66"/>
+      <c r="E22" s="171"/>
+      <c r="F22" s="171"/>
+      <c r="G22" s="171"/>
+      <c r="H22" s="171"/>
+      <c r="I22" s="171"/>
+      <c r="J22" s="171"/>
+      <c r="K22" s="171"/>
+      <c r="L22" s="63"/>
+      <c r="M22" s="63"/>
+      <c r="N22" s="63"/>
+      <c r="O22" s="63"/>
+      <c r="P22" s="63"/>
+      <c r="Q22" s="63"/>
+      <c r="R22" s="63"/>
     </row>
     <row r="23" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
-      <c r="D23" s="109"/>
-      <c r="E23" s="109"/>
-      <c r="F23" s="109"/>
-      <c r="G23" s="109"/>
-      <c r="H23" s="109"/>
-      <c r="I23" s="109"/>
-      <c r="J23" s="109"/>
-      <c r="K23" s="109"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="106"/>
+      <c r="F23" s="106"/>
+      <c r="G23" s="106"/>
+      <c r="H23" s="106"/>
+      <c r="I23" s="106"/>
+      <c r="J23" s="106"/>
+      <c r="K23" s="106"/>
     </row>
     <row r="24" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="175">
+      <c r="D24" s="171">
         <f>Proposal!F26</f>
         <v>0</v>
       </c>
-      <c r="E24" s="175"/>
-      <c r="F24" s="175"/>
-      <c r="G24" s="175"/>
-      <c r="H24" s="175"/>
-      <c r="I24" s="175"/>
-      <c r="J24" s="175"/>
-      <c r="K24" s="175"/>
+      <c r="E24" s="171"/>
+      <c r="F24" s="171"/>
+      <c r="G24" s="171"/>
+      <c r="H24" s="171"/>
+      <c r="I24" s="171"/>
+      <c r="J24" s="171"/>
+      <c r="K24" s="171"/>
     </row>
     <row r="25" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
-      <c r="D25" s="109"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="109"/>
-      <c r="G25" s="109"/>
-      <c r="H25" s="109"/>
-      <c r="I25" s="109"/>
-      <c r="J25" s="109"/>
-      <c r="K25" s="109"/>
+      <c r="D25" s="106"/>
+      <c r="E25" s="106"/>
+      <c r="F25" s="106"/>
+      <c r="G25" s="106"/>
+      <c r="H25" s="106"/>
+      <c r="I25" s="106"/>
+      <c r="J25" s="106"/>
+      <c r="K25" s="106"/>
     </row>
     <row r="26" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="174">
+      <c r="D26" s="170">
         <f>Proposal!F28</f>
         <v>0</v>
       </c>
-      <c r="E26" s="175"/>
-      <c r="F26" s="175"/>
-      <c r="G26" s="175"/>
-      <c r="H26" s="175"/>
-      <c r="I26" s="175"/>
-      <c r="J26" s="175"/>
-      <c r="K26" s="175"/>
+      <c r="E26" s="171"/>
+      <c r="F26" s="171"/>
+      <c r="G26" s="171"/>
+      <c r="H26" s="171"/>
+      <c r="I26" s="171"/>
+      <c r="J26" s="171"/>
+      <c r="K26" s="171"/>
     </row>
     <row r="27" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="173"/>
-      <c r="E27" s="173"/>
-      <c r="F27" s="173"/>
-      <c r="G27" s="173"/>
-      <c r="H27" s="173"/>
-      <c r="I27" s="173"/>
-      <c r="J27" s="173"/>
-      <c r="K27" s="173"/>
+      <c r="D27" s="169"/>
+      <c r="E27" s="169"/>
+      <c r="F27" s="169"/>
+      <c r="G27" s="169"/>
+      <c r="H27" s="169"/>
+      <c r="I27" s="169"/>
+      <c r="J27" s="169"/>
+      <c r="K27" s="169"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2965,10 +2946,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="B1:P7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2981,13 +2962,12 @@
     <col min="10" max="10" width="11.875" style="7" customWidth="1"/>
     <col min="11" max="13" width="11.875" style="3" customWidth="1"/>
     <col min="14" max="15" width="11.875" style="7" customWidth="1"/>
-    <col min="16" max="16" width="11.875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="3" style="3" customWidth="1"/>
-    <col min="18" max="16384" width="10.625" style="3"/>
+    <col min="16" max="18" width="11.875" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="10.625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="str">
         <f>SUBSTITUTE(Proposal!F2, "Broadcast Proposal", "Flow Chart")</f>
@@ -2999,8 +2979,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:16" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -3011,210 +2991,53 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="65">
+    <row r="5" spans="2:16" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="62">
         <f>Proposal!K5</f>
         <v>0</v>
       </c>
-      <c r="C5" s="65">
+      <c r="C5" s="62">
         <f>Proposal!O5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="172">
+      <c r="D5" s="168">
         <f>Proposal!F22</f>
         <v>0</v>
       </c>
-      <c r="E5" s="172"/>
-      <c r="F5" s="172"/>
-      <c r="G5" s="172"/>
-      <c r="H5" s="172"/>
-      <c r="I5" s="172"/>
-      <c r="J5" s="172"/>
-      <c r="K5" s="172"/>
-      <c r="L5" s="172"/>
-      <c r="M5" s="172"/>
-      <c r="N5" s="172"/>
-      <c r="O5" s="172"/>
-      <c r="P5" s="172"/>
-    </row>
-    <row r="6" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="168"/>
+      <c r="F5" s="168"/>
+      <c r="G5" s="168"/>
+      <c r="H5" s="168"/>
+      <c r="I5" s="168"/>
+      <c r="J5" s="168"/>
+      <c r="K5" s="168"/>
+      <c r="L5" s="168"/>
+      <c r="M5" s="168"/>
+      <c r="N5" s="168"/>
+      <c r="O5" s="168"/>
+      <c r="P5" s="168"/>
+    </row>
+    <row r="6" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P6" s="54"/>
     </row>
-    <row r="7" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="54"/>
-      <c r="B7" s="64"/>
-      <c r="C7" s="176"/>
-      <c r="D7" s="176"/>
-      <c r="E7" s="176"/>
-      <c r="F7" s="177"/>
-      <c r="G7" s="176"/>
-      <c r="H7" s="176"/>
-      <c r="I7" s="176"/>
-      <c r="J7" s="177"/>
-      <c r="K7" s="178"/>
-      <c r="L7" s="176"/>
-      <c r="M7" s="176"/>
-      <c r="N7" s="176"/>
-      <c r="O7" s="177"/>
-      <c r="P7" s="29"/>
-    </row>
-    <row r="8" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="54"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="52"/>
-      <c r="O8" s="53"/>
-      <c r="P8" s="57" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" s="130" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="151" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="138"/>
-      <c r="D9" s="139"/>
-      <c r="E9" s="139"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="138"/>
-      <c r="H9" s="139"/>
-      <c r="I9" s="139"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="138"/>
-      <c r="L9" s="139"/>
-      <c r="M9" s="139"/>
-      <c r="N9" s="139"/>
-      <c r="O9" s="56"/>
-      <c r="P9" s="142" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" s="130" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="152" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="141"/>
-      <c r="D10" s="133"/>
-      <c r="E10" s="143"/>
-      <c r="F10" s="144"/>
-      <c r="G10" s="141"/>
-      <c r="H10" s="133"/>
-      <c r="I10" s="143"/>
-      <c r="J10" s="144"/>
-      <c r="K10" s="141"/>
-      <c r="L10" s="133"/>
-      <c r="M10" s="143"/>
-      <c r="N10" s="143"/>
-      <c r="O10" s="136"/>
-      <c r="P10" s="136"/>
-    </row>
-    <row r="11" spans="1:16" s="130" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="152" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="140"/>
-      <c r="D11" s="132"/>
-      <c r="E11" s="145"/>
-      <c r="F11" s="146"/>
-      <c r="G11" s="140"/>
-      <c r="H11" s="132"/>
-      <c r="I11" s="145"/>
-      <c r="J11" s="146"/>
-      <c r="K11" s="140"/>
-      <c r="L11" s="132"/>
-      <c r="M11" s="145"/>
-      <c r="N11" s="145"/>
-      <c r="O11" s="135"/>
-      <c r="P11" s="135"/>
-    </row>
-    <row r="12" spans="1:16" s="130" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="152" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="147"/>
-      <c r="D12" s="134"/>
-      <c r="E12" s="148"/>
-      <c r="F12" s="149"/>
-      <c r="G12" s="147"/>
-      <c r="H12" s="134"/>
-      <c r="I12" s="148"/>
-      <c r="J12" s="149"/>
-      <c r="K12" s="147"/>
-      <c r="L12" s="134"/>
-      <c r="M12" s="148"/>
-      <c r="N12" s="148"/>
-      <c r="O12" s="150"/>
-      <c r="P12" s="150"/>
-    </row>
-    <row r="13" spans="1:16" s="130" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="152" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="58"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="58"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="61"/>
-      <c r="N13" s="61"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-    </row>
-    <row r="14" spans="1:16" s="130" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="154" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="155"/>
-      <c r="D14" s="156"/>
-      <c r="E14" s="156"/>
-      <c r="F14" s="156"/>
-      <c r="G14" s="155"/>
-      <c r="H14" s="156"/>
-      <c r="I14" s="156"/>
-      <c r="J14" s="157"/>
-      <c r="K14" s="155"/>
-      <c r="L14" s="156"/>
-      <c r="M14" s="156"/>
-      <c r="N14" s="156"/>
-      <c r="O14" s="157"/>
-      <c r="P14" s="158"/>
-    </row>
-    <row r="15" spans="1:16" s="130" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="131"/>
-      <c r="D15" s="131"/>
-      <c r="E15" s="153"/>
-      <c r="F15" s="153"/>
-      <c r="G15" s="131"/>
-      <c r="H15" s="131"/>
-      <c r="I15" s="153"/>
-      <c r="J15" s="153"/>
-      <c r="K15" s="131"/>
-      <c r="L15" s="131"/>
-      <c r="M15" s="153"/>
-      <c r="N15" s="153"/>
-      <c r="O15" s="153"/>
+    <row r="7" spans="2:16" s="127" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="128"/>
+      <c r="D7" s="128"/>
+      <c r="E7" s="142"/>
+      <c r="F7" s="142"/>
+      <c r="G7" s="128"/>
+      <c r="H7" s="128"/>
+      <c r="I7" s="142"/>
+      <c r="J7" s="142"/>
+      <c r="K7" s="128"/>
+      <c r="L7" s="128"/>
+      <c r="M7" s="142"/>
+      <c r="N7" s="142"/>
+      <c r="O7" s="142"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="1">
     <mergeCell ref="D5:P5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="K7:O7"/>
   </mergeCells>
   <conditionalFormatting sqref="C4">
     <cfRule type="expression" dxfId="18" priority="3">
@@ -3357,24 +3180,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="180" t="s">
+      <c r="G7" s="176" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="180"/>
-      <c r="I7" s="180"/>
-      <c r="J7" s="180"/>
-      <c r="K7" s="180"/>
-      <c r="L7" s="181"/>
+      <c r="H7" s="176"/>
+      <c r="I7" s="176"/>
+      <c r="J7" s="176"/>
+      <c r="K7" s="176"/>
+      <c r="L7" s="177"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="180" t="s">
+      <c r="N7" s="176" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="180"/>
-      <c r="P7" s="180"/>
-      <c r="Q7" s="180"/>
-      <c r="R7" s="180"/>
-      <c r="S7" s="180"/>
-      <c r="T7" s="181"/>
+      <c r="O7" s="176"/>
+      <c r="P7" s="176"/>
+      <c r="Q7" s="176"/>
+      <c r="R7" s="176"/>
+      <c r="S7" s="176"/>
+      <c r="T7" s="177"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -3450,7 +3273,7 @@
       <c r="G9" s="44">
         <v>2.2218515429524603</v>
       </c>
-      <c r="H9" s="67">
+      <c r="H9" s="64">
         <v>13.331109257714761</v>
       </c>
       <c r="I9" s="14">
@@ -3472,7 +3295,7 @@
       <c r="O9" s="44">
         <v>0.83840543510840237</v>
       </c>
-      <c r="P9" s="67">
+      <c r="P9" s="64">
         <v>5.030432610650414</v>
       </c>
       <c r="Q9" s="14">
@@ -3506,7 +3329,7 @@
       <c r="G10" s="45">
         <v>1.9491242702251876</v>
       </c>
-      <c r="H10" s="68">
+      <c r="H10" s="65">
         <v>9.7456213511259389</v>
       </c>
       <c r="I10" s="16">
@@ -3528,7 +3351,7 @@
       <c r="O10" s="45">
         <v>0.63042261964232194</v>
       </c>
-      <c r="P10" s="68">
+      <c r="P10" s="65">
         <v>3.1521130982116095</v>
       </c>
       <c r="Q10" s="16">
@@ -3564,7 +3387,7 @@
       <c r="G11" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="69">
+      <c r="H11" s="66">
         <f>SUM(H9:H10)</f>
         <v>23.076730608840698</v>
       </c>
@@ -3590,7 +3413,7 @@
       <c r="O11" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="P11" s="69">
+      <c r="P11" s="66">
         <f>SUM(P9:P10)</f>
         <v>8.1825457088620226</v>
       </c>
@@ -3618,24 +3441,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="178" t="s">
+      <c r="G13" s="173" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="176"/>
-      <c r="I13" s="176"/>
-      <c r="J13" s="176"/>
-      <c r="K13" s="176"/>
-      <c r="L13" s="177"/>
+      <c r="H13" s="174"/>
+      <c r="I13" s="174"/>
+      <c r="J13" s="174"/>
+      <c r="K13" s="174"/>
+      <c r="L13" s="175"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="178" t="s">
+      <c r="N13" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="176"/>
-      <c r="P13" s="176"/>
-      <c r="Q13" s="176"/>
-      <c r="R13" s="176"/>
-      <c r="S13" s="176"/>
-      <c r="T13" s="177"/>
+      <c r="O13" s="174"/>
+      <c r="P13" s="174"/>
+      <c r="Q13" s="174"/>
+      <c r="R13" s="174"/>
+      <c r="S13" s="174"/>
+      <c r="T13" s="175"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="35" t="s">
@@ -3709,7 +3532,7 @@
       <c r="G15" s="44">
         <v>2.2919099249374479</v>
       </c>
-      <c r="H15" s="67">
+      <c r="H15" s="64">
         <v>11.45954962468724</v>
       </c>
       <c r="I15" s="14">
@@ -3731,7 +3554,7 @@
       <c r="O15" s="44">
         <v>0.86484164252173046</v>
       </c>
-      <c r="P15" s="67">
+      <c r="P15" s="64">
         <v>4.3242082126086521</v>
       </c>
       <c r="Q15" s="14">
@@ -3764,7 +3587,7 @@
       <c r="G16" s="45">
         <v>2.1401167639699752</v>
       </c>
-      <c r="H16" s="68">
+      <c r="H16" s="65">
         <v>8.5604670558799008</v>
       </c>
       <c r="I16" s="16">
@@ -3786,7 +3609,7 @@
       <c r="O16" s="45">
         <v>0.69219702267958838</v>
       </c>
-      <c r="P16" s="68">
+      <c r="P16" s="65">
         <v>2.7687880907183535</v>
       </c>
       <c r="Q16" s="16">
@@ -3821,7 +3644,7 @@
       <c r="G17" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="69">
+      <c r="H17" s="66">
         <f>SUM(H15:H16)</f>
         <v>20.020016680567139</v>
       </c>
@@ -3847,7 +3670,7 @@
       <c r="O17" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="P17" s="69">
+      <c r="P17" s="66">
         <f>SUM(P15:P16)</f>
         <v>7.0929963033270056</v>
       </c>
@@ -3875,24 +3698,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="178" t="s">
+      <c r="G19" s="173" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="176"/>
-      <c r="I19" s="176"/>
-      <c r="J19" s="176"/>
-      <c r="K19" s="176"/>
-      <c r="L19" s="177"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174"/>
+      <c r="J19" s="174"/>
+      <c r="K19" s="174"/>
+      <c r="L19" s="175"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="178" t="s">
+      <c r="N19" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="176"/>
-      <c r="P19" s="176"/>
-      <c r="Q19" s="176"/>
-      <c r="R19" s="176"/>
-      <c r="S19" s="176"/>
-      <c r="T19" s="177"/>
+      <c r="O19" s="174"/>
+      <c r="P19" s="174"/>
+      <c r="Q19" s="174"/>
+      <c r="R19" s="174"/>
+      <c r="S19" s="174"/>
+      <c r="T19" s="175"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="35" t="s">
@@ -3969,7 +3792,7 @@
         <f t="shared" ref="G21:L21" si="0">SUM(G9,G15)</f>
         <v>4.5137614678899087</v>
       </c>
-      <c r="H21" s="67">
+      <c r="H21" s="64">
         <f t="shared" si="0"/>
         <v>24.790658882401999</v>
       </c>
@@ -3998,7 +3821,7 @@
         <f t="shared" si="1"/>
         <v>1.7032470776301327</v>
       </c>
-      <c r="P21" s="67">
+      <c r="P21" s="64">
         <f t="shared" si="1"/>
         <v>9.3546408232590661</v>
       </c>
@@ -4039,7 +3862,7 @@
         <f t="shared" ref="G22:L22" si="2">SUM(G10,G16)</f>
         <v>4.0892410341951626</v>
       </c>
-      <c r="H22" s="68">
+      <c r="H22" s="65">
         <f t="shared" si="2"/>
         <v>18.306088407005838</v>
       </c>
@@ -4068,7 +3891,7 @@
         <f t="shared" si="3"/>
         <v>1.3226196423219103</v>
       </c>
-      <c r="P22" s="68">
+      <c r="P22" s="65">
         <f t="shared" si="3"/>
         <v>5.920901188929963</v>
       </c>
@@ -4109,7 +3932,7 @@
         <f>SUM(G21:G22)</f>
         <v>8.6030025020850722</v>
       </c>
-      <c r="H23" s="69">
+      <c r="H23" s="66">
         <f t="shared" ref="H23:L23" si="4">SUM(H21:H22)</f>
         <v>43.096747289407837</v>
       </c>
@@ -4137,7 +3960,7 @@
         <f t="shared" ref="O23:T23" si="5">SUM(O21:O22)</f>
         <v>3.025866719952043</v>
       </c>
-      <c r="P23" s="69">
+      <c r="P23" s="66">
         <f t="shared" si="5"/>
         <v>15.275542012189028</v>
       </c>
@@ -4162,25 +3985,25 @@
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="182" t="s">
+      <c r="D25" s="178" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="182"/>
-      <c r="F25" s="182"/>
-      <c r="G25" s="182"/>
-      <c r="H25" s="182"/>
-      <c r="I25" s="182"/>
-      <c r="J25" s="182"/>
-      <c r="K25" s="182"/>
-      <c r="L25" s="182"/>
-      <c r="M25" s="182"/>
-      <c r="N25" s="182"/>
-      <c r="O25" s="182"/>
-      <c r="P25" s="182"/>
-      <c r="Q25" s="182"/>
-      <c r="R25" s="182"/>
-      <c r="S25" s="182"/>
-      <c r="T25" s="182"/>
+      <c r="E25" s="178"/>
+      <c r="F25" s="178"/>
+      <c r="G25" s="178"/>
+      <c r="H25" s="178"/>
+      <c r="I25" s="178"/>
+      <c r="J25" s="178"/>
+      <c r="K25" s="178"/>
+      <c r="L25" s="178"/>
+      <c r="M25" s="178"/>
+      <c r="N25" s="178"/>
+      <c r="O25" s="178"/>
+      <c r="P25" s="178"/>
+      <c r="Q25" s="178"/>
+      <c r="R25" s="178"/>
+      <c r="S25" s="178"/>
+      <c r="T25" s="178"/>
     </row>
     <row r="26" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -4206,25 +4029,25 @@
       <c r="B27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="182" t="s">
+      <c r="D27" s="178" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="182"/>
-      <c r="F27" s="182"/>
-      <c r="G27" s="182"/>
-      <c r="H27" s="182"/>
-      <c r="I27" s="182"/>
-      <c r="J27" s="182"/>
-      <c r="K27" s="182"/>
-      <c r="L27" s="182"/>
-      <c r="M27" s="182"/>
-      <c r="N27" s="182"/>
-      <c r="O27" s="182"/>
-      <c r="P27" s="182"/>
-      <c r="Q27" s="182"/>
-      <c r="R27" s="182"/>
-      <c r="S27" s="182"/>
-      <c r="T27" s="182"/>
+      <c r="E27" s="178"/>
+      <c r="F27" s="178"/>
+      <c r="G27" s="178"/>
+      <c r="H27" s="178"/>
+      <c r="I27" s="178"/>
+      <c r="J27" s="178"/>
+      <c r="K27" s="178"/>
+      <c r="L27" s="178"/>
+      <c r="M27" s="178"/>
+      <c r="N27" s="178"/>
+      <c r="O27" s="178"/>
+      <c r="P27" s="178"/>
+      <c r="Q27" s="178"/>
+      <c r="R27" s="178"/>
+      <c r="S27" s="178"/>
+      <c r="T27" s="178"/>
     </row>
     <row r="28" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
@@ -4250,25 +4073,25 @@
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="182" t="s">
+      <c r="D29" s="178" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="182"/>
-      <c r="F29" s="182"/>
-      <c r="G29" s="182"/>
-      <c r="H29" s="182"/>
-      <c r="I29" s="182"/>
-      <c r="J29" s="182"/>
-      <c r="K29" s="182"/>
-      <c r="L29" s="182"/>
-      <c r="M29" s="182"/>
-      <c r="N29" s="182"/>
-      <c r="O29" s="182"/>
-      <c r="P29" s="182"/>
-      <c r="Q29" s="182"/>
-      <c r="R29" s="182"/>
-      <c r="S29" s="182"/>
-      <c r="T29" s="182"/>
+      <c r="E29" s="178"/>
+      <c r="F29" s="178"/>
+      <c r="G29" s="178"/>
+      <c r="H29" s="178"/>
+      <c r="I29" s="178"/>
+      <c r="J29" s="178"/>
+      <c r="K29" s="178"/>
+      <c r="L29" s="178"/>
+      <c r="M29" s="178"/>
+      <c r="N29" s="178"/>
+      <c r="O29" s="178"/>
+      <c r="P29" s="178"/>
+      <c r="Q29" s="178"/>
+      <c r="R29" s="178"/>
+      <c r="S29" s="178"/>
+      <c r="T29" s="178"/>
     </row>
     <row r="30" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
@@ -4294,25 +4117,25 @@
       <c r="B31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="182" t="s">
+      <c r="D31" s="178" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="182"/>
-      <c r="F31" s="182"/>
-      <c r="G31" s="182"/>
-      <c r="H31" s="182"/>
-      <c r="I31" s="182"/>
-      <c r="J31" s="182"/>
-      <c r="K31" s="182"/>
-      <c r="L31" s="182"/>
-      <c r="M31" s="182"/>
-      <c r="N31" s="182"/>
-      <c r="O31" s="182"/>
-      <c r="P31" s="182"/>
-      <c r="Q31" s="182"/>
-      <c r="R31" s="182"/>
-      <c r="S31" s="182"/>
-      <c r="T31" s="182"/>
+      <c r="E31" s="178"/>
+      <c r="F31" s="178"/>
+      <c r="G31" s="178"/>
+      <c r="H31" s="178"/>
+      <c r="I31" s="178"/>
+      <c r="J31" s="178"/>
+      <c r="K31" s="178"/>
+      <c r="L31" s="178"/>
+      <c r="M31" s="178"/>
+      <c r="N31" s="178"/>
+      <c r="O31" s="178"/>
+      <c r="P31" s="178"/>
+      <c r="Q31" s="178"/>
+      <c r="R31" s="178"/>
+      <c r="S31" s="178"/>
+      <c r="T31" s="178"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -4338,25 +4161,25 @@
       <c r="B33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="182" t="s">
+      <c r="D33" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="182"/>
-      <c r="F33" s="182"/>
-      <c r="G33" s="182"/>
-      <c r="H33" s="182"/>
-      <c r="I33" s="182"/>
-      <c r="J33" s="182"/>
-      <c r="K33" s="182"/>
-      <c r="L33" s="182"/>
-      <c r="M33" s="182"/>
-      <c r="N33" s="182"/>
-      <c r="O33" s="182"/>
-      <c r="P33" s="182"/>
-      <c r="Q33" s="182"/>
-      <c r="R33" s="182"/>
-      <c r="S33" s="182"/>
-      <c r="T33" s="182"/>
+      <c r="E33" s="178"/>
+      <c r="F33" s="178"/>
+      <c r="G33" s="178"/>
+      <c r="H33" s="178"/>
+      <c r="I33" s="178"/>
+      <c r="J33" s="178"/>
+      <c r="K33" s="178"/>
+      <c r="L33" s="178"/>
+      <c r="M33" s="178"/>
+      <c r="N33" s="178"/>
+      <c r="O33" s="178"/>
+      <c r="P33" s="178"/>
+      <c r="Q33" s="178"/>
+      <c r="R33" s="178"/>
+      <c r="S33" s="178"/>
+      <c r="T33" s="178"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -4382,25 +4205,25 @@
       <c r="B35" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="179" t="s">
+      <c r="D35" s="172" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="179"/>
-      <c r="F35" s="179"/>
-      <c r="G35" s="179"/>
-      <c r="H35" s="179"/>
-      <c r="I35" s="179"/>
-      <c r="J35" s="179"/>
-      <c r="K35" s="179"/>
-      <c r="L35" s="179"/>
-      <c r="M35" s="179"/>
-      <c r="N35" s="179"/>
-      <c r="O35" s="179"/>
-      <c r="P35" s="179"/>
-      <c r="Q35" s="179"/>
-      <c r="R35" s="179"/>
-      <c r="S35" s="179"/>
-      <c r="T35" s="179"/>
+      <c r="E35" s="172"/>
+      <c r="F35" s="172"/>
+      <c r="G35" s="172"/>
+      <c r="H35" s="172"/>
+      <c r="I35" s="172"/>
+      <c r="J35" s="172"/>
+      <c r="K35" s="172"/>
+      <c r="L35" s="172"/>
+      <c r="M35" s="172"/>
+      <c r="N35" s="172"/>
+      <c r="O35" s="172"/>
+      <c r="P35" s="172"/>
+      <c r="Q35" s="172"/>
+      <c r="R35" s="172"/>
+      <c r="S35" s="172"/>
+      <c r="T35" s="172"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4542,24 +4365,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="180" t="s">
+      <c r="G7" s="176" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="180"/>
-      <c r="I7" s="180"/>
-      <c r="J7" s="180"/>
-      <c r="K7" s="180"/>
-      <c r="L7" s="181"/>
+      <c r="H7" s="176"/>
+      <c r="I7" s="176"/>
+      <c r="J7" s="176"/>
+      <c r="K7" s="176"/>
+      <c r="L7" s="177"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="180" t="s">
+      <c r="N7" s="176" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="180"/>
-      <c r="P7" s="180"/>
-      <c r="Q7" s="180"/>
-      <c r="R7" s="180"/>
-      <c r="S7" s="180"/>
-      <c r="T7" s="181"/>
+      <c r="O7" s="176"/>
+      <c r="P7" s="176"/>
+      <c r="Q7" s="176"/>
+      <c r="R7" s="176"/>
+      <c r="S7" s="176"/>
+      <c r="T7" s="177"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -4801,24 +4624,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="178" t="s">
+      <c r="G13" s="173" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="176"/>
-      <c r="I13" s="176"/>
-      <c r="J13" s="176"/>
-      <c r="K13" s="176"/>
-      <c r="L13" s="177"/>
+      <c r="H13" s="174"/>
+      <c r="I13" s="174"/>
+      <c r="J13" s="174"/>
+      <c r="K13" s="174"/>
+      <c r="L13" s="175"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="178" t="s">
+      <c r="N13" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="176"/>
-      <c r="P13" s="176"/>
-      <c r="Q13" s="176"/>
-      <c r="R13" s="176"/>
-      <c r="S13" s="176"/>
-      <c r="T13" s="177"/>
+      <c r="O13" s="174"/>
+      <c r="P13" s="174"/>
+      <c r="Q13" s="174"/>
+      <c r="R13" s="174"/>
+      <c r="S13" s="174"/>
+      <c r="T13" s="175"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="35" t="s">
@@ -5056,24 +4879,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="178" t="s">
+      <c r="G19" s="173" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="176"/>
-      <c r="I19" s="176"/>
-      <c r="J19" s="176"/>
-      <c r="K19" s="176"/>
-      <c r="L19" s="177"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="174"/>
+      <c r="J19" s="174"/>
+      <c r="K19" s="174"/>
+      <c r="L19" s="175"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="178" t="s">
+      <c r="N19" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="176"/>
-      <c r="P19" s="176"/>
-      <c r="Q19" s="176"/>
-      <c r="R19" s="176"/>
-      <c r="S19" s="176"/>
-      <c r="T19" s="177"/>
+      <c r="O19" s="174"/>
+      <c r="P19" s="174"/>
+      <c r="Q19" s="174"/>
+      <c r="R19" s="174"/>
+      <c r="S19" s="174"/>
+      <c r="T19" s="175"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="35" t="s">
@@ -5311,24 +5134,24 @@
       <c r="D25" s="6"/>
       <c r="E25" s="20"/>
       <c r="F25" s="25"/>
-      <c r="G25" s="178" t="s">
+      <c r="G25" s="173" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="176"/>
-      <c r="I25" s="176"/>
-      <c r="J25" s="176"/>
-      <c r="K25" s="176"/>
-      <c r="L25" s="177"/>
+      <c r="H25" s="174"/>
+      <c r="I25" s="174"/>
+      <c r="J25" s="174"/>
+      <c r="K25" s="174"/>
+      <c r="L25" s="175"/>
       <c r="M25" s="30"/>
-      <c r="N25" s="178" t="s">
+      <c r="N25" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="176"/>
-      <c r="P25" s="176"/>
-      <c r="Q25" s="176"/>
-      <c r="R25" s="176"/>
-      <c r="S25" s="176"/>
-      <c r="T25" s="177"/>
+      <c r="O25" s="174"/>
+      <c r="P25" s="174"/>
+      <c r="Q25" s="174"/>
+      <c r="R25" s="174"/>
+      <c r="S25" s="174"/>
+      <c r="T25" s="175"/>
     </row>
     <row r="26" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="35" t="s">
@@ -5566,26 +5389,26 @@
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="172" t="s">
+      <c r="C31" s="168" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="172"/>
-      <c r="E31" s="172"/>
-      <c r="F31" s="172"/>
-      <c r="G31" s="172"/>
-      <c r="H31" s="172"/>
-      <c r="I31" s="172"/>
-      <c r="J31" s="172"/>
-      <c r="K31" s="172"/>
-      <c r="L31" s="172"/>
-      <c r="M31" s="172"/>
-      <c r="N31" s="172"/>
-      <c r="O31" s="172"/>
-      <c r="P31" s="172"/>
-      <c r="Q31" s="172"/>
-      <c r="R31" s="172"/>
-      <c r="S31" s="172"/>
-      <c r="T31" s="172"/>
+      <c r="D31" s="168"/>
+      <c r="E31" s="168"/>
+      <c r="F31" s="168"/>
+      <c r="G31" s="168"/>
+      <c r="H31" s="168"/>
+      <c r="I31" s="168"/>
+      <c r="J31" s="168"/>
+      <c r="K31" s="168"/>
+      <c r="L31" s="168"/>
+      <c r="M31" s="168"/>
+      <c r="N31" s="168"/>
+      <c r="O31" s="168"/>
+      <c r="P31" s="168"/>
+      <c r="Q31" s="168"/>
+      <c r="R31" s="168"/>
+      <c r="S31" s="168"/>
+      <c r="T31" s="168"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -5612,26 +5435,26 @@
       <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="172" t="s">
+      <c r="C33" s="168" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="172"/>
-      <c r="E33" s="172"/>
-      <c r="F33" s="172"/>
-      <c r="G33" s="172"/>
-      <c r="H33" s="172"/>
-      <c r="I33" s="172"/>
-      <c r="J33" s="172"/>
-      <c r="K33" s="172"/>
-      <c r="L33" s="172"/>
-      <c r="M33" s="172"/>
-      <c r="N33" s="172"/>
-      <c r="O33" s="172"/>
-      <c r="P33" s="172"/>
-      <c r="Q33" s="172"/>
-      <c r="R33" s="172"/>
-      <c r="S33" s="172"/>
-      <c r="T33" s="172"/>
+      <c r="D33" s="168"/>
+      <c r="E33" s="168"/>
+      <c r="F33" s="168"/>
+      <c r="G33" s="168"/>
+      <c r="H33" s="168"/>
+      <c r="I33" s="168"/>
+      <c r="J33" s="168"/>
+      <c r="K33" s="168"/>
+      <c r="L33" s="168"/>
+      <c r="M33" s="168"/>
+      <c r="N33" s="168"/>
+      <c r="O33" s="168"/>
+      <c r="P33" s="168"/>
+      <c r="Q33" s="168"/>
+      <c r="R33" s="168"/>
+      <c r="S33" s="168"/>
+      <c r="T33" s="168"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -5658,26 +5481,26 @@
       <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="172" t="s">
+      <c r="C35" s="168" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="172"/>
-      <c r="E35" s="172"/>
-      <c r="F35" s="172"/>
-      <c r="G35" s="172"/>
-      <c r="H35" s="172"/>
-      <c r="I35" s="172"/>
-      <c r="J35" s="172"/>
-      <c r="K35" s="172"/>
-      <c r="L35" s="172"/>
-      <c r="M35" s="172"/>
-      <c r="N35" s="172"/>
-      <c r="O35" s="172"/>
-      <c r="P35" s="172"/>
-      <c r="Q35" s="172"/>
-      <c r="R35" s="172"/>
-      <c r="S35" s="172"/>
-      <c r="T35" s="172"/>
+      <c r="D35" s="168"/>
+      <c r="E35" s="168"/>
+      <c r="F35" s="168"/>
+      <c r="G35" s="168"/>
+      <c r="H35" s="168"/>
+      <c r="I35" s="168"/>
+      <c r="J35" s="168"/>
+      <c r="K35" s="168"/>
+      <c r="L35" s="168"/>
+      <c r="M35" s="168"/>
+      <c r="N35" s="168"/>
+      <c r="O35" s="168"/>
+      <c r="P35" s="168"/>
+      <c r="Q35" s="168"/>
+      <c r="R35" s="168"/>
+      <c r="S35" s="168"/>
+      <c r="T35" s="168"/>
     </row>
     <row r="36" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
@@ -5704,26 +5527,26 @@
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="172" t="s">
+      <c r="C37" s="168" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="172"/>
-      <c r="E37" s="172"/>
-      <c r="F37" s="172"/>
-      <c r="G37" s="172"/>
-      <c r="H37" s="172"/>
-      <c r="I37" s="172"/>
-      <c r="J37" s="172"/>
-      <c r="K37" s="172"/>
-      <c r="L37" s="172"/>
-      <c r="M37" s="172"/>
-      <c r="N37" s="172"/>
-      <c r="O37" s="172"/>
-      <c r="P37" s="172"/>
-      <c r="Q37" s="172"/>
-      <c r="R37" s="172"/>
-      <c r="S37" s="172"/>
-      <c r="T37" s="172"/>
+      <c r="D37" s="168"/>
+      <c r="E37" s="168"/>
+      <c r="F37" s="168"/>
+      <c r="G37" s="168"/>
+      <c r="H37" s="168"/>
+      <c r="I37" s="168"/>
+      <c r="J37" s="168"/>
+      <c r="K37" s="168"/>
+      <c r="L37" s="168"/>
+      <c r="M37" s="168"/>
+      <c r="N37" s="168"/>
+      <c r="O37" s="168"/>
+      <c r="P37" s="168"/>
+      <c r="Q37" s="168"/>
+      <c r="R37" s="168"/>
+      <c r="S37" s="168"/>
+      <c r="T37" s="168"/>
     </row>
     <row r="38" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
@@ -5750,26 +5573,26 @@
       <c r="B39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="172" t="s">
+      <c r="C39" s="168" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="172"/>
-      <c r="E39" s="172"/>
-      <c r="F39" s="172"/>
-      <c r="G39" s="172"/>
-      <c r="H39" s="172"/>
-      <c r="I39" s="172"/>
-      <c r="J39" s="172"/>
-      <c r="K39" s="172"/>
-      <c r="L39" s="172"/>
-      <c r="M39" s="172"/>
-      <c r="N39" s="172"/>
-      <c r="O39" s="172"/>
-      <c r="P39" s="172"/>
-      <c r="Q39" s="172"/>
-      <c r="R39" s="172"/>
-      <c r="S39" s="172"/>
-      <c r="T39" s="172"/>
+      <c r="D39" s="168"/>
+      <c r="E39" s="168"/>
+      <c r="F39" s="168"/>
+      <c r="G39" s="168"/>
+      <c r="H39" s="168"/>
+      <c r="I39" s="168"/>
+      <c r="J39" s="168"/>
+      <c r="K39" s="168"/>
+      <c r="L39" s="168"/>
+      <c r="M39" s="168"/>
+      <c r="N39" s="168"/>
+      <c r="O39" s="168"/>
+      <c r="P39" s="168"/>
+      <c r="Q39" s="168"/>
+      <c r="R39" s="168"/>
+      <c r="S39" s="168"/>
+      <c r="T39" s="168"/>
     </row>
     <row r="40" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
@@ -5796,34 +5619,29 @@
       <c r="B41" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="174" t="s">
+      <c r="C41" s="170" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="174"/>
-      <c r="E41" s="174"/>
-      <c r="F41" s="174"/>
-      <c r="G41" s="174"/>
-      <c r="H41" s="174"/>
-      <c r="I41" s="174"/>
-      <c r="J41" s="174"/>
-      <c r="K41" s="174"/>
-      <c r="L41" s="174"/>
-      <c r="M41" s="174"/>
-      <c r="N41" s="174"/>
-      <c r="O41" s="174"/>
-      <c r="P41" s="174"/>
-      <c r="Q41" s="174"/>
-      <c r="R41" s="174"/>
-      <c r="S41" s="174"/>
-      <c r="T41" s="174"/>
+      <c r="D41" s="170"/>
+      <c r="E41" s="170"/>
+      <c r="F41" s="170"/>
+      <c r="G41" s="170"/>
+      <c r="H41" s="170"/>
+      <c r="I41" s="170"/>
+      <c r="J41" s="170"/>
+      <c r="K41" s="170"/>
+      <c r="L41" s="170"/>
+      <c r="M41" s="170"/>
+      <c r="N41" s="170"/>
+      <c r="O41" s="170"/>
+      <c r="P41" s="170"/>
+      <c r="Q41" s="170"/>
+      <c r="R41" s="170"/>
+      <c r="S41" s="170"/>
+      <c r="T41" s="170"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5833,6 +5651,11 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5853,14 +5676,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="0" style="88" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="3" style="88" customWidth="1"/>
-    <col min="3" max="3" width="24.875" style="88" customWidth="1"/>
-    <col min="4" max="4" width="68" style="88" customWidth="1"/>
-    <col min="5" max="5" width="2.375" style="88" customWidth="1"/>
-    <col min="6" max="12" width="10.875" style="88" customWidth="1"/>
-    <col min="13" max="13" width="3" style="88" customWidth="1"/>
-    <col min="14" max="16384" width="10.625" style="88"/>
+    <col min="1" max="1" width="0" style="85" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="85" customWidth="1"/>
+    <col min="3" max="3" width="24.875" style="85" customWidth="1"/>
+    <col min="4" max="4" width="68" style="85" customWidth="1"/>
+    <col min="5" max="5" width="2.375" style="85" customWidth="1"/>
+    <col min="6" max="12" width="10.875" style="85" customWidth="1"/>
+    <col min="13" max="13" width="3" style="85" customWidth="1"/>
+    <col min="14" max="16384" width="10.625" style="85"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5870,95 +5693,95 @@
       </c>
     </row>
     <row r="3" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="3:4" s="107" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="183" t="s">
+    <row r="4" spans="3:4" s="104" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="179" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="183"/>
-    </row>
-    <row r="5" spans="3:4" s="107" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="183" t="s">
+      <c r="D4" s="179"/>
+    </row>
+    <row r="5" spans="3:4" s="104" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="179" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="183"/>
-    </row>
-    <row r="6" spans="3:4" s="107" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="183" t="s">
+      <c r="D5" s="179"/>
+    </row>
+    <row r="6" spans="3:4" s="104" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="179" t="s">
         <v>73</v>
       </c>
-      <c r="D6" s="183"/>
-    </row>
-    <row r="7" spans="3:4" s="107" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="183" t="s">
+      <c r="D6" s="179"/>
+    </row>
+    <row r="7" spans="3:4" s="104" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="179" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="183"/>
-    </row>
-    <row r="8" spans="3:4" s="107" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="183" t="s">
+      <c r="D7" s="179"/>
+    </row>
+    <row r="8" spans="3:4" s="104" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="179" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="183"/>
-    </row>
-    <row r="9" spans="3:4" s="107" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="183" t="s">
+      <c r="D8" s="179"/>
+    </row>
+    <row r="9" spans="3:4" s="104" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="179" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="183"/>
-    </row>
-    <row r="10" spans="3:4" s="107" customFormat="1" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="183" t="s">
+      <c r="D9" s="179"/>
+    </row>
+    <row r="10" spans="3:4" s="104" customFormat="1" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="179" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="183"/>
-    </row>
-    <row r="11" spans="3:4" s="107" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="183" t="s">
+      <c r="D10" s="179"/>
+    </row>
+    <row r="11" spans="3:4" s="104" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="179" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="183"/>
-    </row>
-    <row r="12" spans="3:4" s="107" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="183" t="s">
+      <c r="D11" s="179"/>
+    </row>
+    <row r="12" spans="3:4" s="104" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="179" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="183"/>
-    </row>
-    <row r="13" spans="3:4" s="107" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="183" t="s">
+      <c r="D12" s="179"/>
+    </row>
+    <row r="13" spans="3:4" s="104" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="179" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="183"/>
-    </row>
-    <row r="14" spans="3:4" s="107" customFormat="1" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="183" t="s">
+      <c r="D13" s="179"/>
+    </row>
+    <row r="14" spans="3:4" s="104" customFormat="1" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="179" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="183"/>
-    </row>
-    <row r="15" spans="3:4" s="107" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="183" t="s">
+      <c r="D14" s="179"/>
+    </row>
+    <row r="15" spans="3:4" s="104" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="179" t="s">
         <v>82</v>
       </c>
-      <c r="D15" s="183"/>
-    </row>
-    <row r="16" spans="3:4" s="107" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="183" t="s">
+      <c r="D15" s="179"/>
+    </row>
+    <row r="16" spans="3:4" s="104" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="179" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="183"/>
-    </row>
-    <row r="17" spans="3:4" s="107" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="183" t="s">
+      <c r="D16" s="179"/>
+    </row>
+    <row r="17" spans="3:4" s="104" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="179" t="s">
         <v>84</v>
       </c>
-      <c r="D17" s="183"/>
-    </row>
-    <row r="18" spans="3:4" s="107" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="183" t="s">
+      <c r="D17" s="179"/>
+    </row>
+    <row r="18" spans="3:4" s="104" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="179" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="183"/>
+      <c r="D18" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -5997,20 +5820,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.125" style="88" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="3" style="88" customWidth="1"/>
-    <col min="3" max="3" width="11.375" style="88" customWidth="1"/>
-    <col min="4" max="4" width="9" style="88" customWidth="1"/>
-    <col min="5" max="5" width="7.875" style="88" customWidth="1"/>
-    <col min="6" max="6" width="11.375" style="88" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="88" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="106" customWidth="1"/>
-    <col min="9" max="13" width="11.375" style="88" customWidth="1"/>
-    <col min="14" max="14" width="12.5" style="88" customWidth="1"/>
-    <col min="15" max="20" width="11.375" style="88" customWidth="1"/>
-    <col min="21" max="21" width="12.5" style="88" customWidth="1"/>
-    <col min="22" max="22" width="10.5" style="88" customWidth="1"/>
-    <col min="23" max="16384" width="10.625" style="88"/>
+    <col min="1" max="1" width="5.125" style="85" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="85" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="85" customWidth="1"/>
+    <col min="4" max="4" width="9" style="85" customWidth="1"/>
+    <col min="5" max="5" width="7.875" style="85" customWidth="1"/>
+    <col min="6" max="6" width="11.375" style="85" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="85" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="103" customWidth="1"/>
+    <col min="9" max="13" width="11.375" style="85" customWidth="1"/>
+    <col min="14" max="14" width="12.5" style="85" customWidth="1"/>
+    <col min="15" max="20" width="11.375" style="85" customWidth="1"/>
+    <col min="21" max="21" width="12.5" style="85" customWidth="1"/>
+    <col min="22" max="22" width="10.5" style="85" customWidth="1"/>
+    <col min="23" max="16384" width="10.625" style="85"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6054,24 +5877,24 @@
       </c>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="172"/>
-      <c r="D5" s="172"/>
-      <c r="E5" s="172"/>
-      <c r="F5" s="172"/>
-      <c r="G5" s="172"/>
-      <c r="H5" s="105"/>
-      <c r="I5" s="172"/>
-      <c r="J5" s="172"/>
-      <c r="K5" s="172"/>
-      <c r="L5" s="172"/>
-      <c r="M5" s="172"/>
-      <c r="N5" s="172"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="172"/>
-      <c r="Q5" s="172"/>
-      <c r="R5" s="172"/>
-      <c r="S5" s="172"/>
-      <c r="T5" s="172"/>
+      <c r="C5" s="168"/>
+      <c r="D5" s="168"/>
+      <c r="E5" s="168"/>
+      <c r="F5" s="168"/>
+      <c r="G5" s="168"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="168"/>
+      <c r="J5" s="168"/>
+      <c r="K5" s="168"/>
+      <c r="L5" s="168"/>
+      <c r="M5" s="168"/>
+      <c r="N5" s="168"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="168"/>
+      <c r="Q5" s="168"/>
+      <c r="R5" s="168"/>
+      <c r="S5" s="168"/>
+      <c r="T5" s="168"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I6" s="29"/>
@@ -6080,13 +5903,13 @@
       <c r="L6" s="29"/>
       <c r="M6" s="29"/>
       <c r="N6" s="29"/>
-      <c r="O6" s="137"/>
-      <c r="P6" s="137"/>
-      <c r="Q6" s="137"/>
-      <c r="R6" s="137"/>
-      <c r="S6" s="137"/>
-      <c r="T6" s="137"/>
-      <c r="U6" s="137"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="134"/>
+      <c r="U6" s="134"/>
     </row>
     <row r="7" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="49"/>
@@ -6095,24 +5918,24 @@
       <c r="F7" s="6"/>
       <c r="G7" s="20"/>
       <c r="H7" s="55"/>
-      <c r="I7" s="178" t="s">
+      <c r="I7" s="173" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="176"/>
-      <c r="K7" s="176"/>
-      <c r="L7" s="176"/>
-      <c r="M7" s="176"/>
-      <c r="N7" s="177"/>
-      <c r="O7" s="178"/>
-      <c r="P7" s="176"/>
-      <c r="Q7" s="176"/>
-      <c r="R7" s="176"/>
-      <c r="S7" s="176"/>
-      <c r="T7" s="176"/>
-      <c r="U7" s="177"/>
+      <c r="J7" s="174"/>
+      <c r="K7" s="174"/>
+      <c r="L7" s="174"/>
+      <c r="M7" s="174"/>
+      <c r="N7" s="175"/>
+      <c r="O7" s="173"/>
+      <c r="P7" s="174"/>
+      <c r="Q7" s="174"/>
+      <c r="R7" s="174"/>
+      <c r="S7" s="174"/>
+      <c r="T7" s="174"/>
+      <c r="U7" s="175"/>
     </row>
     <row r="8" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="85" t="s">
         <v>69</v>
       </c>
       <c r="B8" s="24"/>
@@ -6176,23 +5999,23 @@
       <c r="B9" s="24"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="110"/>
-      <c r="F9" s="111"/>
-      <c r="G9" s="125"/>
-      <c r="H9" s="112"/>
-      <c r="I9" s="171"/>
-      <c r="J9" s="114"/>
-      <c r="K9" s="110"/>
-      <c r="L9" s="110"/>
-      <c r="M9" s="115"/>
-      <c r="N9" s="112"/>
-      <c r="O9" s="116"/>
-      <c r="P9" s="113"/>
-      <c r="Q9" s="114"/>
-      <c r="R9" s="110"/>
-      <c r="S9" s="110"/>
-      <c r="T9" s="115"/>
-      <c r="U9" s="112"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="122"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="156"/>
+      <c r="J9" s="111"/>
+      <c r="K9" s="107"/>
+      <c r="L9" s="107"/>
+      <c r="M9" s="112"/>
+      <c r="N9" s="109"/>
+      <c r="O9" s="113"/>
+      <c r="P9" s="110"/>
+      <c r="Q9" s="111"/>
+      <c r="R9" s="107"/>
+      <c r="S9" s="107"/>
+      <c r="T9" s="112"/>
+      <c r="U9" s="109"/>
     </row>
     <row r="10" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="24"/>
@@ -6209,7 +6032,7 @@
       <c r="I10" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="69"/>
+      <c r="J10" s="66"/>
       <c r="K10" s="47" t="s">
         <v>35</v>
       </c>
@@ -6222,7 +6045,7 @@
       <c r="P10" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="Q10" s="69"/>
+      <c r="Q10" s="66"/>
       <c r="R10" s="47" t="s">
         <v>35</v>
       </c>
@@ -6230,7 +6053,7 @@
       <c r="T10" s="43"/>
       <c r="U10" s="39"/>
     </row>
-    <row r="11" spans="1:21" s="106" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" s="103" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="54"/>
       <c r="C11"/>
       <c r="D11"/>
@@ -6252,40 +6075,40 @@
       <c r="T11"/>
       <c r="U11"/>
     </row>
-    <row r="12" spans="1:21" s="106" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" s="103" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="54"/>
       <c r="C12"/>
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12"/>
-      <c r="H12" s="118" t="s">
+      <c r="H12" s="115" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="106" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" s="103" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="54"/>
       <c r="C13"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
-      <c r="H13" s="178"/>
-      <c r="I13" s="176"/>
-      <c r="J13" s="176"/>
-      <c r="K13" s="176"/>
-      <c r="L13" s="176"/>
-      <c r="M13" s="176"/>
-      <c r="N13" s="177"/>
-      <c r="O13" s="178"/>
-      <c r="P13" s="176"/>
-      <c r="Q13" s="176"/>
-      <c r="R13" s="176"/>
-      <c r="S13" s="176"/>
-      <c r="T13" s="176"/>
-      <c r="U13" s="177"/>
-    </row>
-    <row r="14" spans="1:21" s="106" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="173"/>
+      <c r="I13" s="174"/>
+      <c r="J13" s="174"/>
+      <c r="K13" s="174"/>
+      <c r="L13" s="174"/>
+      <c r="M13" s="174"/>
+      <c r="N13" s="175"/>
+      <c r="O13" s="173"/>
+      <c r="P13" s="174"/>
+      <c r="Q13" s="174"/>
+      <c r="R13" s="174"/>
+      <c r="S13" s="174"/>
+      <c r="T13" s="174"/>
+      <c r="U13" s="175"/>
+    </row>
+    <row r="14" spans="1:21" s="103" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="54"/>
       <c r="C14"/>
       <c r="D14"/>
@@ -6335,29 +6158,29 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="106" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" s="103" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="54"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
-      <c r="H15" s="170"/>
-      <c r="I15" s="120"/>
-      <c r="J15" s="121"/>
-      <c r="K15" s="119"/>
-      <c r="L15" s="119"/>
-      <c r="M15" s="122"/>
-      <c r="N15" s="123"/>
-      <c r="O15" s="124"/>
-      <c r="P15" s="120"/>
-      <c r="Q15" s="121"/>
-      <c r="R15" s="119"/>
-      <c r="S15" s="119"/>
-      <c r="T15" s="122"/>
-      <c r="U15" s="123"/>
-    </row>
-    <row r="16" spans="1:21" s="106" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="155"/>
+      <c r="I15" s="117"/>
+      <c r="J15" s="118"/>
+      <c r="K15" s="116"/>
+      <c r="L15" s="116"/>
+      <c r="M15" s="119"/>
+      <c r="N15" s="120"/>
+      <c r="O15" s="121"/>
+      <c r="P15" s="117"/>
+      <c r="Q15" s="118"/>
+      <c r="R15" s="116"/>
+      <c r="S15" s="116"/>
+      <c r="T15" s="119"/>
+      <c r="U15" s="120"/>
+    </row>
+    <row r="16" spans="1:21" s="103" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="54"/>
       <c r="C16"/>
       <c r="D16"/>
@@ -6366,287 +6189,295 @@
       <c r="G16"/>
       <c r="H16" s="41"/>
       <c r="I16" s="46"/>
-      <c r="J16" s="69"/>
+      <c r="J16" s="66"/>
       <c r="K16" s="47"/>
       <c r="L16" s="47"/>
       <c r="M16" s="43"/>
       <c r="N16" s="39"/>
       <c r="O16" s="41"/>
       <c r="P16" s="46"/>
-      <c r="Q16" s="69"/>
+      <c r="Q16" s="66"/>
       <c r="R16" s="47"/>
       <c r="S16" s="47"/>
       <c r="T16" s="43"/>
       <c r="U16" s="39"/>
     </row>
-    <row r="17" spans="1:22" s="160" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="137"/>
+    <row r="17" spans="1:22" s="145" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="134"/>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17"/>
-      <c r="H17" s="164"/>
-      <c r="I17" s="165"/>
-      <c r="J17" s="166"/>
-      <c r="K17" s="167"/>
-      <c r="L17" s="167"/>
-      <c r="M17" s="168"/>
-      <c r="N17" s="169"/>
-      <c r="O17" s="164"/>
-      <c r="P17" s="165"/>
-      <c r="Q17" s="166"/>
-      <c r="R17" s="167"/>
-      <c r="S17" s="167"/>
-      <c r="T17" s="168"/>
-      <c r="U17" s="169"/>
-    </row>
-    <row r="18" spans="1:22" s="106" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="126"/>
+      <c r="H17" s="149"/>
+      <c r="I17" s="150"/>
+      <c r="J17" s="151"/>
+      <c r="K17" s="152"/>
+      <c r="L17" s="152"/>
+      <c r="M17" s="153"/>
+      <c r="N17" s="154"/>
+      <c r="O17" s="149"/>
+      <c r="P17" s="150"/>
+      <c r="Q17" s="151"/>
+      <c r="R17" s="152"/>
+      <c r="S17" s="152"/>
+      <c r="T17" s="153"/>
+      <c r="U17" s="154"/>
+    </row>
+    <row r="18" spans="1:22" s="103" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="123"/>
       <c r="B18"/>
-      <c r="C18" s="127"/>
-      <c r="D18" s="127"/>
-      <c r="E18" s="127"/>
-      <c r="F18" s="127"/>
-      <c r="G18" s="127"/>
-      <c r="H18" s="127"/>
-      <c r="I18" s="127"/>
-      <c r="J18" s="127"/>
-      <c r="K18" s="127"/>
-      <c r="L18" s="127"/>
-      <c r="M18" s="127"/>
-      <c r="N18" s="127"/>
-      <c r="O18" s="127"/>
-      <c r="P18" s="127"/>
-      <c r="Q18" s="127"/>
-      <c r="R18" s="127"/>
-      <c r="S18" s="127"/>
-      <c r="T18" s="127"/>
-      <c r="U18" s="127"/>
+      <c r="C18" s="124"/>
+      <c r="D18" s="124"/>
+      <c r="E18" s="124"/>
+      <c r="F18" s="124"/>
+      <c r="G18" s="124"/>
+      <c r="H18" s="124"/>
+      <c r="I18" s="124"/>
+      <c r="J18" s="124"/>
+      <c r="K18" s="124"/>
+      <c r="L18" s="124"/>
+      <c r="M18" s="124"/>
+      <c r="N18" s="124"/>
+      <c r="O18" s="124"/>
+      <c r="P18" s="124"/>
+      <c r="Q18" s="124"/>
+      <c r="R18" s="124"/>
+      <c r="S18" s="124"/>
+      <c r="T18" s="124"/>
+      <c r="U18" s="124"/>
     </row>
     <row r="19" spans="1:22" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="161"/>
-      <c r="B19" s="162"/>
-      <c r="C19" s="163"/>
-      <c r="D19" s="163"/>
-      <c r="E19" s="163"/>
-      <c r="F19" s="163"/>
-      <c r="G19" s="163"/>
-      <c r="H19" s="163"/>
-      <c r="I19" s="163"/>
-      <c r="J19" s="163"/>
-      <c r="K19" s="163"/>
-      <c r="L19" s="163"/>
-      <c r="M19" s="163"/>
-      <c r="N19" s="163"/>
-      <c r="O19" s="163"/>
-      <c r="P19" s="163"/>
-      <c r="Q19" s="163"/>
-      <c r="R19" s="163"/>
-      <c r="S19" s="163"/>
-      <c r="T19" s="163"/>
-      <c r="U19" s="163"/>
-    </row>
-    <row r="20" spans="1:22" s="129" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="146"/>
+      <c r="B19" s="147"/>
+      <c r="C19" s="148"/>
+      <c r="D19" s="148"/>
+      <c r="E19" s="148"/>
+      <c r="F19" s="148"/>
+      <c r="G19" s="148"/>
+      <c r="H19" s="148"/>
+      <c r="I19" s="148"/>
+      <c r="J19" s="148"/>
+      <c r="K19" s="148"/>
+      <c r="L19" s="148"/>
+      <c r="M19" s="148"/>
+      <c r="N19" s="148"/>
+      <c r="O19" s="148"/>
+      <c r="P19" s="148"/>
+      <c r="Q19" s="148"/>
+      <c r="R19" s="148"/>
+      <c r="S19" s="148"/>
+      <c r="T19" s="148"/>
+      <c r="U19" s="148"/>
+    </row>
+    <row r="20" spans="1:22" s="126" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C20" s="51" t="s">
         <v>42</v>
       </c>
       <c r="D20" s="51"/>
-      <c r="E20" s="108"/>
-      <c r="F20" s="184"/>
-      <c r="G20" s="184"/>
-      <c r="H20" s="184"/>
-      <c r="I20" s="184"/>
-      <c r="J20" s="184"/>
-      <c r="K20" s="184"/>
-      <c r="L20" s="184"/>
-      <c r="M20" s="184"/>
-      <c r="N20" s="184"/>
-      <c r="O20" s="184"/>
-      <c r="P20" s="184"/>
-      <c r="Q20" s="184"/>
-      <c r="R20" s="184"/>
-      <c r="S20" s="184"/>
-      <c r="T20" s="184"/>
-      <c r="U20" s="184"/>
-    </row>
-    <row r="21" spans="1:22" s="129" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="105"/>
+      <c r="F20" s="180"/>
+      <c r="G20" s="180"/>
+      <c r="H20" s="180"/>
+      <c r="I20" s="180"/>
+      <c r="J20" s="180"/>
+      <c r="K20" s="180"/>
+      <c r="L20" s="180"/>
+      <c r="M20" s="180"/>
+      <c r="N20" s="180"/>
+      <c r="O20" s="180"/>
+      <c r="P20" s="180"/>
+      <c r="Q20" s="180"/>
+      <c r="R20" s="180"/>
+      <c r="S20" s="180"/>
+      <c r="T20" s="180"/>
+      <c r="U20" s="180"/>
+    </row>
+    <row r="21" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="F21" s="128"/>
-      <c r="G21" s="128"/>
-      <c r="H21" s="128"/>
-      <c r="I21" s="128"/>
-      <c r="J21" s="128"/>
-      <c r="K21" s="128"/>
-      <c r="L21" s="128"/>
-      <c r="M21" s="128"/>
-      <c r="N21" s="128"/>
-      <c r="O21" s="128"/>
-      <c r="P21" s="128"/>
-      <c r="Q21" s="128"/>
-      <c r="R21" s="128"/>
-      <c r="S21" s="128"/>
-      <c r="T21" s="128"/>
-      <c r="U21" s="128"/>
-    </row>
-    <row r="22" spans="1:22" s="108" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="129"/>
-      <c r="B22" s="129"/>
+      <c r="F21" s="125"/>
+      <c r="G21" s="125"/>
+      <c r="H21" s="125"/>
+      <c r="I21" s="125"/>
+      <c r="J21" s="125"/>
+      <c r="K21" s="125"/>
+      <c r="L21" s="125"/>
+      <c r="M21" s="125"/>
+      <c r="N21" s="125"/>
+      <c r="O21" s="125"/>
+      <c r="P21" s="125"/>
+      <c r="Q21" s="125"/>
+      <c r="R21" s="125"/>
+      <c r="S21" s="125"/>
+      <c r="T21" s="125"/>
+      <c r="U21" s="125"/>
+    </row>
+    <row r="22" spans="1:22" s="105" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="126"/>
+      <c r="B22" s="126"/>
       <c r="C22" s="51" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="51"/>
-      <c r="F22" s="184"/>
-      <c r="G22" s="184"/>
-      <c r="H22" s="184"/>
-      <c r="I22" s="184"/>
-      <c r="J22" s="184"/>
-      <c r="K22" s="184"/>
-      <c r="L22" s="184"/>
-      <c r="M22" s="184"/>
-      <c r="N22" s="184"/>
-      <c r="O22" s="184"/>
-      <c r="P22" s="184"/>
-      <c r="Q22" s="184"/>
-      <c r="R22" s="184"/>
-      <c r="S22" s="184"/>
-      <c r="T22" s="184"/>
-      <c r="U22" s="184"/>
-      <c r="V22" s="129"/>
-    </row>
-    <row r="23" spans="1:22" s="129" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="180"/>
+      <c r="G22" s="180"/>
+      <c r="H22" s="180"/>
+      <c r="I22" s="180"/>
+      <c r="J22" s="180"/>
+      <c r="K22" s="180"/>
+      <c r="L22" s="180"/>
+      <c r="M22" s="180"/>
+      <c r="N22" s="180"/>
+      <c r="O22" s="180"/>
+      <c r="P22" s="180"/>
+      <c r="Q22" s="180"/>
+      <c r="R22" s="180"/>
+      <c r="S22" s="180"/>
+      <c r="T22" s="180"/>
+      <c r="U22" s="180"/>
+      <c r="V22" s="126"/>
+    </row>
+    <row r="23" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="F23" s="109"/>
-      <c r="G23" s="109"/>
-      <c r="H23" s="109"/>
-      <c r="I23" s="109"/>
-      <c r="J23" s="109"/>
-      <c r="K23" s="109"/>
-      <c r="L23" s="109"/>
-      <c r="M23" s="109"/>
-      <c r="N23" s="109"/>
-      <c r="O23" s="109"/>
-      <c r="P23" s="109"/>
-      <c r="Q23" s="109"/>
-      <c r="R23" s="109"/>
-      <c r="S23" s="109"/>
-      <c r="T23" s="109"/>
-      <c r="U23" s="109"/>
-    </row>
-    <row r="24" spans="1:22" s="129" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="106"/>
+      <c r="G23" s="106"/>
+      <c r="H23" s="106"/>
+      <c r="I23" s="106"/>
+      <c r="J23" s="106"/>
+      <c r="K23" s="106"/>
+      <c r="L23" s="106"/>
+      <c r="M23" s="106"/>
+      <c r="N23" s="106"/>
+      <c r="O23" s="106"/>
+      <c r="P23" s="106"/>
+      <c r="Q23" s="106"/>
+      <c r="R23" s="106"/>
+      <c r="S23" s="106"/>
+      <c r="T23" s="106"/>
+      <c r="U23" s="106"/>
+    </row>
+    <row r="24" spans="1:22" s="126" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="51" t="s">
         <v>47</v>
       </c>
       <c r="D24" s="51"/>
-      <c r="E24" s="108"/>
-      <c r="F24" s="184"/>
-      <c r="G24" s="184"/>
-      <c r="H24" s="184"/>
-      <c r="I24" s="184"/>
-      <c r="J24" s="184"/>
-      <c r="K24" s="184"/>
-      <c r="L24" s="184"/>
-      <c r="M24" s="184"/>
-      <c r="N24" s="184"/>
-      <c r="O24" s="184"/>
-      <c r="P24" s="184"/>
-      <c r="Q24" s="184"/>
-      <c r="R24" s="184"/>
-      <c r="S24" s="184"/>
-      <c r="T24" s="184"/>
-      <c r="U24" s="184"/>
-    </row>
-    <row r="25" spans="1:22" s="129" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="105"/>
+      <c r="F24" s="180"/>
+      <c r="G24" s="180"/>
+      <c r="H24" s="180"/>
+      <c r="I24" s="180"/>
+      <c r="J24" s="180"/>
+      <c r="K24" s="180"/>
+      <c r="L24" s="180"/>
+      <c r="M24" s="180"/>
+      <c r="N24" s="180"/>
+      <c r="O24" s="180"/>
+      <c r="P24" s="180"/>
+      <c r="Q24" s="180"/>
+      <c r="R24" s="180"/>
+      <c r="S24" s="180"/>
+      <c r="T24" s="180"/>
+      <c r="U24" s="180"/>
+    </row>
+    <row r="25" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="F25" s="109"/>
-      <c r="G25" s="109"/>
-      <c r="H25" s="109"/>
-      <c r="I25" s="109"/>
-      <c r="J25" s="109"/>
-      <c r="K25" s="109"/>
-      <c r="L25" s="109"/>
-      <c r="M25" s="109"/>
-      <c r="N25" s="109"/>
-      <c r="O25" s="109"/>
-      <c r="P25" s="109"/>
-      <c r="Q25" s="109"/>
-      <c r="R25" s="109"/>
-      <c r="S25" s="109"/>
-      <c r="T25" s="109"/>
-      <c r="U25" s="109"/>
-    </row>
-    <row r="26" spans="1:22" s="108" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="129"/>
-      <c r="B26" s="129"/>
+      <c r="F25" s="106"/>
+      <c r="G25" s="106"/>
+      <c r="H25" s="106"/>
+      <c r="I25" s="106"/>
+      <c r="J25" s="106"/>
+      <c r="K25" s="106"/>
+      <c r="L25" s="106"/>
+      <c r="M25" s="106"/>
+      <c r="N25" s="106"/>
+      <c r="O25" s="106"/>
+      <c r="P25" s="106"/>
+      <c r="Q25" s="106"/>
+      <c r="R25" s="106"/>
+      <c r="S25" s="106"/>
+      <c r="T25" s="106"/>
+      <c r="U25" s="106"/>
+    </row>
+    <row r="26" spans="1:22" s="105" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="126"/>
+      <c r="B26" s="126"/>
       <c r="C26" s="51" t="s">
         <v>48</v>
       </c>
       <c r="D26" s="51"/>
-      <c r="F26" s="175"/>
-      <c r="G26" s="175"/>
-      <c r="H26" s="175"/>
-      <c r="I26" s="175"/>
-      <c r="J26" s="175"/>
-      <c r="K26" s="175"/>
-      <c r="L26" s="175"/>
-      <c r="M26" s="175"/>
-      <c r="N26" s="175"/>
-      <c r="O26" s="175"/>
-      <c r="P26" s="175"/>
-      <c r="Q26" s="175"/>
-      <c r="R26" s="175"/>
-      <c r="S26" s="175"/>
-      <c r="T26" s="175"/>
-      <c r="U26" s="175"/>
-      <c r="V26" s="129"/>
-    </row>
-    <row r="27" spans="1:22" s="129" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="171"/>
+      <c r="G26" s="171"/>
+      <c r="H26" s="171"/>
+      <c r="I26" s="171"/>
+      <c r="J26" s="171"/>
+      <c r="K26" s="171"/>
+      <c r="L26" s="171"/>
+      <c r="M26" s="171"/>
+      <c r="N26" s="171"/>
+      <c r="O26" s="171"/>
+      <c r="P26" s="171"/>
+      <c r="Q26" s="171"/>
+      <c r="R26" s="171"/>
+      <c r="S26" s="171"/>
+      <c r="T26" s="171"/>
+      <c r="U26" s="171"/>
+      <c r="V26" s="126"/>
+    </row>
+    <row r="27" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="F27" s="109"/>
-      <c r="G27" s="109"/>
-      <c r="H27" s="109"/>
-      <c r="I27" s="109"/>
-      <c r="J27" s="109"/>
-      <c r="K27" s="109"/>
-      <c r="L27" s="109"/>
-      <c r="M27" s="109"/>
-      <c r="N27" s="109"/>
-      <c r="O27" s="109"/>
-      <c r="P27" s="109"/>
-      <c r="Q27" s="109"/>
-      <c r="R27" s="109"/>
-      <c r="S27" s="109"/>
-      <c r="T27" s="109"/>
-      <c r="U27" s="109"/>
-    </row>
-    <row r="28" spans="1:22" s="129" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="106"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="106"/>
+      <c r="I27" s="106"/>
+      <c r="J27" s="106"/>
+      <c r="K27" s="106"/>
+      <c r="L27" s="106"/>
+      <c r="M27" s="106"/>
+      <c r="N27" s="106"/>
+      <c r="O27" s="106"/>
+      <c r="P27" s="106"/>
+      <c r="Q27" s="106"/>
+      <c r="R27" s="106"/>
+      <c r="S27" s="106"/>
+      <c r="T27" s="106"/>
+      <c r="U27" s="106"/>
+    </row>
+    <row r="28" spans="1:22" s="126" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="51" t="s">
         <v>49</v>
       </c>
       <c r="D28" s="51"/>
-      <c r="F28" s="174"/>
-      <c r="G28" s="174"/>
-      <c r="H28" s="174"/>
-      <c r="I28" s="174"/>
-      <c r="J28" s="174"/>
-      <c r="K28" s="174"/>
-      <c r="L28" s="174"/>
-      <c r="M28" s="174"/>
-      <c r="N28" s="174"/>
-      <c r="O28" s="174"/>
-      <c r="P28" s="174"/>
-      <c r="Q28" s="174"/>
-      <c r="R28" s="174"/>
-      <c r="S28" s="174"/>
-      <c r="T28" s="174"/>
-      <c r="U28" s="174"/>
+      <c r="F28" s="170"/>
+      <c r="G28" s="170"/>
+      <c r="H28" s="170"/>
+      <c r="I28" s="170"/>
+      <c r="J28" s="170"/>
+      <c r="K28" s="170"/>
+      <c r="L28" s="170"/>
+      <c r="M28" s="170"/>
+      <c r="N28" s="170"/>
+      <c r="O28" s="170"/>
+      <c r="P28" s="170"/>
+      <c r="Q28" s="170"/>
+      <c r="R28" s="170"/>
+      <c r="S28" s="170"/>
+      <c r="T28" s="170"/>
+      <c r="U28" s="170"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
     <mergeCell ref="F28:U28"/>
     <mergeCell ref="F20:U20"/>
     <mergeCell ref="H13:N13"/>
@@ -6655,14 +6486,6 @@
     <mergeCell ref="F24:U24"/>
     <mergeCell ref="F26:U26"/>
     <mergeCell ref="O13:U13"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:U3 C5 C4:O4 Q4 S4:U4 U5 C6:U10 O14:U17 H15:N15 C20:U28">
     <cfRule type="expression" dxfId="15" priority="76">
@@ -6747,6 +6570,1142 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="56" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AABE7EAF-1136-470A-A75B-F26CD2CB0D81}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:Q63"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" style="157" customWidth="1"/>
+    <col min="2" max="2" width="23.125" style="157" customWidth="1"/>
+    <col min="3" max="5" width="11.875" style="157" customWidth="1"/>
+    <col min="6" max="6" width="11.875" style="7" customWidth="1"/>
+    <col min="7" max="9" width="11.875" style="157" customWidth="1"/>
+    <col min="10" max="10" width="11.875" style="7" customWidth="1"/>
+    <col min="11" max="13" width="11.875" style="157" customWidth="1"/>
+    <col min="14" max="15" width="11.875" style="7" customWidth="1"/>
+    <col min="16" max="18" width="11.875" style="157" customWidth="1"/>
+    <col min="19" max="16384" width="10.625" style="157"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="49"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="175"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
+      <c r="I2" s="174"/>
+      <c r="J2" s="175"/>
+      <c r="K2" s="173"/>
+      <c r="L2" s="174"/>
+      <c r="M2" s="174"/>
+      <c r="N2" s="175"/>
+      <c r="O2" s="29"/>
+    </row>
+    <row r="3" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="61"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="158" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="135"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="135"/>
+      <c r="H4" s="136"/>
+      <c r="I4" s="136"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="135"/>
+      <c r="L4" s="136"/>
+      <c r="M4" s="136"/>
+      <c r="N4" s="136"/>
+      <c r="O4" s="139" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="159" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="138"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="133"/>
+      <c r="G5" s="138"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="133"/>
+      <c r="K5" s="138"/>
+      <c r="L5" s="130"/>
+      <c r="M5" s="130"/>
+      <c r="N5" s="130"/>
+      <c r="O5" s="160"/>
+    </row>
+    <row r="6" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="159" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="137"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="137"/>
+      <c r="H6" s="129"/>
+      <c r="I6" s="129"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="137"/>
+      <c r="L6" s="129"/>
+      <c r="M6" s="129"/>
+      <c r="N6" s="129"/>
+      <c r="O6" s="161"/>
+    </row>
+    <row r="7" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="159" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="140"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="141"/>
+      <c r="G7" s="140"/>
+      <c r="H7" s="131"/>
+      <c r="I7" s="131"/>
+      <c r="J7" s="141"/>
+      <c r="K7" s="140"/>
+      <c r="L7" s="131"/>
+      <c r="M7" s="131"/>
+      <c r="N7" s="131"/>
+      <c r="O7" s="162"/>
+    </row>
+    <row r="8" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="159" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="58"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="59"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="163"/>
+    </row>
+    <row r="9" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="143" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="164"/>
+      <c r="D9" s="165"/>
+      <c r="E9" s="165"/>
+      <c r="F9" s="165"/>
+      <c r="G9" s="164"/>
+      <c r="H9" s="165"/>
+      <c r="I9" s="165"/>
+      <c r="J9" s="166"/>
+      <c r="K9" s="164"/>
+      <c r="L9" s="165"/>
+      <c r="M9" s="165"/>
+      <c r="N9" s="165"/>
+      <c r="O9" s="167"/>
+    </row>
+    <row r="11" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="49"/>
+      <c r="C11" s="173"/>
+      <c r="D11" s="174"/>
+      <c r="E11" s="174"/>
+      <c r="F11" s="174"/>
+      <c r="G11" s="175"/>
+      <c r="H11" s="174"/>
+      <c r="I11" s="174"/>
+      <c r="J11" s="174"/>
+      <c r="K11" s="175"/>
+      <c r="L11" s="173"/>
+      <c r="M11" s="174"/>
+      <c r="N11" s="174"/>
+      <c r="O11" s="175"/>
+      <c r="P11" s="29"/>
+    </row>
+    <row r="12" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="61"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="158" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="135"/>
+      <c r="D13" s="136"/>
+      <c r="E13" s="136"/>
+      <c r="F13" s="136"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="135"/>
+      <c r="I13" s="136"/>
+      <c r="J13" s="136"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="135"/>
+      <c r="M13" s="136"/>
+      <c r="N13" s="136"/>
+      <c r="O13" s="56"/>
+      <c r="P13" s="139" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="159" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="138"/>
+      <c r="D14" s="130"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="130"/>
+      <c r="G14" s="133"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="130"/>
+      <c r="J14" s="130"/>
+      <c r="K14" s="133"/>
+      <c r="L14" s="138"/>
+      <c r="M14" s="130"/>
+      <c r="N14" s="130"/>
+      <c r="O14" s="133"/>
+      <c r="P14" s="133"/>
+    </row>
+    <row r="15" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="159" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="137"/>
+      <c r="D15" s="129"/>
+      <c r="E15" s="129"/>
+      <c r="F15" s="129"/>
+      <c r="G15" s="132"/>
+      <c r="H15" s="137"/>
+      <c r="I15" s="129"/>
+      <c r="J15" s="129"/>
+      <c r="K15" s="132"/>
+      <c r="L15" s="137"/>
+      <c r="M15" s="129"/>
+      <c r="N15" s="129"/>
+      <c r="O15" s="132"/>
+      <c r="P15" s="132"/>
+    </row>
+    <row r="16" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="159" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="140"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="131"/>
+      <c r="F16" s="131"/>
+      <c r="G16" s="141"/>
+      <c r="H16" s="140"/>
+      <c r="I16" s="131"/>
+      <c r="J16" s="131"/>
+      <c r="K16" s="141"/>
+      <c r="L16" s="140"/>
+      <c r="M16" s="131"/>
+      <c r="N16" s="131"/>
+      <c r="O16" s="141"/>
+      <c r="P16" s="141"/>
+    </row>
+    <row r="17" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="159" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="58"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="60"/>
+      <c r="P17" s="60"/>
+    </row>
+    <row r="18" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="143" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="164"/>
+      <c r="D18" s="165"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="165"/>
+      <c r="G18" s="165"/>
+      <c r="H18" s="164"/>
+      <c r="I18" s="165"/>
+      <c r="J18" s="165"/>
+      <c r="K18" s="166"/>
+      <c r="L18" s="164"/>
+      <c r="M18" s="165"/>
+      <c r="N18" s="165"/>
+      <c r="O18" s="166"/>
+      <c r="P18" s="167"/>
+    </row>
+    <row r="20" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="49"/>
+      <c r="C20" s="173"/>
+      <c r="D20" s="174"/>
+      <c r="E20" s="174"/>
+      <c r="F20" s="175"/>
+      <c r="G20" s="174"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="174"/>
+      <c r="J20" s="174"/>
+      <c r="K20" s="175"/>
+      <c r="L20" s="173"/>
+      <c r="M20" s="174"/>
+      <c r="N20" s="174"/>
+      <c r="O20" s="175"/>
+      <c r="P20" s="29"/>
+    </row>
+    <row r="21" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="61"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="52"/>
+      <c r="P21" s="57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="158" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="135"/>
+      <c r="D22" s="136"/>
+      <c r="E22" s="136"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="135"/>
+      <c r="H22" s="136"/>
+      <c r="I22" s="136"/>
+      <c r="J22" s="136"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="135"/>
+      <c r="M22" s="136"/>
+      <c r="N22" s="136"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="139" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="159" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="138"/>
+      <c r="D23" s="130"/>
+      <c r="E23" s="130"/>
+      <c r="F23" s="133"/>
+      <c r="G23" s="138"/>
+      <c r="H23" s="130"/>
+      <c r="I23" s="130"/>
+      <c r="J23" s="130"/>
+      <c r="K23" s="133"/>
+      <c r="L23" s="138"/>
+      <c r="M23" s="130"/>
+      <c r="N23" s="130"/>
+      <c r="O23" s="133"/>
+      <c r="P23" s="133"/>
+    </row>
+    <row r="24" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="159" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="137"/>
+      <c r="D24" s="129"/>
+      <c r="E24" s="129"/>
+      <c r="F24" s="132"/>
+      <c r="G24" s="137"/>
+      <c r="H24" s="129"/>
+      <c r="I24" s="129"/>
+      <c r="J24" s="129"/>
+      <c r="K24" s="132"/>
+      <c r="L24" s="137"/>
+      <c r="M24" s="129"/>
+      <c r="N24" s="129"/>
+      <c r="O24" s="132"/>
+      <c r="P24" s="132"/>
+    </row>
+    <row r="25" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="159" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="140"/>
+      <c r="D25" s="131"/>
+      <c r="E25" s="131"/>
+      <c r="F25" s="141"/>
+      <c r="G25" s="140"/>
+      <c r="H25" s="131"/>
+      <c r="I25" s="131"/>
+      <c r="J25" s="131"/>
+      <c r="K25" s="141"/>
+      <c r="L25" s="140"/>
+      <c r="M25" s="131"/>
+      <c r="N25" s="131"/>
+      <c r="O25" s="141"/>
+      <c r="P25" s="141"/>
+    </row>
+    <row r="26" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="159" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="58"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="58"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="60"/>
+    </row>
+    <row r="27" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="143" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" s="164"/>
+      <c r="D27" s="165"/>
+      <c r="E27" s="165"/>
+      <c r="F27" s="165"/>
+      <c r="G27" s="164"/>
+      <c r="H27" s="165"/>
+      <c r="I27" s="165"/>
+      <c r="J27" s="165"/>
+      <c r="K27" s="166"/>
+      <c r="L27" s="164"/>
+      <c r="M27" s="165"/>
+      <c r="N27" s="165"/>
+      <c r="O27" s="166"/>
+      <c r="P27" s="167"/>
+    </row>
+    <row r="29" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="49"/>
+      <c r="C29" s="173"/>
+      <c r="D29" s="174"/>
+      <c r="E29" s="174"/>
+      <c r="F29" s="175"/>
+      <c r="G29" s="174"/>
+      <c r="H29" s="174"/>
+      <c r="I29" s="174"/>
+      <c r="J29" s="175"/>
+      <c r="K29" s="173"/>
+      <c r="L29" s="174"/>
+      <c r="M29" s="174"/>
+      <c r="N29" s="174"/>
+      <c r="O29" s="175"/>
+      <c r="P29" s="29"/>
+    </row>
+    <row r="30" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="61"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="52"/>
+      <c r="L30" s="52"/>
+      <c r="M30" s="52"/>
+      <c r="N30" s="52"/>
+      <c r="O30" s="52"/>
+      <c r="P30" s="57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="158" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="135"/>
+      <c r="D31" s="136"/>
+      <c r="E31" s="136"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="135"/>
+      <c r="H31" s="136"/>
+      <c r="I31" s="136"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="135"/>
+      <c r="L31" s="136"/>
+      <c r="M31" s="136"/>
+      <c r="N31" s="136"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="139" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="159" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="138"/>
+      <c r="D32" s="130"/>
+      <c r="E32" s="130"/>
+      <c r="F32" s="133"/>
+      <c r="G32" s="138"/>
+      <c r="H32" s="130"/>
+      <c r="I32" s="130"/>
+      <c r="J32" s="133"/>
+      <c r="K32" s="138"/>
+      <c r="L32" s="130"/>
+      <c r="M32" s="130"/>
+      <c r="N32" s="130"/>
+      <c r="O32" s="133"/>
+      <c r="P32" s="133"/>
+    </row>
+    <row r="33" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="159" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="137"/>
+      <c r="D33" s="129"/>
+      <c r="E33" s="129"/>
+      <c r="F33" s="132"/>
+      <c r="G33" s="137"/>
+      <c r="H33" s="129"/>
+      <c r="I33" s="129"/>
+      <c r="J33" s="132"/>
+      <c r="K33" s="137"/>
+      <c r="L33" s="129"/>
+      <c r="M33" s="129"/>
+      <c r="N33" s="129"/>
+      <c r="O33" s="132"/>
+      <c r="P33" s="132"/>
+    </row>
+    <row r="34" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="159" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="140"/>
+      <c r="D34" s="131"/>
+      <c r="E34" s="131"/>
+      <c r="F34" s="141"/>
+      <c r="G34" s="140"/>
+      <c r="H34" s="131"/>
+      <c r="I34" s="131"/>
+      <c r="J34" s="141"/>
+      <c r="K34" s="140"/>
+      <c r="L34" s="131"/>
+      <c r="M34" s="131"/>
+      <c r="N34" s="131"/>
+      <c r="O34" s="141"/>
+      <c r="P34" s="141"/>
+    </row>
+    <row r="35" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="159" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="58"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="58"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="59"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="58"/>
+      <c r="L35" s="59"/>
+      <c r="M35" s="59"/>
+      <c r="N35" s="59"/>
+      <c r="O35" s="60"/>
+      <c r="P35" s="60"/>
+    </row>
+    <row r="36" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="143" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="164"/>
+      <c r="D36" s="165"/>
+      <c r="E36" s="165"/>
+      <c r="F36" s="165"/>
+      <c r="G36" s="164"/>
+      <c r="H36" s="165"/>
+      <c r="I36" s="165"/>
+      <c r="J36" s="166"/>
+      <c r="K36" s="164"/>
+      <c r="L36" s="165"/>
+      <c r="M36" s="165"/>
+      <c r="N36" s="165"/>
+      <c r="O36" s="166"/>
+      <c r="P36" s="167"/>
+    </row>
+    <row r="38" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="49"/>
+      <c r="C38" s="173"/>
+      <c r="D38" s="174"/>
+      <c r="E38" s="174"/>
+      <c r="F38" s="174"/>
+      <c r="G38" s="175"/>
+      <c r="H38" s="174"/>
+      <c r="I38" s="174"/>
+      <c r="J38" s="174"/>
+      <c r="K38" s="174"/>
+      <c r="L38" s="175"/>
+      <c r="M38" s="173"/>
+      <c r="N38" s="174"/>
+      <c r="O38" s="174"/>
+      <c r="P38" s="175"/>
+      <c r="Q38" s="29"/>
+    </row>
+    <row r="39" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="61"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="52"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="52"/>
+      <c r="N39" s="52"/>
+      <c r="O39" s="52"/>
+      <c r="P39" s="52"/>
+      <c r="Q39" s="57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="158" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="135"/>
+      <c r="D40" s="136"/>
+      <c r="E40" s="136"/>
+      <c r="F40" s="136"/>
+      <c r="G40" s="56"/>
+      <c r="H40" s="135"/>
+      <c r="I40" s="136"/>
+      <c r="J40" s="136"/>
+      <c r="K40" s="136"/>
+      <c r="L40" s="56"/>
+      <c r="M40" s="135"/>
+      <c r="N40" s="136"/>
+      <c r="O40" s="136"/>
+      <c r="P40" s="56"/>
+      <c r="Q40" s="139" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="159" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="138"/>
+      <c r="D41" s="130"/>
+      <c r="E41" s="130"/>
+      <c r="F41" s="130"/>
+      <c r="G41" s="133"/>
+      <c r="H41" s="138"/>
+      <c r="I41" s="130"/>
+      <c r="J41" s="130"/>
+      <c r="K41" s="130"/>
+      <c r="L41" s="133"/>
+      <c r="M41" s="138"/>
+      <c r="N41" s="130"/>
+      <c r="O41" s="130"/>
+      <c r="P41" s="133"/>
+      <c r="Q41" s="133"/>
+    </row>
+    <row r="42" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="159" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="137"/>
+      <c r="D42" s="129"/>
+      <c r="E42" s="129"/>
+      <c r="F42" s="129"/>
+      <c r="G42" s="132"/>
+      <c r="H42" s="137"/>
+      <c r="I42" s="129"/>
+      <c r="J42" s="129"/>
+      <c r="K42" s="129"/>
+      <c r="L42" s="132"/>
+      <c r="M42" s="137"/>
+      <c r="N42" s="129"/>
+      <c r="O42" s="129"/>
+      <c r="P42" s="132"/>
+      <c r="Q42" s="132"/>
+    </row>
+    <row r="43" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="159" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="140"/>
+      <c r="D43" s="131"/>
+      <c r="E43" s="131"/>
+      <c r="F43" s="131"/>
+      <c r="G43" s="141"/>
+      <c r="H43" s="140"/>
+      <c r="I43" s="131"/>
+      <c r="J43" s="131"/>
+      <c r="K43" s="131"/>
+      <c r="L43" s="141"/>
+      <c r="M43" s="140"/>
+      <c r="N43" s="131"/>
+      <c r="O43" s="131"/>
+      <c r="P43" s="141"/>
+      <c r="Q43" s="141"/>
+    </row>
+    <row r="44" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="159" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="58"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="60"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
+      <c r="K44" s="59"/>
+      <c r="L44" s="60"/>
+      <c r="M44" s="58"/>
+      <c r="N44" s="59"/>
+      <c r="O44" s="59"/>
+      <c r="P44" s="60"/>
+      <c r="Q44" s="60"/>
+    </row>
+    <row r="45" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="143" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="164"/>
+      <c r="D45" s="165"/>
+      <c r="E45" s="165"/>
+      <c r="F45" s="165"/>
+      <c r="G45" s="165"/>
+      <c r="H45" s="164"/>
+      <c r="I45" s="165"/>
+      <c r="J45" s="165"/>
+      <c r="K45" s="165"/>
+      <c r="L45" s="166"/>
+      <c r="M45" s="164"/>
+      <c r="N45" s="165"/>
+      <c r="O45" s="165"/>
+      <c r="P45" s="166"/>
+      <c r="Q45" s="167"/>
+    </row>
+    <row r="47" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="49"/>
+      <c r="C47" s="173"/>
+      <c r="D47" s="174"/>
+      <c r="E47" s="174"/>
+      <c r="F47" s="174"/>
+      <c r="G47" s="175"/>
+      <c r="H47" s="174"/>
+      <c r="I47" s="174"/>
+      <c r="J47" s="174"/>
+      <c r="K47" s="175"/>
+      <c r="L47" s="173"/>
+      <c r="M47" s="174"/>
+      <c r="N47" s="174"/>
+      <c r="O47" s="174"/>
+      <c r="P47" s="175"/>
+      <c r="Q47" s="29"/>
+    </row>
+    <row r="48" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="61"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="53"/>
+      <c r="H48" s="52"/>
+      <c r="I48" s="52"/>
+      <c r="J48" s="52"/>
+      <c r="K48" s="53"/>
+      <c r="L48" s="52"/>
+      <c r="M48" s="52"/>
+      <c r="N48" s="52"/>
+      <c r="O48" s="52"/>
+      <c r="P48" s="52"/>
+      <c r="Q48" s="57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="158" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="135"/>
+      <c r="D49" s="136"/>
+      <c r="E49" s="136"/>
+      <c r="F49" s="136"/>
+      <c r="G49" s="56"/>
+      <c r="H49" s="135"/>
+      <c r="I49" s="136"/>
+      <c r="J49" s="136"/>
+      <c r="K49" s="56"/>
+      <c r="L49" s="135"/>
+      <c r="M49" s="136"/>
+      <c r="N49" s="136"/>
+      <c r="O49" s="136"/>
+      <c r="P49" s="56"/>
+      <c r="Q49" s="139" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="159" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="138"/>
+      <c r="D50" s="130"/>
+      <c r="E50" s="130"/>
+      <c r="F50" s="130"/>
+      <c r="G50" s="133"/>
+      <c r="H50" s="138"/>
+      <c r="I50" s="130"/>
+      <c r="J50" s="130"/>
+      <c r="K50" s="133"/>
+      <c r="L50" s="138"/>
+      <c r="M50" s="130"/>
+      <c r="N50" s="130"/>
+      <c r="O50" s="130"/>
+      <c r="P50" s="133"/>
+      <c r="Q50" s="133"/>
+    </row>
+    <row r="51" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="159" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="137"/>
+      <c r="D51" s="129"/>
+      <c r="E51" s="129"/>
+      <c r="F51" s="129"/>
+      <c r="G51" s="132"/>
+      <c r="H51" s="137"/>
+      <c r="I51" s="129"/>
+      <c r="J51" s="129"/>
+      <c r="K51" s="132"/>
+      <c r="L51" s="137"/>
+      <c r="M51" s="129"/>
+      <c r="N51" s="129"/>
+      <c r="O51" s="129"/>
+      <c r="P51" s="132"/>
+      <c r="Q51" s="132"/>
+    </row>
+    <row r="52" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="159" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="140"/>
+      <c r="D52" s="131"/>
+      <c r="E52" s="131"/>
+      <c r="F52" s="131"/>
+      <c r="G52" s="141"/>
+      <c r="H52" s="140"/>
+      <c r="I52" s="131"/>
+      <c r="J52" s="131"/>
+      <c r="K52" s="141"/>
+      <c r="L52" s="140"/>
+      <c r="M52" s="131"/>
+      <c r="N52" s="131"/>
+      <c r="O52" s="131"/>
+      <c r="P52" s="141"/>
+      <c r="Q52" s="141"/>
+    </row>
+    <row r="53" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="159" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" s="58"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="59"/>
+      <c r="G53" s="60"/>
+      <c r="H53" s="58"/>
+      <c r="I53" s="59"/>
+      <c r="J53" s="59"/>
+      <c r="K53" s="60"/>
+      <c r="L53" s="58"/>
+      <c r="M53" s="59"/>
+      <c r="N53" s="59"/>
+      <c r="O53" s="59"/>
+      <c r="P53" s="60"/>
+      <c r="Q53" s="60"/>
+    </row>
+    <row r="54" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="143" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="164"/>
+      <c r="D54" s="165"/>
+      <c r="E54" s="165"/>
+      <c r="F54" s="165"/>
+      <c r="G54" s="165"/>
+      <c r="H54" s="164"/>
+      <c r="I54" s="165"/>
+      <c r="J54" s="165"/>
+      <c r="K54" s="166"/>
+      <c r="L54" s="164"/>
+      <c r="M54" s="165"/>
+      <c r="N54" s="165"/>
+      <c r="O54" s="165"/>
+      <c r="P54" s="166"/>
+      <c r="Q54" s="167"/>
+    </row>
+    <row r="56" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="49"/>
+      <c r="C56" s="173"/>
+      <c r="D56" s="174"/>
+      <c r="E56" s="174"/>
+      <c r="F56" s="175"/>
+      <c r="G56" s="174"/>
+      <c r="H56" s="174"/>
+      <c r="I56" s="174"/>
+      <c r="J56" s="174"/>
+      <c r="K56" s="175"/>
+      <c r="L56" s="173"/>
+      <c r="M56" s="174"/>
+      <c r="N56" s="174"/>
+      <c r="O56" s="174"/>
+      <c r="P56" s="175"/>
+      <c r="Q56" s="29"/>
+    </row>
+    <row r="57" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="61"/>
+      <c r="C57" s="52"/>
+      <c r="D57" s="52"/>
+      <c r="E57" s="52"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="52"/>
+      <c r="H57" s="52"/>
+      <c r="I57" s="52"/>
+      <c r="J57" s="52"/>
+      <c r="K57" s="53"/>
+      <c r="L57" s="52"/>
+      <c r="M57" s="52"/>
+      <c r="N57" s="52"/>
+      <c r="O57" s="52"/>
+      <c r="P57" s="52"/>
+      <c r="Q57" s="57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="158" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="135"/>
+      <c r="D58" s="136"/>
+      <c r="E58" s="136"/>
+      <c r="F58" s="56"/>
+      <c r="G58" s="135"/>
+      <c r="H58" s="136"/>
+      <c r="I58" s="136"/>
+      <c r="J58" s="136"/>
+      <c r="K58" s="56"/>
+      <c r="L58" s="135"/>
+      <c r="M58" s="136"/>
+      <c r="N58" s="136"/>
+      <c r="O58" s="136"/>
+      <c r="P58" s="56"/>
+      <c r="Q58" s="139" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="159" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="138"/>
+      <c r="D59" s="130"/>
+      <c r="E59" s="130"/>
+      <c r="F59" s="133"/>
+      <c r="G59" s="138"/>
+      <c r="H59" s="130"/>
+      <c r="I59" s="130"/>
+      <c r="J59" s="130"/>
+      <c r="K59" s="133"/>
+      <c r="L59" s="138"/>
+      <c r="M59" s="130"/>
+      <c r="N59" s="130"/>
+      <c r="O59" s="130"/>
+      <c r="P59" s="133"/>
+      <c r="Q59" s="133"/>
+    </row>
+    <row r="60" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="159" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" s="137"/>
+      <c r="D60" s="129"/>
+      <c r="E60" s="129"/>
+      <c r="F60" s="132"/>
+      <c r="G60" s="137"/>
+      <c r="H60" s="129"/>
+      <c r="I60" s="129"/>
+      <c r="J60" s="129"/>
+      <c r="K60" s="132"/>
+      <c r="L60" s="137"/>
+      <c r="M60" s="129"/>
+      <c r="N60" s="129"/>
+      <c r="O60" s="129"/>
+      <c r="P60" s="132"/>
+      <c r="Q60" s="132"/>
+    </row>
+    <row r="61" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="159" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61" s="140"/>
+      <c r="D61" s="131"/>
+      <c r="E61" s="131"/>
+      <c r="F61" s="141"/>
+      <c r="G61" s="140"/>
+      <c r="H61" s="131"/>
+      <c r="I61" s="131"/>
+      <c r="J61" s="131"/>
+      <c r="K61" s="141"/>
+      <c r="L61" s="140"/>
+      <c r="M61" s="131"/>
+      <c r="N61" s="131"/>
+      <c r="O61" s="131"/>
+      <c r="P61" s="141"/>
+      <c r="Q61" s="141"/>
+    </row>
+    <row r="62" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="159" t="s">
+        <v>54</v>
+      </c>
+      <c r="C62" s="58"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="59"/>
+      <c r="F62" s="60"/>
+      <c r="G62" s="58"/>
+      <c r="H62" s="59"/>
+      <c r="I62" s="59"/>
+      <c r="J62" s="59"/>
+      <c r="K62" s="60"/>
+      <c r="L62" s="58"/>
+      <c r="M62" s="59"/>
+      <c r="N62" s="59"/>
+      <c r="O62" s="59"/>
+      <c r="P62" s="60"/>
+      <c r="Q62" s="60"/>
+    </row>
+    <row r="63" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="143" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" s="164"/>
+      <c r="D63" s="165"/>
+      <c r="E63" s="165"/>
+      <c r="F63" s="165"/>
+      <c r="G63" s="164"/>
+      <c r="H63" s="165"/>
+      <c r="I63" s="165"/>
+      <c r="J63" s="165"/>
+      <c r="K63" s="166"/>
+      <c r="L63" s="164"/>
+      <c r="M63" s="165"/>
+      <c r="N63" s="165"/>
+      <c r="O63" s="165"/>
+      <c r="P63" s="166"/>
+      <c r="Q63" s="167"/>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="C56:F56"/>
+    <mergeCell ref="G56:K56"/>
+    <mergeCell ref="L56:P56"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="H38:L38"/>
+    <mergeCell ref="M38:P38"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="H47:K47"/>
+    <mergeCell ref="L47:P47"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:O29"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:O11"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" sqref="C9:N9 C36:O36 C18:O18 C27:O27 C45:P45 C54:P54 C63:P63" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
+  </dataValidations>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="49" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6974,18 +7933,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7008,6 +7967,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -7022,12 +7989,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged PR 7532: PRI-22079 Export Campaign to Excel - All Tabs - Update text patterns in Content Restrictions
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{77FFFB5B-80E2-47F3-B61E-E13D6193EABF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0E86CE11-C4D9-4E83-B7C2-7ED090BED2E2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="27360" windowHeight="15240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Proposal (By Plan)" sheetId="1" state="hidden" r:id="rId4"/>
     <sheet name="Terms &amp; Conditions" sheetId="7" r:id="rId5"/>
     <sheet name="Proposal" sheetId="5" r:id="rId6"/>
-    <sheet name="Flow Chart template tables" sheetId="9" r:id="rId7"/>
+    <sheet name="Flow Chart Template Tables" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -5642,6 +5642,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5651,11 +5656,6 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -6470,6 +6470,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F28:U28"/>
+    <mergeCell ref="F20:U20"/>
+    <mergeCell ref="H13:N13"/>
+    <mergeCell ref="O7:U7"/>
+    <mergeCell ref="F22:U22"/>
+    <mergeCell ref="F24:U24"/>
+    <mergeCell ref="F26:U26"/>
+    <mergeCell ref="O13:U13"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:T5"/>
     <mergeCell ref="E5:G5"/>
@@ -6478,14 +6486,6 @@
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
-    <mergeCell ref="F28:U28"/>
-    <mergeCell ref="F20:U20"/>
-    <mergeCell ref="H13:N13"/>
-    <mergeCell ref="O7:U7"/>
-    <mergeCell ref="F22:U22"/>
-    <mergeCell ref="F24:U24"/>
-    <mergeCell ref="F26:U26"/>
-    <mergeCell ref="O13:U13"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:U3 C5 C4:O4 Q4 S4:U4 U5 C6:U10 O14:U17 H15:N15 C20:U28">
     <cfRule type="expression" dxfId="15" priority="76">
@@ -7679,6 +7679,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:O29"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="G56:K56"/>
     <mergeCell ref="L56:P56"/>
@@ -7688,18 +7700,6 @@
     <mergeCell ref="C47:G47"/>
     <mergeCell ref="H47:K47"/>
     <mergeCell ref="L47:P47"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="K29:O29"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:O11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="C9:N9 C36:O36 C18:O18 C27:O27 C45:P45 C54:P54 C63:P63" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
@@ -7710,6 +7710,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7932,15 +7941,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7948,6 +7948,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7962,14 +7970,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Merged PR 7550: Backmerge
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0E86CE11-C4D9-4E83-B7C2-7ED090BED2E2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{95FF1907-A241-4455-BD7A-9BC1FC65151D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="27360" windowHeight="15240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="90">
   <si>
     <t>Broadcast Proposal Gorilla Glue Q4 '19 - Q1 '20</t>
   </si>
@@ -194,9 +194,6 @@
 Rates quoted above based on multi-quarter commitment.
 Commercially reasonable efforts to hold the rates for the inventory for 10 business days from the proposal date noted above.
 Rates and inventory are subject to change and availability at time of order.</t>
-  </si>
-  <si>
-    <t>Imp.</t>
   </si>
   <si>
     <t>Cost</t>
@@ -2485,7 +2482,7 @@
         <v>7</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>14</v>
@@ -2569,28 +2566,28 @@
     </row>
     <row r="8" spans="3:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="73" t="s">
         <v>58</v>
-      </c>
-      <c r="D8" s="73" t="s">
-        <v>59</v>
       </c>
       <c r="E8" s="73" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G8" s="73" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H8" s="73" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="78" t="s">
         <v>61</v>
-      </c>
-      <c r="J8" s="78" t="s">
-        <v>62</v>
       </c>
       <c r="K8" s="74" t="s">
         <v>26</v>
@@ -2634,7 +2631,7 @@
     </row>
     <row r="12" spans="3:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I12" s="54"/>
     </row>
@@ -2643,11 +2640,11 @@
         <v>19</v>
       </c>
       <c r="D13" s="87" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" s="87"/>
       <c r="F13" s="87" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G13" s="87"/>
       <c r="H13" s="87" t="s">
@@ -2693,13 +2690,13 @@
     </row>
     <row r="16" spans="3:20" s="105" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="99" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" s="95"/>
       <c r="E16" s="95"/>
       <c r="F16" s="98"/>
       <c r="G16" s="100" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H16" s="95"/>
       <c r="I16" s="101"/>
@@ -2985,7 +2982,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>36</v>
@@ -3141,7 +3138,7 @@
         <v>10</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>9</v>
@@ -3174,7 +3171,7 @@
     </row>
     <row r="7" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -3435,7 +3432,7 @@
     </row>
     <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -5642,11 +5639,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5656,6 +5648,11 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5689,97 +5686,97 @@
     <row r="1" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:4" s="104" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="179" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="179"/>
     </row>
     <row r="5" spans="3:4" s="104" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="179" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="179"/>
     </row>
     <row r="6" spans="3:4" s="104" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="179" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="179"/>
     </row>
     <row r="7" spans="3:4" s="104" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="179" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="179"/>
     </row>
     <row r="8" spans="3:4" s="104" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="179" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="179"/>
     </row>
     <row r="9" spans="3:4" s="104" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="179" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="179"/>
     </row>
     <row r="10" spans="3:4" s="104" customFormat="1" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="179" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D10" s="179"/>
     </row>
     <row r="11" spans="3:4" s="104" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="179" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="179"/>
     </row>
     <row r="12" spans="3:4" s="104" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="179" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" s="179"/>
     </row>
     <row r="13" spans="3:4" s="104" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="179" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="179"/>
     </row>
     <row r="14" spans="3:4" s="104" customFormat="1" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="179" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" s="179"/>
     </row>
     <row r="15" spans="3:4" s="104" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="179" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D15" s="179"/>
     </row>
     <row r="16" spans="3:4" s="104" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="179" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" s="179"/>
     </row>
     <row r="17" spans="3:4" s="104" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="179" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" s="179"/>
     </row>
     <row r="18" spans="3:4" s="104" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="179" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D18" s="179"/>
     </row>
@@ -5840,10 +5837,10 @@
     <row r="2" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5864,7 +5861,7 @@
         <v>7</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>14</v>
@@ -5936,14 +5933,14 @@
     </row>
     <row r="8" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="85" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="35" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="36" t="s">
         <v>19</v>
@@ -6021,7 +6018,7 @@
       <c r="B10" s="24"/>
       <c r="C10" s="35"/>
       <c r="D10" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10" s="47"/>
       <c r="F10" s="38" t="s">
@@ -6083,7 +6080,7 @@
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12" s="115" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="103" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6470,6 +6467,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
     <mergeCell ref="F28:U28"/>
     <mergeCell ref="F20:U20"/>
     <mergeCell ref="H13:N13"/>
@@ -6478,14 +6483,6 @@
     <mergeCell ref="F24:U24"/>
     <mergeCell ref="F26:U26"/>
     <mergeCell ref="O13:U13"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:U3 C5 C4:O4 Q4 S4:U4 U5 C6:U10 O14:U17 H15:N15 C20:U28">
     <cfRule type="expression" dxfId="15" priority="76">
@@ -6580,7 +6577,9 @@
   </sheetPr>
   <dimension ref="B1:Q63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6633,7 +6632,7 @@
     </row>
     <row r="4" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="158" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="135"/>
       <c r="D4" s="136"/>
@@ -6671,7 +6670,7 @@
     </row>
     <row r="6" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="159" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="C6" s="137"/>
       <c r="D6" s="129"/>
@@ -6707,7 +6706,7 @@
     </row>
     <row r="8" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="159" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="58"/>
       <c r="D8" s="59"/>
@@ -6725,7 +6724,7 @@
     </row>
     <row r="9" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="143" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="164"/>
       <c r="D9" s="165"/>
@@ -6779,7 +6778,7 @@
     </row>
     <row r="13" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="158" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="135"/>
       <c r="D13" s="136"/>
@@ -6819,7 +6818,7 @@
     </row>
     <row r="15" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="159" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="C15" s="137"/>
       <c r="D15" s="129"/>
@@ -6857,7 +6856,7 @@
     </row>
     <row r="17" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="159" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="58"/>
       <c r="D17" s="59"/>
@@ -6876,7 +6875,7 @@
     </row>
     <row r="18" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="143" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" s="164"/>
       <c r="D18" s="165"/>
@@ -6931,7 +6930,7 @@
     </row>
     <row r="22" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="158" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="135"/>
       <c r="D22" s="136"/>
@@ -6971,7 +6970,7 @@
     </row>
     <row r="24" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="159" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="C24" s="137"/>
       <c r="D24" s="129"/>
@@ -7009,7 +7008,7 @@
     </row>
     <row r="26" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="159" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="58"/>
       <c r="D26" s="59"/>
@@ -7028,7 +7027,7 @@
     </row>
     <row r="27" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="143" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" s="164"/>
       <c r="D27" s="165"/>
@@ -7083,7 +7082,7 @@
     </row>
     <row r="31" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="158" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" s="135"/>
       <c r="D31" s="136"/>
@@ -7123,7 +7122,7 @@
     </row>
     <row r="33" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="159" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="C33" s="137"/>
       <c r="D33" s="129"/>
@@ -7161,7 +7160,7 @@
     </row>
     <row r="35" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="159" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" s="58"/>
       <c r="D35" s="59"/>
@@ -7180,7 +7179,7 @@
     </row>
     <row r="36" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="143" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" s="164"/>
       <c r="D36" s="165"/>
@@ -7237,7 +7236,7 @@
     </row>
     <row r="40" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="158" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C40" s="135"/>
       <c r="D40" s="136"/>
@@ -7279,7 +7278,7 @@
     </row>
     <row r="42" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="159" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="C42" s="137"/>
       <c r="D42" s="129"/>
@@ -7319,7 +7318,7 @@
     </row>
     <row r="44" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="159" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C44" s="58"/>
       <c r="D44" s="59"/>
@@ -7339,7 +7338,7 @@
     </row>
     <row r="45" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="143" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C45" s="164"/>
       <c r="D45" s="165"/>
@@ -7397,7 +7396,7 @@
     </row>
     <row r="49" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="158" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" s="135"/>
       <c r="D49" s="136"/>
@@ -7439,7 +7438,7 @@
     </row>
     <row r="51" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="159" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="C51" s="137"/>
       <c r="D51" s="129"/>
@@ -7479,7 +7478,7 @@
     </row>
     <row r="53" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="159" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C53" s="58"/>
       <c r="D53" s="59"/>
@@ -7499,7 +7498,7 @@
     </row>
     <row r="54" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="143" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C54" s="164"/>
       <c r="D54" s="165"/>
@@ -7557,7 +7556,7 @@
     </row>
     <row r="58" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="158" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C58" s="135"/>
       <c r="D58" s="136"/>
@@ -7599,7 +7598,7 @@
     </row>
     <row r="60" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="159" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="C60" s="137"/>
       <c r="D60" s="129"/>
@@ -7639,7 +7638,7 @@
     </row>
     <row r="62" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="159" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C62" s="58"/>
       <c r="D62" s="59"/>
@@ -7659,7 +7658,7 @@
     </row>
     <row r="63" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="143" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C63" s="164"/>
       <c r="D63" s="165"/>
@@ -7679,18 +7678,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="K29:O29"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="G56:K56"/>
     <mergeCell ref="L56:P56"/>
@@ -7700,6 +7687,18 @@
     <mergeCell ref="C47:G47"/>
     <mergeCell ref="H47:K47"/>
     <mergeCell ref="L47:P47"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:O29"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:O11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="C9:N9 C36:O36 C18:O18 C27:O27 C45:P45 C54:P54 C63:P63" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
@@ -7710,15 +7709,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7941,6 +7931,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7948,14 +7947,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7970,6 +7961,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Merged PR 7560: Backmerge
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{95FF1907-A241-4455-BD7A-9BC1FC65151D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D312C421-F63C-4CA8-95C5-97BA3F7CB93C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="27360" windowHeight="15240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5639,6 +5639,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5648,11 +5653,6 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -6467,6 +6467,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F28:U28"/>
+    <mergeCell ref="F20:U20"/>
+    <mergeCell ref="H13:N13"/>
+    <mergeCell ref="O7:U7"/>
+    <mergeCell ref="F22:U22"/>
+    <mergeCell ref="F24:U24"/>
+    <mergeCell ref="F26:U26"/>
+    <mergeCell ref="O13:U13"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:T5"/>
     <mergeCell ref="E5:G5"/>
@@ -6475,14 +6483,6 @@
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
-    <mergeCell ref="F28:U28"/>
-    <mergeCell ref="F20:U20"/>
-    <mergeCell ref="H13:N13"/>
-    <mergeCell ref="O7:U7"/>
-    <mergeCell ref="F22:U22"/>
-    <mergeCell ref="F24:U24"/>
-    <mergeCell ref="F26:U26"/>
-    <mergeCell ref="O13:U13"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:U3 C5 C4:O4 Q4 S4:U4 U5 C6:U10 O14:U17 H15:N15 C20:U28">
     <cfRule type="expression" dxfId="15" priority="76">
@@ -6577,8 +6577,8 @@
   </sheetPr>
   <dimension ref="B1:Q63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58:Q62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7678,6 +7678,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:O29"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="G56:K56"/>
     <mergeCell ref="L56:P56"/>
@@ -7687,18 +7699,6 @@
     <mergeCell ref="C47:G47"/>
     <mergeCell ref="H47:K47"/>
     <mergeCell ref="L47:P47"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="K29:O29"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:O11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="C9:N9 C36:O36 C18:O18 C27:O27 C45:P45 C54:P54 C63:P63" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
@@ -7709,6 +7709,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7931,15 +7940,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7947,6 +7947,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7961,14 +7969,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Merged PR 7567: Backmerged releases/2020.03 into develop
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D312C421-F63C-4CA8-95C5-97BA3F7CB93C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4FFE7DFA-B30C-4ED1-B48F-559D69B40A92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="27360" windowHeight="15240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="27360" windowHeight="15240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="90">
   <si>
     <t>Broadcast Proposal Gorilla Glue Q4 '19 - Q1 '20</t>
   </si>
@@ -2435,8 +2435,8 @@
   </sheetPr>
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2732,10 +2732,7 @@
       <c r="C18" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="171">
-        <f>Proposal!F20</f>
-        <v>0</v>
-      </c>
+      <c r="D18" s="171"/>
       <c r="E18" s="171"/>
       <c r="F18" s="171"/>
       <c r="G18" s="171"/>
@@ -2773,10 +2770,7 @@
       <c r="C20" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="171">
-        <f>Proposal!F22</f>
-        <v>0</v>
-      </c>
+      <c r="D20" s="171"/>
       <c r="E20" s="171"/>
       <c r="F20" s="171"/>
       <c r="G20" s="171"/>
@@ -2814,10 +2808,7 @@
       <c r="C22" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="171">
-        <f>Proposal!F24</f>
-        <v>0</v>
-      </c>
+      <c r="D22" s="171"/>
       <c r="E22" s="171"/>
       <c r="F22" s="171"/>
       <c r="G22" s="171"/>
@@ -2848,10 +2839,7 @@
       <c r="C24" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="171">
-        <f>Proposal!F26</f>
-        <v>0</v>
-      </c>
+      <c r="D24" s="171"/>
       <c r="E24" s="171"/>
       <c r="F24" s="171"/>
       <c r="G24" s="171"/>
@@ -2875,10 +2863,7 @@
       <c r="C26" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="170">
-        <f>Proposal!F28</f>
-        <v>0</v>
-      </c>
+      <c r="D26" s="170"/>
       <c r="E26" s="171"/>
       <c r="F26" s="171"/>
       <c r="G26" s="171"/>
@@ -2945,7 +2930,7 @@
   </sheetPr>
   <dimension ref="B1:P7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2972,8 +2957,9 @@
       </c>
       <c r="G2" s="4"/>
       <c r="K2" s="4"/>
-      <c r="P2" s="5" t="s">
-        <v>13</v>
+      <c r="P2" s="5" t="str">
+        <f>Proposal!U2</f>
+        <v xml:space="preserve">Created </v>
       </c>
     </row>
     <row r="3" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2997,10 +2983,7 @@
         <f>Proposal!O5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="168">
-        <f>Proposal!F22</f>
-        <v>0</v>
-      </c>
+      <c r="D5" s="168"/>
       <c r="E5" s="168"/>
       <c r="F5" s="168"/>
       <c r="G5" s="168"/>
@@ -6577,7 +6560,7 @@
   </sheetPr>
   <dimension ref="B1:Q63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A52" workbookViewId="0">
       <selection activeCell="C58" sqref="C58:Q62"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Merged PR 7625: PRI-22419 Proposal Tab - Secondary Audiences Template - Fix Formatting
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4FFE7DFA-B30C-4ED1-B48F-559D69B40A92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8500BB96-3032-4FCB-894F-DBD3E3405DBA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="27360" windowHeight="15240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="27360" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="4" r:id="rId1"/>
@@ -1683,98 +1683,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -1857,6 +1766,7 @@
   <colors>
     <mruColors>
       <color rgb="FFF5F8F8"/>
+      <color rgb="FFF8F5F5"/>
       <color rgb="FF3D5261"/>
       <color rgb="FFECF0F3"/>
       <color rgb="FFE5EAED"/>
@@ -2435,8 +2345,8 @@
   </sheetPr>
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:K20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2893,27 +2803,27 @@
     <mergeCell ref="D24:K24"/>
   </mergeCells>
   <conditionalFormatting sqref="L14:R22">
-    <cfRule type="expression" dxfId="23" priority="5">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>$A14="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:K19 C21:K21 C20:D20 C23:K23 C22 C25:K25 C24 C26 C18:D18">
-    <cfRule type="expression" dxfId="22" priority="4">
+    <cfRule type="expression" dxfId="9" priority="4">
       <formula>$A14="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="21" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>$A18="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$A20="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$A22="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2930,7 +2840,7 @@
   </sheetPr>
   <dimension ref="B1:P7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -3020,17 +2930,17 @@
     <mergeCell ref="D5:P5"/>
   </mergeCells>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$A4="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$A5="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$A2="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5622,11 +5532,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5636,6 +5541,11 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5800,7 +5710,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.125" style="85" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="5.75" style="85" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="3" style="85" customWidth="1"/>
     <col min="3" max="3" width="11.375" style="85" customWidth="1"/>
     <col min="4" max="4" width="9" style="85" customWidth="1"/>
@@ -6450,6 +6360,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
     <mergeCell ref="F28:U28"/>
     <mergeCell ref="F20:U20"/>
     <mergeCell ref="H13:N13"/>
@@ -6458,93 +6376,20 @@
     <mergeCell ref="F24:U24"/>
     <mergeCell ref="F26:U26"/>
     <mergeCell ref="O13:U13"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1:U3 C5 C4:O4 Q4 S4:U4 U5 C6:U10 O14:U17 H15:N15 C20:U28">
-    <cfRule type="expression" dxfId="15" priority="76">
+  <conditionalFormatting sqref="C1:U3 C5 C4:N4 P4 R4:U4 U5 C6:U1048576">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R4">
-    <cfRule type="expression" dxfId="14" priority="64">
-      <formula>$A4="Even"</formula>
+  <conditionalFormatting sqref="H1:N1048576">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$A1="EvenSA1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="13" priority="72">
-      <formula>$A5="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="12" priority="71">
-      <formula>$A5="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K5">
-    <cfRule type="expression" dxfId="11" priority="70">
-      <formula>$A5="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M5">
-    <cfRule type="expression" dxfId="10" priority="69">
-      <formula>$A5="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O5">
-    <cfRule type="expression" dxfId="9" priority="68">
-      <formula>$A5="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P4">
-    <cfRule type="expression" dxfId="8" priority="66">
-      <formula>$A4="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P5">
-    <cfRule type="expression" dxfId="7" priority="63">
-      <formula>$A5="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R5">
-    <cfRule type="expression" dxfId="6" priority="62">
-      <formula>$A5="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29:F1048576">
-    <cfRule type="expression" dxfId="5" priority="77">
-      <formula>$A41="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G29:U1048576">
-    <cfRule type="expression" dxfId="4" priority="81">
-      <formula>$A48="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H13:N13">
-    <cfRule type="expression" dxfId="3" priority="47">
-      <formula>$A13="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O13:U13">
-    <cfRule type="expression" dxfId="2" priority="50">
-      <formula>$A13="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H14:N14 H16:N17">
-    <cfRule type="expression" dxfId="1" priority="52">
-      <formula>$A14="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H12">
+  <conditionalFormatting sqref="H1:U1048576">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$A12="Even"</formula>
+      <formula>$A1="EvenSA2"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7661,18 +7506,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="K29:O29"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="G56:K56"/>
     <mergeCell ref="L56:P56"/>
@@ -7682,6 +7515,18 @@
     <mergeCell ref="C47:G47"/>
     <mergeCell ref="H47:K47"/>
     <mergeCell ref="L47:P47"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:O29"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:O11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="C9:N9 C36:O36 C18:O18 C27:O27 C45:P45 C54:P54 C63:P63" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
@@ -7692,15 +7537,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7923,6 +7759,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7930,14 +7775,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7952,6 +7789,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Merged PR 7629: PRI-21942  Add Flight Days to Daypart Sorting
PRI-21942  Implementation and tests
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8500BB96-3032-4FCB-894F-DBD3E3405DBA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A34D29D1-3AC8-4B30-B911-AC22546302CC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="27360" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -227,9 +227,6 @@
   </si>
   <si>
     <t>Cadent:</t>
-  </si>
-  <si>
-    <t>Reciept Acknowledged:</t>
   </si>
   <si>
     <t>:15 equiv., :30</t>
@@ -669,6 +666,9 @@
   </si>
   <si>
     <t xml:space="preserve">Broadcast Proposal </t>
+  </si>
+  <si>
+    <t>Receipt Acknowledged:</t>
   </si>
 </sst>
 </file>
@@ -2392,7 +2392,7 @@
         <v>7</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>14</v>
@@ -2606,7 +2606,7 @@
       <c r="E16" s="95"/>
       <c r="F16" s="98"/>
       <c r="G16" s="100" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="H16" s="95"/>
       <c r="I16" s="101"/>
@@ -2878,7 +2878,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>36</v>
@@ -3031,7 +3031,7 @@
         <v>10</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>9</v>
@@ -5532,6 +5532,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5541,11 +5546,6 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5579,97 +5579,97 @@
     <row r="1" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:4" s="104" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="179" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" s="179"/>
     </row>
     <row r="5" spans="3:4" s="104" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="179" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="179"/>
     </row>
     <row r="6" spans="3:4" s="104" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="179" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="179"/>
     </row>
     <row r="7" spans="3:4" s="104" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="179" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="179"/>
     </row>
     <row r="8" spans="3:4" s="104" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="179" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="179"/>
     </row>
     <row r="9" spans="3:4" s="104" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="179" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" s="179"/>
     </row>
     <row r="10" spans="3:4" s="104" customFormat="1" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="179" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" s="179"/>
     </row>
     <row r="11" spans="3:4" s="104" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="179" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="179"/>
     </row>
     <row r="12" spans="3:4" s="104" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="179" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="179"/>
     </row>
     <row r="13" spans="3:4" s="104" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="179" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" s="179"/>
     </row>
     <row r="14" spans="3:4" s="104" customFormat="1" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="179" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="179"/>
     </row>
     <row r="15" spans="3:4" s="104" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="179" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D15" s="179"/>
     </row>
     <row r="16" spans="3:4" s="104" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="179" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" s="179"/>
     </row>
     <row r="17" spans="3:4" s="104" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="179" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D17" s="179"/>
     </row>
     <row r="18" spans="3:4" s="104" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="179" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" s="179"/>
     </row>
@@ -5730,10 +5730,10 @@
     <row r="2" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5754,7 +5754,7 @@
         <v>7</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>14</v>
@@ -5826,14 +5826,14 @@
     </row>
     <row r="8" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="85" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="24"/>
       <c r="C8" s="35" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8" s="36" t="s">
         <v>19</v>
@@ -5911,7 +5911,7 @@
       <c r="B10" s="24"/>
       <c r="C10" s="35"/>
       <c r="D10" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="47"/>
       <c r="F10" s="38" t="s">
@@ -5973,7 +5973,7 @@
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12" s="115" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="103" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6360,6 +6360,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F28:U28"/>
+    <mergeCell ref="F20:U20"/>
+    <mergeCell ref="H13:N13"/>
+    <mergeCell ref="O7:U7"/>
+    <mergeCell ref="F22:U22"/>
+    <mergeCell ref="F24:U24"/>
+    <mergeCell ref="F26:U26"/>
+    <mergeCell ref="O13:U13"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:T5"/>
     <mergeCell ref="E5:G5"/>
@@ -6368,14 +6376,6 @@
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
-    <mergeCell ref="F28:U28"/>
-    <mergeCell ref="F20:U20"/>
-    <mergeCell ref="H13:N13"/>
-    <mergeCell ref="O7:U7"/>
-    <mergeCell ref="F22:U22"/>
-    <mergeCell ref="F24:U24"/>
-    <mergeCell ref="F26:U26"/>
-    <mergeCell ref="O13:U13"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:U3 C5 C4:N4 P4 R4:U4 U5 C6:U1048576">
     <cfRule type="expression" dxfId="2" priority="3">
@@ -6552,7 +6552,7 @@
     </row>
     <row r="9" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="143" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="164"/>
       <c r="D9" s="165"/>
@@ -6703,7 +6703,7 @@
     </row>
     <row r="18" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="143" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" s="164"/>
       <c r="D18" s="165"/>
@@ -6855,7 +6855,7 @@
     </row>
     <row r="27" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="143" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27" s="164"/>
       <c r="D27" s="165"/>
@@ -7007,7 +7007,7 @@
     </row>
     <row r="36" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="143" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C36" s="164"/>
       <c r="D36" s="165"/>
@@ -7166,7 +7166,7 @@
     </row>
     <row r="45" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="143" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C45" s="164"/>
       <c r="D45" s="165"/>
@@ -7326,7 +7326,7 @@
     </row>
     <row r="54" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="143" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C54" s="164"/>
       <c r="D54" s="165"/>
@@ -7486,7 +7486,7 @@
     </row>
     <row r="63" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="143" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C63" s="164"/>
       <c r="D63" s="165"/>
@@ -7506,6 +7506,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:O29"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="G56:K56"/>
     <mergeCell ref="L56:P56"/>
@@ -7515,18 +7527,6 @@
     <mergeCell ref="C47:G47"/>
     <mergeCell ref="H47:K47"/>
     <mergeCell ref="L47:P47"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="K29:O29"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:O11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="C9:N9 C36:O36 C18:O18 C27:O27 C45:P45 C54:P54 C63:P63" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
@@ -7537,6 +7537,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7759,15 +7768,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7775,6 +7775,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7789,14 +7797,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Merged PR 8125: Backmerged releases/2020.04 into develop
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A34D29D1-3AC8-4B30-B911-AC22546302CC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{218018CF-6366-42FE-BA2A-5D89B5843371}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="27360" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1144,7 +1144,7 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1675,6 +1675,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5532,11 +5535,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5546,6 +5544,11 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -6360,6 +6363,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
     <mergeCell ref="F28:U28"/>
     <mergeCell ref="F20:U20"/>
     <mergeCell ref="H13:N13"/>
@@ -6368,14 +6379,6 @@
     <mergeCell ref="F24:U24"/>
     <mergeCell ref="F26:U26"/>
     <mergeCell ref="O13:U13"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:U3 C5 C4:N4 P4 R4:U4 U5 C6:U1048576">
     <cfRule type="expression" dxfId="2" priority="3">
@@ -6405,8 +6408,8 @@
   </sheetPr>
   <dimension ref="B1:Q63"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58:Q62"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" activeCellId="6" sqref="B56 B47 B38 B29 B20 B11 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6425,7 +6428,7 @@
   <sheetData>
     <row r="1" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="49"/>
+      <c r="B2" s="181"/>
       <c r="C2" s="173"/>
       <c r="D2" s="174"/>
       <c r="E2" s="174"/>
@@ -6569,7 +6572,7 @@
       <c r="O9" s="167"/>
     </row>
     <row r="11" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="49"/>
+      <c r="B11" s="181"/>
       <c r="C11" s="173"/>
       <c r="D11" s="174"/>
       <c r="E11" s="174"/>
@@ -6721,7 +6724,7 @@
       <c r="P18" s="167"/>
     </row>
     <row r="20" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="49"/>
+      <c r="B20" s="181"/>
       <c r="C20" s="173"/>
       <c r="D20" s="174"/>
       <c r="E20" s="174"/>
@@ -6873,7 +6876,7 @@
       <c r="P27" s="167"/>
     </row>
     <row r="29" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="49"/>
+      <c r="B29" s="181"/>
       <c r="C29" s="173"/>
       <c r="D29" s="174"/>
       <c r="E29" s="174"/>
@@ -7025,7 +7028,7 @@
       <c r="P36" s="167"/>
     </row>
     <row r="38" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="49"/>
+      <c r="B38" s="181"/>
       <c r="C38" s="173"/>
       <c r="D38" s="174"/>
       <c r="E38" s="174"/>
@@ -7185,7 +7188,7 @@
       <c r="Q45" s="167"/>
     </row>
     <row r="47" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="49"/>
+      <c r="B47" s="181"/>
       <c r="C47" s="173"/>
       <c r="D47" s="174"/>
       <c r="E47" s="174"/>
@@ -7345,7 +7348,7 @@
       <c r="Q54" s="167"/>
     </row>
     <row r="56" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="49"/>
+      <c r="B56" s="181"/>
       <c r="C56" s="173"/>
       <c r="D56" s="174"/>
       <c r="E56" s="174"/>
@@ -7506,18 +7509,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="K29:O29"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="G56:K56"/>
     <mergeCell ref="L56:P56"/>
@@ -7527,6 +7518,18 @@
     <mergeCell ref="C47:G47"/>
     <mergeCell ref="H47:K47"/>
     <mergeCell ref="L47:P47"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:O29"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:O11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="C9:N9 C36:O36 C18:O18 C27:O27 C45:P45 C54:P54 C63:P63" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
@@ -7537,15 +7540,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7768,6 +7762,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -7775,14 +7778,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7797,6 +7792,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Merged PR 9171: backmerge
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{218018CF-6366-42FE-BA2A-5D89B5843371}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B3122A62-23AF-46CF-8FA5-7F7F2A60E9A5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="27360" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1637,6 +1637,9 @@
     <xf numFmtId="1" fontId="12" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
@@ -1675,9 +1678,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1686,35 +1686,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF5F8F8"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -2416,11 +2388,11 @@
         <f>Proposal!E5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="168">
+      <c r="E5" s="169">
         <f>Proposal!I5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="168"/>
+      <c r="F5" s="169"/>
       <c r="G5" s="62">
         <f>Proposal!K5</f>
         <v>0</v>
@@ -2683,14 +2655,14 @@
       <c r="C20" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="171"/>
-      <c r="E20" s="171"/>
-      <c r="F20" s="171"/>
-      <c r="G20" s="171"/>
-      <c r="H20" s="171"/>
-      <c r="I20" s="171"/>
-      <c r="J20" s="171"/>
-      <c r="K20" s="171"/>
+      <c r="D20" s="172"/>
+      <c r="E20" s="172"/>
+      <c r="F20" s="172"/>
+      <c r="G20" s="172"/>
+      <c r="H20" s="172"/>
+      <c r="I20" s="172"/>
+      <c r="J20" s="172"/>
+      <c r="K20" s="172"/>
       <c r="L20" s="114"/>
       <c r="M20" s="114"/>
       <c r="N20" s="114"/>
@@ -2721,14 +2693,14 @@
       <c r="C22" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="171"/>
-      <c r="E22" s="171"/>
-      <c r="F22" s="171"/>
-      <c r="G22" s="171"/>
-      <c r="H22" s="171"/>
-      <c r="I22" s="171"/>
-      <c r="J22" s="171"/>
-      <c r="K22" s="171"/>
+      <c r="D22" s="172"/>
+      <c r="E22" s="172"/>
+      <c r="F22" s="172"/>
+      <c r="G22" s="172"/>
+      <c r="H22" s="172"/>
+      <c r="I22" s="172"/>
+      <c r="J22" s="172"/>
+      <c r="K22" s="172"/>
       <c r="L22" s="63"/>
       <c r="M22" s="63"/>
       <c r="N22" s="63"/>
@@ -2752,14 +2724,14 @@
       <c r="C24" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="171"/>
-      <c r="E24" s="171"/>
-      <c r="F24" s="171"/>
-      <c r="G24" s="171"/>
-      <c r="H24" s="171"/>
-      <c r="I24" s="171"/>
-      <c r="J24" s="171"/>
-      <c r="K24" s="171"/>
+      <c r="D24" s="172"/>
+      <c r="E24" s="172"/>
+      <c r="F24" s="172"/>
+      <c r="G24" s="172"/>
+      <c r="H24" s="172"/>
+      <c r="I24" s="172"/>
+      <c r="J24" s="172"/>
+      <c r="K24" s="172"/>
     </row>
     <row r="25" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
@@ -2776,24 +2748,24 @@
       <c r="C26" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="170"/>
-      <c r="E26" s="171"/>
-      <c r="F26" s="171"/>
-      <c r="G26" s="171"/>
-      <c r="H26" s="171"/>
-      <c r="I26" s="171"/>
-      <c r="J26" s="171"/>
-      <c r="K26" s="171"/>
+      <c r="D26" s="171"/>
+      <c r="E26" s="172"/>
+      <c r="F26" s="172"/>
+      <c r="G26" s="172"/>
+      <c r="H26" s="172"/>
+      <c r="I26" s="172"/>
+      <c r="J26" s="172"/>
+      <c r="K26" s="172"/>
     </row>
     <row r="27" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="169"/>
-      <c r="E27" s="169"/>
-      <c r="F27" s="169"/>
-      <c r="G27" s="169"/>
-      <c r="H27" s="169"/>
-      <c r="I27" s="169"/>
-      <c r="J27" s="169"/>
-      <c r="K27" s="169"/>
+      <c r="D27" s="170"/>
+      <c r="E27" s="170"/>
+      <c r="F27" s="170"/>
+      <c r="G27" s="170"/>
+      <c r="H27" s="170"/>
+      <c r="I27" s="170"/>
+      <c r="J27" s="170"/>
+      <c r="K27" s="170"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2805,29 +2777,9 @@
     <mergeCell ref="D22:K22"/>
     <mergeCell ref="D24:K24"/>
   </mergeCells>
-  <conditionalFormatting sqref="L14:R22">
-    <cfRule type="expression" dxfId="10" priority="5">
-      <formula>$A14="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C19:K19 C21:K21 C20:D20 C23:K23 C22 C25:K25 C24 C26 C18:D18">
-    <cfRule type="expression" dxfId="9" priority="4">
-      <formula>$A14="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="8" priority="3">
-      <formula>$A18="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
-    <cfRule type="expression" dxfId="7" priority="2">
-      <formula>$A20="Even"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="expression" dxfId="6" priority="1">
-      <formula>$A22="Even"</formula>
+  <conditionalFormatting sqref="C1:K1048576">
+    <cfRule type="expression" dxfId="6" priority="5">
+      <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2896,19 +2848,19 @@
         <f>Proposal!O5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="168"/>
-      <c r="E5" s="168"/>
-      <c r="F5" s="168"/>
-      <c r="G5" s="168"/>
-      <c r="H5" s="168"/>
-      <c r="I5" s="168"/>
-      <c r="J5" s="168"/>
-      <c r="K5" s="168"/>
-      <c r="L5" s="168"/>
-      <c r="M5" s="168"/>
-      <c r="N5" s="168"/>
-      <c r="O5" s="168"/>
-      <c r="P5" s="168"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="169"/>
+      <c r="H5" s="169"/>
+      <c r="I5" s="169"/>
+      <c r="J5" s="169"/>
+      <c r="K5" s="169"/>
+      <c r="L5" s="169"/>
+      <c r="M5" s="169"/>
+      <c r="N5" s="169"/>
+      <c r="O5" s="169"/>
+      <c r="P5" s="169"/>
     </row>
     <row r="6" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P6" s="54"/>
@@ -3073,24 +3025,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="176" t="s">
+      <c r="G7" s="177" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="176"/>
-      <c r="I7" s="176"/>
-      <c r="J7" s="176"/>
-      <c r="K7" s="176"/>
-      <c r="L7" s="177"/>
+      <c r="H7" s="177"/>
+      <c r="I7" s="177"/>
+      <c r="J7" s="177"/>
+      <c r="K7" s="177"/>
+      <c r="L7" s="178"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="176" t="s">
+      <c r="N7" s="177" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="176"/>
-      <c r="P7" s="176"/>
-      <c r="Q7" s="176"/>
-      <c r="R7" s="176"/>
-      <c r="S7" s="176"/>
-      <c r="T7" s="177"/>
+      <c r="O7" s="177"/>
+      <c r="P7" s="177"/>
+      <c r="Q7" s="177"/>
+      <c r="R7" s="177"/>
+      <c r="S7" s="177"/>
+      <c r="T7" s="178"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -3334,24 +3286,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="173" t="s">
+      <c r="G13" s="174" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="174"/>
-      <c r="I13" s="174"/>
-      <c r="J13" s="174"/>
-      <c r="K13" s="174"/>
-      <c r="L13" s="175"/>
+      <c r="H13" s="175"/>
+      <c r="I13" s="175"/>
+      <c r="J13" s="175"/>
+      <c r="K13" s="175"/>
+      <c r="L13" s="176"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="173" t="s">
+      <c r="N13" s="174" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="174"/>
-      <c r="P13" s="174"/>
-      <c r="Q13" s="174"/>
-      <c r="R13" s="174"/>
-      <c r="S13" s="174"/>
-      <c r="T13" s="175"/>
+      <c r="O13" s="175"/>
+      <c r="P13" s="175"/>
+      <c r="Q13" s="175"/>
+      <c r="R13" s="175"/>
+      <c r="S13" s="175"/>
+      <c r="T13" s="176"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="35" t="s">
@@ -3591,24 +3543,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="173" t="s">
+      <c r="G19" s="174" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174"/>
-      <c r="J19" s="174"/>
-      <c r="K19" s="174"/>
-      <c r="L19" s="175"/>
+      <c r="H19" s="175"/>
+      <c r="I19" s="175"/>
+      <c r="J19" s="175"/>
+      <c r="K19" s="175"/>
+      <c r="L19" s="176"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="173" t="s">
+      <c r="N19" s="174" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="174"/>
-      <c r="P19" s="174"/>
-      <c r="Q19" s="174"/>
-      <c r="R19" s="174"/>
-      <c r="S19" s="174"/>
-      <c r="T19" s="175"/>
+      <c r="O19" s="175"/>
+      <c r="P19" s="175"/>
+      <c r="Q19" s="175"/>
+      <c r="R19" s="175"/>
+      <c r="S19" s="175"/>
+      <c r="T19" s="176"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="35" t="s">
@@ -3878,25 +3830,25 @@
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="178" t="s">
+      <c r="D25" s="179" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="178"/>
-      <c r="F25" s="178"/>
-      <c r="G25" s="178"/>
-      <c r="H25" s="178"/>
-      <c r="I25" s="178"/>
-      <c r="J25" s="178"/>
-      <c r="K25" s="178"/>
-      <c r="L25" s="178"/>
-      <c r="M25" s="178"/>
-      <c r="N25" s="178"/>
-      <c r="O25" s="178"/>
-      <c r="P25" s="178"/>
-      <c r="Q25" s="178"/>
-      <c r="R25" s="178"/>
-      <c r="S25" s="178"/>
-      <c r="T25" s="178"/>
+      <c r="E25" s="179"/>
+      <c r="F25" s="179"/>
+      <c r="G25" s="179"/>
+      <c r="H25" s="179"/>
+      <c r="I25" s="179"/>
+      <c r="J25" s="179"/>
+      <c r="K25" s="179"/>
+      <c r="L25" s="179"/>
+      <c r="M25" s="179"/>
+      <c r="N25" s="179"/>
+      <c r="O25" s="179"/>
+      <c r="P25" s="179"/>
+      <c r="Q25" s="179"/>
+      <c r="R25" s="179"/>
+      <c r="S25" s="179"/>
+      <c r="T25" s="179"/>
     </row>
     <row r="26" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -3922,25 +3874,25 @@
       <c r="B27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="178" t="s">
+      <c r="D27" s="179" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="178"/>
-      <c r="F27" s="178"/>
-      <c r="G27" s="178"/>
-      <c r="H27" s="178"/>
-      <c r="I27" s="178"/>
-      <c r="J27" s="178"/>
-      <c r="K27" s="178"/>
-      <c r="L27" s="178"/>
-      <c r="M27" s="178"/>
-      <c r="N27" s="178"/>
-      <c r="O27" s="178"/>
-      <c r="P27" s="178"/>
-      <c r="Q27" s="178"/>
-      <c r="R27" s="178"/>
-      <c r="S27" s="178"/>
-      <c r="T27" s="178"/>
+      <c r="E27" s="179"/>
+      <c r="F27" s="179"/>
+      <c r="G27" s="179"/>
+      <c r="H27" s="179"/>
+      <c r="I27" s="179"/>
+      <c r="J27" s="179"/>
+      <c r="K27" s="179"/>
+      <c r="L27" s="179"/>
+      <c r="M27" s="179"/>
+      <c r="N27" s="179"/>
+      <c r="O27" s="179"/>
+      <c r="P27" s="179"/>
+      <c r="Q27" s="179"/>
+      <c r="R27" s="179"/>
+      <c r="S27" s="179"/>
+      <c r="T27" s="179"/>
     </row>
     <row r="28" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
@@ -3966,25 +3918,25 @@
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="178" t="s">
+      <c r="D29" s="179" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="178"/>
-      <c r="F29" s="178"/>
-      <c r="G29" s="178"/>
-      <c r="H29" s="178"/>
-      <c r="I29" s="178"/>
-      <c r="J29" s="178"/>
-      <c r="K29" s="178"/>
-      <c r="L29" s="178"/>
-      <c r="M29" s="178"/>
-      <c r="N29" s="178"/>
-      <c r="O29" s="178"/>
-      <c r="P29" s="178"/>
-      <c r="Q29" s="178"/>
-      <c r="R29" s="178"/>
-      <c r="S29" s="178"/>
-      <c r="T29" s="178"/>
+      <c r="E29" s="179"/>
+      <c r="F29" s="179"/>
+      <c r="G29" s="179"/>
+      <c r="H29" s="179"/>
+      <c r="I29" s="179"/>
+      <c r="J29" s="179"/>
+      <c r="K29" s="179"/>
+      <c r="L29" s="179"/>
+      <c r="M29" s="179"/>
+      <c r="N29" s="179"/>
+      <c r="O29" s="179"/>
+      <c r="P29" s="179"/>
+      <c r="Q29" s="179"/>
+      <c r="R29" s="179"/>
+      <c r="S29" s="179"/>
+      <c r="T29" s="179"/>
     </row>
     <row r="30" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
@@ -4010,25 +3962,25 @@
       <c r="B31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="178" t="s">
+      <c r="D31" s="179" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="178"/>
-      <c r="F31" s="178"/>
-      <c r="G31" s="178"/>
-      <c r="H31" s="178"/>
-      <c r="I31" s="178"/>
-      <c r="J31" s="178"/>
-      <c r="K31" s="178"/>
-      <c r="L31" s="178"/>
-      <c r="M31" s="178"/>
-      <c r="N31" s="178"/>
-      <c r="O31" s="178"/>
-      <c r="P31" s="178"/>
-      <c r="Q31" s="178"/>
-      <c r="R31" s="178"/>
-      <c r="S31" s="178"/>
-      <c r="T31" s="178"/>
+      <c r="E31" s="179"/>
+      <c r="F31" s="179"/>
+      <c r="G31" s="179"/>
+      <c r="H31" s="179"/>
+      <c r="I31" s="179"/>
+      <c r="J31" s="179"/>
+      <c r="K31" s="179"/>
+      <c r="L31" s="179"/>
+      <c r="M31" s="179"/>
+      <c r="N31" s="179"/>
+      <c r="O31" s="179"/>
+      <c r="P31" s="179"/>
+      <c r="Q31" s="179"/>
+      <c r="R31" s="179"/>
+      <c r="S31" s="179"/>
+      <c r="T31" s="179"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -4054,25 +4006,25 @@
       <c r="B33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="178" t="s">
+      <c r="D33" s="179" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="178"/>
-      <c r="F33" s="178"/>
-      <c r="G33" s="178"/>
-      <c r="H33" s="178"/>
-      <c r="I33" s="178"/>
-      <c r="J33" s="178"/>
-      <c r="K33" s="178"/>
-      <c r="L33" s="178"/>
-      <c r="M33" s="178"/>
-      <c r="N33" s="178"/>
-      <c r="O33" s="178"/>
-      <c r="P33" s="178"/>
-      <c r="Q33" s="178"/>
-      <c r="R33" s="178"/>
-      <c r="S33" s="178"/>
-      <c r="T33" s="178"/>
+      <c r="E33" s="179"/>
+      <c r="F33" s="179"/>
+      <c r="G33" s="179"/>
+      <c r="H33" s="179"/>
+      <c r="I33" s="179"/>
+      <c r="J33" s="179"/>
+      <c r="K33" s="179"/>
+      <c r="L33" s="179"/>
+      <c r="M33" s="179"/>
+      <c r="N33" s="179"/>
+      <c r="O33" s="179"/>
+      <c r="P33" s="179"/>
+      <c r="Q33" s="179"/>
+      <c r="R33" s="179"/>
+      <c r="S33" s="179"/>
+      <c r="T33" s="179"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -4098,25 +4050,25 @@
       <c r="B35" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="172" t="s">
+      <c r="D35" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="172"/>
-      <c r="F35" s="172"/>
-      <c r="G35" s="172"/>
-      <c r="H35" s="172"/>
-      <c r="I35" s="172"/>
-      <c r="J35" s="172"/>
-      <c r="K35" s="172"/>
-      <c r="L35" s="172"/>
-      <c r="M35" s="172"/>
-      <c r="N35" s="172"/>
-      <c r="O35" s="172"/>
-      <c r="P35" s="172"/>
-      <c r="Q35" s="172"/>
-      <c r="R35" s="172"/>
-      <c r="S35" s="172"/>
-      <c r="T35" s="172"/>
+      <c r="E35" s="173"/>
+      <c r="F35" s="173"/>
+      <c r="G35" s="173"/>
+      <c r="H35" s="173"/>
+      <c r="I35" s="173"/>
+      <c r="J35" s="173"/>
+      <c r="K35" s="173"/>
+      <c r="L35" s="173"/>
+      <c r="M35" s="173"/>
+      <c r="N35" s="173"/>
+      <c r="O35" s="173"/>
+      <c r="P35" s="173"/>
+      <c r="Q35" s="173"/>
+      <c r="R35" s="173"/>
+      <c r="S35" s="173"/>
+      <c r="T35" s="173"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4258,24 +4210,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="176" t="s">
+      <c r="G7" s="177" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="176"/>
-      <c r="I7" s="176"/>
-      <c r="J7" s="176"/>
-      <c r="K7" s="176"/>
-      <c r="L7" s="177"/>
+      <c r="H7" s="177"/>
+      <c r="I7" s="177"/>
+      <c r="J7" s="177"/>
+      <c r="K7" s="177"/>
+      <c r="L7" s="178"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="176" t="s">
+      <c r="N7" s="177" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="176"/>
-      <c r="P7" s="176"/>
-      <c r="Q7" s="176"/>
-      <c r="R7" s="176"/>
-      <c r="S7" s="176"/>
-      <c r="T7" s="177"/>
+      <c r="O7" s="177"/>
+      <c r="P7" s="177"/>
+      <c r="Q7" s="177"/>
+      <c r="R7" s="177"/>
+      <c r="S7" s="177"/>
+      <c r="T7" s="178"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -4517,24 +4469,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="173" t="s">
+      <c r="G13" s="174" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="174"/>
-      <c r="I13" s="174"/>
-      <c r="J13" s="174"/>
-      <c r="K13" s="174"/>
-      <c r="L13" s="175"/>
+      <c r="H13" s="175"/>
+      <c r="I13" s="175"/>
+      <c r="J13" s="175"/>
+      <c r="K13" s="175"/>
+      <c r="L13" s="176"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="173" t="s">
+      <c r="N13" s="174" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="174"/>
-      <c r="P13" s="174"/>
-      <c r="Q13" s="174"/>
-      <c r="R13" s="174"/>
-      <c r="S13" s="174"/>
-      <c r="T13" s="175"/>
+      <c r="O13" s="175"/>
+      <c r="P13" s="175"/>
+      <c r="Q13" s="175"/>
+      <c r="R13" s="175"/>
+      <c r="S13" s="175"/>
+      <c r="T13" s="176"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="35" t="s">
@@ -4772,24 +4724,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="173" t="s">
+      <c r="G19" s="174" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="174"/>
-      <c r="I19" s="174"/>
-      <c r="J19" s="174"/>
-      <c r="K19" s="174"/>
-      <c r="L19" s="175"/>
+      <c r="H19" s="175"/>
+      <c r="I19" s="175"/>
+      <c r="J19" s="175"/>
+      <c r="K19" s="175"/>
+      <c r="L19" s="176"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="173" t="s">
+      <c r="N19" s="174" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="174"/>
-      <c r="P19" s="174"/>
-      <c r="Q19" s="174"/>
-      <c r="R19" s="174"/>
-      <c r="S19" s="174"/>
-      <c r="T19" s="175"/>
+      <c r="O19" s="175"/>
+      <c r="P19" s="175"/>
+      <c r="Q19" s="175"/>
+      <c r="R19" s="175"/>
+      <c r="S19" s="175"/>
+      <c r="T19" s="176"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="35" t="s">
@@ -5027,24 +4979,24 @@
       <c r="D25" s="6"/>
       <c r="E25" s="20"/>
       <c r="F25" s="25"/>
-      <c r="G25" s="173" t="s">
+      <c r="G25" s="174" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="174"/>
-      <c r="I25" s="174"/>
-      <c r="J25" s="174"/>
-      <c r="K25" s="174"/>
-      <c r="L25" s="175"/>
+      <c r="H25" s="175"/>
+      <c r="I25" s="175"/>
+      <c r="J25" s="175"/>
+      <c r="K25" s="175"/>
+      <c r="L25" s="176"/>
       <c r="M25" s="30"/>
-      <c r="N25" s="173" t="s">
+      <c r="N25" s="174" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="174"/>
-      <c r="P25" s="174"/>
-      <c r="Q25" s="174"/>
-      <c r="R25" s="174"/>
-      <c r="S25" s="174"/>
-      <c r="T25" s="175"/>
+      <c r="O25" s="175"/>
+      <c r="P25" s="175"/>
+      <c r="Q25" s="175"/>
+      <c r="R25" s="175"/>
+      <c r="S25" s="175"/>
+      <c r="T25" s="176"/>
     </row>
     <row r="26" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="35" t="s">
@@ -5282,26 +5234,26 @@
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="168" t="s">
+      <c r="C31" s="169" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="168"/>
-      <c r="E31" s="168"/>
-      <c r="F31" s="168"/>
-      <c r="G31" s="168"/>
-      <c r="H31" s="168"/>
-      <c r="I31" s="168"/>
-      <c r="J31" s="168"/>
-      <c r="K31" s="168"/>
-      <c r="L31" s="168"/>
-      <c r="M31" s="168"/>
-      <c r="N31" s="168"/>
-      <c r="O31" s="168"/>
-      <c r="P31" s="168"/>
-      <c r="Q31" s="168"/>
-      <c r="R31" s="168"/>
-      <c r="S31" s="168"/>
-      <c r="T31" s="168"/>
+      <c r="D31" s="169"/>
+      <c r="E31" s="169"/>
+      <c r="F31" s="169"/>
+      <c r="G31" s="169"/>
+      <c r="H31" s="169"/>
+      <c r="I31" s="169"/>
+      <c r="J31" s="169"/>
+      <c r="K31" s="169"/>
+      <c r="L31" s="169"/>
+      <c r="M31" s="169"/>
+      <c r="N31" s="169"/>
+      <c r="O31" s="169"/>
+      <c r="P31" s="169"/>
+      <c r="Q31" s="169"/>
+      <c r="R31" s="169"/>
+      <c r="S31" s="169"/>
+      <c r="T31" s="169"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -5328,26 +5280,26 @@
       <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="168" t="s">
+      <c r="C33" s="169" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="168"/>
-      <c r="E33" s="168"/>
-      <c r="F33" s="168"/>
-      <c r="G33" s="168"/>
-      <c r="H33" s="168"/>
-      <c r="I33" s="168"/>
-      <c r="J33" s="168"/>
-      <c r="K33" s="168"/>
-      <c r="L33" s="168"/>
-      <c r="M33" s="168"/>
-      <c r="N33" s="168"/>
-      <c r="O33" s="168"/>
-      <c r="P33" s="168"/>
-      <c r="Q33" s="168"/>
-      <c r="R33" s="168"/>
-      <c r="S33" s="168"/>
-      <c r="T33" s="168"/>
+      <c r="D33" s="169"/>
+      <c r="E33" s="169"/>
+      <c r="F33" s="169"/>
+      <c r="G33" s="169"/>
+      <c r="H33" s="169"/>
+      <c r="I33" s="169"/>
+      <c r="J33" s="169"/>
+      <c r="K33" s="169"/>
+      <c r="L33" s="169"/>
+      <c r="M33" s="169"/>
+      <c r="N33" s="169"/>
+      <c r="O33" s="169"/>
+      <c r="P33" s="169"/>
+      <c r="Q33" s="169"/>
+      <c r="R33" s="169"/>
+      <c r="S33" s="169"/>
+      <c r="T33" s="169"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -5374,26 +5326,26 @@
       <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="168" t="s">
+      <c r="C35" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="168"/>
-      <c r="E35" s="168"/>
-      <c r="F35" s="168"/>
-      <c r="G35" s="168"/>
-      <c r="H35" s="168"/>
-      <c r="I35" s="168"/>
-      <c r="J35" s="168"/>
-      <c r="K35" s="168"/>
-      <c r="L35" s="168"/>
-      <c r="M35" s="168"/>
-      <c r="N35" s="168"/>
-      <c r="O35" s="168"/>
-      <c r="P35" s="168"/>
-      <c r="Q35" s="168"/>
-      <c r="R35" s="168"/>
-      <c r="S35" s="168"/>
-      <c r="T35" s="168"/>
+      <c r="D35" s="169"/>
+      <c r="E35" s="169"/>
+      <c r="F35" s="169"/>
+      <c r="G35" s="169"/>
+      <c r="H35" s="169"/>
+      <c r="I35" s="169"/>
+      <c r="J35" s="169"/>
+      <c r="K35" s="169"/>
+      <c r="L35" s="169"/>
+      <c r="M35" s="169"/>
+      <c r="N35" s="169"/>
+      <c r="O35" s="169"/>
+      <c r="P35" s="169"/>
+      <c r="Q35" s="169"/>
+      <c r="R35" s="169"/>
+      <c r="S35" s="169"/>
+      <c r="T35" s="169"/>
     </row>
     <row r="36" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
@@ -5420,26 +5372,26 @@
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="168" t="s">
+      <c r="C37" s="169" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="168"/>
-      <c r="E37" s="168"/>
-      <c r="F37" s="168"/>
-      <c r="G37" s="168"/>
-      <c r="H37" s="168"/>
-      <c r="I37" s="168"/>
-      <c r="J37" s="168"/>
-      <c r="K37" s="168"/>
-      <c r="L37" s="168"/>
-      <c r="M37" s="168"/>
-      <c r="N37" s="168"/>
-      <c r="O37" s="168"/>
-      <c r="P37" s="168"/>
-      <c r="Q37" s="168"/>
-      <c r="R37" s="168"/>
-      <c r="S37" s="168"/>
-      <c r="T37" s="168"/>
+      <c r="D37" s="169"/>
+      <c r="E37" s="169"/>
+      <c r="F37" s="169"/>
+      <c r="G37" s="169"/>
+      <c r="H37" s="169"/>
+      <c r="I37" s="169"/>
+      <c r="J37" s="169"/>
+      <c r="K37" s="169"/>
+      <c r="L37" s="169"/>
+      <c r="M37" s="169"/>
+      <c r="N37" s="169"/>
+      <c r="O37" s="169"/>
+      <c r="P37" s="169"/>
+      <c r="Q37" s="169"/>
+      <c r="R37" s="169"/>
+      <c r="S37" s="169"/>
+      <c r="T37" s="169"/>
     </row>
     <row r="38" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
@@ -5466,26 +5418,26 @@
       <c r="B39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="168" t="s">
+      <c r="C39" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="168"/>
-      <c r="E39" s="168"/>
-      <c r="F39" s="168"/>
-      <c r="G39" s="168"/>
-      <c r="H39" s="168"/>
-      <c r="I39" s="168"/>
-      <c r="J39" s="168"/>
-      <c r="K39" s="168"/>
-      <c r="L39" s="168"/>
-      <c r="M39" s="168"/>
-      <c r="N39" s="168"/>
-      <c r="O39" s="168"/>
-      <c r="P39" s="168"/>
-      <c r="Q39" s="168"/>
-      <c r="R39" s="168"/>
-      <c r="S39" s="168"/>
-      <c r="T39" s="168"/>
+      <c r="D39" s="169"/>
+      <c r="E39" s="169"/>
+      <c r="F39" s="169"/>
+      <c r="G39" s="169"/>
+      <c r="H39" s="169"/>
+      <c r="I39" s="169"/>
+      <c r="J39" s="169"/>
+      <c r="K39" s="169"/>
+      <c r="L39" s="169"/>
+      <c r="M39" s="169"/>
+      <c r="N39" s="169"/>
+      <c r="O39" s="169"/>
+      <c r="P39" s="169"/>
+      <c r="Q39" s="169"/>
+      <c r="R39" s="169"/>
+      <c r="S39" s="169"/>
+      <c r="T39" s="169"/>
     </row>
     <row r="40" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
@@ -5512,26 +5464,26 @@
       <c r="B41" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="170" t="s">
+      <c r="C41" s="171" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="170"/>
-      <c r="E41" s="170"/>
-      <c r="F41" s="170"/>
-      <c r="G41" s="170"/>
-      <c r="H41" s="170"/>
-      <c r="I41" s="170"/>
-      <c r="J41" s="170"/>
-      <c r="K41" s="170"/>
-      <c r="L41" s="170"/>
-      <c r="M41" s="170"/>
-      <c r="N41" s="170"/>
-      <c r="O41" s="170"/>
-      <c r="P41" s="170"/>
-      <c r="Q41" s="170"/>
-      <c r="R41" s="170"/>
-      <c r="S41" s="170"/>
-      <c r="T41" s="170"/>
+      <c r="D41" s="171"/>
+      <c r="E41" s="171"/>
+      <c r="F41" s="171"/>
+      <c r="G41" s="171"/>
+      <c r="H41" s="171"/>
+      <c r="I41" s="171"/>
+      <c r="J41" s="171"/>
+      <c r="K41" s="171"/>
+      <c r="L41" s="171"/>
+      <c r="M41" s="171"/>
+      <c r="N41" s="171"/>
+      <c r="O41" s="171"/>
+      <c r="P41" s="171"/>
+      <c r="Q41" s="171"/>
+      <c r="R41" s="171"/>
+      <c r="S41" s="171"/>
+      <c r="T41" s="171"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -5587,94 +5539,94 @@
     </row>
     <row r="3" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:4" s="104" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="179" t="s">
+      <c r="C4" s="180" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="179"/>
+      <c r="D4" s="180"/>
     </row>
     <row r="5" spans="3:4" s="104" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="179" t="s">
+      <c r="C5" s="180" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="179"/>
+      <c r="D5" s="180"/>
     </row>
     <row r="6" spans="3:4" s="104" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="179" t="s">
+      <c r="C6" s="180" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="179"/>
+      <c r="D6" s="180"/>
     </row>
     <row r="7" spans="3:4" s="104" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="179" t="s">
+      <c r="C7" s="180" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="179"/>
+      <c r="D7" s="180"/>
     </row>
     <row r="8" spans="3:4" s="104" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="179" t="s">
+      <c r="C8" s="180" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="179"/>
+      <c r="D8" s="180"/>
     </row>
     <row r="9" spans="3:4" s="104" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="179" t="s">
+      <c r="C9" s="180" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="179"/>
+      <c r="D9" s="180"/>
     </row>
     <row r="10" spans="3:4" s="104" customFormat="1" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="179" t="s">
+      <c r="C10" s="180" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="179"/>
+      <c r="D10" s="180"/>
     </row>
     <row r="11" spans="3:4" s="104" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="179" t="s">
+      <c r="C11" s="180" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="179"/>
+      <c r="D11" s="180"/>
     </row>
     <row r="12" spans="3:4" s="104" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="179" t="s">
+      <c r="C12" s="180" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="179"/>
+      <c r="D12" s="180"/>
     </row>
     <row r="13" spans="3:4" s="104" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="179" t="s">
+      <c r="C13" s="180" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="179"/>
+      <c r="D13" s="180"/>
     </row>
     <row r="14" spans="3:4" s="104" customFormat="1" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="179" t="s">
+      <c r="C14" s="180" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="179"/>
+      <c r="D14" s="180"/>
     </row>
     <row r="15" spans="3:4" s="104" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="179" t="s">
+      <c r="C15" s="180" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="179"/>
+      <c r="D15" s="180"/>
     </row>
     <row r="16" spans="3:4" s="104" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="179" t="s">
+      <c r="C16" s="180" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="179"/>
+      <c r="D16" s="180"/>
     </row>
     <row r="17" spans="3:4" s="104" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="179" t="s">
+      <c r="C17" s="180" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="179"/>
+      <c r="D17" s="180"/>
     </row>
     <row r="18" spans="3:4" s="104" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="179" t="s">
+      <c r="C18" s="180" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="179"/>
+      <c r="D18" s="180"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -5770,24 +5722,24 @@
       </c>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="168"/>
-      <c r="D5" s="168"/>
-      <c r="E5" s="168"/>
-      <c r="F5" s="168"/>
-      <c r="G5" s="168"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="169"/>
       <c r="H5" s="102"/>
-      <c r="I5" s="168"/>
-      <c r="J5" s="168"/>
-      <c r="K5" s="168"/>
-      <c r="L5" s="168"/>
-      <c r="M5" s="168"/>
-      <c r="N5" s="168"/>
+      <c r="I5" s="169"/>
+      <c r="J5" s="169"/>
+      <c r="K5" s="169"/>
+      <c r="L5" s="169"/>
+      <c r="M5" s="169"/>
+      <c r="N5" s="169"/>
       <c r="O5" s="62"/>
-      <c r="P5" s="168"/>
-      <c r="Q5" s="168"/>
-      <c r="R5" s="168"/>
-      <c r="S5" s="168"/>
-      <c r="T5" s="168"/>
+      <c r="P5" s="169"/>
+      <c r="Q5" s="169"/>
+      <c r="R5" s="169"/>
+      <c r="S5" s="169"/>
+      <c r="T5" s="169"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I6" s="29"/>
@@ -5811,21 +5763,21 @@
       <c r="F7" s="6"/>
       <c r="G7" s="20"/>
       <c r="H7" s="55"/>
-      <c r="I7" s="173" t="s">
+      <c r="I7" s="174" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="174"/>
-      <c r="K7" s="174"/>
-      <c r="L7" s="174"/>
-      <c r="M7" s="174"/>
-      <c r="N7" s="175"/>
-      <c r="O7" s="173"/>
-      <c r="P7" s="174"/>
-      <c r="Q7" s="174"/>
-      <c r="R7" s="174"/>
-      <c r="S7" s="174"/>
-      <c r="T7" s="174"/>
-      <c r="U7" s="175"/>
+      <c r="J7" s="175"/>
+      <c r="K7" s="175"/>
+      <c r="L7" s="175"/>
+      <c r="M7" s="175"/>
+      <c r="N7" s="176"/>
+      <c r="O7" s="174"/>
+      <c r="P7" s="175"/>
+      <c r="Q7" s="175"/>
+      <c r="R7" s="175"/>
+      <c r="S7" s="175"/>
+      <c r="T7" s="175"/>
+      <c r="U7" s="176"/>
     </row>
     <row r="8" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="85" t="s">
@@ -5986,20 +5938,20 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
-      <c r="H13" s="173"/>
-      <c r="I13" s="174"/>
-      <c r="J13" s="174"/>
-      <c r="K13" s="174"/>
-      <c r="L13" s="174"/>
-      <c r="M13" s="174"/>
-      <c r="N13" s="175"/>
-      <c r="O13" s="173"/>
-      <c r="P13" s="174"/>
-      <c r="Q13" s="174"/>
-      <c r="R13" s="174"/>
-      <c r="S13" s="174"/>
-      <c r="T13" s="174"/>
-      <c r="U13" s="175"/>
+      <c r="H13" s="174"/>
+      <c r="I13" s="175"/>
+      <c r="J13" s="175"/>
+      <c r="K13" s="175"/>
+      <c r="L13" s="175"/>
+      <c r="M13" s="175"/>
+      <c r="N13" s="176"/>
+      <c r="O13" s="174"/>
+      <c r="P13" s="175"/>
+      <c r="Q13" s="175"/>
+      <c r="R13" s="175"/>
+      <c r="S13" s="175"/>
+      <c r="T13" s="175"/>
+      <c r="U13" s="176"/>
     </row>
     <row r="14" spans="1:21" s="103" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="54"/>
@@ -6169,22 +6121,22 @@
       </c>
       <c r="D20" s="51"/>
       <c r="E20" s="105"/>
-      <c r="F20" s="180"/>
-      <c r="G20" s="180"/>
-      <c r="H20" s="180"/>
-      <c r="I20" s="180"/>
-      <c r="J20" s="180"/>
-      <c r="K20" s="180"/>
-      <c r="L20" s="180"/>
-      <c r="M20" s="180"/>
-      <c r="N20" s="180"/>
-      <c r="O20" s="180"/>
-      <c r="P20" s="180"/>
-      <c r="Q20" s="180"/>
-      <c r="R20" s="180"/>
-      <c r="S20" s="180"/>
-      <c r="T20" s="180"/>
-      <c r="U20" s="180"/>
+      <c r="F20" s="181"/>
+      <c r="G20" s="181"/>
+      <c r="H20" s="181"/>
+      <c r="I20" s="181"/>
+      <c r="J20" s="181"/>
+      <c r="K20" s="181"/>
+      <c r="L20" s="181"/>
+      <c r="M20" s="181"/>
+      <c r="N20" s="181"/>
+      <c r="O20" s="181"/>
+      <c r="P20" s="181"/>
+      <c r="Q20" s="181"/>
+      <c r="R20" s="181"/>
+      <c r="S20" s="181"/>
+      <c r="T20" s="181"/>
+      <c r="U20" s="181"/>
     </row>
     <row r="21" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
@@ -6213,22 +6165,22 @@
         <v>36</v>
       </c>
       <c r="D22" s="51"/>
-      <c r="F22" s="180"/>
-      <c r="G22" s="180"/>
-      <c r="H22" s="180"/>
-      <c r="I22" s="180"/>
-      <c r="J22" s="180"/>
-      <c r="K22" s="180"/>
-      <c r="L22" s="180"/>
-      <c r="M22" s="180"/>
-      <c r="N22" s="180"/>
-      <c r="O22" s="180"/>
-      <c r="P22" s="180"/>
-      <c r="Q22" s="180"/>
-      <c r="R22" s="180"/>
-      <c r="S22" s="180"/>
-      <c r="T22" s="180"/>
-      <c r="U22" s="180"/>
+      <c r="F22" s="181"/>
+      <c r="G22" s="181"/>
+      <c r="H22" s="181"/>
+      <c r="I22" s="181"/>
+      <c r="J22" s="181"/>
+      <c r="K22" s="181"/>
+      <c r="L22" s="181"/>
+      <c r="M22" s="181"/>
+      <c r="N22" s="181"/>
+      <c r="O22" s="181"/>
+      <c r="P22" s="181"/>
+      <c r="Q22" s="181"/>
+      <c r="R22" s="181"/>
+      <c r="S22" s="181"/>
+      <c r="T22" s="181"/>
+      <c r="U22" s="181"/>
       <c r="V22" s="126"/>
     </row>
     <row r="23" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -6257,22 +6209,22 @@
       </c>
       <c r="D24" s="51"/>
       <c r="E24" s="105"/>
-      <c r="F24" s="180"/>
-      <c r="G24" s="180"/>
-      <c r="H24" s="180"/>
-      <c r="I24" s="180"/>
-      <c r="J24" s="180"/>
-      <c r="K24" s="180"/>
-      <c r="L24" s="180"/>
-      <c r="M24" s="180"/>
-      <c r="N24" s="180"/>
-      <c r="O24" s="180"/>
-      <c r="P24" s="180"/>
-      <c r="Q24" s="180"/>
-      <c r="R24" s="180"/>
-      <c r="S24" s="180"/>
-      <c r="T24" s="180"/>
-      <c r="U24" s="180"/>
+      <c r="F24" s="181"/>
+      <c r="G24" s="181"/>
+      <c r="H24" s="181"/>
+      <c r="I24" s="181"/>
+      <c r="J24" s="181"/>
+      <c r="K24" s="181"/>
+      <c r="L24" s="181"/>
+      <c r="M24" s="181"/>
+      <c r="N24" s="181"/>
+      <c r="O24" s="181"/>
+      <c r="P24" s="181"/>
+      <c r="Q24" s="181"/>
+      <c r="R24" s="181"/>
+      <c r="S24" s="181"/>
+      <c r="T24" s="181"/>
+      <c r="U24" s="181"/>
     </row>
     <row r="25" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
@@ -6301,22 +6253,22 @@
         <v>48</v>
       </c>
       <c r="D26" s="51"/>
-      <c r="F26" s="171"/>
-      <c r="G26" s="171"/>
-      <c r="H26" s="171"/>
-      <c r="I26" s="171"/>
-      <c r="J26" s="171"/>
-      <c r="K26" s="171"/>
-      <c r="L26" s="171"/>
-      <c r="M26" s="171"/>
-      <c r="N26" s="171"/>
-      <c r="O26" s="171"/>
-      <c r="P26" s="171"/>
-      <c r="Q26" s="171"/>
-      <c r="R26" s="171"/>
-      <c r="S26" s="171"/>
-      <c r="T26" s="171"/>
-      <c r="U26" s="171"/>
+      <c r="F26" s="172"/>
+      <c r="G26" s="172"/>
+      <c r="H26" s="172"/>
+      <c r="I26" s="172"/>
+      <c r="J26" s="172"/>
+      <c r="K26" s="172"/>
+      <c r="L26" s="172"/>
+      <c r="M26" s="172"/>
+      <c r="N26" s="172"/>
+      <c r="O26" s="172"/>
+      <c r="P26" s="172"/>
+      <c r="Q26" s="172"/>
+      <c r="R26" s="172"/>
+      <c r="S26" s="172"/>
+      <c r="T26" s="172"/>
+      <c r="U26" s="172"/>
       <c r="V26" s="126"/>
     </row>
     <row r="27" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -6344,22 +6296,22 @@
         <v>49</v>
       </c>
       <c r="D28" s="51"/>
-      <c r="F28" s="170"/>
-      <c r="G28" s="170"/>
-      <c r="H28" s="170"/>
-      <c r="I28" s="170"/>
-      <c r="J28" s="170"/>
-      <c r="K28" s="170"/>
-      <c r="L28" s="170"/>
-      <c r="M28" s="170"/>
-      <c r="N28" s="170"/>
-      <c r="O28" s="170"/>
-      <c r="P28" s="170"/>
-      <c r="Q28" s="170"/>
-      <c r="R28" s="170"/>
-      <c r="S28" s="170"/>
-      <c r="T28" s="170"/>
-      <c r="U28" s="170"/>
+      <c r="F28" s="171"/>
+      <c r="G28" s="171"/>
+      <c r="H28" s="171"/>
+      <c r="I28" s="171"/>
+      <c r="J28" s="171"/>
+      <c r="K28" s="171"/>
+      <c r="L28" s="171"/>
+      <c r="M28" s="171"/>
+      <c r="N28" s="171"/>
+      <c r="O28" s="171"/>
+      <c r="P28" s="171"/>
+      <c r="Q28" s="171"/>
+      <c r="R28" s="171"/>
+      <c r="S28" s="171"/>
+      <c r="T28" s="171"/>
+      <c r="U28" s="171"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -6428,19 +6380,19 @@
   <sheetData>
     <row r="1" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="181"/>
-      <c r="C2" s="173"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="175"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
-      <c r="I2" s="174"/>
-      <c r="J2" s="175"/>
-      <c r="K2" s="173"/>
-      <c r="L2" s="174"/>
-      <c r="M2" s="174"/>
-      <c r="N2" s="175"/>
+      <c r="B2" s="168"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="175"/>
+      <c r="E2" s="175"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="175"/>
+      <c r="I2" s="175"/>
+      <c r="J2" s="176"/>
+      <c r="K2" s="174"/>
+      <c r="L2" s="175"/>
+      <c r="M2" s="175"/>
+      <c r="N2" s="176"/>
       <c r="O2" s="29"/>
     </row>
     <row r="3" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6572,20 +6524,20 @@
       <c r="O9" s="167"/>
     </row>
     <row r="11" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="181"/>
-      <c r="C11" s="173"/>
-      <c r="D11" s="174"/>
-      <c r="E11" s="174"/>
-      <c r="F11" s="174"/>
-      <c r="G11" s="175"/>
-      <c r="H11" s="174"/>
-      <c r="I11" s="174"/>
-      <c r="J11" s="174"/>
-      <c r="K11" s="175"/>
-      <c r="L11" s="173"/>
-      <c r="M11" s="174"/>
-      <c r="N11" s="174"/>
-      <c r="O11" s="175"/>
+      <c r="B11" s="168"/>
+      <c r="C11" s="174"/>
+      <c r="D11" s="175"/>
+      <c r="E11" s="175"/>
+      <c r="F11" s="175"/>
+      <c r="G11" s="176"/>
+      <c r="H11" s="175"/>
+      <c r="I11" s="175"/>
+      <c r="J11" s="175"/>
+      <c r="K11" s="176"/>
+      <c r="L11" s="174"/>
+      <c r="M11" s="175"/>
+      <c r="N11" s="175"/>
+      <c r="O11" s="176"/>
       <c r="P11" s="29"/>
     </row>
     <row r="12" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6724,20 +6676,20 @@
       <c r="P18" s="167"/>
     </row>
     <row r="20" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="181"/>
-      <c r="C20" s="173"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="174"/>
-      <c r="F20" s="175"/>
-      <c r="G20" s="174"/>
-      <c r="H20" s="174"/>
-      <c r="I20" s="174"/>
-      <c r="J20" s="174"/>
-      <c r="K20" s="175"/>
-      <c r="L20" s="173"/>
-      <c r="M20" s="174"/>
-      <c r="N20" s="174"/>
-      <c r="O20" s="175"/>
+      <c r="B20" s="168"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="175"/>
+      <c r="E20" s="175"/>
+      <c r="F20" s="176"/>
+      <c r="G20" s="175"/>
+      <c r="H20" s="175"/>
+      <c r="I20" s="175"/>
+      <c r="J20" s="175"/>
+      <c r="K20" s="176"/>
+      <c r="L20" s="174"/>
+      <c r="M20" s="175"/>
+      <c r="N20" s="175"/>
+      <c r="O20" s="176"/>
       <c r="P20" s="29"/>
     </row>
     <row r="21" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6876,20 +6828,20 @@
       <c r="P27" s="167"/>
     </row>
     <row r="29" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="181"/>
-      <c r="C29" s="173"/>
-      <c r="D29" s="174"/>
-      <c r="E29" s="174"/>
-      <c r="F29" s="175"/>
-      <c r="G29" s="174"/>
-      <c r="H29" s="174"/>
-      <c r="I29" s="174"/>
-      <c r="J29" s="175"/>
-      <c r="K29" s="173"/>
-      <c r="L29" s="174"/>
-      <c r="M29" s="174"/>
-      <c r="N29" s="174"/>
-      <c r="O29" s="175"/>
+      <c r="B29" s="168"/>
+      <c r="C29" s="174"/>
+      <c r="D29" s="175"/>
+      <c r="E29" s="175"/>
+      <c r="F29" s="176"/>
+      <c r="G29" s="175"/>
+      <c r="H29" s="175"/>
+      <c r="I29" s="175"/>
+      <c r="J29" s="176"/>
+      <c r="K29" s="174"/>
+      <c r="L29" s="175"/>
+      <c r="M29" s="175"/>
+      <c r="N29" s="175"/>
+      <c r="O29" s="176"/>
       <c r="P29" s="29"/>
     </row>
     <row r="30" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7028,21 +6980,21 @@
       <c r="P36" s="167"/>
     </row>
     <row r="38" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="181"/>
-      <c r="C38" s="173"/>
-      <c r="D38" s="174"/>
-      <c r="E38" s="174"/>
-      <c r="F38" s="174"/>
-      <c r="G38" s="175"/>
-      <c r="H38" s="174"/>
-      <c r="I38" s="174"/>
-      <c r="J38" s="174"/>
-      <c r="K38" s="174"/>
-      <c r="L38" s="175"/>
-      <c r="M38" s="173"/>
-      <c r="N38" s="174"/>
-      <c r="O38" s="174"/>
-      <c r="P38" s="175"/>
+      <c r="B38" s="168"/>
+      <c r="C38" s="174"/>
+      <c r="D38" s="175"/>
+      <c r="E38" s="175"/>
+      <c r="F38" s="175"/>
+      <c r="G38" s="176"/>
+      <c r="H38" s="175"/>
+      <c r="I38" s="175"/>
+      <c r="J38" s="175"/>
+      <c r="K38" s="175"/>
+      <c r="L38" s="176"/>
+      <c r="M38" s="174"/>
+      <c r="N38" s="175"/>
+      <c r="O38" s="175"/>
+      <c r="P38" s="176"/>
       <c r="Q38" s="29"/>
     </row>
     <row r="39" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7188,21 +7140,21 @@
       <c r="Q45" s="167"/>
     </row>
     <row r="47" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="181"/>
-      <c r="C47" s="173"/>
-      <c r="D47" s="174"/>
-      <c r="E47" s="174"/>
-      <c r="F47" s="174"/>
-      <c r="G47" s="175"/>
-      <c r="H47" s="174"/>
-      <c r="I47" s="174"/>
-      <c r="J47" s="174"/>
-      <c r="K47" s="175"/>
-      <c r="L47" s="173"/>
-      <c r="M47" s="174"/>
-      <c r="N47" s="174"/>
-      <c r="O47" s="174"/>
-      <c r="P47" s="175"/>
+      <c r="B47" s="168"/>
+      <c r="C47" s="174"/>
+      <c r="D47" s="175"/>
+      <c r="E47" s="175"/>
+      <c r="F47" s="175"/>
+      <c r="G47" s="176"/>
+      <c r="H47" s="175"/>
+      <c r="I47" s="175"/>
+      <c r="J47" s="175"/>
+      <c r="K47" s="176"/>
+      <c r="L47" s="174"/>
+      <c r="M47" s="175"/>
+      <c r="N47" s="175"/>
+      <c r="O47" s="175"/>
+      <c r="P47" s="176"/>
       <c r="Q47" s="29"/>
     </row>
     <row r="48" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7348,21 +7300,21 @@
       <c r="Q54" s="167"/>
     </row>
     <row r="56" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="181"/>
-      <c r="C56" s="173"/>
-      <c r="D56" s="174"/>
-      <c r="E56" s="174"/>
-      <c r="F56" s="175"/>
-      <c r="G56" s="174"/>
-      <c r="H56" s="174"/>
-      <c r="I56" s="174"/>
-      <c r="J56" s="174"/>
-      <c r="K56" s="175"/>
-      <c r="L56" s="173"/>
-      <c r="M56" s="174"/>
-      <c r="N56" s="174"/>
-      <c r="O56" s="174"/>
-      <c r="P56" s="175"/>
+      <c r="B56" s="168"/>
+      <c r="C56" s="174"/>
+      <c r="D56" s="175"/>
+      <c r="E56" s="175"/>
+      <c r="F56" s="176"/>
+      <c r="G56" s="175"/>
+      <c r="H56" s="175"/>
+      <c r="I56" s="175"/>
+      <c r="J56" s="175"/>
+      <c r="K56" s="176"/>
+      <c r="L56" s="174"/>
+      <c r="M56" s="175"/>
+      <c r="N56" s="175"/>
+      <c r="O56" s="175"/>
+      <c r="P56" s="176"/>
       <c r="Q56" s="29"/>
     </row>
     <row r="57" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7540,6 +7492,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7762,22 +7729,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7794,29 +7771,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged PR 9338: Backmerge 1019 and 1020 into develop
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B3122A62-23AF-46CF-8FA5-7F7F2A60E9A5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DA99B150-1A51-4C43-B164-FFBC06E7FD5D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="27360" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2320,8 +2320,8 @@
   </sheetPr>
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2693,14 +2693,14 @@
       <c r="C22" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="172"/>
-      <c r="E22" s="172"/>
-      <c r="F22" s="172"/>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172"/>
-      <c r="J22" s="172"/>
-      <c r="K22" s="172"/>
+      <c r="D22" s="171"/>
+      <c r="E22" s="171"/>
+      <c r="F22" s="171"/>
+      <c r="G22" s="171"/>
+      <c r="H22" s="171"/>
+      <c r="I22" s="171"/>
+      <c r="J22" s="171"/>
+      <c r="K22" s="171"/>
       <c r="L22" s="63"/>
       <c r="M22" s="63"/>
       <c r="N22" s="63"/>
@@ -5487,6 +5487,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5496,11 +5501,6 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -6315,6 +6315,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="F28:U28"/>
+    <mergeCell ref="F20:U20"/>
+    <mergeCell ref="H13:N13"/>
+    <mergeCell ref="O7:U7"/>
+    <mergeCell ref="F22:U22"/>
+    <mergeCell ref="F24:U24"/>
+    <mergeCell ref="F26:U26"/>
+    <mergeCell ref="O13:U13"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:T5"/>
     <mergeCell ref="E5:G5"/>
@@ -6323,14 +6331,6 @@
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
-    <mergeCell ref="F28:U28"/>
-    <mergeCell ref="F20:U20"/>
-    <mergeCell ref="H13:N13"/>
-    <mergeCell ref="O7:U7"/>
-    <mergeCell ref="F22:U22"/>
-    <mergeCell ref="F24:U24"/>
-    <mergeCell ref="F26:U26"/>
-    <mergeCell ref="O13:U13"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:U3 C5 C4:N4 P4 R4:U4 U5 C6:U1048576">
     <cfRule type="expression" dxfId="2" priority="3">
@@ -7461,6 +7461,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="L11:O11"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:O29"/>
     <mergeCell ref="C56:F56"/>
     <mergeCell ref="G56:K56"/>
     <mergeCell ref="L56:P56"/>
@@ -7470,18 +7482,6 @@
     <mergeCell ref="C47:G47"/>
     <mergeCell ref="H47:K47"/>
     <mergeCell ref="L47:P47"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="K29:O29"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:O11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="C9:N9 C36:O36 C18:O18 C27:O27 C45:P45 C54:P54 C63:P63" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
@@ -7492,18 +7492,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7730,14 +7730,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -7750,6 +7742,14 @@
     <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Merged PR 13008: BP-3071_Campaign Export-Flow Chart tab- Quarterly/Monthly table-Total Hiatus...
BP-3071_Campaign Export-Flow Chart tab- Quarterly/Monthly table-Total Hiatus days displayed with a $ sign
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DA99B150-1A51-4C43-B164-FFBC06E7FD5D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325B9DD5-DD1A-461E-AA99-77B19CF44296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="27360" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="4" r:id="rId1"/>
@@ -21,17 +21,26 @@
     <sheet name="Proposal" sheetId="5" r:id="rId6"/>
     <sheet name="Flow Chart Template Tables" sheetId="9" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="91">
   <si>
     <t>Broadcast Proposal Gorilla Glue Q4 '19 - Q1 '20</t>
   </si>
@@ -669,6 +678,9 @@
   </si>
   <si>
     <t>Receipt Acknowledged:</t>
+  </si>
+  <si>
+    <t>Total Monthly Cost</t>
   </si>
 </sst>
 </file>
@@ -1144,7 +1156,7 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1625,21 +1637,15 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="1" fontId="12" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
@@ -1678,6 +1684,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2320,7 +2359,7 @@
   </sheetPr>
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B22" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B16" workbookViewId="0">
       <selection activeCell="D22" sqref="D22:K22"/>
     </sheetView>
   </sheetViews>
@@ -2388,11 +2427,11 @@
         <f>Proposal!E5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="169">
+      <c r="E5" s="167">
         <f>Proposal!I5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="169"/>
+      <c r="F5" s="167"/>
       <c r="G5" s="62">
         <f>Proposal!K5</f>
         <v>0</v>
@@ -2617,14 +2656,14 @@
       <c r="C18" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="171"/>
-      <c r="E18" s="171"/>
-      <c r="F18" s="171"/>
-      <c r="G18" s="171"/>
-      <c r="H18" s="171"/>
-      <c r="I18" s="171"/>
-      <c r="J18" s="171"/>
-      <c r="K18" s="171"/>
+      <c r="D18" s="169"/>
+      <c r="E18" s="169"/>
+      <c r="F18" s="169"/>
+      <c r="G18" s="169"/>
+      <c r="H18" s="169"/>
+      <c r="I18" s="169"/>
+      <c r="J18" s="169"/>
+      <c r="K18" s="169"/>
       <c r="L18" s="114"/>
       <c r="M18" s="114"/>
       <c r="N18" s="114"/>
@@ -2655,14 +2694,14 @@
       <c r="C20" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="172"/>
-      <c r="E20" s="172"/>
-      <c r="F20" s="172"/>
-      <c r="G20" s="172"/>
-      <c r="H20" s="172"/>
-      <c r="I20" s="172"/>
-      <c r="J20" s="172"/>
-      <c r="K20" s="172"/>
+      <c r="D20" s="170"/>
+      <c r="E20" s="170"/>
+      <c r="F20" s="170"/>
+      <c r="G20" s="170"/>
+      <c r="H20" s="170"/>
+      <c r="I20" s="170"/>
+      <c r="J20" s="170"/>
+      <c r="K20" s="170"/>
       <c r="L20" s="114"/>
       <c r="M20" s="114"/>
       <c r="N20" s="114"/>
@@ -2693,14 +2732,14 @@
       <c r="C22" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="171"/>
-      <c r="E22" s="171"/>
-      <c r="F22" s="171"/>
-      <c r="G22" s="171"/>
-      <c r="H22" s="171"/>
-      <c r="I22" s="171"/>
-      <c r="J22" s="171"/>
-      <c r="K22" s="171"/>
+      <c r="D22" s="169"/>
+      <c r="E22" s="169"/>
+      <c r="F22" s="169"/>
+      <c r="G22" s="169"/>
+      <c r="H22" s="169"/>
+      <c r="I22" s="169"/>
+      <c r="J22" s="169"/>
+      <c r="K22" s="169"/>
       <c r="L22" s="63"/>
       <c r="M22" s="63"/>
       <c r="N22" s="63"/>
@@ -2724,14 +2763,14 @@
       <c r="C24" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="172"/>
-      <c r="E24" s="172"/>
-      <c r="F24" s="172"/>
-      <c r="G24" s="172"/>
-      <c r="H24" s="172"/>
-      <c r="I24" s="172"/>
-      <c r="J24" s="172"/>
-      <c r="K24" s="172"/>
+      <c r="D24" s="170"/>
+      <c r="E24" s="170"/>
+      <c r="F24" s="170"/>
+      <c r="G24" s="170"/>
+      <c r="H24" s="170"/>
+      <c r="I24" s="170"/>
+      <c r="J24" s="170"/>
+      <c r="K24" s="170"/>
     </row>
     <row r="25" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
@@ -2748,24 +2787,24 @@
       <c r="C26" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="171"/>
-      <c r="E26" s="172"/>
-      <c r="F26" s="172"/>
-      <c r="G26" s="172"/>
-      <c r="H26" s="172"/>
-      <c r="I26" s="172"/>
-      <c r="J26" s="172"/>
-      <c r="K26" s="172"/>
+      <c r="D26" s="169"/>
+      <c r="E26" s="170"/>
+      <c r="F26" s="170"/>
+      <c r="G26" s="170"/>
+      <c r="H26" s="170"/>
+      <c r="I26" s="170"/>
+      <c r="J26" s="170"/>
+      <c r="K26" s="170"/>
     </row>
     <row r="27" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="170"/>
-      <c r="E27" s="170"/>
-      <c r="F27" s="170"/>
-      <c r="G27" s="170"/>
-      <c r="H27" s="170"/>
-      <c r="I27" s="170"/>
-      <c r="J27" s="170"/>
-      <c r="K27" s="170"/>
+      <c r="D27" s="168"/>
+      <c r="E27" s="168"/>
+      <c r="F27" s="168"/>
+      <c r="G27" s="168"/>
+      <c r="H27" s="168"/>
+      <c r="I27" s="168"/>
+      <c r="J27" s="168"/>
+      <c r="K27" s="168"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2795,7 +2834,7 @@
   </sheetPr>
   <dimension ref="B1:P7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2848,19 +2887,19 @@
         <f>Proposal!O5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="169"/>
-      <c r="H5" s="169"/>
-      <c r="I5" s="169"/>
-      <c r="J5" s="169"/>
-      <c r="K5" s="169"/>
-      <c r="L5" s="169"/>
-      <c r="M5" s="169"/>
-      <c r="N5" s="169"/>
-      <c r="O5" s="169"/>
-      <c r="P5" s="169"/>
+      <c r="D5" s="167"/>
+      <c r="E5" s="167"/>
+      <c r="F5" s="167"/>
+      <c r="G5" s="167"/>
+      <c r="H5" s="167"/>
+      <c r="I5" s="167"/>
+      <c r="J5" s="167"/>
+      <c r="K5" s="167"/>
+      <c r="L5" s="167"/>
+      <c r="M5" s="167"/>
+      <c r="N5" s="167"/>
+      <c r="O5" s="167"/>
+      <c r="P5" s="167"/>
     </row>
     <row r="6" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P6" s="54"/>
@@ -3025,24 +3064,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="177" t="s">
+      <c r="G7" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="177"/>
-      <c r="I7" s="177"/>
-      <c r="J7" s="177"/>
-      <c r="K7" s="177"/>
-      <c r="L7" s="178"/>
+      <c r="H7" s="175"/>
+      <c r="I7" s="175"/>
+      <c r="J7" s="175"/>
+      <c r="K7" s="175"/>
+      <c r="L7" s="176"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="177" t="s">
+      <c r="N7" s="175" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="177"/>
-      <c r="P7" s="177"/>
-      <c r="Q7" s="177"/>
-      <c r="R7" s="177"/>
-      <c r="S7" s="177"/>
-      <c r="T7" s="178"/>
+      <c r="O7" s="175"/>
+      <c r="P7" s="175"/>
+      <c r="Q7" s="175"/>
+      <c r="R7" s="175"/>
+      <c r="S7" s="175"/>
+      <c r="T7" s="176"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -3286,24 +3325,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="174" t="s">
+      <c r="G13" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="175"/>
-      <c r="I13" s="175"/>
-      <c r="J13" s="175"/>
-      <c r="K13" s="175"/>
-      <c r="L13" s="176"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
+      <c r="L13" s="174"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="174" t="s">
+      <c r="N13" s="172" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="175"/>
-      <c r="P13" s="175"/>
-      <c r="Q13" s="175"/>
-      <c r="R13" s="175"/>
-      <c r="S13" s="175"/>
-      <c r="T13" s="176"/>
+      <c r="O13" s="173"/>
+      <c r="P13" s="173"/>
+      <c r="Q13" s="173"/>
+      <c r="R13" s="173"/>
+      <c r="S13" s="173"/>
+      <c r="T13" s="174"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="35" t="s">
@@ -3543,24 +3582,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="174" t="s">
+      <c r="G19" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="175"/>
-      <c r="I19" s="175"/>
-      <c r="J19" s="175"/>
-      <c r="K19" s="175"/>
-      <c r="L19" s="176"/>
+      <c r="H19" s="173"/>
+      <c r="I19" s="173"/>
+      <c r="J19" s="173"/>
+      <c r="K19" s="173"/>
+      <c r="L19" s="174"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="174" t="s">
+      <c r="N19" s="172" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="175"/>
-      <c r="P19" s="175"/>
-      <c r="Q19" s="175"/>
-      <c r="R19" s="175"/>
-      <c r="S19" s="175"/>
-      <c r="T19" s="176"/>
+      <c r="O19" s="173"/>
+      <c r="P19" s="173"/>
+      <c r="Q19" s="173"/>
+      <c r="R19" s="173"/>
+      <c r="S19" s="173"/>
+      <c r="T19" s="174"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="35" t="s">
@@ -3830,25 +3869,25 @@
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="179" t="s">
+      <c r="D25" s="177" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="179"/>
-      <c r="F25" s="179"/>
-      <c r="G25" s="179"/>
-      <c r="H25" s="179"/>
-      <c r="I25" s="179"/>
-      <c r="J25" s="179"/>
-      <c r="K25" s="179"/>
-      <c r="L25" s="179"/>
-      <c r="M25" s="179"/>
-      <c r="N25" s="179"/>
-      <c r="O25" s="179"/>
-      <c r="P25" s="179"/>
-      <c r="Q25" s="179"/>
-      <c r="R25" s="179"/>
-      <c r="S25" s="179"/>
-      <c r="T25" s="179"/>
+      <c r="E25" s="177"/>
+      <c r="F25" s="177"/>
+      <c r="G25" s="177"/>
+      <c r="H25" s="177"/>
+      <c r="I25" s="177"/>
+      <c r="J25" s="177"/>
+      <c r="K25" s="177"/>
+      <c r="L25" s="177"/>
+      <c r="M25" s="177"/>
+      <c r="N25" s="177"/>
+      <c r="O25" s="177"/>
+      <c r="P25" s="177"/>
+      <c r="Q25" s="177"/>
+      <c r="R25" s="177"/>
+      <c r="S25" s="177"/>
+      <c r="T25" s="177"/>
     </row>
     <row r="26" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -3874,25 +3913,25 @@
       <c r="B27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="179" t="s">
+      <c r="D27" s="177" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="179"/>
-      <c r="F27" s="179"/>
-      <c r="G27" s="179"/>
-      <c r="H27" s="179"/>
-      <c r="I27" s="179"/>
-      <c r="J27" s="179"/>
-      <c r="K27" s="179"/>
-      <c r="L27" s="179"/>
-      <c r="M27" s="179"/>
-      <c r="N27" s="179"/>
-      <c r="O27" s="179"/>
-      <c r="P27" s="179"/>
-      <c r="Q27" s="179"/>
-      <c r="R27" s="179"/>
-      <c r="S27" s="179"/>
-      <c r="T27" s="179"/>
+      <c r="E27" s="177"/>
+      <c r="F27" s="177"/>
+      <c r="G27" s="177"/>
+      <c r="H27" s="177"/>
+      <c r="I27" s="177"/>
+      <c r="J27" s="177"/>
+      <c r="K27" s="177"/>
+      <c r="L27" s="177"/>
+      <c r="M27" s="177"/>
+      <c r="N27" s="177"/>
+      <c r="O27" s="177"/>
+      <c r="P27" s="177"/>
+      <c r="Q27" s="177"/>
+      <c r="R27" s="177"/>
+      <c r="S27" s="177"/>
+      <c r="T27" s="177"/>
     </row>
     <row r="28" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
@@ -3918,25 +3957,25 @@
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="179" t="s">
+      <c r="D29" s="177" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="179"/>
-      <c r="F29" s="179"/>
-      <c r="G29" s="179"/>
-      <c r="H29" s="179"/>
-      <c r="I29" s="179"/>
-      <c r="J29" s="179"/>
-      <c r="K29" s="179"/>
-      <c r="L29" s="179"/>
-      <c r="M29" s="179"/>
-      <c r="N29" s="179"/>
-      <c r="O29" s="179"/>
-      <c r="P29" s="179"/>
-      <c r="Q29" s="179"/>
-      <c r="R29" s="179"/>
-      <c r="S29" s="179"/>
-      <c r="T29" s="179"/>
+      <c r="E29" s="177"/>
+      <c r="F29" s="177"/>
+      <c r="G29" s="177"/>
+      <c r="H29" s="177"/>
+      <c r="I29" s="177"/>
+      <c r="J29" s="177"/>
+      <c r="K29" s="177"/>
+      <c r="L29" s="177"/>
+      <c r="M29" s="177"/>
+      <c r="N29" s="177"/>
+      <c r="O29" s="177"/>
+      <c r="P29" s="177"/>
+      <c r="Q29" s="177"/>
+      <c r="R29" s="177"/>
+      <c r="S29" s="177"/>
+      <c r="T29" s="177"/>
     </row>
     <row r="30" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
@@ -3962,25 +4001,25 @@
       <c r="B31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="179" t="s">
+      <c r="D31" s="177" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="179"/>
-      <c r="F31" s="179"/>
-      <c r="G31" s="179"/>
-      <c r="H31" s="179"/>
-      <c r="I31" s="179"/>
-      <c r="J31" s="179"/>
-      <c r="K31" s="179"/>
-      <c r="L31" s="179"/>
-      <c r="M31" s="179"/>
-      <c r="N31" s="179"/>
-      <c r="O31" s="179"/>
-      <c r="P31" s="179"/>
-      <c r="Q31" s="179"/>
-      <c r="R31" s="179"/>
-      <c r="S31" s="179"/>
-      <c r="T31" s="179"/>
+      <c r="E31" s="177"/>
+      <c r="F31" s="177"/>
+      <c r="G31" s="177"/>
+      <c r="H31" s="177"/>
+      <c r="I31" s="177"/>
+      <c r="J31" s="177"/>
+      <c r="K31" s="177"/>
+      <c r="L31" s="177"/>
+      <c r="M31" s="177"/>
+      <c r="N31" s="177"/>
+      <c r="O31" s="177"/>
+      <c r="P31" s="177"/>
+      <c r="Q31" s="177"/>
+      <c r="R31" s="177"/>
+      <c r="S31" s="177"/>
+      <c r="T31" s="177"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -4006,25 +4045,25 @@
       <c r="B33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="179" t="s">
+      <c r="D33" s="177" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="179"/>
-      <c r="F33" s="179"/>
-      <c r="G33" s="179"/>
-      <c r="H33" s="179"/>
-      <c r="I33" s="179"/>
-      <c r="J33" s="179"/>
-      <c r="K33" s="179"/>
-      <c r="L33" s="179"/>
-      <c r="M33" s="179"/>
-      <c r="N33" s="179"/>
-      <c r="O33" s="179"/>
-      <c r="P33" s="179"/>
-      <c r="Q33" s="179"/>
-      <c r="R33" s="179"/>
-      <c r="S33" s="179"/>
-      <c r="T33" s="179"/>
+      <c r="E33" s="177"/>
+      <c r="F33" s="177"/>
+      <c r="G33" s="177"/>
+      <c r="H33" s="177"/>
+      <c r="I33" s="177"/>
+      <c r="J33" s="177"/>
+      <c r="K33" s="177"/>
+      <c r="L33" s="177"/>
+      <c r="M33" s="177"/>
+      <c r="N33" s="177"/>
+      <c r="O33" s="177"/>
+      <c r="P33" s="177"/>
+      <c r="Q33" s="177"/>
+      <c r="R33" s="177"/>
+      <c r="S33" s="177"/>
+      <c r="T33" s="177"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -4050,25 +4089,25 @@
       <c r="B35" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="173" t="s">
+      <c r="D35" s="171" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="173"/>
-      <c r="F35" s="173"/>
-      <c r="G35" s="173"/>
-      <c r="H35" s="173"/>
-      <c r="I35" s="173"/>
-      <c r="J35" s="173"/>
-      <c r="K35" s="173"/>
-      <c r="L35" s="173"/>
-      <c r="M35" s="173"/>
-      <c r="N35" s="173"/>
-      <c r="O35" s="173"/>
-      <c r="P35" s="173"/>
-      <c r="Q35" s="173"/>
-      <c r="R35" s="173"/>
-      <c r="S35" s="173"/>
-      <c r="T35" s="173"/>
+      <c r="E35" s="171"/>
+      <c r="F35" s="171"/>
+      <c r="G35" s="171"/>
+      <c r="H35" s="171"/>
+      <c r="I35" s="171"/>
+      <c r="J35" s="171"/>
+      <c r="K35" s="171"/>
+      <c r="L35" s="171"/>
+      <c r="M35" s="171"/>
+      <c r="N35" s="171"/>
+      <c r="O35" s="171"/>
+      <c r="P35" s="171"/>
+      <c r="Q35" s="171"/>
+      <c r="R35" s="171"/>
+      <c r="S35" s="171"/>
+      <c r="T35" s="171"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4210,24 +4249,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="177" t="s">
+      <c r="G7" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="177"/>
-      <c r="I7" s="177"/>
-      <c r="J7" s="177"/>
-      <c r="K7" s="177"/>
-      <c r="L7" s="178"/>
+      <c r="H7" s="175"/>
+      <c r="I7" s="175"/>
+      <c r="J7" s="175"/>
+      <c r="K7" s="175"/>
+      <c r="L7" s="176"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="177" t="s">
+      <c r="N7" s="175" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="177"/>
-      <c r="P7" s="177"/>
-      <c r="Q7" s="177"/>
-      <c r="R7" s="177"/>
-      <c r="S7" s="177"/>
-      <c r="T7" s="178"/>
+      <c r="O7" s="175"/>
+      <c r="P7" s="175"/>
+      <c r="Q7" s="175"/>
+      <c r="R7" s="175"/>
+      <c r="S7" s="175"/>
+      <c r="T7" s="176"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -4469,24 +4508,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="174" t="s">
+      <c r="G13" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="175"/>
-      <c r="I13" s="175"/>
-      <c r="J13" s="175"/>
-      <c r="K13" s="175"/>
-      <c r="L13" s="176"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
+      <c r="L13" s="174"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="174" t="s">
+      <c r="N13" s="172" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="175"/>
-      <c r="P13" s="175"/>
-      <c r="Q13" s="175"/>
-      <c r="R13" s="175"/>
-      <c r="S13" s="175"/>
-      <c r="T13" s="176"/>
+      <c r="O13" s="173"/>
+      <c r="P13" s="173"/>
+      <c r="Q13" s="173"/>
+      <c r="R13" s="173"/>
+      <c r="S13" s="173"/>
+      <c r="T13" s="174"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="35" t="s">
@@ -4724,24 +4763,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="174" t="s">
+      <c r="G19" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="175"/>
-      <c r="I19" s="175"/>
-      <c r="J19" s="175"/>
-      <c r="K19" s="175"/>
-      <c r="L19" s="176"/>
+      <c r="H19" s="173"/>
+      <c r="I19" s="173"/>
+      <c r="J19" s="173"/>
+      <c r="K19" s="173"/>
+      <c r="L19" s="174"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="174" t="s">
+      <c r="N19" s="172" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="175"/>
-      <c r="P19" s="175"/>
-      <c r="Q19" s="175"/>
-      <c r="R19" s="175"/>
-      <c r="S19" s="175"/>
-      <c r="T19" s="176"/>
+      <c r="O19" s="173"/>
+      <c r="P19" s="173"/>
+      <c r="Q19" s="173"/>
+      <c r="R19" s="173"/>
+      <c r="S19" s="173"/>
+      <c r="T19" s="174"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="35" t="s">
@@ -4979,24 +5018,24 @@
       <c r="D25" s="6"/>
       <c r="E25" s="20"/>
       <c r="F25" s="25"/>
-      <c r="G25" s="174" t="s">
+      <c r="G25" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="175"/>
-      <c r="I25" s="175"/>
-      <c r="J25" s="175"/>
-      <c r="K25" s="175"/>
-      <c r="L25" s="176"/>
+      <c r="H25" s="173"/>
+      <c r="I25" s="173"/>
+      <c r="J25" s="173"/>
+      <c r="K25" s="173"/>
+      <c r="L25" s="174"/>
       <c r="M25" s="30"/>
-      <c r="N25" s="174" t="s">
+      <c r="N25" s="172" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="175"/>
-      <c r="P25" s="175"/>
-      <c r="Q25" s="175"/>
-      <c r="R25" s="175"/>
-      <c r="S25" s="175"/>
-      <c r="T25" s="176"/>
+      <c r="O25" s="173"/>
+      <c r="P25" s="173"/>
+      <c r="Q25" s="173"/>
+      <c r="R25" s="173"/>
+      <c r="S25" s="173"/>
+      <c r="T25" s="174"/>
     </row>
     <row r="26" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="35" t="s">
@@ -5234,26 +5273,26 @@
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="169" t="s">
+      <c r="C31" s="167" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="169"/>
-      <c r="E31" s="169"/>
-      <c r="F31" s="169"/>
-      <c r="G31" s="169"/>
-      <c r="H31" s="169"/>
-      <c r="I31" s="169"/>
-      <c r="J31" s="169"/>
-      <c r="K31" s="169"/>
-      <c r="L31" s="169"/>
-      <c r="M31" s="169"/>
-      <c r="N31" s="169"/>
-      <c r="O31" s="169"/>
-      <c r="P31" s="169"/>
-      <c r="Q31" s="169"/>
-      <c r="R31" s="169"/>
-      <c r="S31" s="169"/>
-      <c r="T31" s="169"/>
+      <c r="D31" s="167"/>
+      <c r="E31" s="167"/>
+      <c r="F31" s="167"/>
+      <c r="G31" s="167"/>
+      <c r="H31" s="167"/>
+      <c r="I31" s="167"/>
+      <c r="J31" s="167"/>
+      <c r="K31" s="167"/>
+      <c r="L31" s="167"/>
+      <c r="M31" s="167"/>
+      <c r="N31" s="167"/>
+      <c r="O31" s="167"/>
+      <c r="P31" s="167"/>
+      <c r="Q31" s="167"/>
+      <c r="R31" s="167"/>
+      <c r="S31" s="167"/>
+      <c r="T31" s="167"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -5280,26 +5319,26 @@
       <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="169" t="s">
+      <c r="C33" s="167" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="169"/>
-      <c r="E33" s="169"/>
-      <c r="F33" s="169"/>
-      <c r="G33" s="169"/>
-      <c r="H33" s="169"/>
-      <c r="I33" s="169"/>
-      <c r="J33" s="169"/>
-      <c r="K33" s="169"/>
-      <c r="L33" s="169"/>
-      <c r="M33" s="169"/>
-      <c r="N33" s="169"/>
-      <c r="O33" s="169"/>
-      <c r="P33" s="169"/>
-      <c r="Q33" s="169"/>
-      <c r="R33" s="169"/>
-      <c r="S33" s="169"/>
-      <c r="T33" s="169"/>
+      <c r="D33" s="167"/>
+      <c r="E33" s="167"/>
+      <c r="F33" s="167"/>
+      <c r="G33" s="167"/>
+      <c r="H33" s="167"/>
+      <c r="I33" s="167"/>
+      <c r="J33" s="167"/>
+      <c r="K33" s="167"/>
+      <c r="L33" s="167"/>
+      <c r="M33" s="167"/>
+      <c r="N33" s="167"/>
+      <c r="O33" s="167"/>
+      <c r="P33" s="167"/>
+      <c r="Q33" s="167"/>
+      <c r="R33" s="167"/>
+      <c r="S33" s="167"/>
+      <c r="T33" s="167"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -5326,26 +5365,26 @@
       <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="169" t="s">
+      <c r="C35" s="167" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="169"/>
-      <c r="E35" s="169"/>
-      <c r="F35" s="169"/>
-      <c r="G35" s="169"/>
-      <c r="H35" s="169"/>
-      <c r="I35" s="169"/>
-      <c r="J35" s="169"/>
-      <c r="K35" s="169"/>
-      <c r="L35" s="169"/>
-      <c r="M35" s="169"/>
-      <c r="N35" s="169"/>
-      <c r="O35" s="169"/>
-      <c r="P35" s="169"/>
-      <c r="Q35" s="169"/>
-      <c r="R35" s="169"/>
-      <c r="S35" s="169"/>
-      <c r="T35" s="169"/>
+      <c r="D35" s="167"/>
+      <c r="E35" s="167"/>
+      <c r="F35" s="167"/>
+      <c r="G35" s="167"/>
+      <c r="H35" s="167"/>
+      <c r="I35" s="167"/>
+      <c r="J35" s="167"/>
+      <c r="K35" s="167"/>
+      <c r="L35" s="167"/>
+      <c r="M35" s="167"/>
+      <c r="N35" s="167"/>
+      <c r="O35" s="167"/>
+      <c r="P35" s="167"/>
+      <c r="Q35" s="167"/>
+      <c r="R35" s="167"/>
+      <c r="S35" s="167"/>
+      <c r="T35" s="167"/>
     </row>
     <row r="36" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
@@ -5372,26 +5411,26 @@
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="169" t="s">
+      <c r="C37" s="167" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="169"/>
-      <c r="E37" s="169"/>
-      <c r="F37" s="169"/>
-      <c r="G37" s="169"/>
-      <c r="H37" s="169"/>
-      <c r="I37" s="169"/>
-      <c r="J37" s="169"/>
-      <c r="K37" s="169"/>
-      <c r="L37" s="169"/>
-      <c r="M37" s="169"/>
-      <c r="N37" s="169"/>
-      <c r="O37" s="169"/>
-      <c r="P37" s="169"/>
-      <c r="Q37" s="169"/>
-      <c r="R37" s="169"/>
-      <c r="S37" s="169"/>
-      <c r="T37" s="169"/>
+      <c r="D37" s="167"/>
+      <c r="E37" s="167"/>
+      <c r="F37" s="167"/>
+      <c r="G37" s="167"/>
+      <c r="H37" s="167"/>
+      <c r="I37" s="167"/>
+      <c r="J37" s="167"/>
+      <c r="K37" s="167"/>
+      <c r="L37" s="167"/>
+      <c r="M37" s="167"/>
+      <c r="N37" s="167"/>
+      <c r="O37" s="167"/>
+      <c r="P37" s="167"/>
+      <c r="Q37" s="167"/>
+      <c r="R37" s="167"/>
+      <c r="S37" s="167"/>
+      <c r="T37" s="167"/>
     </row>
     <row r="38" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
@@ -5418,26 +5457,26 @@
       <c r="B39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="169" t="s">
+      <c r="C39" s="167" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="169"/>
-      <c r="E39" s="169"/>
-      <c r="F39" s="169"/>
-      <c r="G39" s="169"/>
-      <c r="H39" s="169"/>
-      <c r="I39" s="169"/>
-      <c r="J39" s="169"/>
-      <c r="K39" s="169"/>
-      <c r="L39" s="169"/>
-      <c r="M39" s="169"/>
-      <c r="N39" s="169"/>
-      <c r="O39" s="169"/>
-      <c r="P39" s="169"/>
-      <c r="Q39" s="169"/>
-      <c r="R39" s="169"/>
-      <c r="S39" s="169"/>
-      <c r="T39" s="169"/>
+      <c r="D39" s="167"/>
+      <c r="E39" s="167"/>
+      <c r="F39" s="167"/>
+      <c r="G39" s="167"/>
+      <c r="H39" s="167"/>
+      <c r="I39" s="167"/>
+      <c r="J39" s="167"/>
+      <c r="K39" s="167"/>
+      <c r="L39" s="167"/>
+      <c r="M39" s="167"/>
+      <c r="N39" s="167"/>
+      <c r="O39" s="167"/>
+      <c r="P39" s="167"/>
+      <c r="Q39" s="167"/>
+      <c r="R39" s="167"/>
+      <c r="S39" s="167"/>
+      <c r="T39" s="167"/>
     </row>
     <row r="40" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
@@ -5464,34 +5503,29 @@
       <c r="B41" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="171" t="s">
+      <c r="C41" s="169" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="171"/>
-      <c r="E41" s="171"/>
-      <c r="F41" s="171"/>
-      <c r="G41" s="171"/>
-      <c r="H41" s="171"/>
-      <c r="I41" s="171"/>
-      <c r="J41" s="171"/>
-      <c r="K41" s="171"/>
-      <c r="L41" s="171"/>
-      <c r="M41" s="171"/>
-      <c r="N41" s="171"/>
-      <c r="O41" s="171"/>
-      <c r="P41" s="171"/>
-      <c r="Q41" s="171"/>
-      <c r="R41" s="171"/>
-      <c r="S41" s="171"/>
-      <c r="T41" s="171"/>
+      <c r="D41" s="169"/>
+      <c r="E41" s="169"/>
+      <c r="F41" s="169"/>
+      <c r="G41" s="169"/>
+      <c r="H41" s="169"/>
+      <c r="I41" s="169"/>
+      <c r="J41" s="169"/>
+      <c r="K41" s="169"/>
+      <c r="L41" s="169"/>
+      <c r="M41" s="169"/>
+      <c r="N41" s="169"/>
+      <c r="O41" s="169"/>
+      <c r="P41" s="169"/>
+      <c r="Q41" s="169"/>
+      <c r="R41" s="169"/>
+      <c r="S41" s="169"/>
+      <c r="T41" s="169"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5501,6 +5535,11 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5539,94 +5578,94 @@
     </row>
     <row r="3" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:4" s="104" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="180" t="s">
+      <c r="C4" s="178" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="180"/>
+      <c r="D4" s="178"/>
     </row>
     <row r="5" spans="3:4" s="104" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="180" t="s">
+      <c r="C5" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="180"/>
+      <c r="D5" s="178"/>
     </row>
     <row r="6" spans="3:4" s="104" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="180" t="s">
+      <c r="C6" s="178" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="180"/>
+      <c r="D6" s="178"/>
     </row>
     <row r="7" spans="3:4" s="104" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="180" t="s">
+      <c r="C7" s="178" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="180"/>
+      <c r="D7" s="178"/>
     </row>
     <row r="8" spans="3:4" s="104" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="180" t="s">
+      <c r="C8" s="178" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="180"/>
+      <c r="D8" s="178"/>
     </row>
     <row r="9" spans="3:4" s="104" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="180" t="s">
+      <c r="C9" s="178" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="180"/>
+      <c r="D9" s="178"/>
     </row>
     <row r="10" spans="3:4" s="104" customFormat="1" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="180" t="s">
+      <c r="C10" s="178" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="180"/>
+      <c r="D10" s="178"/>
     </row>
     <row r="11" spans="3:4" s="104" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="180" t="s">
+      <c r="C11" s="178" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="180"/>
+      <c r="D11" s="178"/>
     </row>
     <row r="12" spans="3:4" s="104" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="180" t="s">
+      <c r="C12" s="178" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="180"/>
+      <c r="D12" s="178"/>
     </row>
     <row r="13" spans="3:4" s="104" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="180" t="s">
+      <c r="C13" s="178" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="180"/>
+      <c r="D13" s="178"/>
     </row>
     <row r="14" spans="3:4" s="104" customFormat="1" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="180" t="s">
+      <c r="C14" s="178" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="180"/>
+      <c r="D14" s="178"/>
     </row>
     <row r="15" spans="3:4" s="104" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="180" t="s">
+      <c r="C15" s="178" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="180"/>
+      <c r="D15" s="178"/>
     </row>
     <row r="16" spans="3:4" s="104" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="180" t="s">
+      <c r="C16" s="178" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="180"/>
+      <c r="D16" s="178"/>
     </row>
     <row r="17" spans="3:4" s="104" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="180" t="s">
+      <c r="C17" s="178" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="180"/>
+      <c r="D17" s="178"/>
     </row>
     <row r="18" spans="3:4" s="104" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="180" t="s">
+      <c r="C18" s="178" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="180"/>
+      <c r="D18" s="178"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -5722,24 +5761,24 @@
       </c>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="169"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="169"/>
+      <c r="C5" s="167"/>
+      <c r="D5" s="167"/>
+      <c r="E5" s="167"/>
+      <c r="F5" s="167"/>
+      <c r="G5" s="167"/>
       <c r="H5" s="102"/>
-      <c r="I5" s="169"/>
-      <c r="J5" s="169"/>
-      <c r="K5" s="169"/>
-      <c r="L5" s="169"/>
-      <c r="M5" s="169"/>
-      <c r="N5" s="169"/>
+      <c r="I5" s="167"/>
+      <c r="J5" s="167"/>
+      <c r="K5" s="167"/>
+      <c r="L5" s="167"/>
+      <c r="M5" s="167"/>
+      <c r="N5" s="167"/>
       <c r="O5" s="62"/>
-      <c r="P5" s="169"/>
-      <c r="Q5" s="169"/>
-      <c r="R5" s="169"/>
-      <c r="S5" s="169"/>
-      <c r="T5" s="169"/>
+      <c r="P5" s="167"/>
+      <c r="Q5" s="167"/>
+      <c r="R5" s="167"/>
+      <c r="S5" s="167"/>
+      <c r="T5" s="167"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I6" s="29"/>
@@ -5763,21 +5802,21 @@
       <c r="F7" s="6"/>
       <c r="G7" s="20"/>
       <c r="H7" s="55"/>
-      <c r="I7" s="174" t="s">
+      <c r="I7" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="175"/>
-      <c r="K7" s="175"/>
-      <c r="L7" s="175"/>
-      <c r="M7" s="175"/>
-      <c r="N7" s="176"/>
-      <c r="O7" s="174"/>
-      <c r="P7" s="175"/>
-      <c r="Q7" s="175"/>
-      <c r="R7" s="175"/>
-      <c r="S7" s="175"/>
-      <c r="T7" s="175"/>
-      <c r="U7" s="176"/>
+      <c r="J7" s="173"/>
+      <c r="K7" s="173"/>
+      <c r="L7" s="173"/>
+      <c r="M7" s="173"/>
+      <c r="N7" s="174"/>
+      <c r="O7" s="172"/>
+      <c r="P7" s="173"/>
+      <c r="Q7" s="173"/>
+      <c r="R7" s="173"/>
+      <c r="S7" s="173"/>
+      <c r="T7" s="173"/>
+      <c r="U7" s="174"/>
     </row>
     <row r="8" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="85" t="s">
@@ -5938,20 +5977,20 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
-      <c r="H13" s="174"/>
-      <c r="I13" s="175"/>
-      <c r="J13" s="175"/>
-      <c r="K13" s="175"/>
-      <c r="L13" s="175"/>
-      <c r="M13" s="175"/>
-      <c r="N13" s="176"/>
-      <c r="O13" s="174"/>
-      <c r="P13" s="175"/>
-      <c r="Q13" s="175"/>
-      <c r="R13" s="175"/>
-      <c r="S13" s="175"/>
-      <c r="T13" s="175"/>
-      <c r="U13" s="176"/>
+      <c r="H13" s="172"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
+      <c r="L13" s="173"/>
+      <c r="M13" s="173"/>
+      <c r="N13" s="174"/>
+      <c r="O13" s="172"/>
+      <c r="P13" s="173"/>
+      <c r="Q13" s="173"/>
+      <c r="R13" s="173"/>
+      <c r="S13" s="173"/>
+      <c r="T13" s="173"/>
+      <c r="U13" s="174"/>
     </row>
     <row r="14" spans="1:21" s="103" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="54"/>
@@ -6121,22 +6160,22 @@
       </c>
       <c r="D20" s="51"/>
       <c r="E20" s="105"/>
-      <c r="F20" s="181"/>
-      <c r="G20" s="181"/>
-      <c r="H20" s="181"/>
-      <c r="I20" s="181"/>
-      <c r="J20" s="181"/>
-      <c r="K20" s="181"/>
-      <c r="L20" s="181"/>
-      <c r="M20" s="181"/>
-      <c r="N20" s="181"/>
-      <c r="O20" s="181"/>
-      <c r="P20" s="181"/>
-      <c r="Q20" s="181"/>
-      <c r="R20" s="181"/>
-      <c r="S20" s="181"/>
-      <c r="T20" s="181"/>
-      <c r="U20" s="181"/>
+      <c r="F20" s="179"/>
+      <c r="G20" s="179"/>
+      <c r="H20" s="179"/>
+      <c r="I20" s="179"/>
+      <c r="J20" s="179"/>
+      <c r="K20" s="179"/>
+      <c r="L20" s="179"/>
+      <c r="M20" s="179"/>
+      <c r="N20" s="179"/>
+      <c r="O20" s="179"/>
+      <c r="P20" s="179"/>
+      <c r="Q20" s="179"/>
+      <c r="R20" s="179"/>
+      <c r="S20" s="179"/>
+      <c r="T20" s="179"/>
+      <c r="U20" s="179"/>
     </row>
     <row r="21" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
@@ -6165,22 +6204,22 @@
         <v>36</v>
       </c>
       <c r="D22" s="51"/>
-      <c r="F22" s="181"/>
-      <c r="G22" s="181"/>
-      <c r="H22" s="181"/>
-      <c r="I22" s="181"/>
-      <c r="J22" s="181"/>
-      <c r="K22" s="181"/>
-      <c r="L22" s="181"/>
-      <c r="M22" s="181"/>
-      <c r="N22" s="181"/>
-      <c r="O22" s="181"/>
-      <c r="P22" s="181"/>
-      <c r="Q22" s="181"/>
-      <c r="R22" s="181"/>
-      <c r="S22" s="181"/>
-      <c r="T22" s="181"/>
-      <c r="U22" s="181"/>
+      <c r="F22" s="179"/>
+      <c r="G22" s="179"/>
+      <c r="H22" s="179"/>
+      <c r="I22" s="179"/>
+      <c r="J22" s="179"/>
+      <c r="K22" s="179"/>
+      <c r="L22" s="179"/>
+      <c r="M22" s="179"/>
+      <c r="N22" s="179"/>
+      <c r="O22" s="179"/>
+      <c r="P22" s="179"/>
+      <c r="Q22" s="179"/>
+      <c r="R22" s="179"/>
+      <c r="S22" s="179"/>
+      <c r="T22" s="179"/>
+      <c r="U22" s="179"/>
       <c r="V22" s="126"/>
     </row>
     <row r="23" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -6209,22 +6248,22 @@
       </c>
       <c r="D24" s="51"/>
       <c r="E24" s="105"/>
-      <c r="F24" s="181"/>
-      <c r="G24" s="181"/>
-      <c r="H24" s="181"/>
-      <c r="I24" s="181"/>
-      <c r="J24" s="181"/>
-      <c r="K24" s="181"/>
-      <c r="L24" s="181"/>
-      <c r="M24" s="181"/>
-      <c r="N24" s="181"/>
-      <c r="O24" s="181"/>
-      <c r="P24" s="181"/>
-      <c r="Q24" s="181"/>
-      <c r="R24" s="181"/>
-      <c r="S24" s="181"/>
-      <c r="T24" s="181"/>
-      <c r="U24" s="181"/>
+      <c r="F24" s="179"/>
+      <c r="G24" s="179"/>
+      <c r="H24" s="179"/>
+      <c r="I24" s="179"/>
+      <c r="J24" s="179"/>
+      <c r="K24" s="179"/>
+      <c r="L24" s="179"/>
+      <c r="M24" s="179"/>
+      <c r="N24" s="179"/>
+      <c r="O24" s="179"/>
+      <c r="P24" s="179"/>
+      <c r="Q24" s="179"/>
+      <c r="R24" s="179"/>
+      <c r="S24" s="179"/>
+      <c r="T24" s="179"/>
+      <c r="U24" s="179"/>
     </row>
     <row r="25" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
@@ -6253,22 +6292,22 @@
         <v>48</v>
       </c>
       <c r="D26" s="51"/>
-      <c r="F26" s="172"/>
-      <c r="G26" s="172"/>
-      <c r="H26" s="172"/>
-      <c r="I26" s="172"/>
-      <c r="J26" s="172"/>
-      <c r="K26" s="172"/>
-      <c r="L26" s="172"/>
-      <c r="M26" s="172"/>
-      <c r="N26" s="172"/>
-      <c r="O26" s="172"/>
-      <c r="P26" s="172"/>
-      <c r="Q26" s="172"/>
-      <c r="R26" s="172"/>
-      <c r="S26" s="172"/>
-      <c r="T26" s="172"/>
-      <c r="U26" s="172"/>
+      <c r="F26" s="170"/>
+      <c r="G26" s="170"/>
+      <c r="H26" s="170"/>
+      <c r="I26" s="170"/>
+      <c r="J26" s="170"/>
+      <c r="K26" s="170"/>
+      <c r="L26" s="170"/>
+      <c r="M26" s="170"/>
+      <c r="N26" s="170"/>
+      <c r="O26" s="170"/>
+      <c r="P26" s="170"/>
+      <c r="Q26" s="170"/>
+      <c r="R26" s="170"/>
+      <c r="S26" s="170"/>
+      <c r="T26" s="170"/>
+      <c r="U26" s="170"/>
       <c r="V26" s="126"/>
     </row>
     <row r="27" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -6296,25 +6335,33 @@
         <v>49</v>
       </c>
       <c r="D28" s="51"/>
-      <c r="F28" s="171"/>
-      <c r="G28" s="171"/>
-      <c r="H28" s="171"/>
-      <c r="I28" s="171"/>
-      <c r="J28" s="171"/>
-      <c r="K28" s="171"/>
-      <c r="L28" s="171"/>
-      <c r="M28" s="171"/>
-      <c r="N28" s="171"/>
-      <c r="O28" s="171"/>
-      <c r="P28" s="171"/>
-      <c r="Q28" s="171"/>
-      <c r="R28" s="171"/>
-      <c r="S28" s="171"/>
-      <c r="T28" s="171"/>
-      <c r="U28" s="171"/>
+      <c r="F28" s="169"/>
+      <c r="G28" s="169"/>
+      <c r="H28" s="169"/>
+      <c r="I28" s="169"/>
+      <c r="J28" s="169"/>
+      <c r="K28" s="169"/>
+      <c r="L28" s="169"/>
+      <c r="M28" s="169"/>
+      <c r="N28" s="169"/>
+      <c r="O28" s="169"/>
+      <c r="P28" s="169"/>
+      <c r="Q28" s="169"/>
+      <c r="R28" s="169"/>
+      <c r="S28" s="169"/>
+      <c r="T28" s="169"/>
+      <c r="U28" s="169"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
     <mergeCell ref="F28:U28"/>
     <mergeCell ref="F20:U20"/>
     <mergeCell ref="H13:N13"/>
@@ -6323,14 +6370,6 @@
     <mergeCell ref="F24:U24"/>
     <mergeCell ref="F26:U26"/>
     <mergeCell ref="O13:U13"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:U3 C5 C4:N4 P4 R4:U4 U5 C6:U1048576">
     <cfRule type="expression" dxfId="2" priority="3">
@@ -6358,10 +6397,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Q63"/>
+  <dimension ref="B1:Q70"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" activeCellId="6" sqref="B56 B47 B38 B29 B20 B11 B2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6380,19 +6419,19 @@
   <sheetData>
     <row r="1" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="168"/>
-      <c r="C2" s="174"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="175"/>
-      <c r="H2" s="175"/>
-      <c r="I2" s="175"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="174"/>
-      <c r="L2" s="175"/>
-      <c r="M2" s="175"/>
-      <c r="N2" s="176"/>
+      <c r="B2" s="165"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="173"/>
+      <c r="H2" s="173"/>
+      <c r="I2" s="173"/>
+      <c r="J2" s="174"/>
+      <c r="K2" s="172"/>
+      <c r="L2" s="173"/>
+      <c r="M2" s="173"/>
+      <c r="N2" s="174"/>
       <c r="O2" s="29"/>
     </row>
     <row r="3" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6505,986 +6544,1142 @@
       <c r="N8" s="59"/>
       <c r="O8" s="163"/>
     </row>
-    <row r="9" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="143" t="s">
+    <row r="9" spans="2:16" s="166" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="164"/>
-      <c r="D9" s="165"/>
-      <c r="E9" s="165"/>
-      <c r="F9" s="165"/>
-      <c r="G9" s="164"/>
-      <c r="H9" s="165"/>
-      <c r="I9" s="165"/>
-      <c r="J9" s="166"/>
-      <c r="K9" s="164"/>
-      <c r="L9" s="165"/>
-      <c r="M9" s="165"/>
-      <c r="N9" s="165"/>
-      <c r="O9" s="167"/>
-    </row>
-    <row r="11" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="168"/>
-      <c r="C11" s="174"/>
-      <c r="D11" s="175"/>
-      <c r="E11" s="175"/>
-      <c r="F11" s="175"/>
-      <c r="G11" s="176"/>
-      <c r="H11" s="175"/>
-      <c r="I11" s="175"/>
-      <c r="J11" s="175"/>
-      <c r="K11" s="176"/>
-      <c r="L11" s="174"/>
-      <c r="M11" s="175"/>
-      <c r="N11" s="175"/>
-      <c r="O11" s="176"/>
-      <c r="P11" s="29"/>
+      <c r="C9" s="184"/>
+      <c r="D9" s="185"/>
+      <c r="E9" s="185"/>
+      <c r="F9" s="185"/>
+      <c r="G9" s="184"/>
+      <c r="H9" s="185"/>
+      <c r="I9" s="185"/>
+      <c r="J9" s="186"/>
+      <c r="K9" s="184"/>
+      <c r="L9" s="185"/>
+      <c r="M9" s="185"/>
+      <c r="N9" s="185"/>
+      <c r="O9" s="187"/>
+    </row>
+    <row r="10" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="143" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="180"/>
+      <c r="D10" s="181"/>
+      <c r="E10" s="181"/>
+      <c r="F10" s="182"/>
+      <c r="G10" s="180"/>
+      <c r="H10" s="181"/>
+      <c r="I10" s="181"/>
+      <c r="J10" s="182"/>
+      <c r="K10" s="180"/>
+      <c r="L10" s="181"/>
+      <c r="M10" s="181"/>
+      <c r="N10" s="182"/>
+      <c r="O10" s="183"/>
     </row>
     <row r="12" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="61"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="57" t="s">
+      <c r="B12" s="165"/>
+      <c r="C12" s="172"/>
+      <c r="D12" s="173"/>
+      <c r="E12" s="173"/>
+      <c r="F12" s="173"/>
+      <c r="G12" s="174"/>
+      <c r="H12" s="173"/>
+      <c r="I12" s="173"/>
+      <c r="J12" s="173"/>
+      <c r="K12" s="174"/>
+      <c r="L12" s="172"/>
+      <c r="M12" s="173"/>
+      <c r="N12" s="173"/>
+      <c r="O12" s="174"/>
+      <c r="P12" s="29"/>
+    </row>
+    <row r="13" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="61"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="57" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="158" t="s">
+    <row r="14" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="158" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="135"/>
-      <c r="D13" s="136"/>
-      <c r="E13" s="136"/>
-      <c r="F13" s="136"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="135"/>
-      <c r="I13" s="136"/>
-      <c r="J13" s="136"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="135"/>
-      <c r="M13" s="136"/>
-      <c r="N13" s="136"/>
-      <c r="O13" s="56"/>
-      <c r="P13" s="139" t="s">
+      <c r="C14" s="135"/>
+      <c r="D14" s="136"/>
+      <c r="E14" s="136"/>
+      <c r="F14" s="136"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="135"/>
+      <c r="I14" s="136"/>
+      <c r="J14" s="136"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="135"/>
+      <c r="M14" s="136"/>
+      <c r="N14" s="136"/>
+      <c r="O14" s="56"/>
+      <c r="P14" s="139" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="159" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="138"/>
-      <c r="D14" s="130"/>
-      <c r="E14" s="130"/>
-      <c r="F14" s="130"/>
-      <c r="G14" s="133"/>
-      <c r="H14" s="138"/>
-      <c r="I14" s="130"/>
-      <c r="J14" s="130"/>
-      <c r="K14" s="133"/>
-      <c r="L14" s="138"/>
-      <c r="M14" s="130"/>
-      <c r="N14" s="130"/>
-      <c r="O14" s="133"/>
-      <c r="P14" s="133"/>
     </row>
     <row r="15" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="159" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="137"/>
-      <c r="D15" s="129"/>
-      <c r="E15" s="129"/>
-      <c r="F15" s="129"/>
-      <c r="G15" s="132"/>
-      <c r="H15" s="137"/>
-      <c r="I15" s="129"/>
-      <c r="J15" s="129"/>
-      <c r="K15" s="132"/>
-      <c r="L15" s="137"/>
-      <c r="M15" s="129"/>
-      <c r="N15" s="129"/>
-      <c r="O15" s="132"/>
-      <c r="P15" s="132"/>
+        <v>19</v>
+      </c>
+      <c r="C15" s="138"/>
+      <c r="D15" s="130"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="130"/>
+      <c r="G15" s="133"/>
+      <c r="H15" s="138"/>
+      <c r="I15" s="130"/>
+      <c r="J15" s="130"/>
+      <c r="K15" s="133"/>
+      <c r="L15" s="138"/>
+      <c r="M15" s="130"/>
+      <c r="N15" s="130"/>
+      <c r="O15" s="133"/>
+      <c r="P15" s="133"/>
     </row>
     <row r="16" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="159" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="140"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="141"/>
-      <c r="H16" s="140"/>
-      <c r="I16" s="131"/>
-      <c r="J16" s="131"/>
-      <c r="K16" s="141"/>
-      <c r="L16" s="140"/>
-      <c r="M16" s="131"/>
-      <c r="N16" s="131"/>
-      <c r="O16" s="141"/>
-      <c r="P16" s="141"/>
+        <v>24</v>
+      </c>
+      <c r="C16" s="137"/>
+      <c r="D16" s="129"/>
+      <c r="E16" s="129"/>
+      <c r="F16" s="129"/>
+      <c r="G16" s="132"/>
+      <c r="H16" s="137"/>
+      <c r="I16" s="129"/>
+      <c r="J16" s="129"/>
+      <c r="K16" s="132"/>
+      <c r="L16" s="137"/>
+      <c r="M16" s="129"/>
+      <c r="N16" s="129"/>
+      <c r="O16" s="132"/>
+      <c r="P16" s="132"/>
     </row>
     <row r="17" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="159" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="140"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="131"/>
+      <c r="G17" s="141"/>
+      <c r="H17" s="140"/>
+      <c r="I17" s="131"/>
+      <c r="J17" s="131"/>
+      <c r="K17" s="141"/>
+      <c r="L17" s="140"/>
+      <c r="M17" s="131"/>
+      <c r="N17" s="131"/>
+      <c r="O17" s="141"/>
+      <c r="P17" s="141"/>
+    </row>
+    <row r="18" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="58"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="58"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="59"/>
-      <c r="O17" s="60"/>
-      <c r="P17" s="60"/>
-    </row>
-    <row r="18" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="143" t="s">
+      <c r="C18" s="58"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
+    </row>
+    <row r="19" spans="2:16" s="166" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="164"/>
-      <c r="D18" s="165"/>
-      <c r="E18" s="165"/>
-      <c r="F18" s="165"/>
-      <c r="G18" s="165"/>
-      <c r="H18" s="164"/>
-      <c r="I18" s="165"/>
-      <c r="J18" s="165"/>
-      <c r="K18" s="166"/>
-      <c r="L18" s="164"/>
-      <c r="M18" s="165"/>
-      <c r="N18" s="165"/>
-      <c r="O18" s="166"/>
-      <c r="P18" s="167"/>
+      <c r="C19" s="184"/>
+      <c r="D19" s="185"/>
+      <c r="E19" s="185"/>
+      <c r="F19" s="185"/>
+      <c r="G19" s="185"/>
+      <c r="H19" s="184"/>
+      <c r="I19" s="185"/>
+      <c r="J19" s="185"/>
+      <c r="K19" s="186"/>
+      <c r="L19" s="184"/>
+      <c r="M19" s="185"/>
+      <c r="N19" s="185"/>
+      <c r="O19" s="186"/>
+      <c r="P19" s="186"/>
     </row>
     <row r="20" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="168"/>
-      <c r="C20" s="174"/>
-      <c r="D20" s="175"/>
-      <c r="E20" s="175"/>
-      <c r="F20" s="176"/>
-      <c r="G20" s="175"/>
-      <c r="H20" s="175"/>
-      <c r="I20" s="175"/>
-      <c r="J20" s="175"/>
-      <c r="K20" s="176"/>
-      <c r="L20" s="174"/>
-      <c r="M20" s="175"/>
-      <c r="N20" s="175"/>
-      <c r="O20" s="176"/>
-      <c r="P20" s="29"/>
-    </row>
-    <row r="21" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="61"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="52"/>
-      <c r="O21" s="52"/>
-      <c r="P21" s="57" t="s">
+      <c r="B20" s="143" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="180"/>
+      <c r="D20" s="181"/>
+      <c r="E20" s="181"/>
+      <c r="F20" s="181"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="180"/>
+      <c r="I20" s="181"/>
+      <c r="J20" s="181"/>
+      <c r="K20" s="182"/>
+      <c r="L20" s="188"/>
+      <c r="M20" s="189"/>
+      <c r="N20" s="189"/>
+      <c r="O20" s="190"/>
+      <c r="P20" s="164"/>
+    </row>
+    <row r="22" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="165"/>
+      <c r="C22" s="172"/>
+      <c r="D22" s="173"/>
+      <c r="E22" s="173"/>
+      <c r="F22" s="174"/>
+      <c r="G22" s="173"/>
+      <c r="H22" s="173"/>
+      <c r="I22" s="173"/>
+      <c r="J22" s="173"/>
+      <c r="K22" s="174"/>
+      <c r="L22" s="172"/>
+      <c r="M22" s="173"/>
+      <c r="N22" s="173"/>
+      <c r="O22" s="174"/>
+      <c r="P22" s="29"/>
+    </row>
+    <row r="23" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="61"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="52"/>
+      <c r="P23" s="57" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="158" t="s">
+    <row r="24" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="158" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="135"/>
-      <c r="D22" s="136"/>
-      <c r="E22" s="136"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="135"/>
-      <c r="H22" s="136"/>
-      <c r="I22" s="136"/>
-      <c r="J22" s="136"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="135"/>
-      <c r="M22" s="136"/>
-      <c r="N22" s="136"/>
-      <c r="O22" s="56"/>
-      <c r="P22" s="139" t="s">
+      <c r="C24" s="135"/>
+      <c r="D24" s="136"/>
+      <c r="E24" s="136"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="135"/>
+      <c r="H24" s="136"/>
+      <c r="I24" s="136"/>
+      <c r="J24" s="136"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="135"/>
+      <c r="M24" s="136"/>
+      <c r="N24" s="136"/>
+      <c r="O24" s="56"/>
+      <c r="P24" s="139" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="159" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="138"/>
-      <c r="D23" s="130"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="133"/>
-      <c r="G23" s="138"/>
-      <c r="H23" s="130"/>
-      <c r="I23" s="130"/>
-      <c r="J23" s="130"/>
-      <c r="K23" s="133"/>
-      <c r="L23" s="138"/>
-      <c r="M23" s="130"/>
-      <c r="N23" s="130"/>
-      <c r="O23" s="133"/>
-      <c r="P23" s="133"/>
-    </row>
-    <row r="24" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="159" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="137"/>
-      <c r="D24" s="129"/>
-      <c r="E24" s="129"/>
-      <c r="F24" s="132"/>
-      <c r="G24" s="137"/>
-      <c r="H24" s="129"/>
-      <c r="I24" s="129"/>
-      <c r="J24" s="129"/>
-      <c r="K24" s="132"/>
-      <c r="L24" s="137"/>
-      <c r="M24" s="129"/>
-      <c r="N24" s="129"/>
-      <c r="O24" s="132"/>
-      <c r="P24" s="132"/>
     </row>
     <row r="25" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="159" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="140"/>
-      <c r="D25" s="131"/>
-      <c r="E25" s="131"/>
-      <c r="F25" s="141"/>
-      <c r="G25" s="140"/>
-      <c r="H25" s="131"/>
-      <c r="I25" s="131"/>
-      <c r="J25" s="131"/>
-      <c r="K25" s="141"/>
-      <c r="L25" s="140"/>
-      <c r="M25" s="131"/>
-      <c r="N25" s="131"/>
-      <c r="O25" s="141"/>
-      <c r="P25" s="141"/>
+        <v>19</v>
+      </c>
+      <c r="C25" s="138"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="130"/>
+      <c r="F25" s="133"/>
+      <c r="G25" s="138"/>
+      <c r="H25" s="130"/>
+      <c r="I25" s="130"/>
+      <c r="J25" s="130"/>
+      <c r="K25" s="133"/>
+      <c r="L25" s="138"/>
+      <c r="M25" s="130"/>
+      <c r="N25" s="130"/>
+      <c r="O25" s="133"/>
+      <c r="P25" s="133"/>
     </row>
     <row r="26" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="159" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="137"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="129"/>
+      <c r="F26" s="132"/>
+      <c r="G26" s="137"/>
+      <c r="H26" s="129"/>
+      <c r="I26" s="129"/>
+      <c r="J26" s="129"/>
+      <c r="K26" s="132"/>
+      <c r="L26" s="137"/>
+      <c r="M26" s="129"/>
+      <c r="N26" s="129"/>
+      <c r="O26" s="132"/>
+      <c r="P26" s="132"/>
+    </row>
+    <row r="27" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="159" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="140"/>
+      <c r="D27" s="131"/>
+      <c r="E27" s="131"/>
+      <c r="F27" s="141"/>
+      <c r="G27" s="140"/>
+      <c r="H27" s="131"/>
+      <c r="I27" s="131"/>
+      <c r="J27" s="131"/>
+      <c r="K27" s="141"/>
+      <c r="L27" s="140"/>
+      <c r="M27" s="131"/>
+      <c r="N27" s="131"/>
+      <c r="O27" s="141"/>
+      <c r="P27" s="141"/>
+    </row>
+    <row r="28" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="59"/>
-      <c r="K26" s="60"/>
-      <c r="L26" s="58"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="59"/>
-      <c r="O26" s="60"/>
-      <c r="P26" s="60"/>
-    </row>
-    <row r="27" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="143" t="s">
+      <c r="C28" s="58"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="59"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="60"/>
+      <c r="P28" s="60"/>
+    </row>
+    <row r="29" spans="2:16" s="166" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="164"/>
-      <c r="D27" s="165"/>
-      <c r="E27" s="165"/>
-      <c r="F27" s="165"/>
-      <c r="G27" s="164"/>
-      <c r="H27" s="165"/>
-      <c r="I27" s="165"/>
-      <c r="J27" s="165"/>
-      <c r="K27" s="166"/>
-      <c r="L27" s="164"/>
-      <c r="M27" s="165"/>
-      <c r="N27" s="165"/>
-      <c r="O27" s="166"/>
-      <c r="P27" s="167"/>
-    </row>
-    <row r="29" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="168"/>
-      <c r="C29" s="174"/>
-      <c r="D29" s="175"/>
-      <c r="E29" s="175"/>
-      <c r="F29" s="176"/>
-      <c r="G29" s="175"/>
-      <c r="H29" s="175"/>
-      <c r="I29" s="175"/>
-      <c r="J29" s="176"/>
-      <c r="K29" s="174"/>
-      <c r="L29" s="175"/>
-      <c r="M29" s="175"/>
-      <c r="N29" s="175"/>
-      <c r="O29" s="176"/>
-      <c r="P29" s="29"/>
+      <c r="C29" s="184"/>
+      <c r="D29" s="185"/>
+      <c r="E29" s="185"/>
+      <c r="F29" s="185"/>
+      <c r="G29" s="184"/>
+      <c r="H29" s="185"/>
+      <c r="I29" s="185"/>
+      <c r="J29" s="185"/>
+      <c r="K29" s="186"/>
+      <c r="L29" s="184"/>
+      <c r="M29" s="185"/>
+      <c r="N29" s="185"/>
+      <c r="O29" s="186"/>
+      <c r="P29" s="186"/>
     </row>
     <row r="30" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="61"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="52"/>
-      <c r="L30" s="52"/>
-      <c r="M30" s="52"/>
-      <c r="N30" s="52"/>
-      <c r="O30" s="52"/>
-      <c r="P30" s="57" t="s">
+      <c r="B30" s="143" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="180"/>
+      <c r="D30" s="181"/>
+      <c r="E30" s="181"/>
+      <c r="F30" s="182"/>
+      <c r="G30" s="180"/>
+      <c r="H30" s="181"/>
+      <c r="I30" s="181"/>
+      <c r="J30" s="181"/>
+      <c r="K30" s="182"/>
+      <c r="L30" s="180"/>
+      <c r="M30" s="181"/>
+      <c r="N30" s="181"/>
+      <c r="O30" s="182"/>
+      <c r="P30" s="183"/>
+    </row>
+    <row r="32" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="165"/>
+      <c r="C32" s="172"/>
+      <c r="D32" s="173"/>
+      <c r="E32" s="173"/>
+      <c r="F32" s="174"/>
+      <c r="G32" s="173"/>
+      <c r="H32" s="173"/>
+      <c r="I32" s="173"/>
+      <c r="J32" s="174"/>
+      <c r="K32" s="172"/>
+      <c r="L32" s="173"/>
+      <c r="M32" s="173"/>
+      <c r="N32" s="173"/>
+      <c r="O32" s="174"/>
+      <c r="P32" s="29"/>
+    </row>
+    <row r="33" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="61"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="52"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="52"/>
+      <c r="M33" s="52"/>
+      <c r="N33" s="52"/>
+      <c r="O33" s="52"/>
+      <c r="P33" s="57" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="158" t="s">
+    <row r="34" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="158" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="135"/>
-      <c r="D31" s="136"/>
-      <c r="E31" s="136"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="135"/>
-      <c r="H31" s="136"/>
-      <c r="I31" s="136"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="135"/>
-      <c r="L31" s="136"/>
-      <c r="M31" s="136"/>
-      <c r="N31" s="136"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="139" t="s">
+      <c r="C34" s="135"/>
+      <c r="D34" s="136"/>
+      <c r="E34" s="136"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="135"/>
+      <c r="H34" s="136"/>
+      <c r="I34" s="136"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="135"/>
+      <c r="L34" s="136"/>
+      <c r="M34" s="136"/>
+      <c r="N34" s="136"/>
+      <c r="O34" s="56"/>
+      <c r="P34" s="139" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="159" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="138"/>
-      <c r="D32" s="130"/>
-      <c r="E32" s="130"/>
-      <c r="F32" s="133"/>
-      <c r="G32" s="138"/>
-      <c r="H32" s="130"/>
-      <c r="I32" s="130"/>
-      <c r="J32" s="133"/>
-      <c r="K32" s="138"/>
-      <c r="L32" s="130"/>
-      <c r="M32" s="130"/>
-      <c r="N32" s="130"/>
-      <c r="O32" s="133"/>
-      <c r="P32" s="133"/>
-    </row>
-    <row r="33" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="159" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" s="137"/>
-      <c r="D33" s="129"/>
-      <c r="E33" s="129"/>
-      <c r="F33" s="132"/>
-      <c r="G33" s="137"/>
-      <c r="H33" s="129"/>
-      <c r="I33" s="129"/>
-      <c r="J33" s="132"/>
-      <c r="K33" s="137"/>
-      <c r="L33" s="129"/>
-      <c r="M33" s="129"/>
-      <c r="N33" s="129"/>
-      <c r="O33" s="132"/>
-      <c r="P33" s="132"/>
-    </row>
-    <row r="34" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="159" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="140"/>
-      <c r="D34" s="131"/>
-      <c r="E34" s="131"/>
-      <c r="F34" s="141"/>
-      <c r="G34" s="140"/>
-      <c r="H34" s="131"/>
-      <c r="I34" s="131"/>
-      <c r="J34" s="141"/>
-      <c r="K34" s="140"/>
-      <c r="L34" s="131"/>
-      <c r="M34" s="131"/>
-      <c r="N34" s="131"/>
-      <c r="O34" s="141"/>
-      <c r="P34" s="141"/>
     </row>
     <row r="35" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="159" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="138"/>
+      <c r="D35" s="130"/>
+      <c r="E35" s="130"/>
+      <c r="F35" s="133"/>
+      <c r="G35" s="138"/>
+      <c r="H35" s="130"/>
+      <c r="I35" s="130"/>
+      <c r="J35" s="133"/>
+      <c r="K35" s="138"/>
+      <c r="L35" s="130"/>
+      <c r="M35" s="130"/>
+      <c r="N35" s="130"/>
+      <c r="O35" s="133"/>
+      <c r="P35" s="133"/>
+    </row>
+    <row r="36" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="159" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="137"/>
+      <c r="D36" s="129"/>
+      <c r="E36" s="129"/>
+      <c r="F36" s="132"/>
+      <c r="G36" s="137"/>
+      <c r="H36" s="129"/>
+      <c r="I36" s="129"/>
+      <c r="J36" s="132"/>
+      <c r="K36" s="137"/>
+      <c r="L36" s="129"/>
+      <c r="M36" s="129"/>
+      <c r="N36" s="129"/>
+      <c r="O36" s="132"/>
+      <c r="P36" s="132"/>
+    </row>
+    <row r="37" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="159" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="140"/>
+      <c r="D37" s="131"/>
+      <c r="E37" s="131"/>
+      <c r="F37" s="141"/>
+      <c r="G37" s="140"/>
+      <c r="H37" s="131"/>
+      <c r="I37" s="131"/>
+      <c r="J37" s="141"/>
+      <c r="K37" s="140"/>
+      <c r="L37" s="131"/>
+      <c r="M37" s="131"/>
+      <c r="N37" s="131"/>
+      <c r="O37" s="141"/>
+      <c r="P37" s="141"/>
+    </row>
+    <row r="38" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="58"/>
-      <c r="D35" s="59"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="59"/>
-      <c r="I35" s="59"/>
-      <c r="J35" s="60"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="59"/>
-      <c r="M35" s="59"/>
-      <c r="N35" s="59"/>
-      <c r="O35" s="60"/>
-      <c r="P35" s="60"/>
-    </row>
-    <row r="36" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="143" t="s">
+      <c r="C38" s="58"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="58"/>
+      <c r="H38" s="59"/>
+      <c r="I38" s="59"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="58"/>
+      <c r="L38" s="59"/>
+      <c r="M38" s="59"/>
+      <c r="N38" s="59"/>
+      <c r="O38" s="60"/>
+      <c r="P38" s="60"/>
+    </row>
+    <row r="39" spans="2:17" s="166" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="164"/>
-      <c r="D36" s="165"/>
-      <c r="E36" s="165"/>
-      <c r="F36" s="165"/>
-      <c r="G36" s="164"/>
-      <c r="H36" s="165"/>
-      <c r="I36" s="165"/>
-      <c r="J36" s="166"/>
-      <c r="K36" s="164"/>
-      <c r="L36" s="165"/>
-      <c r="M36" s="165"/>
-      <c r="N36" s="165"/>
-      <c r="O36" s="166"/>
-      <c r="P36" s="167"/>
-    </row>
-    <row r="38" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="168"/>
-      <c r="C38" s="174"/>
-      <c r="D38" s="175"/>
-      <c r="E38" s="175"/>
-      <c r="F38" s="175"/>
-      <c r="G38" s="176"/>
-      <c r="H38" s="175"/>
-      <c r="I38" s="175"/>
-      <c r="J38" s="175"/>
-      <c r="K38" s="175"/>
-      <c r="L38" s="176"/>
-      <c r="M38" s="174"/>
-      <c r="N38" s="175"/>
-      <c r="O38" s="175"/>
-      <c r="P38" s="176"/>
-      <c r="Q38" s="29"/>
-    </row>
-    <row r="39" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="61"/>
-      <c r="C39" s="52"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="53"/>
-      <c r="H39" s="52"/>
-      <c r="I39" s="52"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="52"/>
-      <c r="L39" s="53"/>
-      <c r="M39" s="52"/>
-      <c r="N39" s="52"/>
-      <c r="O39" s="52"/>
-      <c r="P39" s="52"/>
-      <c r="Q39" s="57" t="s">
+      <c r="C39" s="184"/>
+      <c r="D39" s="185"/>
+      <c r="E39" s="185"/>
+      <c r="F39" s="185"/>
+      <c r="G39" s="184"/>
+      <c r="H39" s="185"/>
+      <c r="I39" s="185"/>
+      <c r="J39" s="186"/>
+      <c r="K39" s="184"/>
+      <c r="L39" s="185"/>
+      <c r="M39" s="185"/>
+      <c r="N39" s="185"/>
+      <c r="O39" s="186"/>
+      <c r="P39" s="186"/>
+    </row>
+    <row r="40" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="143" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="180"/>
+      <c r="D40" s="181"/>
+      <c r="E40" s="181"/>
+      <c r="F40" s="182"/>
+      <c r="G40" s="180"/>
+      <c r="H40" s="181"/>
+      <c r="I40" s="181"/>
+      <c r="J40" s="182"/>
+      <c r="K40" s="180"/>
+      <c r="L40" s="181"/>
+      <c r="M40" s="181"/>
+      <c r="N40" s="181"/>
+      <c r="O40" s="182"/>
+      <c r="P40" s="183"/>
+    </row>
+    <row r="42" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="165"/>
+      <c r="C42" s="172"/>
+      <c r="D42" s="173"/>
+      <c r="E42" s="173"/>
+      <c r="F42" s="173"/>
+      <c r="G42" s="174"/>
+      <c r="H42" s="173"/>
+      <c r="I42" s="173"/>
+      <c r="J42" s="173"/>
+      <c r="K42" s="173"/>
+      <c r="L42" s="174"/>
+      <c r="M42" s="172"/>
+      <c r="N42" s="173"/>
+      <c r="O42" s="173"/>
+      <c r="P42" s="174"/>
+      <c r="Q42" s="29"/>
+    </row>
+    <row r="43" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="61"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="52"/>
+      <c r="K43" s="52"/>
+      <c r="L43" s="53"/>
+      <c r="M43" s="52"/>
+      <c r="N43" s="52"/>
+      <c r="O43" s="52"/>
+      <c r="P43" s="52"/>
+      <c r="Q43" s="57" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="158" t="s">
+    <row r="44" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="158" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="135"/>
-      <c r="D40" s="136"/>
-      <c r="E40" s="136"/>
-      <c r="F40" s="136"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="135"/>
-      <c r="I40" s="136"/>
-      <c r="J40" s="136"/>
-      <c r="K40" s="136"/>
-      <c r="L40" s="56"/>
-      <c r="M40" s="135"/>
-      <c r="N40" s="136"/>
-      <c r="O40" s="136"/>
-      <c r="P40" s="56"/>
-      <c r="Q40" s="139" t="s">
+      <c r="C44" s="135"/>
+      <c r="D44" s="136"/>
+      <c r="E44" s="136"/>
+      <c r="F44" s="136"/>
+      <c r="G44" s="56"/>
+      <c r="H44" s="135"/>
+      <c r="I44" s="136"/>
+      <c r="J44" s="136"/>
+      <c r="K44" s="136"/>
+      <c r="L44" s="56"/>
+      <c r="M44" s="135"/>
+      <c r="N44" s="136"/>
+      <c r="O44" s="136"/>
+      <c r="P44" s="56"/>
+      <c r="Q44" s="139" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="159" t="s">
+    <row r="45" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="159" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="138"/>
-      <c r="D41" s="130"/>
-      <c r="E41" s="130"/>
-      <c r="F41" s="130"/>
-      <c r="G41" s="133"/>
-      <c r="H41" s="138"/>
-      <c r="I41" s="130"/>
-      <c r="J41" s="130"/>
-      <c r="K41" s="130"/>
-      <c r="L41" s="133"/>
-      <c r="M41" s="138"/>
-      <c r="N41" s="130"/>
-      <c r="O41" s="130"/>
-      <c r="P41" s="133"/>
-      <c r="Q41" s="133"/>
-    </row>
-    <row r="42" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="159" t="s">
+      <c r="C45" s="138"/>
+      <c r="D45" s="130"/>
+      <c r="E45" s="130"/>
+      <c r="F45" s="130"/>
+      <c r="G45" s="133"/>
+      <c r="H45" s="138"/>
+      <c r="I45" s="130"/>
+      <c r="J45" s="130"/>
+      <c r="K45" s="130"/>
+      <c r="L45" s="133"/>
+      <c r="M45" s="138"/>
+      <c r="N45" s="130"/>
+      <c r="O45" s="130"/>
+      <c r="P45" s="133"/>
+      <c r="Q45" s="133"/>
+    </row>
+    <row r="46" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="159" t="s">
         <v>24</v>
       </c>
-      <c r="C42" s="137"/>
-      <c r="D42" s="129"/>
-      <c r="E42" s="129"/>
-      <c r="F42" s="129"/>
-      <c r="G42" s="132"/>
-      <c r="H42" s="137"/>
-      <c r="I42" s="129"/>
-      <c r="J42" s="129"/>
-      <c r="K42" s="129"/>
-      <c r="L42" s="132"/>
-      <c r="M42" s="137"/>
-      <c r="N42" s="129"/>
-      <c r="O42" s="129"/>
-      <c r="P42" s="132"/>
-      <c r="Q42" s="132"/>
-    </row>
-    <row r="43" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="159" t="s">
+      <c r="C46" s="137"/>
+      <c r="D46" s="129"/>
+      <c r="E46" s="129"/>
+      <c r="F46" s="129"/>
+      <c r="G46" s="132"/>
+      <c r="H46" s="137"/>
+      <c r="I46" s="129"/>
+      <c r="J46" s="129"/>
+      <c r="K46" s="129"/>
+      <c r="L46" s="132"/>
+      <c r="M46" s="137"/>
+      <c r="N46" s="129"/>
+      <c r="O46" s="129"/>
+      <c r="P46" s="132"/>
+      <c r="Q46" s="132"/>
+    </row>
+    <row r="47" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="159" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="140"/>
-      <c r="D43" s="131"/>
-      <c r="E43" s="131"/>
-      <c r="F43" s="131"/>
-      <c r="G43" s="141"/>
-      <c r="H43" s="140"/>
-      <c r="I43" s="131"/>
-      <c r="J43" s="131"/>
-      <c r="K43" s="131"/>
-      <c r="L43" s="141"/>
-      <c r="M43" s="140"/>
-      <c r="N43" s="131"/>
-      <c r="O43" s="131"/>
-      <c r="P43" s="141"/>
-      <c r="Q43" s="141"/>
-    </row>
-    <row r="44" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="159" t="s">
+      <c r="C47" s="140"/>
+      <c r="D47" s="131"/>
+      <c r="E47" s="131"/>
+      <c r="F47" s="131"/>
+      <c r="G47" s="141"/>
+      <c r="H47" s="140"/>
+      <c r="I47" s="131"/>
+      <c r="J47" s="131"/>
+      <c r="K47" s="131"/>
+      <c r="L47" s="141"/>
+      <c r="M47" s="140"/>
+      <c r="N47" s="131"/>
+      <c r="O47" s="131"/>
+      <c r="P47" s="141"/>
+      <c r="Q47" s="141"/>
+    </row>
+    <row r="48" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="58"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="60"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
-      <c r="K44" s="59"/>
-      <c r="L44" s="60"/>
-      <c r="M44" s="58"/>
-      <c r="N44" s="59"/>
-      <c r="O44" s="59"/>
-      <c r="P44" s="60"/>
-      <c r="Q44" s="60"/>
-    </row>
-    <row r="45" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="143" t="s">
+      <c r="C48" s="58"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="60"/>
+      <c r="H48" s="58"/>
+      <c r="I48" s="59"/>
+      <c r="J48" s="59"/>
+      <c r="K48" s="59"/>
+      <c r="L48" s="60"/>
+      <c r="M48" s="58"/>
+      <c r="N48" s="59"/>
+      <c r="O48" s="59"/>
+      <c r="P48" s="60"/>
+      <c r="Q48" s="60"/>
+    </row>
+    <row r="49" spans="2:17" s="166" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="164"/>
-      <c r="D45" s="165"/>
-      <c r="E45" s="165"/>
-      <c r="F45" s="165"/>
-      <c r="G45" s="165"/>
-      <c r="H45" s="164"/>
-      <c r="I45" s="165"/>
-      <c r="J45" s="165"/>
-      <c r="K45" s="165"/>
-      <c r="L45" s="166"/>
-      <c r="M45" s="164"/>
-      <c r="N45" s="165"/>
-      <c r="O45" s="165"/>
-      <c r="P45" s="166"/>
-      <c r="Q45" s="167"/>
-    </row>
-    <row r="47" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="168"/>
-      <c r="C47" s="174"/>
-      <c r="D47" s="175"/>
-      <c r="E47" s="175"/>
-      <c r="F47" s="175"/>
-      <c r="G47" s="176"/>
-      <c r="H47" s="175"/>
-      <c r="I47" s="175"/>
-      <c r="J47" s="175"/>
-      <c r="K47" s="176"/>
-      <c r="L47" s="174"/>
-      <c r="M47" s="175"/>
-      <c r="N47" s="175"/>
-      <c r="O47" s="175"/>
-      <c r="P47" s="176"/>
-      <c r="Q47" s="29"/>
-    </row>
-    <row r="48" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="61"/>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="52"/>
-      <c r="I48" s="52"/>
-      <c r="J48" s="52"/>
-      <c r="K48" s="53"/>
-      <c r="L48" s="52"/>
-      <c r="M48" s="52"/>
-      <c r="N48" s="52"/>
-      <c r="O48" s="52"/>
-      <c r="P48" s="52"/>
-      <c r="Q48" s="57" t="s">
+      <c r="C49" s="184"/>
+      <c r="D49" s="185"/>
+      <c r="E49" s="185"/>
+      <c r="F49" s="185"/>
+      <c r="G49" s="185"/>
+      <c r="H49" s="184"/>
+      <c r="I49" s="185"/>
+      <c r="J49" s="185"/>
+      <c r="K49" s="185"/>
+      <c r="L49" s="186"/>
+      <c r="M49" s="184"/>
+      <c r="N49" s="185"/>
+      <c r="O49" s="185"/>
+      <c r="P49" s="186"/>
+      <c r="Q49" s="186"/>
+    </row>
+    <row r="50" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="143" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="180"/>
+      <c r="D50" s="181"/>
+      <c r="E50" s="181"/>
+      <c r="F50" s="181"/>
+      <c r="G50" s="182"/>
+      <c r="H50" s="180"/>
+      <c r="I50" s="181"/>
+      <c r="J50" s="181"/>
+      <c r="K50" s="181"/>
+      <c r="L50" s="182"/>
+      <c r="M50" s="180"/>
+      <c r="N50" s="181"/>
+      <c r="O50" s="181"/>
+      <c r="P50" s="182"/>
+      <c r="Q50" s="183"/>
+    </row>
+    <row r="52" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="165"/>
+      <c r="C52" s="172"/>
+      <c r="D52" s="173"/>
+      <c r="E52" s="173"/>
+      <c r="F52" s="173"/>
+      <c r="G52" s="174"/>
+      <c r="H52" s="173"/>
+      <c r="I52" s="173"/>
+      <c r="J52" s="173"/>
+      <c r="K52" s="174"/>
+      <c r="L52" s="172"/>
+      <c r="M52" s="173"/>
+      <c r="N52" s="173"/>
+      <c r="O52" s="173"/>
+      <c r="P52" s="174"/>
+      <c r="Q52" s="29"/>
+    </row>
+    <row r="53" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="61"/>
+      <c r="C53" s="52"/>
+      <c r="D53" s="52"/>
+      <c r="E53" s="52"/>
+      <c r="F53" s="52"/>
+      <c r="G53" s="53"/>
+      <c r="H53" s="52"/>
+      <c r="I53" s="52"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="53"/>
+      <c r="L53" s="52"/>
+      <c r="M53" s="52"/>
+      <c r="N53" s="52"/>
+      <c r="O53" s="52"/>
+      <c r="P53" s="52"/>
+      <c r="Q53" s="57" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="158" t="s">
+    <row r="54" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="158" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="135"/>
-      <c r="D49" s="136"/>
-      <c r="E49" s="136"/>
-      <c r="F49" s="136"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="135"/>
-      <c r="I49" s="136"/>
-      <c r="J49" s="136"/>
-      <c r="K49" s="56"/>
-      <c r="L49" s="135"/>
-      <c r="M49" s="136"/>
-      <c r="N49" s="136"/>
-      <c r="O49" s="136"/>
-      <c r="P49" s="56"/>
-      <c r="Q49" s="139" t="s">
+      <c r="C54" s="135"/>
+      <c r="D54" s="136"/>
+      <c r="E54" s="136"/>
+      <c r="F54" s="136"/>
+      <c r="G54" s="56"/>
+      <c r="H54" s="135"/>
+      <c r="I54" s="136"/>
+      <c r="J54" s="136"/>
+      <c r="K54" s="56"/>
+      <c r="L54" s="135"/>
+      <c r="M54" s="136"/>
+      <c r="N54" s="136"/>
+      <c r="O54" s="136"/>
+      <c r="P54" s="56"/>
+      <c r="Q54" s="139" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="159" t="s">
+    <row r="55" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="159" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="138"/>
-      <c r="D50" s="130"/>
-      <c r="E50" s="130"/>
-      <c r="F50" s="130"/>
-      <c r="G50" s="133"/>
-      <c r="H50" s="138"/>
-      <c r="I50" s="130"/>
-      <c r="J50" s="130"/>
-      <c r="K50" s="133"/>
-      <c r="L50" s="138"/>
-      <c r="M50" s="130"/>
-      <c r="N50" s="130"/>
-      <c r="O50" s="130"/>
-      <c r="P50" s="133"/>
-      <c r="Q50" s="133"/>
-    </row>
-    <row r="51" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="159" t="s">
+      <c r="C55" s="138"/>
+      <c r="D55" s="130"/>
+      <c r="E55" s="130"/>
+      <c r="F55" s="130"/>
+      <c r="G55" s="133"/>
+      <c r="H55" s="138"/>
+      <c r="I55" s="130"/>
+      <c r="J55" s="130"/>
+      <c r="K55" s="133"/>
+      <c r="L55" s="138"/>
+      <c r="M55" s="130"/>
+      <c r="N55" s="130"/>
+      <c r="O55" s="130"/>
+      <c r="P55" s="133"/>
+      <c r="Q55" s="133"/>
+    </row>
+    <row r="56" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="159" t="s">
         <v>24</v>
       </c>
-      <c r="C51" s="137"/>
-      <c r="D51" s="129"/>
-      <c r="E51" s="129"/>
-      <c r="F51" s="129"/>
-      <c r="G51" s="132"/>
-      <c r="H51" s="137"/>
-      <c r="I51" s="129"/>
-      <c r="J51" s="129"/>
-      <c r="K51" s="132"/>
-      <c r="L51" s="137"/>
-      <c r="M51" s="129"/>
-      <c r="N51" s="129"/>
-      <c r="O51" s="129"/>
-      <c r="P51" s="132"/>
-      <c r="Q51" s="132"/>
-    </row>
-    <row r="52" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="159" t="s">
+      <c r="C56" s="137"/>
+      <c r="D56" s="129"/>
+      <c r="E56" s="129"/>
+      <c r="F56" s="129"/>
+      <c r="G56" s="132"/>
+      <c r="H56" s="137"/>
+      <c r="I56" s="129"/>
+      <c r="J56" s="129"/>
+      <c r="K56" s="132"/>
+      <c r="L56" s="137"/>
+      <c r="M56" s="129"/>
+      <c r="N56" s="129"/>
+      <c r="O56" s="129"/>
+      <c r="P56" s="132"/>
+      <c r="Q56" s="132"/>
+    </row>
+    <row r="57" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="159" t="s">
         <v>26</v>
       </c>
-      <c r="C52" s="140"/>
-      <c r="D52" s="131"/>
-      <c r="E52" s="131"/>
-      <c r="F52" s="131"/>
-      <c r="G52" s="141"/>
-      <c r="H52" s="140"/>
-      <c r="I52" s="131"/>
-      <c r="J52" s="131"/>
-      <c r="K52" s="141"/>
-      <c r="L52" s="140"/>
-      <c r="M52" s="131"/>
-      <c r="N52" s="131"/>
-      <c r="O52" s="131"/>
-      <c r="P52" s="141"/>
-      <c r="Q52" s="141"/>
-    </row>
-    <row r="53" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="159" t="s">
+      <c r="C57" s="140"/>
+      <c r="D57" s="131"/>
+      <c r="E57" s="131"/>
+      <c r="F57" s="131"/>
+      <c r="G57" s="141"/>
+      <c r="H57" s="140"/>
+      <c r="I57" s="131"/>
+      <c r="J57" s="131"/>
+      <c r="K57" s="141"/>
+      <c r="L57" s="140"/>
+      <c r="M57" s="131"/>
+      <c r="N57" s="131"/>
+      <c r="O57" s="131"/>
+      <c r="P57" s="141"/>
+      <c r="Q57" s="141"/>
+    </row>
+    <row r="58" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="58"/>
-      <c r="D53" s="59"/>
-      <c r="E53" s="59"/>
-      <c r="F53" s="59"/>
-      <c r="G53" s="60"/>
-      <c r="H53" s="58"/>
-      <c r="I53" s="59"/>
-      <c r="J53" s="59"/>
-      <c r="K53" s="60"/>
-      <c r="L53" s="58"/>
-      <c r="M53" s="59"/>
-      <c r="N53" s="59"/>
-      <c r="O53" s="59"/>
-      <c r="P53" s="60"/>
-      <c r="Q53" s="60"/>
-    </row>
-    <row r="54" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="143" t="s">
+      <c r="C58" s="58"/>
+      <c r="D58" s="59"/>
+      <c r="E58" s="59"/>
+      <c r="F58" s="59"/>
+      <c r="G58" s="60"/>
+      <c r="H58" s="58"/>
+      <c r="I58" s="59"/>
+      <c r="J58" s="59"/>
+      <c r="K58" s="60"/>
+      <c r="L58" s="58"/>
+      <c r="M58" s="59"/>
+      <c r="N58" s="59"/>
+      <c r="O58" s="59"/>
+      <c r="P58" s="60"/>
+      <c r="Q58" s="60"/>
+    </row>
+    <row r="59" spans="2:17" s="166" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="C54" s="164"/>
-      <c r="D54" s="165"/>
-      <c r="E54" s="165"/>
-      <c r="F54" s="165"/>
-      <c r="G54" s="165"/>
-      <c r="H54" s="164"/>
-      <c r="I54" s="165"/>
-      <c r="J54" s="165"/>
-      <c r="K54" s="166"/>
-      <c r="L54" s="164"/>
-      <c r="M54" s="165"/>
-      <c r="N54" s="165"/>
-      <c r="O54" s="165"/>
-      <c r="P54" s="166"/>
-      <c r="Q54" s="167"/>
-    </row>
-    <row r="56" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="168"/>
-      <c r="C56" s="174"/>
-      <c r="D56" s="175"/>
-      <c r="E56" s="175"/>
-      <c r="F56" s="176"/>
-      <c r="G56" s="175"/>
-      <c r="H56" s="175"/>
-      <c r="I56" s="175"/>
-      <c r="J56" s="175"/>
-      <c r="K56" s="176"/>
-      <c r="L56" s="174"/>
-      <c r="M56" s="175"/>
-      <c r="N56" s="175"/>
-      <c r="O56" s="175"/>
-      <c r="P56" s="176"/>
-      <c r="Q56" s="29"/>
-    </row>
-    <row r="57" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="61"/>
-      <c r="C57" s="52"/>
-      <c r="D57" s="52"/>
-      <c r="E57" s="52"/>
-      <c r="F57" s="53"/>
-      <c r="G57" s="52"/>
-      <c r="H57" s="52"/>
-      <c r="I57" s="52"/>
-      <c r="J57" s="52"/>
-      <c r="K57" s="53"/>
-      <c r="L57" s="52"/>
-      <c r="M57" s="52"/>
-      <c r="N57" s="52"/>
-      <c r="O57" s="52"/>
-      <c r="P57" s="52"/>
-      <c r="Q57" s="57" t="s">
+      <c r="C59" s="184"/>
+      <c r="D59" s="185"/>
+      <c r="E59" s="185"/>
+      <c r="F59" s="185"/>
+      <c r="G59" s="185"/>
+      <c r="H59" s="184"/>
+      <c r="I59" s="185"/>
+      <c r="J59" s="185"/>
+      <c r="K59" s="186"/>
+      <c r="L59" s="184"/>
+      <c r="M59" s="185"/>
+      <c r="N59" s="185"/>
+      <c r="O59" s="185"/>
+      <c r="P59" s="186"/>
+      <c r="Q59" s="186"/>
+    </row>
+    <row r="60" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="143" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="180"/>
+      <c r="D60" s="181"/>
+      <c r="E60" s="181"/>
+      <c r="F60" s="181"/>
+      <c r="G60" s="182"/>
+      <c r="H60" s="180"/>
+      <c r="I60" s="181"/>
+      <c r="J60" s="181"/>
+      <c r="K60" s="182"/>
+      <c r="L60" s="180"/>
+      <c r="M60" s="181"/>
+      <c r="N60" s="181"/>
+      <c r="O60" s="181"/>
+      <c r="P60" s="182"/>
+      <c r="Q60" s="183"/>
+    </row>
+    <row r="62" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="165"/>
+      <c r="C62" s="172"/>
+      <c r="D62" s="173"/>
+      <c r="E62" s="173"/>
+      <c r="F62" s="174"/>
+      <c r="G62" s="173"/>
+      <c r="H62" s="173"/>
+      <c r="I62" s="173"/>
+      <c r="J62" s="173"/>
+      <c r="K62" s="174"/>
+      <c r="L62" s="172"/>
+      <c r="M62" s="173"/>
+      <c r="N62" s="173"/>
+      <c r="O62" s="173"/>
+      <c r="P62" s="174"/>
+      <c r="Q62" s="29"/>
+    </row>
+    <row r="63" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="61"/>
+      <c r="C63" s="52"/>
+      <c r="D63" s="52"/>
+      <c r="E63" s="52"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="52"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="52"/>
+      <c r="K63" s="53"/>
+      <c r="L63" s="52"/>
+      <c r="M63" s="52"/>
+      <c r="N63" s="52"/>
+      <c r="O63" s="52"/>
+      <c r="P63" s="52"/>
+      <c r="Q63" s="57" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="158" t="s">
+    <row r="64" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="158" t="s">
         <v>54</v>
       </c>
-      <c r="C58" s="135"/>
-      <c r="D58" s="136"/>
-      <c r="E58" s="136"/>
-      <c r="F58" s="56"/>
-      <c r="G58" s="135"/>
-      <c r="H58" s="136"/>
-      <c r="I58" s="136"/>
-      <c r="J58" s="136"/>
-      <c r="K58" s="56"/>
-      <c r="L58" s="135"/>
-      <c r="M58" s="136"/>
-      <c r="N58" s="136"/>
-      <c r="O58" s="136"/>
-      <c r="P58" s="56"/>
-      <c r="Q58" s="139" t="s">
+      <c r="C64" s="135"/>
+      <c r="D64" s="136"/>
+      <c r="E64" s="136"/>
+      <c r="F64" s="56"/>
+      <c r="G64" s="135"/>
+      <c r="H64" s="136"/>
+      <c r="I64" s="136"/>
+      <c r="J64" s="136"/>
+      <c r="K64" s="56"/>
+      <c r="L64" s="135"/>
+      <c r="M64" s="136"/>
+      <c r="N64" s="136"/>
+      <c r="O64" s="136"/>
+      <c r="P64" s="56"/>
+      <c r="Q64" s="139" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="159" t="s">
+    <row r="65" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="159" t="s">
         <v>19</v>
       </c>
-      <c r="C59" s="138"/>
-      <c r="D59" s="130"/>
-      <c r="E59" s="130"/>
-      <c r="F59" s="133"/>
-      <c r="G59" s="138"/>
-      <c r="H59" s="130"/>
-      <c r="I59" s="130"/>
-      <c r="J59" s="130"/>
-      <c r="K59" s="133"/>
-      <c r="L59" s="138"/>
-      <c r="M59" s="130"/>
-      <c r="N59" s="130"/>
-      <c r="O59" s="130"/>
-      <c r="P59" s="133"/>
-      <c r="Q59" s="133"/>
-    </row>
-    <row r="60" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="159" t="s">
+      <c r="C65" s="138"/>
+      <c r="D65" s="130"/>
+      <c r="E65" s="130"/>
+      <c r="F65" s="133"/>
+      <c r="G65" s="138"/>
+      <c r="H65" s="130"/>
+      <c r="I65" s="130"/>
+      <c r="J65" s="130"/>
+      <c r="K65" s="133"/>
+      <c r="L65" s="138"/>
+      <c r="M65" s="130"/>
+      <c r="N65" s="130"/>
+      <c r="O65" s="130"/>
+      <c r="P65" s="133"/>
+      <c r="Q65" s="133"/>
+    </row>
+    <row r="66" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="159" t="s">
         <v>24</v>
       </c>
-      <c r="C60" s="137"/>
-      <c r="D60" s="129"/>
-      <c r="E60" s="129"/>
-      <c r="F60" s="132"/>
-      <c r="G60" s="137"/>
-      <c r="H60" s="129"/>
-      <c r="I60" s="129"/>
-      <c r="J60" s="129"/>
-      <c r="K60" s="132"/>
-      <c r="L60" s="137"/>
-      <c r="M60" s="129"/>
-      <c r="N60" s="129"/>
-      <c r="O60" s="129"/>
-      <c r="P60" s="132"/>
-      <c r="Q60" s="132"/>
-    </row>
-    <row r="61" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="159" t="s">
+      <c r="C66" s="137"/>
+      <c r="D66" s="129"/>
+      <c r="E66" s="129"/>
+      <c r="F66" s="132"/>
+      <c r="G66" s="137"/>
+      <c r="H66" s="129"/>
+      <c r="I66" s="129"/>
+      <c r="J66" s="129"/>
+      <c r="K66" s="132"/>
+      <c r="L66" s="137"/>
+      <c r="M66" s="129"/>
+      <c r="N66" s="129"/>
+      <c r="O66" s="129"/>
+      <c r="P66" s="132"/>
+      <c r="Q66" s="132"/>
+    </row>
+    <row r="67" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="159" t="s">
         <v>26</v>
       </c>
-      <c r="C61" s="140"/>
-      <c r="D61" s="131"/>
-      <c r="E61" s="131"/>
-      <c r="F61" s="141"/>
-      <c r="G61" s="140"/>
-      <c r="H61" s="131"/>
-      <c r="I61" s="131"/>
-      <c r="J61" s="131"/>
-      <c r="K61" s="141"/>
-      <c r="L61" s="140"/>
-      <c r="M61" s="131"/>
-      <c r="N61" s="131"/>
-      <c r="O61" s="131"/>
-      <c r="P61" s="141"/>
-      <c r="Q61" s="141"/>
-    </row>
-    <row r="62" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="159" t="s">
+      <c r="C67" s="140"/>
+      <c r="D67" s="131"/>
+      <c r="E67" s="131"/>
+      <c r="F67" s="141"/>
+      <c r="G67" s="140"/>
+      <c r="H67" s="131"/>
+      <c r="I67" s="131"/>
+      <c r="J67" s="131"/>
+      <c r="K67" s="141"/>
+      <c r="L67" s="140"/>
+      <c r="M67" s="131"/>
+      <c r="N67" s="131"/>
+      <c r="O67" s="131"/>
+      <c r="P67" s="141"/>
+      <c r="Q67" s="141"/>
+    </row>
+    <row r="68" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="159" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="58"/>
-      <c r="D62" s="59"/>
-      <c r="E62" s="59"/>
-      <c r="F62" s="60"/>
-      <c r="G62" s="58"/>
-      <c r="H62" s="59"/>
-      <c r="I62" s="59"/>
-      <c r="J62" s="59"/>
-      <c r="K62" s="60"/>
-      <c r="L62" s="58"/>
-      <c r="M62" s="59"/>
-      <c r="N62" s="59"/>
-      <c r="O62" s="59"/>
-      <c r="P62" s="60"/>
-      <c r="Q62" s="60"/>
-    </row>
-    <row r="63" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="143" t="s">
+      <c r="C68" s="58"/>
+      <c r="D68" s="59"/>
+      <c r="E68" s="59"/>
+      <c r="F68" s="60"/>
+      <c r="G68" s="58"/>
+      <c r="H68" s="59"/>
+      <c r="I68" s="59"/>
+      <c r="J68" s="59"/>
+      <c r="K68" s="60"/>
+      <c r="L68" s="58"/>
+      <c r="M68" s="59"/>
+      <c r="N68" s="59"/>
+      <c r="O68" s="59"/>
+      <c r="P68" s="60"/>
+      <c r="Q68" s="60"/>
+    </row>
+    <row r="69" spans="2:17" s="166" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="C63" s="164"/>
-      <c r="D63" s="165"/>
-      <c r="E63" s="165"/>
-      <c r="F63" s="165"/>
-      <c r="G63" s="164"/>
-      <c r="H63" s="165"/>
-      <c r="I63" s="165"/>
-      <c r="J63" s="165"/>
-      <c r="K63" s="166"/>
-      <c r="L63" s="164"/>
-      <c r="M63" s="165"/>
-      <c r="N63" s="165"/>
-      <c r="O63" s="165"/>
-      <c r="P63" s="166"/>
-      <c r="Q63" s="167"/>
+      <c r="C69" s="184"/>
+      <c r="D69" s="185"/>
+      <c r="E69" s="185"/>
+      <c r="F69" s="185"/>
+      <c r="G69" s="184"/>
+      <c r="H69" s="185"/>
+      <c r="I69" s="185"/>
+      <c r="J69" s="185"/>
+      <c r="K69" s="186"/>
+      <c r="L69" s="184"/>
+      <c r="M69" s="185"/>
+      <c r="N69" s="185"/>
+      <c r="O69" s="185"/>
+      <c r="P69" s="186"/>
+      <c r="Q69" s="186"/>
+    </row>
+    <row r="70" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="143" t="s">
+        <v>90</v>
+      </c>
+      <c r="C70" s="180"/>
+      <c r="D70" s="181"/>
+      <c r="E70" s="181"/>
+      <c r="F70" s="182"/>
+      <c r="G70" s="180"/>
+      <c r="H70" s="181"/>
+      <c r="I70" s="181"/>
+      <c r="J70" s="181"/>
+      <c r="K70" s="182"/>
+      <c r="L70" s="180"/>
+      <c r="M70" s="181"/>
+      <c r="N70" s="181"/>
+      <c r="O70" s="181"/>
+      <c r="P70" s="182"/>
+      <c r="Q70" s="183"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="42">
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="L20:O20"/>
+    <mergeCell ref="C70:F70"/>
+    <mergeCell ref="G70:K70"/>
+    <mergeCell ref="L70:P70"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="L60:P60"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="H50:L50"/>
+    <mergeCell ref="M50:P50"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="K40:O40"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="G62:K62"/>
+    <mergeCell ref="L62:P62"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="M42:P42"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="L52:P52"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="K32:O32"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="L30:O30"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="L11:O11"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="K29:O29"/>
-    <mergeCell ref="C56:F56"/>
-    <mergeCell ref="G56:K56"/>
-    <mergeCell ref="L56:P56"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="H38:L38"/>
-    <mergeCell ref="M38:P38"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="H47:K47"/>
-    <mergeCell ref="L47:P47"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" sqref="C9:N9 C36:O36 C18:O18 C27:O27 C45:P45 C54:P54 C63:P63" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
+    <dataValidation allowBlank="1" sqref="L20 M50 K10 K40 L60 L70 C10 G10 C20 H20 C70 G70 C60 H60 C50 H50 C40 G40 C30 G30 L30" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="49" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -7498,15 +7693,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7729,6 +7915,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
   <ds:schemaRefs>
@@ -7747,14 +7942,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7771,4 +7958,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged PR 17788: BP-5359_QA and Stage - User is getting error when User enters value in Impres...
BP-5359_QA and Stage - User is getting error when User enters value in Impression per unit field' with delivery type as Custom by week ad length' while creating a new plan
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325B9DD5-DD1A-461E-AA99-77B19CF44296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8420BA5C-7C2F-4C34-8392-BEEB17A07FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="92">
   <si>
     <t>Broadcast Proposal Gorilla Glue Q4 '19 - Q1 '20</t>
   </si>
@@ -681,6 +681,9 @@
   </si>
   <si>
     <t>Total Monthly Cost</t>
+  </si>
+  <si>
+    <t>Fluidity</t>
   </si>
 </sst>
 </file>
@@ -1156,7 +1159,7 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="191">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1649,6 +1652,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -1694,21 +1718,6 @@
     <xf numFmtId="164" fontId="12" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1717,6 +1726,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1725,7 +1737,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF5F8F8"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2359,8 +2378,8 @@
   </sheetPr>
   <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:K22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2409,12 +2428,15 @@
         <v>68</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2427,11 +2449,11 @@
         <f>Proposal!E5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="167">
+      <c r="E5" s="174">
         <f>Proposal!I5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="167"/>
+      <c r="F5" s="174"/>
       <c r="G5" s="62">
         <f>Proposal!K5</f>
         <v>0</v>
@@ -2444,16 +2466,20 @@
         <f>Proposal!O5</f>
         <v>0</v>
       </c>
-      <c r="J5" s="62">
+      <c r="J5" s="193">
         <f>Proposal!P5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="62">
-        <f>Proposal!R5</f>
+      <c r="K5" s="167">
+        <f>Proposal!Q5</f>
         <v>0</v>
       </c>
-      <c r="L5" s="62">
-        <f>Proposal!U5</f>
+      <c r="L5" s="167">
+        <f>Proposal!S5</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="167">
+        <f>Proposal!V5</f>
         <v>0</v>
       </c>
     </row>
@@ -2656,14 +2682,14 @@
       <c r="C18" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="169"/>
-      <c r="E18" s="169"/>
-      <c r="F18" s="169"/>
-      <c r="G18" s="169"/>
-      <c r="H18" s="169"/>
-      <c r="I18" s="169"/>
-      <c r="J18" s="169"/>
-      <c r="K18" s="169"/>
+      <c r="D18" s="176"/>
+      <c r="E18" s="176"/>
+      <c r="F18" s="176"/>
+      <c r="G18" s="176"/>
+      <c r="H18" s="176"/>
+      <c r="I18" s="176"/>
+      <c r="J18" s="176"/>
+      <c r="K18" s="176"/>
       <c r="L18" s="114"/>
       <c r="M18" s="114"/>
       <c r="N18" s="114"/>
@@ -2694,14 +2720,14 @@
       <c r="C20" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="170"/>
-      <c r="E20" s="170"/>
-      <c r="F20" s="170"/>
-      <c r="G20" s="170"/>
-      <c r="H20" s="170"/>
-      <c r="I20" s="170"/>
-      <c r="J20" s="170"/>
-      <c r="K20" s="170"/>
+      <c r="D20" s="177"/>
+      <c r="E20" s="177"/>
+      <c r="F20" s="177"/>
+      <c r="G20" s="177"/>
+      <c r="H20" s="177"/>
+      <c r="I20" s="177"/>
+      <c r="J20" s="177"/>
+      <c r="K20" s="177"/>
       <c r="L20" s="114"/>
       <c r="M20" s="114"/>
       <c r="N20" s="114"/>
@@ -2732,14 +2758,14 @@
       <c r="C22" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="169"/>
-      <c r="E22" s="169"/>
-      <c r="F22" s="169"/>
-      <c r="G22" s="169"/>
-      <c r="H22" s="169"/>
-      <c r="I22" s="169"/>
-      <c r="J22" s="169"/>
-      <c r="K22" s="169"/>
+      <c r="D22" s="176"/>
+      <c r="E22" s="176"/>
+      <c r="F22" s="176"/>
+      <c r="G22" s="176"/>
+      <c r="H22" s="176"/>
+      <c r="I22" s="176"/>
+      <c r="J22" s="176"/>
+      <c r="K22" s="176"/>
       <c r="L22" s="63"/>
       <c r="M22" s="63"/>
       <c r="N22" s="63"/>
@@ -2763,14 +2789,14 @@
       <c r="C24" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="170"/>
-      <c r="E24" s="170"/>
-      <c r="F24" s="170"/>
-      <c r="G24" s="170"/>
-      <c r="H24" s="170"/>
-      <c r="I24" s="170"/>
-      <c r="J24" s="170"/>
-      <c r="K24" s="170"/>
+      <c r="D24" s="177"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="177"/>
+      <c r="G24" s="177"/>
+      <c r="H24" s="177"/>
+      <c r="I24" s="177"/>
+      <c r="J24" s="177"/>
+      <c r="K24" s="177"/>
     </row>
     <row r="25" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
@@ -2787,24 +2813,24 @@
       <c r="C26" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="169"/>
-      <c r="E26" s="170"/>
-      <c r="F26" s="170"/>
-      <c r="G26" s="170"/>
-      <c r="H26" s="170"/>
-      <c r="I26" s="170"/>
-      <c r="J26" s="170"/>
-      <c r="K26" s="170"/>
+      <c r="D26" s="176"/>
+      <c r="E26" s="177"/>
+      <c r="F26" s="177"/>
+      <c r="G26" s="177"/>
+      <c r="H26" s="177"/>
+      <c r="I26" s="177"/>
+      <c r="J26" s="177"/>
+      <c r="K26" s="177"/>
     </row>
     <row r="27" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="168"/>
-      <c r="E27" s="168"/>
-      <c r="F27" s="168"/>
-      <c r="G27" s="168"/>
-      <c r="H27" s="168"/>
-      <c r="I27" s="168"/>
-      <c r="J27" s="168"/>
-      <c r="K27" s="168"/>
+      <c r="D27" s="175"/>
+      <c r="E27" s="175"/>
+      <c r="F27" s="175"/>
+      <c r="G27" s="175"/>
+      <c r="H27" s="175"/>
+      <c r="I27" s="175"/>
+      <c r="J27" s="175"/>
+      <c r="K27" s="175"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2816,8 +2842,8 @@
     <mergeCell ref="D22:K22"/>
     <mergeCell ref="D24:K24"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1:K1048576">
-    <cfRule type="expression" dxfId="6" priority="5">
+  <conditionalFormatting sqref="C1:K3 C6:K1048576 C4:I5 K4:L4 L5">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2887,19 +2913,19 @@
         <f>Proposal!O5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="167"/>
-      <c r="E5" s="167"/>
-      <c r="F5" s="167"/>
-      <c r="G5" s="167"/>
-      <c r="H5" s="167"/>
-      <c r="I5" s="167"/>
-      <c r="J5" s="167"/>
-      <c r="K5" s="167"/>
-      <c r="L5" s="167"/>
-      <c r="M5" s="167"/>
-      <c r="N5" s="167"/>
-      <c r="O5" s="167"/>
-      <c r="P5" s="167"/>
+      <c r="D5" s="174"/>
+      <c r="E5" s="174"/>
+      <c r="F5" s="174"/>
+      <c r="G5" s="174"/>
+      <c r="H5" s="174"/>
+      <c r="I5" s="174"/>
+      <c r="J5" s="174"/>
+      <c r="K5" s="174"/>
+      <c r="L5" s="174"/>
+      <c r="M5" s="174"/>
+      <c r="N5" s="174"/>
+      <c r="O5" s="174"/>
+      <c r="P5" s="174"/>
     </row>
     <row r="6" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P6" s="54"/>
@@ -2924,17 +2950,17 @@
     <mergeCell ref="D5:P5"/>
   </mergeCells>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>$A4="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$A5="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$A2="Even"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3064,24 +3090,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="175" t="s">
+      <c r="G7" s="182" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="175"/>
-      <c r="I7" s="175"/>
-      <c r="J7" s="175"/>
-      <c r="K7" s="175"/>
-      <c r="L7" s="176"/>
+      <c r="H7" s="182"/>
+      <c r="I7" s="182"/>
+      <c r="J7" s="182"/>
+      <c r="K7" s="182"/>
+      <c r="L7" s="183"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="175" t="s">
+      <c r="N7" s="182" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="175"/>
-      <c r="P7" s="175"/>
-      <c r="Q7" s="175"/>
-      <c r="R7" s="175"/>
-      <c r="S7" s="175"/>
-      <c r="T7" s="176"/>
+      <c r="O7" s="182"/>
+      <c r="P7" s="182"/>
+      <c r="Q7" s="182"/>
+      <c r="R7" s="182"/>
+      <c r="S7" s="182"/>
+      <c r="T7" s="183"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -3325,24 +3351,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="172" t="s">
+      <c r="G13" s="179" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
-      <c r="L13" s="174"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="180"/>
+      <c r="J13" s="180"/>
+      <c r="K13" s="180"/>
+      <c r="L13" s="181"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="172" t="s">
+      <c r="N13" s="179" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="173"/>
-      <c r="P13" s="173"/>
-      <c r="Q13" s="173"/>
-      <c r="R13" s="173"/>
-      <c r="S13" s="173"/>
-      <c r="T13" s="174"/>
+      <c r="O13" s="180"/>
+      <c r="P13" s="180"/>
+      <c r="Q13" s="180"/>
+      <c r="R13" s="180"/>
+      <c r="S13" s="180"/>
+      <c r="T13" s="181"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="35" t="s">
@@ -3582,24 +3608,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="172" t="s">
+      <c r="G19" s="179" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="173"/>
-      <c r="I19" s="173"/>
-      <c r="J19" s="173"/>
-      <c r="K19" s="173"/>
-      <c r="L19" s="174"/>
+      <c r="H19" s="180"/>
+      <c r="I19" s="180"/>
+      <c r="J19" s="180"/>
+      <c r="K19" s="180"/>
+      <c r="L19" s="181"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="172" t="s">
+      <c r="N19" s="179" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="173"/>
-      <c r="P19" s="173"/>
-      <c r="Q19" s="173"/>
-      <c r="R19" s="173"/>
-      <c r="S19" s="173"/>
-      <c r="T19" s="174"/>
+      <c r="O19" s="180"/>
+      <c r="P19" s="180"/>
+      <c r="Q19" s="180"/>
+      <c r="R19" s="180"/>
+      <c r="S19" s="180"/>
+      <c r="T19" s="181"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="35" t="s">
@@ -3869,25 +3895,25 @@
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="177" t="s">
+      <c r="D25" s="184" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="177"/>
-      <c r="F25" s="177"/>
-      <c r="G25" s="177"/>
-      <c r="H25" s="177"/>
-      <c r="I25" s="177"/>
-      <c r="J25" s="177"/>
-      <c r="K25" s="177"/>
-      <c r="L25" s="177"/>
-      <c r="M25" s="177"/>
-      <c r="N25" s="177"/>
-      <c r="O25" s="177"/>
-      <c r="P25" s="177"/>
-      <c r="Q25" s="177"/>
-      <c r="R25" s="177"/>
-      <c r="S25" s="177"/>
-      <c r="T25" s="177"/>
+      <c r="E25" s="184"/>
+      <c r="F25" s="184"/>
+      <c r="G25" s="184"/>
+      <c r="H25" s="184"/>
+      <c r="I25" s="184"/>
+      <c r="J25" s="184"/>
+      <c r="K25" s="184"/>
+      <c r="L25" s="184"/>
+      <c r="M25" s="184"/>
+      <c r="N25" s="184"/>
+      <c r="O25" s="184"/>
+      <c r="P25" s="184"/>
+      <c r="Q25" s="184"/>
+      <c r="R25" s="184"/>
+      <c r="S25" s="184"/>
+      <c r="T25" s="184"/>
     </row>
     <row r="26" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -3913,25 +3939,25 @@
       <c r="B27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="177" t="s">
+      <c r="D27" s="184" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="177"/>
-      <c r="F27" s="177"/>
-      <c r="G27" s="177"/>
-      <c r="H27" s="177"/>
-      <c r="I27" s="177"/>
-      <c r="J27" s="177"/>
-      <c r="K27" s="177"/>
-      <c r="L27" s="177"/>
-      <c r="M27" s="177"/>
-      <c r="N27" s="177"/>
-      <c r="O27" s="177"/>
-      <c r="P27" s="177"/>
-      <c r="Q27" s="177"/>
-      <c r="R27" s="177"/>
-      <c r="S27" s="177"/>
-      <c r="T27" s="177"/>
+      <c r="E27" s="184"/>
+      <c r="F27" s="184"/>
+      <c r="G27" s="184"/>
+      <c r="H27" s="184"/>
+      <c r="I27" s="184"/>
+      <c r="J27" s="184"/>
+      <c r="K27" s="184"/>
+      <c r="L27" s="184"/>
+      <c r="M27" s="184"/>
+      <c r="N27" s="184"/>
+      <c r="O27" s="184"/>
+      <c r="P27" s="184"/>
+      <c r="Q27" s="184"/>
+      <c r="R27" s="184"/>
+      <c r="S27" s="184"/>
+      <c r="T27" s="184"/>
     </row>
     <row r="28" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
@@ -3957,25 +3983,25 @@
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="177" t="s">
+      <c r="D29" s="184" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="177"/>
-      <c r="F29" s="177"/>
-      <c r="G29" s="177"/>
-      <c r="H29" s="177"/>
-      <c r="I29" s="177"/>
-      <c r="J29" s="177"/>
-      <c r="K29" s="177"/>
-      <c r="L29" s="177"/>
-      <c r="M29" s="177"/>
-      <c r="N29" s="177"/>
-      <c r="O29" s="177"/>
-      <c r="P29" s="177"/>
-      <c r="Q29" s="177"/>
-      <c r="R29" s="177"/>
-      <c r="S29" s="177"/>
-      <c r="T29" s="177"/>
+      <c r="E29" s="184"/>
+      <c r="F29" s="184"/>
+      <c r="G29" s="184"/>
+      <c r="H29" s="184"/>
+      <c r="I29" s="184"/>
+      <c r="J29" s="184"/>
+      <c r="K29" s="184"/>
+      <c r="L29" s="184"/>
+      <c r="M29" s="184"/>
+      <c r="N29" s="184"/>
+      <c r="O29" s="184"/>
+      <c r="P29" s="184"/>
+      <c r="Q29" s="184"/>
+      <c r="R29" s="184"/>
+      <c r="S29" s="184"/>
+      <c r="T29" s="184"/>
     </row>
     <row r="30" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
@@ -4001,25 +4027,25 @@
       <c r="B31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="177" t="s">
+      <c r="D31" s="184" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="177"/>
-      <c r="F31" s="177"/>
-      <c r="G31" s="177"/>
-      <c r="H31" s="177"/>
-      <c r="I31" s="177"/>
-      <c r="J31" s="177"/>
-      <c r="K31" s="177"/>
-      <c r="L31" s="177"/>
-      <c r="M31" s="177"/>
-      <c r="N31" s="177"/>
-      <c r="O31" s="177"/>
-      <c r="P31" s="177"/>
-      <c r="Q31" s="177"/>
-      <c r="R31" s="177"/>
-      <c r="S31" s="177"/>
-      <c r="T31" s="177"/>
+      <c r="E31" s="184"/>
+      <c r="F31" s="184"/>
+      <c r="G31" s="184"/>
+      <c r="H31" s="184"/>
+      <c r="I31" s="184"/>
+      <c r="J31" s="184"/>
+      <c r="K31" s="184"/>
+      <c r="L31" s="184"/>
+      <c r="M31" s="184"/>
+      <c r="N31" s="184"/>
+      <c r="O31" s="184"/>
+      <c r="P31" s="184"/>
+      <c r="Q31" s="184"/>
+      <c r="R31" s="184"/>
+      <c r="S31" s="184"/>
+      <c r="T31" s="184"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -4045,25 +4071,25 @@
       <c r="B33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="177" t="s">
+      <c r="D33" s="184" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="177"/>
-      <c r="F33" s="177"/>
-      <c r="G33" s="177"/>
-      <c r="H33" s="177"/>
-      <c r="I33" s="177"/>
-      <c r="J33" s="177"/>
-      <c r="K33" s="177"/>
-      <c r="L33" s="177"/>
-      <c r="M33" s="177"/>
-      <c r="N33" s="177"/>
-      <c r="O33" s="177"/>
-      <c r="P33" s="177"/>
-      <c r="Q33" s="177"/>
-      <c r="R33" s="177"/>
-      <c r="S33" s="177"/>
-      <c r="T33" s="177"/>
+      <c r="E33" s="184"/>
+      <c r="F33" s="184"/>
+      <c r="G33" s="184"/>
+      <c r="H33" s="184"/>
+      <c r="I33" s="184"/>
+      <c r="J33" s="184"/>
+      <c r="K33" s="184"/>
+      <c r="L33" s="184"/>
+      <c r="M33" s="184"/>
+      <c r="N33" s="184"/>
+      <c r="O33" s="184"/>
+      <c r="P33" s="184"/>
+      <c r="Q33" s="184"/>
+      <c r="R33" s="184"/>
+      <c r="S33" s="184"/>
+      <c r="T33" s="184"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -4089,25 +4115,25 @@
       <c r="B35" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="171" t="s">
+      <c r="D35" s="178" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="171"/>
-      <c r="F35" s="171"/>
-      <c r="G35" s="171"/>
-      <c r="H35" s="171"/>
-      <c r="I35" s="171"/>
-      <c r="J35" s="171"/>
-      <c r="K35" s="171"/>
-      <c r="L35" s="171"/>
-      <c r="M35" s="171"/>
-      <c r="N35" s="171"/>
-      <c r="O35" s="171"/>
-      <c r="P35" s="171"/>
-      <c r="Q35" s="171"/>
-      <c r="R35" s="171"/>
-      <c r="S35" s="171"/>
-      <c r="T35" s="171"/>
+      <c r="E35" s="178"/>
+      <c r="F35" s="178"/>
+      <c r="G35" s="178"/>
+      <c r="H35" s="178"/>
+      <c r="I35" s="178"/>
+      <c r="J35" s="178"/>
+      <c r="K35" s="178"/>
+      <c r="L35" s="178"/>
+      <c r="M35" s="178"/>
+      <c r="N35" s="178"/>
+      <c r="O35" s="178"/>
+      <c r="P35" s="178"/>
+      <c r="Q35" s="178"/>
+      <c r="R35" s="178"/>
+      <c r="S35" s="178"/>
+      <c r="T35" s="178"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4249,24 +4275,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="20"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="175" t="s">
+      <c r="G7" s="182" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="175"/>
-      <c r="I7" s="175"/>
-      <c r="J7" s="175"/>
-      <c r="K7" s="175"/>
-      <c r="L7" s="176"/>
+      <c r="H7" s="182"/>
+      <c r="I7" s="182"/>
+      <c r="J7" s="182"/>
+      <c r="K7" s="182"/>
+      <c r="L7" s="183"/>
       <c r="M7" s="30"/>
-      <c r="N7" s="175" t="s">
+      <c r="N7" s="182" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="175"/>
-      <c r="P7" s="175"/>
-      <c r="Q7" s="175"/>
-      <c r="R7" s="175"/>
-      <c r="S7" s="175"/>
-      <c r="T7" s="176"/>
+      <c r="O7" s="182"/>
+      <c r="P7" s="182"/>
+      <c r="Q7" s="182"/>
+      <c r="R7" s="182"/>
+      <c r="S7" s="182"/>
+      <c r="T7" s="183"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -4508,24 +4534,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="20"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="172" t="s">
+      <c r="G13" s="179" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
-      <c r="L13" s="174"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="180"/>
+      <c r="J13" s="180"/>
+      <c r="K13" s="180"/>
+      <c r="L13" s="181"/>
       <c r="M13" s="30"/>
-      <c r="N13" s="172" t="s">
+      <c r="N13" s="179" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="173"/>
-      <c r="P13" s="173"/>
-      <c r="Q13" s="173"/>
-      <c r="R13" s="173"/>
-      <c r="S13" s="173"/>
-      <c r="T13" s="174"/>
+      <c r="O13" s="180"/>
+      <c r="P13" s="180"/>
+      <c r="Q13" s="180"/>
+      <c r="R13" s="180"/>
+      <c r="S13" s="180"/>
+      <c r="T13" s="181"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="35" t="s">
@@ -4763,24 +4789,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="20"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="172" t="s">
+      <c r="G19" s="179" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="173"/>
-      <c r="I19" s="173"/>
-      <c r="J19" s="173"/>
-      <c r="K19" s="173"/>
-      <c r="L19" s="174"/>
+      <c r="H19" s="180"/>
+      <c r="I19" s="180"/>
+      <c r="J19" s="180"/>
+      <c r="K19" s="180"/>
+      <c r="L19" s="181"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="172" t="s">
+      <c r="N19" s="179" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="173"/>
-      <c r="P19" s="173"/>
-      <c r="Q19" s="173"/>
-      <c r="R19" s="173"/>
-      <c r="S19" s="173"/>
-      <c r="T19" s="174"/>
+      <c r="O19" s="180"/>
+      <c r="P19" s="180"/>
+      <c r="Q19" s="180"/>
+      <c r="R19" s="180"/>
+      <c r="S19" s="180"/>
+      <c r="T19" s="181"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="35" t="s">
@@ -5018,24 +5044,24 @@
       <c r="D25" s="6"/>
       <c r="E25" s="20"/>
       <c r="F25" s="25"/>
-      <c r="G25" s="172" t="s">
+      <c r="G25" s="179" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="173"/>
-      <c r="I25" s="173"/>
-      <c r="J25" s="173"/>
-      <c r="K25" s="173"/>
-      <c r="L25" s="174"/>
+      <c r="H25" s="180"/>
+      <c r="I25" s="180"/>
+      <c r="J25" s="180"/>
+      <c r="K25" s="180"/>
+      <c r="L25" s="181"/>
       <c r="M25" s="30"/>
-      <c r="N25" s="172" t="s">
+      <c r="N25" s="179" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="173"/>
-      <c r="P25" s="173"/>
-      <c r="Q25" s="173"/>
-      <c r="R25" s="173"/>
-      <c r="S25" s="173"/>
-      <c r="T25" s="174"/>
+      <c r="O25" s="180"/>
+      <c r="P25" s="180"/>
+      <c r="Q25" s="180"/>
+      <c r="R25" s="180"/>
+      <c r="S25" s="180"/>
+      <c r="T25" s="181"/>
     </row>
     <row r="26" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="35" t="s">
@@ -5273,26 +5299,26 @@
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="167" t="s">
+      <c r="C31" s="174" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="167"/>
-      <c r="E31" s="167"/>
-      <c r="F31" s="167"/>
-      <c r="G31" s="167"/>
-      <c r="H31" s="167"/>
-      <c r="I31" s="167"/>
-      <c r="J31" s="167"/>
-      <c r="K31" s="167"/>
-      <c r="L31" s="167"/>
-      <c r="M31" s="167"/>
-      <c r="N31" s="167"/>
-      <c r="O31" s="167"/>
-      <c r="P31" s="167"/>
-      <c r="Q31" s="167"/>
-      <c r="R31" s="167"/>
-      <c r="S31" s="167"/>
-      <c r="T31" s="167"/>
+      <c r="D31" s="174"/>
+      <c r="E31" s="174"/>
+      <c r="F31" s="174"/>
+      <c r="G31" s="174"/>
+      <c r="H31" s="174"/>
+      <c r="I31" s="174"/>
+      <c r="J31" s="174"/>
+      <c r="K31" s="174"/>
+      <c r="L31" s="174"/>
+      <c r="M31" s="174"/>
+      <c r="N31" s="174"/>
+      <c r="O31" s="174"/>
+      <c r="P31" s="174"/>
+      <c r="Q31" s="174"/>
+      <c r="R31" s="174"/>
+      <c r="S31" s="174"/>
+      <c r="T31" s="174"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -5319,26 +5345,26 @@
       <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="167" t="s">
+      <c r="C33" s="174" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="167"/>
-      <c r="E33" s="167"/>
-      <c r="F33" s="167"/>
-      <c r="G33" s="167"/>
-      <c r="H33" s="167"/>
-      <c r="I33" s="167"/>
-      <c r="J33" s="167"/>
-      <c r="K33" s="167"/>
-      <c r="L33" s="167"/>
-      <c r="M33" s="167"/>
-      <c r="N33" s="167"/>
-      <c r="O33" s="167"/>
-      <c r="P33" s="167"/>
-      <c r="Q33" s="167"/>
-      <c r="R33" s="167"/>
-      <c r="S33" s="167"/>
-      <c r="T33" s="167"/>
+      <c r="D33" s="174"/>
+      <c r="E33" s="174"/>
+      <c r="F33" s="174"/>
+      <c r="G33" s="174"/>
+      <c r="H33" s="174"/>
+      <c r="I33" s="174"/>
+      <c r="J33" s="174"/>
+      <c r="K33" s="174"/>
+      <c r="L33" s="174"/>
+      <c r="M33" s="174"/>
+      <c r="N33" s="174"/>
+      <c r="O33" s="174"/>
+      <c r="P33" s="174"/>
+      <c r="Q33" s="174"/>
+      <c r="R33" s="174"/>
+      <c r="S33" s="174"/>
+      <c r="T33" s="174"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -5365,26 +5391,26 @@
       <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="167" t="s">
+      <c r="C35" s="174" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="167"/>
-      <c r="E35" s="167"/>
-      <c r="F35" s="167"/>
-      <c r="G35" s="167"/>
-      <c r="H35" s="167"/>
-      <c r="I35" s="167"/>
-      <c r="J35" s="167"/>
-      <c r="K35" s="167"/>
-      <c r="L35" s="167"/>
-      <c r="M35" s="167"/>
-      <c r="N35" s="167"/>
-      <c r="O35" s="167"/>
-      <c r="P35" s="167"/>
-      <c r="Q35" s="167"/>
-      <c r="R35" s="167"/>
-      <c r="S35" s="167"/>
-      <c r="T35" s="167"/>
+      <c r="D35" s="174"/>
+      <c r="E35" s="174"/>
+      <c r="F35" s="174"/>
+      <c r="G35" s="174"/>
+      <c r="H35" s="174"/>
+      <c r="I35" s="174"/>
+      <c r="J35" s="174"/>
+      <c r="K35" s="174"/>
+      <c r="L35" s="174"/>
+      <c r="M35" s="174"/>
+      <c r="N35" s="174"/>
+      <c r="O35" s="174"/>
+      <c r="P35" s="174"/>
+      <c r="Q35" s="174"/>
+      <c r="R35" s="174"/>
+      <c r="S35" s="174"/>
+      <c r="T35" s="174"/>
     </row>
     <row r="36" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
@@ -5411,26 +5437,26 @@
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="167" t="s">
+      <c r="C37" s="174" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="167"/>
-      <c r="E37" s="167"/>
-      <c r="F37" s="167"/>
-      <c r="G37" s="167"/>
-      <c r="H37" s="167"/>
-      <c r="I37" s="167"/>
-      <c r="J37" s="167"/>
-      <c r="K37" s="167"/>
-      <c r="L37" s="167"/>
-      <c r="M37" s="167"/>
-      <c r="N37" s="167"/>
-      <c r="O37" s="167"/>
-      <c r="P37" s="167"/>
-      <c r="Q37" s="167"/>
-      <c r="R37" s="167"/>
-      <c r="S37" s="167"/>
-      <c r="T37" s="167"/>
+      <c r="D37" s="174"/>
+      <c r="E37" s="174"/>
+      <c r="F37" s="174"/>
+      <c r="G37" s="174"/>
+      <c r="H37" s="174"/>
+      <c r="I37" s="174"/>
+      <c r="J37" s="174"/>
+      <c r="K37" s="174"/>
+      <c r="L37" s="174"/>
+      <c r="M37" s="174"/>
+      <c r="N37" s="174"/>
+      <c r="O37" s="174"/>
+      <c r="P37" s="174"/>
+      <c r="Q37" s="174"/>
+      <c r="R37" s="174"/>
+      <c r="S37" s="174"/>
+      <c r="T37" s="174"/>
     </row>
     <row r="38" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
@@ -5457,26 +5483,26 @@
       <c r="B39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="167" t="s">
+      <c r="C39" s="174" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="167"/>
-      <c r="E39" s="167"/>
-      <c r="F39" s="167"/>
-      <c r="G39" s="167"/>
-      <c r="H39" s="167"/>
-      <c r="I39" s="167"/>
-      <c r="J39" s="167"/>
-      <c r="K39" s="167"/>
-      <c r="L39" s="167"/>
-      <c r="M39" s="167"/>
-      <c r="N39" s="167"/>
-      <c r="O39" s="167"/>
-      <c r="P39" s="167"/>
-      <c r="Q39" s="167"/>
-      <c r="R39" s="167"/>
-      <c r="S39" s="167"/>
-      <c r="T39" s="167"/>
+      <c r="D39" s="174"/>
+      <c r="E39" s="174"/>
+      <c r="F39" s="174"/>
+      <c r="G39" s="174"/>
+      <c r="H39" s="174"/>
+      <c r="I39" s="174"/>
+      <c r="J39" s="174"/>
+      <c r="K39" s="174"/>
+      <c r="L39" s="174"/>
+      <c r="M39" s="174"/>
+      <c r="N39" s="174"/>
+      <c r="O39" s="174"/>
+      <c r="P39" s="174"/>
+      <c r="Q39" s="174"/>
+      <c r="R39" s="174"/>
+      <c r="S39" s="174"/>
+      <c r="T39" s="174"/>
     </row>
     <row r="40" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
@@ -5503,29 +5529,34 @@
       <c r="B41" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="169" t="s">
+      <c r="C41" s="176" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="169"/>
-      <c r="E41" s="169"/>
-      <c r="F41" s="169"/>
-      <c r="G41" s="169"/>
-      <c r="H41" s="169"/>
-      <c r="I41" s="169"/>
-      <c r="J41" s="169"/>
-      <c r="K41" s="169"/>
-      <c r="L41" s="169"/>
-      <c r="M41" s="169"/>
-      <c r="N41" s="169"/>
-      <c r="O41" s="169"/>
-      <c r="P41" s="169"/>
-      <c r="Q41" s="169"/>
-      <c r="R41" s="169"/>
-      <c r="S41" s="169"/>
-      <c r="T41" s="169"/>
+      <c r="D41" s="176"/>
+      <c r="E41" s="176"/>
+      <c r="F41" s="176"/>
+      <c r="G41" s="176"/>
+      <c r="H41" s="176"/>
+      <c r="I41" s="176"/>
+      <c r="J41" s="176"/>
+      <c r="K41" s="176"/>
+      <c r="L41" s="176"/>
+      <c r="M41" s="176"/>
+      <c r="N41" s="176"/>
+      <c r="O41" s="176"/>
+      <c r="P41" s="176"/>
+      <c r="Q41" s="176"/>
+      <c r="R41" s="176"/>
+      <c r="S41" s="176"/>
+      <c r="T41" s="176"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5535,11 +5566,6 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5578,94 +5604,94 @@
     </row>
     <row r="3" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:4" s="104" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="178" t="s">
+      <c r="C4" s="185" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="178"/>
+      <c r="D4" s="185"/>
     </row>
     <row r="5" spans="3:4" s="104" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="178" t="s">
+      <c r="C5" s="185" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="178"/>
+      <c r="D5" s="185"/>
     </row>
     <row r="6" spans="3:4" s="104" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="178" t="s">
+      <c r="C6" s="185" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="178"/>
+      <c r="D6" s="185"/>
     </row>
     <row r="7" spans="3:4" s="104" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="178" t="s">
+      <c r="C7" s="185" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="178"/>
+      <c r="D7" s="185"/>
     </row>
     <row r="8" spans="3:4" s="104" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="178" t="s">
+      <c r="C8" s="185" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="178"/>
+      <c r="D8" s="185"/>
     </row>
     <row r="9" spans="3:4" s="104" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="178" t="s">
+      <c r="C9" s="185" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="178"/>
+      <c r="D9" s="185"/>
     </row>
     <row r="10" spans="3:4" s="104" customFormat="1" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="178" t="s">
+      <c r="C10" s="185" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="178"/>
+      <c r="D10" s="185"/>
     </row>
     <row r="11" spans="3:4" s="104" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="178" t="s">
+      <c r="C11" s="185" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="178"/>
+      <c r="D11" s="185"/>
     </row>
     <row r="12" spans="3:4" s="104" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="178" t="s">
+      <c r="C12" s="185" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="178"/>
+      <c r="D12" s="185"/>
     </row>
     <row r="13" spans="3:4" s="104" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="178" t="s">
+      <c r="C13" s="185" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="178"/>
+      <c r="D13" s="185"/>
     </row>
     <row r="14" spans="3:4" s="104" customFormat="1" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="178" t="s">
+      <c r="C14" s="185" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="178"/>
+      <c r="D14" s="185"/>
     </row>
     <row r="15" spans="3:4" s="104" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="178" t="s">
+      <c r="C15" s="185" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="178"/>
+      <c r="D15" s="185"/>
     </row>
     <row r="16" spans="3:4" s="104" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="178" t="s">
+      <c r="C16" s="185" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="178"/>
+      <c r="D16" s="185"/>
     </row>
     <row r="17" spans="3:4" s="104" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="178" t="s">
+      <c r="C17" s="185" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="178"/>
+      <c r="D17" s="185"/>
     </row>
     <row r="18" spans="3:4" s="104" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="178" t="s">
+      <c r="C18" s="185" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="178"/>
+      <c r="D18" s="185"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -5698,8 +5724,8 @@
   </sheetPr>
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:D5"/>
+    <sheetView showGridLines="0" topLeftCell="I1" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5712,9 +5738,13 @@
     <col min="6" max="6" width="11.375" style="85" customWidth="1"/>
     <col min="7" max="7" width="12.5" style="85" customWidth="1"/>
     <col min="8" max="8" width="12.5" style="103" customWidth="1"/>
-    <col min="9" max="13" width="11.375" style="85" customWidth="1"/>
+    <col min="9" max="12" width="11.375" style="85" customWidth="1"/>
+    <col min="13" max="13" width="14.5" style="85" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.5" style="85" customWidth="1"/>
-    <col min="15" max="20" width="11.375" style="85" customWidth="1"/>
+    <col min="15" max="15" width="10" style="85" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.375" style="85" customWidth="1"/>
+    <col min="17" max="17" width="21.125" style="85" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="11.375" style="85" customWidth="1"/>
     <col min="21" max="21" width="12.5" style="85" customWidth="1"/>
     <col min="22" max="22" width="10.5" style="85" customWidth="1"/>
     <col min="23" max="16384" width="10.625" style="85"/>
@@ -5751,6 +5781,9 @@
         <v>68</v>
       </c>
       <c r="P4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="R4" s="1" t="s">
@@ -5761,24 +5794,24 @@
       </c>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="167"/>
-      <c r="D5" s="167"/>
-      <c r="E5" s="167"/>
-      <c r="F5" s="167"/>
-      <c r="G5" s="167"/>
+      <c r="C5" s="174"/>
+      <c r="D5" s="174"/>
+      <c r="E5" s="174"/>
+      <c r="F5" s="174"/>
+      <c r="G5" s="174"/>
       <c r="H5" s="102"/>
-      <c r="I5" s="167"/>
-      <c r="J5" s="167"/>
-      <c r="K5" s="167"/>
-      <c r="L5" s="167"/>
-      <c r="M5" s="167"/>
-      <c r="N5" s="167"/>
+      <c r="I5" s="174"/>
+      <c r="J5" s="174"/>
+      <c r="K5" s="174"/>
+      <c r="L5" s="174"/>
+      <c r="M5" s="174"/>
+      <c r="N5" s="174"/>
       <c r="O5" s="62"/>
-      <c r="P5" s="167"/>
-      <c r="Q5" s="167"/>
-      <c r="R5" s="167"/>
-      <c r="S5" s="167"/>
-      <c r="T5" s="167"/>
+      <c r="P5" s="168"/>
+      <c r="Q5" s="168"/>
+      <c r="R5" s="174"/>
+      <c r="S5" s="174"/>
+      <c r="T5" s="174"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I6" s="29"/>
@@ -5802,21 +5835,21 @@
       <c r="F7" s="6"/>
       <c r="G7" s="20"/>
       <c r="H7" s="55"/>
-      <c r="I7" s="172" t="s">
+      <c r="I7" s="179" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="173"/>
-      <c r="K7" s="173"/>
-      <c r="L7" s="173"/>
-      <c r="M7" s="173"/>
-      <c r="N7" s="174"/>
-      <c r="O7" s="172"/>
-      <c r="P7" s="173"/>
-      <c r="Q7" s="173"/>
-      <c r="R7" s="173"/>
-      <c r="S7" s="173"/>
-      <c r="T7" s="173"/>
-      <c r="U7" s="174"/>
+      <c r="J7" s="180"/>
+      <c r="K7" s="180"/>
+      <c r="L7" s="180"/>
+      <c r="M7" s="180"/>
+      <c r="N7" s="181"/>
+      <c r="O7" s="179"/>
+      <c r="P7" s="180"/>
+      <c r="Q7" s="180"/>
+      <c r="R7" s="180"/>
+      <c r="S7" s="180"/>
+      <c r="T7" s="180"/>
+      <c r="U7" s="181"/>
     </row>
     <row r="8" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="85" t="s">
@@ -5977,20 +6010,20 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
-      <c r="H13" s="172"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="173"/>
-      <c r="K13" s="173"/>
-      <c r="L13" s="173"/>
-      <c r="M13" s="173"/>
-      <c r="N13" s="174"/>
-      <c r="O13" s="172"/>
-      <c r="P13" s="173"/>
-      <c r="Q13" s="173"/>
-      <c r="R13" s="173"/>
-      <c r="S13" s="173"/>
-      <c r="T13" s="173"/>
-      <c r="U13" s="174"/>
+      <c r="H13" s="179"/>
+      <c r="I13" s="180"/>
+      <c r="J13" s="180"/>
+      <c r="K13" s="180"/>
+      <c r="L13" s="180"/>
+      <c r="M13" s="180"/>
+      <c r="N13" s="181"/>
+      <c r="O13" s="179"/>
+      <c r="P13" s="180"/>
+      <c r="Q13" s="180"/>
+      <c r="R13" s="180"/>
+      <c r="S13" s="180"/>
+      <c r="T13" s="180"/>
+      <c r="U13" s="181"/>
     </row>
     <row r="14" spans="1:21" s="103" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="54"/>
@@ -6160,22 +6193,22 @@
       </c>
       <c r="D20" s="51"/>
       <c r="E20" s="105"/>
-      <c r="F20" s="179"/>
-      <c r="G20" s="179"/>
-      <c r="H20" s="179"/>
-      <c r="I20" s="179"/>
-      <c r="J20" s="179"/>
-      <c r="K20" s="179"/>
-      <c r="L20" s="179"/>
-      <c r="M20" s="179"/>
-      <c r="N20" s="179"/>
-      <c r="O20" s="179"/>
-      <c r="P20" s="179"/>
-      <c r="Q20" s="179"/>
-      <c r="R20" s="179"/>
-      <c r="S20" s="179"/>
-      <c r="T20" s="179"/>
-      <c r="U20" s="179"/>
+      <c r="F20" s="186"/>
+      <c r="G20" s="186"/>
+      <c r="H20" s="186"/>
+      <c r="I20" s="186"/>
+      <c r="J20" s="186"/>
+      <c r="K20" s="186"/>
+      <c r="L20" s="186"/>
+      <c r="M20" s="186"/>
+      <c r="N20" s="186"/>
+      <c r="O20" s="186"/>
+      <c r="P20" s="186"/>
+      <c r="Q20" s="186"/>
+      <c r="R20" s="186"/>
+      <c r="S20" s="186"/>
+      <c r="T20" s="186"/>
+      <c r="U20" s="186"/>
     </row>
     <row r="21" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
@@ -6204,22 +6237,22 @@
         <v>36</v>
       </c>
       <c r="D22" s="51"/>
-      <c r="F22" s="179"/>
-      <c r="G22" s="179"/>
-      <c r="H22" s="179"/>
-      <c r="I22" s="179"/>
-      <c r="J22" s="179"/>
-      <c r="K22" s="179"/>
-      <c r="L22" s="179"/>
-      <c r="M22" s="179"/>
-      <c r="N22" s="179"/>
-      <c r="O22" s="179"/>
-      <c r="P22" s="179"/>
-      <c r="Q22" s="179"/>
-      <c r="R22" s="179"/>
-      <c r="S22" s="179"/>
-      <c r="T22" s="179"/>
-      <c r="U22" s="179"/>
+      <c r="F22" s="186"/>
+      <c r="G22" s="186"/>
+      <c r="H22" s="186"/>
+      <c r="I22" s="186"/>
+      <c r="J22" s="186"/>
+      <c r="K22" s="186"/>
+      <c r="L22" s="186"/>
+      <c r="M22" s="186"/>
+      <c r="N22" s="186"/>
+      <c r="O22" s="186"/>
+      <c r="P22" s="186"/>
+      <c r="Q22" s="186"/>
+      <c r="R22" s="186"/>
+      <c r="S22" s="186"/>
+      <c r="T22" s="186"/>
+      <c r="U22" s="186"/>
       <c r="V22" s="126"/>
     </row>
     <row r="23" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -6248,22 +6281,22 @@
       </c>
       <c r="D24" s="51"/>
       <c r="E24" s="105"/>
-      <c r="F24" s="179"/>
-      <c r="G24" s="179"/>
-      <c r="H24" s="179"/>
-      <c r="I24" s="179"/>
-      <c r="J24" s="179"/>
-      <c r="K24" s="179"/>
-      <c r="L24" s="179"/>
-      <c r="M24" s="179"/>
-      <c r="N24" s="179"/>
-      <c r="O24" s="179"/>
-      <c r="P24" s="179"/>
-      <c r="Q24" s="179"/>
-      <c r="R24" s="179"/>
-      <c r="S24" s="179"/>
-      <c r="T24" s="179"/>
-      <c r="U24" s="179"/>
+      <c r="F24" s="186"/>
+      <c r="G24" s="186"/>
+      <c r="H24" s="186"/>
+      <c r="I24" s="186"/>
+      <c r="J24" s="186"/>
+      <c r="K24" s="186"/>
+      <c r="L24" s="186"/>
+      <c r="M24" s="186"/>
+      <c r="N24" s="186"/>
+      <c r="O24" s="186"/>
+      <c r="P24" s="186"/>
+      <c r="Q24" s="186"/>
+      <c r="R24" s="186"/>
+      <c r="S24" s="186"/>
+      <c r="T24" s="186"/>
+      <c r="U24" s="186"/>
     </row>
     <row r="25" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
@@ -6292,22 +6325,22 @@
         <v>48</v>
       </c>
       <c r="D26" s="51"/>
-      <c r="F26" s="170"/>
-      <c r="G26" s="170"/>
-      <c r="H26" s="170"/>
-      <c r="I26" s="170"/>
-      <c r="J26" s="170"/>
-      <c r="K26" s="170"/>
-      <c r="L26" s="170"/>
-      <c r="M26" s="170"/>
-      <c r="N26" s="170"/>
-      <c r="O26" s="170"/>
-      <c r="P26" s="170"/>
-      <c r="Q26" s="170"/>
-      <c r="R26" s="170"/>
-      <c r="S26" s="170"/>
-      <c r="T26" s="170"/>
-      <c r="U26" s="170"/>
+      <c r="F26" s="177"/>
+      <c r="G26" s="177"/>
+      <c r="H26" s="177"/>
+      <c r="I26" s="177"/>
+      <c r="J26" s="177"/>
+      <c r="K26" s="177"/>
+      <c r="L26" s="177"/>
+      <c r="M26" s="177"/>
+      <c r="N26" s="177"/>
+      <c r="O26" s="177"/>
+      <c r="P26" s="177"/>
+      <c r="Q26" s="177"/>
+      <c r="R26" s="177"/>
+      <c r="S26" s="177"/>
+      <c r="T26" s="177"/>
+      <c r="U26" s="177"/>
       <c r="V26" s="126"/>
     </row>
     <row r="27" spans="1:22" s="126" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -6335,33 +6368,25 @@
         <v>49</v>
       </c>
       <c r="D28" s="51"/>
-      <c r="F28" s="169"/>
-      <c r="G28" s="169"/>
-      <c r="H28" s="169"/>
-      <c r="I28" s="169"/>
-      <c r="J28" s="169"/>
-      <c r="K28" s="169"/>
-      <c r="L28" s="169"/>
-      <c r="M28" s="169"/>
-      <c r="N28" s="169"/>
-      <c r="O28" s="169"/>
-      <c r="P28" s="169"/>
-      <c r="Q28" s="169"/>
-      <c r="R28" s="169"/>
-      <c r="S28" s="169"/>
-      <c r="T28" s="169"/>
-      <c r="U28" s="169"/>
+      <c r="F28" s="176"/>
+      <c r="G28" s="176"/>
+      <c r="H28" s="176"/>
+      <c r="I28" s="176"/>
+      <c r="J28" s="176"/>
+      <c r="K28" s="176"/>
+      <c r="L28" s="176"/>
+      <c r="M28" s="176"/>
+      <c r="N28" s="176"/>
+      <c r="O28" s="176"/>
+      <c r="P28" s="176"/>
+      <c r="Q28" s="176"/>
+      <c r="R28" s="176"/>
+      <c r="S28" s="176"/>
+      <c r="T28" s="176"/>
+      <c r="U28" s="176"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
+  <mergeCells count="15">
     <mergeCell ref="F28:U28"/>
     <mergeCell ref="F20:U20"/>
     <mergeCell ref="H13:N13"/>
@@ -6370,19 +6395,26 @@
     <mergeCell ref="F24:U24"/>
     <mergeCell ref="F26:U26"/>
     <mergeCell ref="O13:U13"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1:U3 C5 C4:N4 P4 R4:U4 U5 C6:U1048576">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="C1:U3 C5 C4:N4 Q4:U4 U5 C6:U1048576">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$A1="Even"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:N1048576">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$A1="EvenSA1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:U1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="H1:U3 H5:U1048576 H4:O4 Q4:U4">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$A1="EvenSA2"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6399,7 +6431,7 @@
   </sheetPr>
   <dimension ref="B1:Q70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -6420,18 +6452,18 @@
     <row r="1" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="165"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="173"/>
-      <c r="I2" s="173"/>
-      <c r="J2" s="174"/>
-      <c r="K2" s="172"/>
-      <c r="L2" s="173"/>
-      <c r="M2" s="173"/>
-      <c r="N2" s="174"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="181"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="180"/>
+      <c r="I2" s="180"/>
+      <c r="J2" s="181"/>
+      <c r="K2" s="179"/>
+      <c r="L2" s="180"/>
+      <c r="M2" s="180"/>
+      <c r="N2" s="181"/>
       <c r="O2" s="29"/>
     </row>
     <row r="3" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6548,53 +6580,53 @@
       <c r="B9" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="184"/>
-      <c r="D9" s="185"/>
-      <c r="E9" s="185"/>
-      <c r="F9" s="185"/>
-      <c r="G9" s="184"/>
-      <c r="H9" s="185"/>
-      <c r="I9" s="185"/>
-      <c r="J9" s="186"/>
-      <c r="K9" s="184"/>
-      <c r="L9" s="185"/>
-      <c r="M9" s="185"/>
-      <c r="N9" s="185"/>
-      <c r="O9" s="187"/>
+      <c r="C9" s="170"/>
+      <c r="D9" s="171"/>
+      <c r="E9" s="171"/>
+      <c r="F9" s="171"/>
+      <c r="G9" s="170"/>
+      <c r="H9" s="171"/>
+      <c r="I9" s="171"/>
+      <c r="J9" s="172"/>
+      <c r="K9" s="170"/>
+      <c r="L9" s="171"/>
+      <c r="M9" s="171"/>
+      <c r="N9" s="171"/>
+      <c r="O9" s="173"/>
     </row>
     <row r="10" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="180"/>
-      <c r="D10" s="181"/>
-      <c r="E10" s="181"/>
-      <c r="F10" s="182"/>
-      <c r="G10" s="180"/>
-      <c r="H10" s="181"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="182"/>
-      <c r="K10" s="180"/>
-      <c r="L10" s="181"/>
-      <c r="M10" s="181"/>
-      <c r="N10" s="182"/>
-      <c r="O10" s="183"/>
+      <c r="C10" s="187"/>
+      <c r="D10" s="188"/>
+      <c r="E10" s="188"/>
+      <c r="F10" s="189"/>
+      <c r="G10" s="187"/>
+      <c r="H10" s="188"/>
+      <c r="I10" s="188"/>
+      <c r="J10" s="189"/>
+      <c r="K10" s="187"/>
+      <c r="L10" s="188"/>
+      <c r="M10" s="188"/>
+      <c r="N10" s="189"/>
+      <c r="O10" s="169"/>
     </row>
     <row r="12" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="165"/>
-      <c r="C12" s="172"/>
-      <c r="D12" s="173"/>
-      <c r="E12" s="173"/>
-      <c r="F12" s="173"/>
-      <c r="G12" s="174"/>
-      <c r="H12" s="173"/>
-      <c r="I12" s="173"/>
-      <c r="J12" s="173"/>
-      <c r="K12" s="174"/>
-      <c r="L12" s="172"/>
-      <c r="M12" s="173"/>
-      <c r="N12" s="173"/>
-      <c r="O12" s="174"/>
+      <c r="C12" s="179"/>
+      <c r="D12" s="180"/>
+      <c r="E12" s="180"/>
+      <c r="F12" s="180"/>
+      <c r="G12" s="181"/>
+      <c r="H12" s="180"/>
+      <c r="I12" s="180"/>
+      <c r="J12" s="180"/>
+      <c r="K12" s="181"/>
+      <c r="L12" s="179"/>
+      <c r="M12" s="180"/>
+      <c r="N12" s="180"/>
+      <c r="O12" s="181"/>
       <c r="P12" s="29"/>
     </row>
     <row r="13" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6717,55 +6749,55 @@
       <c r="B19" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="184"/>
-      <c r="D19" s="185"/>
-      <c r="E19" s="185"/>
-      <c r="F19" s="185"/>
-      <c r="G19" s="185"/>
-      <c r="H19" s="184"/>
-      <c r="I19" s="185"/>
-      <c r="J19" s="185"/>
-      <c r="K19" s="186"/>
-      <c r="L19" s="184"/>
-      <c r="M19" s="185"/>
-      <c r="N19" s="185"/>
-      <c r="O19" s="186"/>
-      <c r="P19" s="186"/>
+      <c r="C19" s="170"/>
+      <c r="D19" s="171"/>
+      <c r="E19" s="171"/>
+      <c r="F19" s="171"/>
+      <c r="G19" s="171"/>
+      <c r="H19" s="170"/>
+      <c r="I19" s="171"/>
+      <c r="J19" s="171"/>
+      <c r="K19" s="172"/>
+      <c r="L19" s="170"/>
+      <c r="M19" s="171"/>
+      <c r="N19" s="171"/>
+      <c r="O19" s="172"/>
+      <c r="P19" s="172"/>
     </row>
     <row r="20" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="180"/>
-      <c r="D20" s="181"/>
-      <c r="E20" s="181"/>
-      <c r="F20" s="181"/>
-      <c r="G20" s="182"/>
-      <c r="H20" s="180"/>
-      <c r="I20" s="181"/>
-      <c r="J20" s="181"/>
-      <c r="K20" s="182"/>
-      <c r="L20" s="188"/>
-      <c r="M20" s="189"/>
-      <c r="N20" s="189"/>
-      <c r="O20" s="190"/>
+      <c r="C20" s="187"/>
+      <c r="D20" s="188"/>
+      <c r="E20" s="188"/>
+      <c r="F20" s="188"/>
+      <c r="G20" s="189"/>
+      <c r="H20" s="187"/>
+      <c r="I20" s="188"/>
+      <c r="J20" s="188"/>
+      <c r="K20" s="189"/>
+      <c r="L20" s="190"/>
+      <c r="M20" s="191"/>
+      <c r="N20" s="191"/>
+      <c r="O20" s="192"/>
       <c r="P20" s="164"/>
     </row>
     <row r="22" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="165"/>
-      <c r="C22" s="172"/>
-      <c r="D22" s="173"/>
-      <c r="E22" s="173"/>
-      <c r="F22" s="174"/>
-      <c r="G22" s="173"/>
-      <c r="H22" s="173"/>
-      <c r="I22" s="173"/>
-      <c r="J22" s="173"/>
-      <c r="K22" s="174"/>
-      <c r="L22" s="172"/>
-      <c r="M22" s="173"/>
-      <c r="N22" s="173"/>
-      <c r="O22" s="174"/>
+      <c r="C22" s="179"/>
+      <c r="D22" s="180"/>
+      <c r="E22" s="180"/>
+      <c r="F22" s="181"/>
+      <c r="G22" s="180"/>
+      <c r="H22" s="180"/>
+      <c r="I22" s="180"/>
+      <c r="J22" s="180"/>
+      <c r="K22" s="181"/>
+      <c r="L22" s="179"/>
+      <c r="M22" s="180"/>
+      <c r="N22" s="180"/>
+      <c r="O22" s="181"/>
       <c r="P22" s="29"/>
     </row>
     <row r="23" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6888,55 +6920,55 @@
       <c r="B29" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="184"/>
-      <c r="D29" s="185"/>
-      <c r="E29" s="185"/>
-      <c r="F29" s="185"/>
-      <c r="G29" s="184"/>
-      <c r="H29" s="185"/>
-      <c r="I29" s="185"/>
-      <c r="J29" s="185"/>
-      <c r="K29" s="186"/>
-      <c r="L29" s="184"/>
-      <c r="M29" s="185"/>
-      <c r="N29" s="185"/>
-      <c r="O29" s="186"/>
-      <c r="P29" s="186"/>
+      <c r="C29" s="170"/>
+      <c r="D29" s="171"/>
+      <c r="E29" s="171"/>
+      <c r="F29" s="171"/>
+      <c r="G29" s="170"/>
+      <c r="H29" s="171"/>
+      <c r="I29" s="171"/>
+      <c r="J29" s="171"/>
+      <c r="K29" s="172"/>
+      <c r="L29" s="170"/>
+      <c r="M29" s="171"/>
+      <c r="N29" s="171"/>
+      <c r="O29" s="172"/>
+      <c r="P29" s="172"/>
     </row>
     <row r="30" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="180"/>
-      <c r="D30" s="181"/>
-      <c r="E30" s="181"/>
-      <c r="F30" s="182"/>
-      <c r="G30" s="180"/>
-      <c r="H30" s="181"/>
-      <c r="I30" s="181"/>
-      <c r="J30" s="181"/>
-      <c r="K30" s="182"/>
-      <c r="L30" s="180"/>
-      <c r="M30" s="181"/>
-      <c r="N30" s="181"/>
-      <c r="O30" s="182"/>
-      <c r="P30" s="183"/>
+      <c r="C30" s="187"/>
+      <c r="D30" s="188"/>
+      <c r="E30" s="188"/>
+      <c r="F30" s="189"/>
+      <c r="G30" s="187"/>
+      <c r="H30" s="188"/>
+      <c r="I30" s="188"/>
+      <c r="J30" s="188"/>
+      <c r="K30" s="189"/>
+      <c r="L30" s="187"/>
+      <c r="M30" s="188"/>
+      <c r="N30" s="188"/>
+      <c r="O30" s="189"/>
+      <c r="P30" s="169"/>
     </row>
     <row r="32" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="165"/>
-      <c r="C32" s="172"/>
-      <c r="D32" s="173"/>
-      <c r="E32" s="173"/>
-      <c r="F32" s="174"/>
-      <c r="G32" s="173"/>
-      <c r="H32" s="173"/>
-      <c r="I32" s="173"/>
-      <c r="J32" s="174"/>
-      <c r="K32" s="172"/>
-      <c r="L32" s="173"/>
-      <c r="M32" s="173"/>
-      <c r="N32" s="173"/>
-      <c r="O32" s="174"/>
+      <c r="C32" s="179"/>
+      <c r="D32" s="180"/>
+      <c r="E32" s="180"/>
+      <c r="F32" s="181"/>
+      <c r="G32" s="180"/>
+      <c r="H32" s="180"/>
+      <c r="I32" s="180"/>
+      <c r="J32" s="181"/>
+      <c r="K32" s="179"/>
+      <c r="L32" s="180"/>
+      <c r="M32" s="180"/>
+      <c r="N32" s="180"/>
+      <c r="O32" s="181"/>
       <c r="P32" s="29"/>
     </row>
     <row r="33" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7059,56 +7091,56 @@
       <c r="B39" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="184"/>
-      <c r="D39" s="185"/>
-      <c r="E39" s="185"/>
-      <c r="F39" s="185"/>
-      <c r="G39" s="184"/>
-      <c r="H39" s="185"/>
-      <c r="I39" s="185"/>
-      <c r="J39" s="186"/>
-      <c r="K39" s="184"/>
-      <c r="L39" s="185"/>
-      <c r="M39" s="185"/>
-      <c r="N39" s="185"/>
-      <c r="O39" s="186"/>
-      <c r="P39" s="186"/>
+      <c r="C39" s="170"/>
+      <c r="D39" s="171"/>
+      <c r="E39" s="171"/>
+      <c r="F39" s="171"/>
+      <c r="G39" s="170"/>
+      <c r="H39" s="171"/>
+      <c r="I39" s="171"/>
+      <c r="J39" s="172"/>
+      <c r="K39" s="170"/>
+      <c r="L39" s="171"/>
+      <c r="M39" s="171"/>
+      <c r="N39" s="171"/>
+      <c r="O39" s="172"/>
+      <c r="P39" s="172"/>
     </row>
     <row r="40" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="180"/>
-      <c r="D40" s="181"/>
-      <c r="E40" s="181"/>
-      <c r="F40" s="182"/>
-      <c r="G40" s="180"/>
-      <c r="H40" s="181"/>
-      <c r="I40" s="181"/>
-      <c r="J40" s="182"/>
-      <c r="K40" s="180"/>
-      <c r="L40" s="181"/>
-      <c r="M40" s="181"/>
-      <c r="N40" s="181"/>
-      <c r="O40" s="182"/>
-      <c r="P40" s="183"/>
+      <c r="C40" s="187"/>
+      <c r="D40" s="188"/>
+      <c r="E40" s="188"/>
+      <c r="F40" s="189"/>
+      <c r="G40" s="187"/>
+      <c r="H40" s="188"/>
+      <c r="I40" s="188"/>
+      <c r="J40" s="189"/>
+      <c r="K40" s="187"/>
+      <c r="L40" s="188"/>
+      <c r="M40" s="188"/>
+      <c r="N40" s="188"/>
+      <c r="O40" s="189"/>
+      <c r="P40" s="169"/>
     </row>
     <row r="42" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="165"/>
-      <c r="C42" s="172"/>
-      <c r="D42" s="173"/>
-      <c r="E42" s="173"/>
-      <c r="F42" s="173"/>
-      <c r="G42" s="174"/>
-      <c r="H42" s="173"/>
-      <c r="I42" s="173"/>
-      <c r="J42" s="173"/>
-      <c r="K42" s="173"/>
-      <c r="L42" s="174"/>
-      <c r="M42" s="172"/>
-      <c r="N42" s="173"/>
-      <c r="O42" s="173"/>
-      <c r="P42" s="174"/>
+      <c r="C42" s="179"/>
+      <c r="D42" s="180"/>
+      <c r="E42" s="180"/>
+      <c r="F42" s="180"/>
+      <c r="G42" s="181"/>
+      <c r="H42" s="180"/>
+      <c r="I42" s="180"/>
+      <c r="J42" s="180"/>
+      <c r="K42" s="180"/>
+      <c r="L42" s="181"/>
+      <c r="M42" s="179"/>
+      <c r="N42" s="180"/>
+      <c r="O42" s="180"/>
+      <c r="P42" s="181"/>
       <c r="Q42" s="29"/>
     </row>
     <row r="43" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7237,58 +7269,58 @@
       <c r="B49" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="C49" s="184"/>
-      <c r="D49" s="185"/>
-      <c r="E49" s="185"/>
-      <c r="F49" s="185"/>
-      <c r="G49" s="185"/>
-      <c r="H49" s="184"/>
-      <c r="I49" s="185"/>
-      <c r="J49" s="185"/>
-      <c r="K49" s="185"/>
-      <c r="L49" s="186"/>
-      <c r="M49" s="184"/>
-      <c r="N49" s="185"/>
-      <c r="O49" s="185"/>
-      <c r="P49" s="186"/>
-      <c r="Q49" s="186"/>
+      <c r="C49" s="170"/>
+      <c r="D49" s="171"/>
+      <c r="E49" s="171"/>
+      <c r="F49" s="171"/>
+      <c r="G49" s="171"/>
+      <c r="H49" s="170"/>
+      <c r="I49" s="171"/>
+      <c r="J49" s="171"/>
+      <c r="K49" s="171"/>
+      <c r="L49" s="172"/>
+      <c r="M49" s="170"/>
+      <c r="N49" s="171"/>
+      <c r="O49" s="171"/>
+      <c r="P49" s="172"/>
+      <c r="Q49" s="172"/>
     </row>
     <row r="50" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="C50" s="180"/>
-      <c r="D50" s="181"/>
-      <c r="E50" s="181"/>
-      <c r="F50" s="181"/>
-      <c r="G50" s="182"/>
-      <c r="H50" s="180"/>
-      <c r="I50" s="181"/>
-      <c r="J50" s="181"/>
-      <c r="K50" s="181"/>
-      <c r="L50" s="182"/>
-      <c r="M50" s="180"/>
-      <c r="N50" s="181"/>
-      <c r="O50" s="181"/>
-      <c r="P50" s="182"/>
-      <c r="Q50" s="183"/>
+      <c r="C50" s="187"/>
+      <c r="D50" s="188"/>
+      <c r="E50" s="188"/>
+      <c r="F50" s="188"/>
+      <c r="G50" s="189"/>
+      <c r="H50" s="187"/>
+      <c r="I50" s="188"/>
+      <c r="J50" s="188"/>
+      <c r="K50" s="188"/>
+      <c r="L50" s="189"/>
+      <c r="M50" s="187"/>
+      <c r="N50" s="188"/>
+      <c r="O50" s="188"/>
+      <c r="P50" s="189"/>
+      <c r="Q50" s="169"/>
     </row>
     <row r="52" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="165"/>
-      <c r="C52" s="172"/>
-      <c r="D52" s="173"/>
-      <c r="E52" s="173"/>
-      <c r="F52" s="173"/>
-      <c r="G52" s="174"/>
-      <c r="H52" s="173"/>
-      <c r="I52" s="173"/>
-      <c r="J52" s="173"/>
-      <c r="K52" s="174"/>
-      <c r="L52" s="172"/>
-      <c r="M52" s="173"/>
-      <c r="N52" s="173"/>
-      <c r="O52" s="173"/>
-      <c r="P52" s="174"/>
+      <c r="C52" s="179"/>
+      <c r="D52" s="180"/>
+      <c r="E52" s="180"/>
+      <c r="F52" s="180"/>
+      <c r="G52" s="181"/>
+      <c r="H52" s="180"/>
+      <c r="I52" s="180"/>
+      <c r="J52" s="180"/>
+      <c r="K52" s="181"/>
+      <c r="L52" s="179"/>
+      <c r="M52" s="180"/>
+      <c r="N52" s="180"/>
+      <c r="O52" s="180"/>
+      <c r="P52" s="181"/>
       <c r="Q52" s="29"/>
     </row>
     <row r="53" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7417,58 +7449,58 @@
       <c r="B59" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="C59" s="184"/>
-      <c r="D59" s="185"/>
-      <c r="E59" s="185"/>
-      <c r="F59" s="185"/>
-      <c r="G59" s="185"/>
-      <c r="H59" s="184"/>
-      <c r="I59" s="185"/>
-      <c r="J59" s="185"/>
-      <c r="K59" s="186"/>
-      <c r="L59" s="184"/>
-      <c r="M59" s="185"/>
-      <c r="N59" s="185"/>
-      <c r="O59" s="185"/>
-      <c r="P59" s="186"/>
-      <c r="Q59" s="186"/>
+      <c r="C59" s="170"/>
+      <c r="D59" s="171"/>
+      <c r="E59" s="171"/>
+      <c r="F59" s="171"/>
+      <c r="G59" s="171"/>
+      <c r="H59" s="170"/>
+      <c r="I59" s="171"/>
+      <c r="J59" s="171"/>
+      <c r="K59" s="172"/>
+      <c r="L59" s="170"/>
+      <c r="M59" s="171"/>
+      <c r="N59" s="171"/>
+      <c r="O59" s="171"/>
+      <c r="P59" s="172"/>
+      <c r="Q59" s="172"/>
     </row>
     <row r="60" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="C60" s="180"/>
-      <c r="D60" s="181"/>
-      <c r="E60" s="181"/>
-      <c r="F60" s="181"/>
-      <c r="G60" s="182"/>
-      <c r="H60" s="180"/>
-      <c r="I60" s="181"/>
-      <c r="J60" s="181"/>
-      <c r="K60" s="182"/>
-      <c r="L60" s="180"/>
-      <c r="M60" s="181"/>
-      <c r="N60" s="181"/>
-      <c r="O60" s="181"/>
-      <c r="P60" s="182"/>
-      <c r="Q60" s="183"/>
+      <c r="C60" s="187"/>
+      <c r="D60" s="188"/>
+      <c r="E60" s="188"/>
+      <c r="F60" s="188"/>
+      <c r="G60" s="189"/>
+      <c r="H60" s="187"/>
+      <c r="I60" s="188"/>
+      <c r="J60" s="188"/>
+      <c r="K60" s="189"/>
+      <c r="L60" s="187"/>
+      <c r="M60" s="188"/>
+      <c r="N60" s="188"/>
+      <c r="O60" s="188"/>
+      <c r="P60" s="189"/>
+      <c r="Q60" s="169"/>
     </row>
     <row r="62" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="165"/>
-      <c r="C62" s="172"/>
-      <c r="D62" s="173"/>
-      <c r="E62" s="173"/>
-      <c r="F62" s="174"/>
-      <c r="G62" s="173"/>
-      <c r="H62" s="173"/>
-      <c r="I62" s="173"/>
-      <c r="J62" s="173"/>
-      <c r="K62" s="174"/>
-      <c r="L62" s="172"/>
-      <c r="M62" s="173"/>
-      <c r="N62" s="173"/>
-      <c r="O62" s="173"/>
-      <c r="P62" s="174"/>
+      <c r="C62" s="179"/>
+      <c r="D62" s="180"/>
+      <c r="E62" s="180"/>
+      <c r="F62" s="181"/>
+      <c r="G62" s="180"/>
+      <c r="H62" s="180"/>
+      <c r="I62" s="180"/>
+      <c r="J62" s="180"/>
+      <c r="K62" s="181"/>
+      <c r="L62" s="179"/>
+      <c r="M62" s="180"/>
+      <c r="N62" s="180"/>
+      <c r="O62" s="180"/>
+      <c r="P62" s="181"/>
       <c r="Q62" s="29"/>
     </row>
     <row r="63" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7597,44 +7629,70 @@
       <c r="B69" s="159" t="s">
         <v>86</v>
       </c>
-      <c r="C69" s="184"/>
-      <c r="D69" s="185"/>
-      <c r="E69" s="185"/>
-      <c r="F69" s="185"/>
-      <c r="G69" s="184"/>
-      <c r="H69" s="185"/>
-      <c r="I69" s="185"/>
-      <c r="J69" s="185"/>
-      <c r="K69" s="186"/>
-      <c r="L69" s="184"/>
-      <c r="M69" s="185"/>
-      <c r="N69" s="185"/>
-      <c r="O69" s="185"/>
-      <c r="P69" s="186"/>
-      <c r="Q69" s="186"/>
+      <c r="C69" s="170"/>
+      <c r="D69" s="171"/>
+      <c r="E69" s="171"/>
+      <c r="F69" s="171"/>
+      <c r="G69" s="170"/>
+      <c r="H69" s="171"/>
+      <c r="I69" s="171"/>
+      <c r="J69" s="171"/>
+      <c r="K69" s="172"/>
+      <c r="L69" s="170"/>
+      <c r="M69" s="171"/>
+      <c r="N69" s="171"/>
+      <c r="O69" s="171"/>
+      <c r="P69" s="172"/>
+      <c r="Q69" s="172"/>
     </row>
     <row r="70" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="143" t="s">
         <v>90</v>
       </c>
-      <c r="C70" s="180"/>
-      <c r="D70" s="181"/>
-      <c r="E70" s="181"/>
-      <c r="F70" s="182"/>
-      <c r="G70" s="180"/>
-      <c r="H70" s="181"/>
-      <c r="I70" s="181"/>
-      <c r="J70" s="181"/>
-      <c r="K70" s="182"/>
-      <c r="L70" s="180"/>
-      <c r="M70" s="181"/>
-      <c r="N70" s="181"/>
-      <c r="O70" s="181"/>
-      <c r="P70" s="182"/>
-      <c r="Q70" s="183"/>
+      <c r="C70" s="187"/>
+      <c r="D70" s="188"/>
+      <c r="E70" s="188"/>
+      <c r="F70" s="189"/>
+      <c r="G70" s="187"/>
+      <c r="H70" s="188"/>
+      <c r="I70" s="188"/>
+      <c r="J70" s="188"/>
+      <c r="K70" s="189"/>
+      <c r="L70" s="187"/>
+      <c r="M70" s="188"/>
+      <c r="N70" s="188"/>
+      <c r="O70" s="188"/>
+      <c r="P70" s="189"/>
+      <c r="Q70" s="169"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="K32:O32"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="G62:K62"/>
+    <mergeCell ref="L62:P62"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="M42:P42"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="L52:P52"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="L20:O20"/>
@@ -7651,32 +7709,6 @@
     <mergeCell ref="G40:J40"/>
     <mergeCell ref="K40:O40"/>
     <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="G62:K62"/>
-    <mergeCell ref="L62:P62"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="M42:P42"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="L52:P52"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="K32:O32"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:N10"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="L20 M50 K10 K40 L60 L70 C10 G10 C20 H20 C70 G70 C60 H60 C50 H50 C40 G40 C30 G30 L30" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
@@ -7693,6 +7725,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7915,15 +7956,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
   <ds:schemaRefs>
@@ -7942,6 +7974,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7958,12 +7998,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged PR 18015: BP-5855 : User is able to see incorrect values in the Account Executive', 'Client Contact and Status field for Unified Campaign plans
User is able to see incorrect values in the Account Executive', 'Client Contact and Status field for Unified Campaign plans
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA383E30-C536-4188-8AC2-549088DA63EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7B93C9-CEF0-477D-A976-01AF02B066D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2269,7 +2269,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2361,7 +2361,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="46" t="str">
-        <f>IF(Proposal!P5=0,"")</f>
+        <f>IF(Proposal!Q5=0,"")</f>
         <v/>
       </c>
       <c r="L5" s="46" t="str">
@@ -5389,6 +5389,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5398,11 +5403,6 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5562,7 +5562,7 @@
   <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="I1" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+      <selection activeCell="R5" sqref="R5:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6207,13 +6207,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
     <mergeCell ref="F28:U28"/>
     <mergeCell ref="F20:U20"/>
     <mergeCell ref="H13:N13"/>
@@ -6222,6 +6215,13 @@
     <mergeCell ref="F24:U24"/>
     <mergeCell ref="F26:U26"/>
     <mergeCell ref="O13:U13"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:U3 C5 C4:N4 Q4:U4 U5 C6:U1048576">
     <cfRule type="expression" dxfId="2" priority="3">
@@ -7481,6 +7481,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="K32:O32"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="G62:K62"/>
+    <mergeCell ref="L62:P62"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="M42:P42"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="L52:P52"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="L20:O20"/>
@@ -7497,32 +7523,6 @@
     <mergeCell ref="G40:J40"/>
     <mergeCell ref="K40:O40"/>
     <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="G62:K62"/>
-    <mergeCell ref="L62:P62"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="M42:P42"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="L52:P52"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="K32:O32"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:N10"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="L20 M50 K10 K40 L60 L70 C10 G10 C20 H20 C70 G70 C60 H60 C50 H50 C40 G40 C30 G30 L30" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
@@ -7533,6 +7533,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7755,22 +7770,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7787,29 +7812,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged PR 18064: BP-5855: User is able to see incorrect values in the Account Executive', 'Client Contact and Status field for Unified Campaign plans
User is able to see incorrect values in the Account Executive', 'Client Contact and Status field for Unified Campaign plans
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7B93C9-CEF0-477D-A976-01AF02B066D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F39EF6-2A0C-4557-BB48-E0A11C283920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24870" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="4" r:id="rId1"/>
@@ -2269,7 +2269,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2361,11 +2361,11 @@
         <v>0</v>
       </c>
       <c r="K5" s="46" t="str">
-        <f>IF(Proposal!Q5=0,"")</f>
+        <f>IF(Proposal!Q5=0,"",Proposal!Q5)</f>
         <v/>
       </c>
       <c r="L5" s="46" t="str">
-        <f>IF(Proposal!R5=0,"")</f>
+        <f>IF(Proposal!R5=0,"",Proposal!R5)</f>
         <v/>
       </c>
       <c r="M5" s="46">
@@ -5389,11 +5389,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5403,6 +5398,11 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5562,7 +5562,7 @@
   <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="I1" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5:T5"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6207,6 +6207,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
     <mergeCell ref="F28:U28"/>
     <mergeCell ref="F20:U20"/>
     <mergeCell ref="H13:N13"/>
@@ -6215,13 +6222,6 @@
     <mergeCell ref="F24:U24"/>
     <mergeCell ref="F26:U26"/>
     <mergeCell ref="O13:U13"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:U3 C5 C4:N4 Q4:U4 U5 C6:U1048576">
     <cfRule type="expression" dxfId="2" priority="3">
@@ -7481,32 +7481,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="K32:O32"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="G62:K62"/>
-    <mergeCell ref="L62:P62"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="M42:P42"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="L52:P52"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="L20:O20"/>
@@ -7523,6 +7497,32 @@
     <mergeCell ref="G40:J40"/>
     <mergeCell ref="K40:O40"/>
     <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="G62:K62"/>
+    <mergeCell ref="L62:P62"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="M42:P42"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="L52:P52"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="K32:O32"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="L20 M50 K10 K40 L60 L70 C10 G10 C20 H20 C70 G70 C60 H60 C50 H50 C40 G40 C30 G30 L30" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
@@ -7533,21 +7533,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7770,32 +7755,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7812,4 +7787,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged PR 18072: BP-5685 : Open market file export implementation DB Script Fixed
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F39EF6-2A0C-4557-BB48-E0A11C283920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F57890D-419E-42CB-9D52-B941400ABD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24870" windowHeight="11250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="9720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="4" r:id="rId1"/>
@@ -2268,7 +2268,7 @@
   </sheetPr>
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -5389,6 +5389,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5398,11 +5403,6 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5561,8 +5561,8 @@
   </sheetPr>
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="I1" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6207,13 +6207,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
     <mergeCell ref="F28:U28"/>
     <mergeCell ref="F20:U20"/>
     <mergeCell ref="H13:N13"/>
@@ -6222,6 +6215,13 @@
     <mergeCell ref="F24:U24"/>
     <mergeCell ref="F26:U26"/>
     <mergeCell ref="O13:U13"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:U3 C5 C4:N4 Q4:U4 U5 C6:U1048576">
     <cfRule type="expression" dxfId="2" priority="3">
@@ -7481,6 +7481,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="K32:O32"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="G62:K62"/>
+    <mergeCell ref="L62:P62"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="M42:P42"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="L52:P52"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="L20:O20"/>
@@ -7497,32 +7523,6 @@
     <mergeCell ref="G40:J40"/>
     <mergeCell ref="K40:O40"/>
     <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="G62:K62"/>
-    <mergeCell ref="L62:P62"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="M42:P42"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="L52:P52"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="K32:O32"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:N10"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="L20 M50 K10 K40 L60 L70 C10 G10 C20 H20 C70 G70 C60 H60 C50 H50 C40 G40 C30 G30 L30" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
@@ -7533,6 +7533,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7755,22 +7770,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7787,29 +7812,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged PR 18091: BP-5808_Program_Genres_ForeignKey
BP-5808_Program_Genres_ForeignKey
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F57890D-419E-42CB-9D52-B941400ABD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA49A774-64D6-4532-9E37-6BE41DCD0B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="9720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9810" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="4" r:id="rId1"/>
@@ -2269,7 +2269,7 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2356,10 +2356,7 @@
         <f>Proposal!O5</f>
         <v>0</v>
       </c>
-      <c r="J5" s="46">
-        <f>Proposal!P5</f>
-        <v>0</v>
-      </c>
+      <c r="J5" s="46"/>
       <c r="K5" s="46" t="str">
         <f>IF(Proposal!Q5=0,"",Proposal!Q5)</f>
         <v/>
@@ -5389,11 +5386,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5403,6 +5395,11 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -6207,6 +6204,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
     <mergeCell ref="F28:U28"/>
     <mergeCell ref="F20:U20"/>
     <mergeCell ref="H13:N13"/>
@@ -6215,13 +6219,6 @@
     <mergeCell ref="F24:U24"/>
     <mergeCell ref="F26:U26"/>
     <mergeCell ref="O13:U13"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:U3 C5 C4:N4 Q4:U4 U5 C6:U1048576">
     <cfRule type="expression" dxfId="2" priority="3">
@@ -7481,32 +7478,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="K32:O32"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="G62:K62"/>
-    <mergeCell ref="L62:P62"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="M42:P42"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="L52:P52"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="L20:O20"/>
@@ -7523,6 +7494,32 @@
     <mergeCell ref="G40:J40"/>
     <mergeCell ref="K40:O40"/>
     <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="G62:K62"/>
+    <mergeCell ref="L62:P62"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="M42:P42"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="L52:P52"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="K32:O32"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="L20 M50 K10 K40 L60 L70 C10 G10 C20 H20 C70 G70 C60 H60 C50 H50 C40 G40 C30 G30 L30" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
@@ -7533,21 +7530,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7770,32 +7752,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7812,4 +7784,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged PR 18094: BP-5855_  Projects Broadcast Project KPI-5312  BP-5855  User is able to see incorrect values in the Account Executive', 'Client Contact and Status field for Unified Campaign plans
BP-5855_  Projects Broadcast Project KPI-5312  BP-5855  User is able to see incorrect values in the Account Executive', 'Client Contact and Status field for Unified Campaign plans
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA49A774-64D6-4532-9E37-6BE41DCD0B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54C5504-DCC9-4590-BDF2-9657D2B5FE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9810" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="4" r:id="rId1"/>
@@ -690,12 +690,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="#,##0.000"/>
+    <numFmt numFmtId="169" formatCode="\ 0;\-0;;@\,"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -1159,7 +1160,7 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1626,6 +1627,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2268,8 +2272,8 @@
   </sheetPr>
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2357,13 +2361,13 @@
         <v>0</v>
       </c>
       <c r="J5" s="46"/>
-      <c r="K5" s="46" t="str">
-        <f>IF(Proposal!Q5=0,"",Proposal!Q5)</f>
-        <v/>
-      </c>
-      <c r="L5" s="46" t="str">
-        <f>IF(Proposal!R5=0,"",Proposal!R5)</f>
-        <v/>
+      <c r="K5" s="159">
+        <f>Proposal!Q5</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="159">
+        <f>Proposal!R5</f>
+        <v>0</v>
       </c>
       <c r="M5" s="46">
         <f>Proposal!V5</f>
@@ -5386,6 +5390,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5395,11 +5404,6 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5558,8 +5562,8 @@
   </sheetPr>
   <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5:T5"/>
+    <sheetView showGridLines="0" topLeftCell="I1" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6204,13 +6208,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
     <mergeCell ref="F28:U28"/>
     <mergeCell ref="F20:U20"/>
     <mergeCell ref="H13:N13"/>
@@ -6219,6 +6216,13 @@
     <mergeCell ref="F24:U24"/>
     <mergeCell ref="F26:U26"/>
     <mergeCell ref="O13:U13"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:U3 C5 C4:N4 Q4:U4 U5 C6:U1048576">
     <cfRule type="expression" dxfId="2" priority="3">
@@ -7478,6 +7482,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="K32:O32"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="G62:K62"/>
+    <mergeCell ref="L62:P62"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="M42:P42"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="L52:P52"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="L20:O20"/>
@@ -7494,32 +7524,6 @@
     <mergeCell ref="G40:J40"/>
     <mergeCell ref="K40:O40"/>
     <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="G62:K62"/>
-    <mergeCell ref="L62:P62"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="M42:P42"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="L52:P52"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="K32:O32"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:N10"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="L20 M50 K10 K40 L60 L70 C10 G10 C20 H20 C70 G70 C60 H60 C50 H50 C40 G40 C30 G30 L30" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
@@ -7530,6 +7534,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7752,22 +7771,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7784,29 +7813,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged PR 19879: BS-273-Fluidity percentage is not reflected in Contract tab of Excel if Unified Campaign is exported
Fluidity percentage is not reflected in Contract tab of Excel if Unified Campaign is exported
</commit_message>
<xml_diff>
--- a/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
+++ b/Source/Tam/Maestro/UI/BroadcastComposerWeb/App_Data/Template - Campaign Export With Secondary Audiences.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git1\Broadcast\Source\Tam\Maestro\UI\BroadcastComposerWeb\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54C5504-DCC9-4590-BDF2-9657D2B5FE59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5078B5BE-9A88-45E2-9A99-63E8DF01E446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1571,6 +1571,9 @@
     <xf numFmtId="1" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
@@ -1627,9 +1630,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2272,8 +2272,8 @@
   </sheetPr>
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2343,11 +2343,11 @@
         <f>Proposal!E5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="140">
+      <c r="E5" s="141">
         <f>Proposal!I5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="140"/>
+      <c r="F5" s="141"/>
       <c r="G5" s="46">
         <f>Proposal!K5</f>
         <v>0</v>
@@ -2360,12 +2360,15 @@
         <f>Proposal!O5</f>
         <v>0</v>
       </c>
-      <c r="J5" s="46"/>
-      <c r="K5" s="159">
+      <c r="J5" s="46">
+        <f>Proposal!P5</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="140">
         <f>Proposal!Q5</f>
         <v>0</v>
       </c>
-      <c r="L5" s="159">
+      <c r="L5" s="140">
         <f>Proposal!R5</f>
         <v>0</v>
       </c>
@@ -2535,14 +2538,14 @@
       <c r="C18" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="142"/>
-      <c r="E18" s="142"/>
-      <c r="F18" s="142"/>
-      <c r="G18" s="142"/>
-      <c r="H18" s="142"/>
-      <c r="I18" s="142"/>
-      <c r="J18" s="142"/>
-      <c r="K18" s="142"/>
+      <c r="D18" s="143"/>
+      <c r="E18" s="143"/>
+      <c r="F18" s="143"/>
+      <c r="G18" s="143"/>
+      <c r="H18" s="143"/>
+      <c r="I18" s="143"/>
+      <c r="J18" s="143"/>
+      <c r="K18" s="143"/>
       <c r="L18" s="103"/>
       <c r="M18" s="103"/>
       <c r="N18" s="103"/>
@@ -2573,14 +2576,14 @@
       <c r="C20" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="143"/>
-      <c r="E20" s="143"/>
-      <c r="F20" s="143"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="143"/>
-      <c r="I20" s="143"/>
-      <c r="J20" s="143"/>
-      <c r="K20" s="143"/>
+      <c r="D20" s="144"/>
+      <c r="E20" s="144"/>
+      <c r="F20" s="144"/>
+      <c r="G20" s="144"/>
+      <c r="H20" s="144"/>
+      <c r="I20" s="144"/>
+      <c r="J20" s="144"/>
+      <c r="K20" s="144"/>
       <c r="L20" s="103"/>
       <c r="M20" s="103"/>
       <c r="N20" s="103"/>
@@ -2611,14 +2614,14 @@
       <c r="C22" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="142"/>
-      <c r="E22" s="142"/>
-      <c r="F22" s="142"/>
-      <c r="G22" s="142"/>
-      <c r="H22" s="142"/>
-      <c r="I22" s="142"/>
-      <c r="J22" s="142"/>
-      <c r="K22" s="142"/>
+      <c r="D22" s="143"/>
+      <c r="E22" s="143"/>
+      <c r="F22" s="143"/>
+      <c r="G22" s="143"/>
+      <c r="H22" s="143"/>
+      <c r="I22" s="143"/>
+      <c r="J22" s="143"/>
+      <c r="K22" s="143"/>
       <c r="L22" s="56"/>
       <c r="M22" s="56"/>
       <c r="N22" s="56"/>
@@ -2642,14 +2645,14 @@
       <c r="C24" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="143"/>
-      <c r="E24" s="143"/>
-      <c r="F24" s="143"/>
-      <c r="G24" s="143"/>
-      <c r="H24" s="143"/>
-      <c r="I24" s="143"/>
-      <c r="J24" s="143"/>
-      <c r="K24" s="143"/>
+      <c r="D24" s="144"/>
+      <c r="E24" s="144"/>
+      <c r="F24" s="144"/>
+      <c r="G24" s="144"/>
+      <c r="H24" s="144"/>
+      <c r="I24" s="144"/>
+      <c r="J24" s="144"/>
+      <c r="K24" s="144"/>
     </row>
     <row r="25" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
@@ -2666,24 +2669,24 @@
       <c r="C26" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="142"/>
-      <c r="E26" s="143"/>
-      <c r="F26" s="143"/>
-      <c r="G26" s="143"/>
-      <c r="H26" s="143"/>
-      <c r="I26" s="143"/>
-      <c r="J26" s="143"/>
-      <c r="K26" s="143"/>
+      <c r="D26" s="143"/>
+      <c r="E26" s="144"/>
+      <c r="F26" s="144"/>
+      <c r="G26" s="144"/>
+      <c r="H26" s="144"/>
+      <c r="I26" s="144"/>
+      <c r="J26" s="144"/>
+      <c r="K26" s="144"/>
     </row>
     <row r="27" spans="3:18" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="141"/>
-      <c r="E27" s="141"/>
-      <c r="F27" s="141"/>
-      <c r="G27" s="141"/>
-      <c r="H27" s="141"/>
-      <c r="I27" s="141"/>
-      <c r="J27" s="141"/>
-      <c r="K27" s="141"/>
+      <c r="D27" s="142"/>
+      <c r="E27" s="142"/>
+      <c r="F27" s="142"/>
+      <c r="G27" s="142"/>
+      <c r="H27" s="142"/>
+      <c r="I27" s="142"/>
+      <c r="J27" s="142"/>
+      <c r="K27" s="142"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2760,19 +2763,19 @@
         <f>Proposal!O5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="140"/>
-      <c r="E5" s="140"/>
-      <c r="F5" s="140"/>
-      <c r="G5" s="140"/>
-      <c r="H5" s="140"/>
-      <c r="I5" s="140"/>
-      <c r="J5" s="140"/>
-      <c r="K5" s="140"/>
-      <c r="L5" s="140"/>
-      <c r="M5" s="140"/>
-      <c r="N5" s="140"/>
-      <c r="O5" s="140"/>
-      <c r="P5" s="140"/>
+      <c r="D5" s="141"/>
+      <c r="E5" s="141"/>
+      <c r="F5" s="141"/>
+      <c r="G5" s="141"/>
+      <c r="H5" s="141"/>
+      <c r="I5" s="141"/>
+      <c r="J5" s="141"/>
+      <c r="K5" s="141"/>
+      <c r="L5" s="141"/>
+      <c r="M5" s="141"/>
+      <c r="N5" s="141"/>
+      <c r="O5" s="141"/>
+      <c r="P5" s="141"/>
     </row>
     <row r="7" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="6"/>
@@ -2932,24 +2935,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="17"/>
       <c r="F7" s="22"/>
-      <c r="G7" s="148" t="s">
+      <c r="G7" s="149" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="148"/>
-      <c r="I7" s="148"/>
-      <c r="J7" s="148"/>
-      <c r="K7" s="148"/>
-      <c r="L7" s="149"/>
+      <c r="H7" s="149"/>
+      <c r="I7" s="149"/>
+      <c r="J7" s="149"/>
+      <c r="K7" s="149"/>
+      <c r="L7" s="150"/>
       <c r="M7" s="26"/>
-      <c r="N7" s="148" t="s">
+      <c r="N7" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="148"/>
-      <c r="P7" s="148"/>
-      <c r="Q7" s="148"/>
-      <c r="R7" s="148"/>
-      <c r="S7" s="148"/>
-      <c r="T7" s="149"/>
+      <c r="O7" s="149"/>
+      <c r="P7" s="149"/>
+      <c r="Q7" s="149"/>
+      <c r="R7" s="149"/>
+      <c r="S7" s="149"/>
+      <c r="T7" s="150"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
@@ -3193,24 +3196,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="17"/>
       <c r="F13" s="22"/>
-      <c r="G13" s="145" t="s">
+      <c r="G13" s="146" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="146"/>
-      <c r="I13" s="146"/>
-      <c r="J13" s="146"/>
-      <c r="K13" s="146"/>
-      <c r="L13" s="147"/>
+      <c r="H13" s="147"/>
+      <c r="I13" s="147"/>
+      <c r="J13" s="147"/>
+      <c r="K13" s="147"/>
+      <c r="L13" s="148"/>
       <c r="M13" s="26"/>
-      <c r="N13" s="145" t="s">
+      <c r="N13" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="146"/>
-      <c r="P13" s="146"/>
-      <c r="Q13" s="146"/>
-      <c r="R13" s="146"/>
-      <c r="S13" s="146"/>
-      <c r="T13" s="147"/>
+      <c r="O13" s="147"/>
+      <c r="P13" s="147"/>
+      <c r="Q13" s="147"/>
+      <c r="R13" s="147"/>
+      <c r="S13" s="147"/>
+      <c r="T13" s="148"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="31" t="s">
@@ -3450,24 +3453,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="17"/>
       <c r="F19" s="22"/>
-      <c r="G19" s="145" t="s">
+      <c r="G19" s="146" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="146"/>
-      <c r="I19" s="146"/>
-      <c r="J19" s="146"/>
-      <c r="K19" s="146"/>
-      <c r="L19" s="147"/>
+      <c r="H19" s="147"/>
+      <c r="I19" s="147"/>
+      <c r="J19" s="147"/>
+      <c r="K19" s="147"/>
+      <c r="L19" s="148"/>
       <c r="M19" s="26"/>
-      <c r="N19" s="145" t="s">
+      <c r="N19" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="146"/>
-      <c r="P19" s="146"/>
-      <c r="Q19" s="146"/>
-      <c r="R19" s="146"/>
-      <c r="S19" s="146"/>
-      <c r="T19" s="147"/>
+      <c r="O19" s="147"/>
+      <c r="P19" s="147"/>
+      <c r="Q19" s="147"/>
+      <c r="R19" s="147"/>
+      <c r="S19" s="147"/>
+      <c r="T19" s="148"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="31" t="s">
@@ -3737,25 +3740,25 @@
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="150" t="s">
+      <c r="D25" s="151" t="s">
         <v>43</v>
       </c>
-      <c r="E25" s="150"/>
-      <c r="F25" s="150"/>
-      <c r="G25" s="150"/>
-      <c r="H25" s="150"/>
-      <c r="I25" s="150"/>
-      <c r="J25" s="150"/>
-      <c r="K25" s="150"/>
-      <c r="L25" s="150"/>
-      <c r="M25" s="150"/>
-      <c r="N25" s="150"/>
-      <c r="O25" s="150"/>
-      <c r="P25" s="150"/>
-      <c r="Q25" s="150"/>
-      <c r="R25" s="150"/>
-      <c r="S25" s="150"/>
-      <c r="T25" s="150"/>
+      <c r="E25" s="151"/>
+      <c r="F25" s="151"/>
+      <c r="G25" s="151"/>
+      <c r="H25" s="151"/>
+      <c r="I25" s="151"/>
+      <c r="J25" s="151"/>
+      <c r="K25" s="151"/>
+      <c r="L25" s="151"/>
+      <c r="M25" s="151"/>
+      <c r="N25" s="151"/>
+      <c r="O25" s="151"/>
+      <c r="P25" s="151"/>
+      <c r="Q25" s="151"/>
+      <c r="R25" s="151"/>
+      <c r="S25" s="151"/>
+      <c r="T25" s="151"/>
     </row>
     <row r="26" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -3781,25 +3784,25 @@
       <c r="B27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="150" t="s">
+      <c r="D27" s="151" t="s">
         <v>45</v>
       </c>
-      <c r="E27" s="150"/>
-      <c r="F27" s="150"/>
-      <c r="G27" s="150"/>
-      <c r="H27" s="150"/>
-      <c r="I27" s="150"/>
-      <c r="J27" s="150"/>
-      <c r="K27" s="150"/>
-      <c r="L27" s="150"/>
-      <c r="M27" s="150"/>
-      <c r="N27" s="150"/>
-      <c r="O27" s="150"/>
-      <c r="P27" s="150"/>
-      <c r="Q27" s="150"/>
-      <c r="R27" s="150"/>
-      <c r="S27" s="150"/>
-      <c r="T27" s="150"/>
+      <c r="E27" s="151"/>
+      <c r="F27" s="151"/>
+      <c r="G27" s="151"/>
+      <c r="H27" s="151"/>
+      <c r="I27" s="151"/>
+      <c r="J27" s="151"/>
+      <c r="K27" s="151"/>
+      <c r="L27" s="151"/>
+      <c r="M27" s="151"/>
+      <c r="N27" s="151"/>
+      <c r="O27" s="151"/>
+      <c r="P27" s="151"/>
+      <c r="Q27" s="151"/>
+      <c r="R27" s="151"/>
+      <c r="S27" s="151"/>
+      <c r="T27" s="151"/>
     </row>
     <row r="28" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
@@ -3825,25 +3828,25 @@
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="150" t="s">
+      <c r="D29" s="151" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="150"/>
-      <c r="F29" s="150"/>
-      <c r="G29" s="150"/>
-      <c r="H29" s="150"/>
-      <c r="I29" s="150"/>
-      <c r="J29" s="150"/>
-      <c r="K29" s="150"/>
-      <c r="L29" s="150"/>
-      <c r="M29" s="150"/>
-      <c r="N29" s="150"/>
-      <c r="O29" s="150"/>
-      <c r="P29" s="150"/>
-      <c r="Q29" s="150"/>
-      <c r="R29" s="150"/>
-      <c r="S29" s="150"/>
-      <c r="T29" s="150"/>
+      <c r="E29" s="151"/>
+      <c r="F29" s="151"/>
+      <c r="G29" s="151"/>
+      <c r="H29" s="151"/>
+      <c r="I29" s="151"/>
+      <c r="J29" s="151"/>
+      <c r="K29" s="151"/>
+      <c r="L29" s="151"/>
+      <c r="M29" s="151"/>
+      <c r="N29" s="151"/>
+      <c r="O29" s="151"/>
+      <c r="P29" s="151"/>
+      <c r="Q29" s="151"/>
+      <c r="R29" s="151"/>
+      <c r="S29" s="151"/>
+      <c r="T29" s="151"/>
     </row>
     <row r="30" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
@@ -3869,25 +3872,25 @@
       <c r="B31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="150" t="s">
+      <c r="D31" s="151" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="150"/>
-      <c r="F31" s="150"/>
-      <c r="G31" s="150"/>
-      <c r="H31" s="150"/>
-      <c r="I31" s="150"/>
-      <c r="J31" s="150"/>
-      <c r="K31" s="150"/>
-      <c r="L31" s="150"/>
-      <c r="M31" s="150"/>
-      <c r="N31" s="150"/>
-      <c r="O31" s="150"/>
-      <c r="P31" s="150"/>
-      <c r="Q31" s="150"/>
-      <c r="R31" s="150"/>
-      <c r="S31" s="150"/>
-      <c r="T31" s="150"/>
+      <c r="E31" s="151"/>
+      <c r="F31" s="151"/>
+      <c r="G31" s="151"/>
+      <c r="H31" s="151"/>
+      <c r="I31" s="151"/>
+      <c r="J31" s="151"/>
+      <c r="K31" s="151"/>
+      <c r="L31" s="151"/>
+      <c r="M31" s="151"/>
+      <c r="N31" s="151"/>
+      <c r="O31" s="151"/>
+      <c r="P31" s="151"/>
+      <c r="Q31" s="151"/>
+      <c r="R31" s="151"/>
+      <c r="S31" s="151"/>
+      <c r="T31" s="151"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -3913,25 +3916,25 @@
       <c r="B33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="150" t="s">
+      <c r="D33" s="151" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="150"/>
-      <c r="F33" s="150"/>
-      <c r="G33" s="150"/>
-      <c r="H33" s="150"/>
-      <c r="I33" s="150"/>
-      <c r="J33" s="150"/>
-      <c r="K33" s="150"/>
-      <c r="L33" s="150"/>
-      <c r="M33" s="150"/>
-      <c r="N33" s="150"/>
-      <c r="O33" s="150"/>
-      <c r="P33" s="150"/>
-      <c r="Q33" s="150"/>
-      <c r="R33" s="150"/>
-      <c r="S33" s="150"/>
-      <c r="T33" s="150"/>
+      <c r="E33" s="151"/>
+      <c r="F33" s="151"/>
+      <c r="G33" s="151"/>
+      <c r="H33" s="151"/>
+      <c r="I33" s="151"/>
+      <c r="J33" s="151"/>
+      <c r="K33" s="151"/>
+      <c r="L33" s="151"/>
+      <c r="M33" s="151"/>
+      <c r="N33" s="151"/>
+      <c r="O33" s="151"/>
+      <c r="P33" s="151"/>
+      <c r="Q33" s="151"/>
+      <c r="R33" s="151"/>
+      <c r="S33" s="151"/>
+      <c r="T33" s="151"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -3957,25 +3960,25 @@
       <c r="B35" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="144" t="s">
+      <c r="D35" s="145" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="144"/>
-      <c r="F35" s="144"/>
-      <c r="G35" s="144"/>
-      <c r="H35" s="144"/>
-      <c r="I35" s="144"/>
-      <c r="J35" s="144"/>
-      <c r="K35" s="144"/>
-      <c r="L35" s="144"/>
-      <c r="M35" s="144"/>
-      <c r="N35" s="144"/>
-      <c r="O35" s="144"/>
-      <c r="P35" s="144"/>
-      <c r="Q35" s="144"/>
-      <c r="R35" s="144"/>
-      <c r="S35" s="144"/>
-      <c r="T35" s="144"/>
+      <c r="E35" s="145"/>
+      <c r="F35" s="145"/>
+      <c r="G35" s="145"/>
+      <c r="H35" s="145"/>
+      <c r="I35" s="145"/>
+      <c r="J35" s="145"/>
+      <c r="K35" s="145"/>
+      <c r="L35" s="145"/>
+      <c r="M35" s="145"/>
+      <c r="N35" s="145"/>
+      <c r="O35" s="145"/>
+      <c r="P35" s="145"/>
+      <c r="Q35" s="145"/>
+      <c r="R35" s="145"/>
+      <c r="S35" s="145"/>
+      <c r="T35" s="145"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4113,24 +4116,24 @@
       <c r="D7" s="6"/>
       <c r="E7" s="17"/>
       <c r="F7" s="22"/>
-      <c r="G7" s="148" t="s">
+      <c r="G7" s="149" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="148"/>
-      <c r="I7" s="148"/>
-      <c r="J7" s="148"/>
-      <c r="K7" s="148"/>
-      <c r="L7" s="149"/>
+      <c r="H7" s="149"/>
+      <c r="I7" s="149"/>
+      <c r="J7" s="149"/>
+      <c r="K7" s="149"/>
+      <c r="L7" s="150"/>
       <c r="M7" s="26"/>
-      <c r="N7" s="148" t="s">
+      <c r="N7" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="O7" s="148"/>
-      <c r="P7" s="148"/>
-      <c r="Q7" s="148"/>
-      <c r="R7" s="148"/>
-      <c r="S7" s="148"/>
-      <c r="T7" s="149"/>
+      <c r="O7" s="149"/>
+      <c r="P7" s="149"/>
+      <c r="Q7" s="149"/>
+      <c r="R7" s="149"/>
+      <c r="S7" s="149"/>
+      <c r="T7" s="150"/>
     </row>
     <row r="8" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
@@ -4372,24 +4375,24 @@
       <c r="D13" s="6"/>
       <c r="E13" s="17"/>
       <c r="F13" s="22"/>
-      <c r="G13" s="145" t="s">
+      <c r="G13" s="146" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="146"/>
-      <c r="I13" s="146"/>
-      <c r="J13" s="146"/>
-      <c r="K13" s="146"/>
-      <c r="L13" s="147"/>
+      <c r="H13" s="147"/>
+      <c r="I13" s="147"/>
+      <c r="J13" s="147"/>
+      <c r="K13" s="147"/>
+      <c r="L13" s="148"/>
       <c r="M13" s="26"/>
-      <c r="N13" s="145" t="s">
+      <c r="N13" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="146"/>
-      <c r="P13" s="146"/>
-      <c r="Q13" s="146"/>
-      <c r="R13" s="146"/>
-      <c r="S13" s="146"/>
-      <c r="T13" s="147"/>
+      <c r="O13" s="147"/>
+      <c r="P13" s="147"/>
+      <c r="Q13" s="147"/>
+      <c r="R13" s="147"/>
+      <c r="S13" s="147"/>
+      <c r="T13" s="148"/>
     </row>
     <row r="14" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="31" t="s">
@@ -4627,24 +4630,24 @@
       <c r="D19" s="6"/>
       <c r="E19" s="17"/>
       <c r="F19" s="22"/>
-      <c r="G19" s="145" t="s">
+      <c r="G19" s="146" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="146"/>
-      <c r="I19" s="146"/>
-      <c r="J19" s="146"/>
-      <c r="K19" s="146"/>
-      <c r="L19" s="147"/>
+      <c r="H19" s="147"/>
+      <c r="I19" s="147"/>
+      <c r="J19" s="147"/>
+      <c r="K19" s="147"/>
+      <c r="L19" s="148"/>
       <c r="M19" s="26"/>
-      <c r="N19" s="145" t="s">
+      <c r="N19" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="146"/>
-      <c r="P19" s="146"/>
-      <c r="Q19" s="146"/>
-      <c r="R19" s="146"/>
-      <c r="S19" s="146"/>
-      <c r="T19" s="147"/>
+      <c r="O19" s="147"/>
+      <c r="P19" s="147"/>
+      <c r="Q19" s="147"/>
+      <c r="R19" s="147"/>
+      <c r="S19" s="147"/>
+      <c r="T19" s="148"/>
     </row>
     <row r="20" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="31" t="s">
@@ -4882,24 +4885,24 @@
       <c r="D25" s="6"/>
       <c r="E25" s="17"/>
       <c r="F25" s="22"/>
-      <c r="G25" s="145" t="s">
+      <c r="G25" s="146" t="s">
         <v>28</v>
       </c>
-      <c r="H25" s="146"/>
-      <c r="I25" s="146"/>
-      <c r="J25" s="146"/>
-      <c r="K25" s="146"/>
-      <c r="L25" s="147"/>
+      <c r="H25" s="147"/>
+      <c r="I25" s="147"/>
+      <c r="J25" s="147"/>
+      <c r="K25" s="147"/>
+      <c r="L25" s="148"/>
       <c r="M25" s="26"/>
-      <c r="N25" s="145" t="s">
+      <c r="N25" s="146" t="s">
         <v>10</v>
       </c>
-      <c r="O25" s="146"/>
-      <c r="P25" s="146"/>
-      <c r="Q25" s="146"/>
-      <c r="R25" s="146"/>
-      <c r="S25" s="146"/>
-      <c r="T25" s="147"/>
+      <c r="O25" s="147"/>
+      <c r="P25" s="147"/>
+      <c r="Q25" s="147"/>
+      <c r="R25" s="147"/>
+      <c r="S25" s="147"/>
+      <c r="T25" s="148"/>
     </row>
     <row r="26" spans="2:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="31" t="s">
@@ -5137,26 +5140,26 @@
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="140" t="s">
+      <c r="C31" s="141" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="140"/>
-      <c r="E31" s="140"/>
-      <c r="F31" s="140"/>
-      <c r="G31" s="140"/>
-      <c r="H31" s="140"/>
-      <c r="I31" s="140"/>
-      <c r="J31" s="140"/>
-      <c r="K31" s="140"/>
-      <c r="L31" s="140"/>
-      <c r="M31" s="140"/>
-      <c r="N31" s="140"/>
-      <c r="O31" s="140"/>
-      <c r="P31" s="140"/>
-      <c r="Q31" s="140"/>
-      <c r="R31" s="140"/>
-      <c r="S31" s="140"/>
-      <c r="T31" s="140"/>
+      <c r="D31" s="141"/>
+      <c r="E31" s="141"/>
+      <c r="F31" s="141"/>
+      <c r="G31" s="141"/>
+      <c r="H31" s="141"/>
+      <c r="I31" s="141"/>
+      <c r="J31" s="141"/>
+      <c r="K31" s="141"/>
+      <c r="L31" s="141"/>
+      <c r="M31" s="141"/>
+      <c r="N31" s="141"/>
+      <c r="O31" s="141"/>
+      <c r="P31" s="141"/>
+      <c r="Q31" s="141"/>
+      <c r="R31" s="141"/>
+      <c r="S31" s="141"/>
+      <c r="T31" s="141"/>
     </row>
     <row r="32" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
@@ -5183,26 +5186,26 @@
       <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="140" t="s">
+      <c r="C33" s="141" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="140"/>
-      <c r="E33" s="140"/>
-      <c r="F33" s="140"/>
-      <c r="G33" s="140"/>
-      <c r="H33" s="140"/>
-      <c r="I33" s="140"/>
-      <c r="J33" s="140"/>
-      <c r="K33" s="140"/>
-      <c r="L33" s="140"/>
-      <c r="M33" s="140"/>
-      <c r="N33" s="140"/>
-      <c r="O33" s="140"/>
-      <c r="P33" s="140"/>
-      <c r="Q33" s="140"/>
-      <c r="R33" s="140"/>
-      <c r="S33" s="140"/>
-      <c r="T33" s="140"/>
+      <c r="D33" s="141"/>
+      <c r="E33" s="141"/>
+      <c r="F33" s="141"/>
+      <c r="G33" s="141"/>
+      <c r="H33" s="141"/>
+      <c r="I33" s="141"/>
+      <c r="J33" s="141"/>
+      <c r="K33" s="141"/>
+      <c r="L33" s="141"/>
+      <c r="M33" s="141"/>
+      <c r="N33" s="141"/>
+      <c r="O33" s="141"/>
+      <c r="P33" s="141"/>
+      <c r="Q33" s="141"/>
+      <c r="R33" s="141"/>
+      <c r="S33" s="141"/>
+      <c r="T33" s="141"/>
     </row>
     <row r="34" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
@@ -5229,26 +5232,26 @@
       <c r="B35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="140" t="s">
+      <c r="C35" s="141" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="140"/>
-      <c r="E35" s="140"/>
-      <c r="F35" s="140"/>
-      <c r="G35" s="140"/>
-      <c r="H35" s="140"/>
-      <c r="I35" s="140"/>
-      <c r="J35" s="140"/>
-      <c r="K35" s="140"/>
-      <c r="L35" s="140"/>
-      <c r="M35" s="140"/>
-      <c r="N35" s="140"/>
-      <c r="O35" s="140"/>
-      <c r="P35" s="140"/>
-      <c r="Q35" s="140"/>
-      <c r="R35" s="140"/>
-      <c r="S35" s="140"/>
-      <c r="T35" s="140"/>
+      <c r="D35" s="141"/>
+      <c r="E35" s="141"/>
+      <c r="F35" s="141"/>
+      <c r="G35" s="141"/>
+      <c r="H35" s="141"/>
+      <c r="I35" s="141"/>
+      <c r="J35" s="141"/>
+      <c r="K35" s="141"/>
+      <c r="L35" s="141"/>
+      <c r="M35" s="141"/>
+      <c r="N35" s="141"/>
+      <c r="O35" s="141"/>
+      <c r="P35" s="141"/>
+      <c r="Q35" s="141"/>
+      <c r="R35" s="141"/>
+      <c r="S35" s="141"/>
+      <c r="T35" s="141"/>
     </row>
     <row r="36" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
@@ -5275,26 +5278,26 @@
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="140" t="s">
+      <c r="C37" s="141" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="140"/>
-      <c r="E37" s="140"/>
-      <c r="F37" s="140"/>
-      <c r="G37" s="140"/>
-      <c r="H37" s="140"/>
-      <c r="I37" s="140"/>
-      <c r="J37" s="140"/>
-      <c r="K37" s="140"/>
-      <c r="L37" s="140"/>
-      <c r="M37" s="140"/>
-      <c r="N37" s="140"/>
-      <c r="O37" s="140"/>
-      <c r="P37" s="140"/>
-      <c r="Q37" s="140"/>
-      <c r="R37" s="140"/>
-      <c r="S37" s="140"/>
-      <c r="T37" s="140"/>
+      <c r="D37" s="141"/>
+      <c r="E37" s="141"/>
+      <c r="F37" s="141"/>
+      <c r="G37" s="141"/>
+      <c r="H37" s="141"/>
+      <c r="I37" s="141"/>
+      <c r="J37" s="141"/>
+      <c r="K37" s="141"/>
+      <c r="L37" s="141"/>
+      <c r="M37" s="141"/>
+      <c r="N37" s="141"/>
+      <c r="O37" s="141"/>
+      <c r="P37" s="141"/>
+      <c r="Q37" s="141"/>
+      <c r="R37" s="141"/>
+      <c r="S37" s="141"/>
+      <c r="T37" s="141"/>
     </row>
     <row r="38" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
@@ -5321,26 +5324,26 @@
       <c r="B39" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="140" t="s">
+      <c r="C39" s="141" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="140"/>
-      <c r="E39" s="140"/>
-      <c r="F39" s="140"/>
-      <c r="G39" s="140"/>
-      <c r="H39" s="140"/>
-      <c r="I39" s="140"/>
-      <c r="J39" s="140"/>
-      <c r="K39" s="140"/>
-      <c r="L39" s="140"/>
-      <c r="M39" s="140"/>
-      <c r="N39" s="140"/>
-      <c r="O39" s="140"/>
-      <c r="P39" s="140"/>
-      <c r="Q39" s="140"/>
-      <c r="R39" s="140"/>
-      <c r="S39" s="140"/>
-      <c r="T39" s="140"/>
+      <c r="D39" s="141"/>
+      <c r="E39" s="141"/>
+      <c r="F39" s="141"/>
+      <c r="G39" s="141"/>
+      <c r="H39" s="141"/>
+      <c r="I39" s="141"/>
+      <c r="J39" s="141"/>
+      <c r="K39" s="141"/>
+      <c r="L39" s="141"/>
+      <c r="M39" s="141"/>
+      <c r="N39" s="141"/>
+      <c r="O39" s="141"/>
+      <c r="P39" s="141"/>
+      <c r="Q39" s="141"/>
+      <c r="R39" s="141"/>
+      <c r="S39" s="141"/>
+      <c r="T39" s="141"/>
     </row>
     <row r="40" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
@@ -5367,34 +5370,29 @@
       <c r="B41" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="142" t="s">
+      <c r="C41" s="143" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="142"/>
-      <c r="E41" s="142"/>
-      <c r="F41" s="142"/>
-      <c r="G41" s="142"/>
-      <c r="H41" s="142"/>
-      <c r="I41" s="142"/>
-      <c r="J41" s="142"/>
-      <c r="K41" s="142"/>
-      <c r="L41" s="142"/>
-      <c r="M41" s="142"/>
-      <c r="N41" s="142"/>
-      <c r="O41" s="142"/>
-      <c r="P41" s="142"/>
-      <c r="Q41" s="142"/>
-      <c r="R41" s="142"/>
-      <c r="S41" s="142"/>
-      <c r="T41" s="142"/>
+      <c r="D41" s="143"/>
+      <c r="E41" s="143"/>
+      <c r="F41" s="143"/>
+      <c r="G41" s="143"/>
+      <c r="H41" s="143"/>
+      <c r="I41" s="143"/>
+      <c r="J41" s="143"/>
+      <c r="K41" s="143"/>
+      <c r="L41" s="143"/>
+      <c r="M41" s="143"/>
+      <c r="N41" s="143"/>
+      <c r="O41" s="143"/>
+      <c r="P41" s="143"/>
+      <c r="Q41" s="143"/>
+      <c r="R41" s="143"/>
+      <c r="S41" s="143"/>
+      <c r="T41" s="143"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="N7:T7"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="N13:T13"/>
-    <mergeCell ref="C35:T35"/>
     <mergeCell ref="C37:T37"/>
     <mergeCell ref="C39:T39"/>
     <mergeCell ref="C41:T41"/>
@@ -5404,6 +5402,11 @@
     <mergeCell ref="N25:T25"/>
     <mergeCell ref="C31:T31"/>
     <mergeCell ref="C33:T33"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="N7:T7"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="N13:T13"/>
+    <mergeCell ref="C35:T35"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -5442,94 +5445,94 @@
     </row>
     <row r="3" spans="3:4" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:4" s="93" customFormat="1" ht="104.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="151" t="s">
+      <c r="C4" s="152" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="151"/>
+      <c r="D4" s="152"/>
     </row>
     <row r="5" spans="3:4" s="93" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="151" t="s">
+      <c r="C5" s="152" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="151"/>
+      <c r="D5" s="152"/>
     </row>
     <row r="6" spans="3:4" s="93" customFormat="1" ht="209.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="151" t="s">
+      <c r="C6" s="152" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="151"/>
+      <c r="D6" s="152"/>
     </row>
     <row r="7" spans="3:4" s="93" customFormat="1" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="151" t="s">
+      <c r="C7" s="152" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="151"/>
+      <c r="D7" s="152"/>
     </row>
     <row r="8" spans="3:4" s="93" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="151" t="s">
+      <c r="C8" s="152" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="151"/>
+      <c r="D8" s="152"/>
     </row>
     <row r="9" spans="3:4" s="93" customFormat="1" ht="200.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="151" t="s">
+      <c r="C9" s="152" t="s">
         <v>74</v>
       </c>
-      <c r="D9" s="151"/>
+      <c r="D9" s="152"/>
     </row>
     <row r="10" spans="3:4" s="93" customFormat="1" ht="147.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="151" t="s">
+      <c r="C10" s="152" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="151"/>
+      <c r="D10" s="152"/>
     </row>
     <row r="11" spans="3:4" s="93" customFormat="1" ht="134.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="151" t="s">
+      <c r="C11" s="152" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="151"/>
+      <c r="D11" s="152"/>
     </row>
     <row r="12" spans="3:4" s="93" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="151" t="s">
+      <c r="C12" s="152" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="151"/>
+      <c r="D12" s="152"/>
     </row>
     <row r="13" spans="3:4" s="93" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="151" t="s">
+      <c r="C13" s="152" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="151"/>
+      <c r="D13" s="152"/>
     </row>
     <row r="14" spans="3:4" s="93" customFormat="1" ht="128.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="151" t="s">
+      <c r="C14" s="152" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="151"/>
+      <c r="D14" s="152"/>
     </row>
     <row r="15" spans="3:4" s="93" customFormat="1" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="151" t="s">
+      <c r="C15" s="152" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="151"/>
+      <c r="D15" s="152"/>
     </row>
     <row r="16" spans="3:4" s="93" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="151" t="s">
+      <c r="C16" s="152" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="151"/>
+      <c r="D16" s="152"/>
     </row>
     <row r="17" spans="3:4" s="93" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="151" t="s">
+      <c r="C17" s="152" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="151"/>
+      <c r="D17" s="152"/>
     </row>
     <row r="18" spans="3:4" s="93" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="151" t="s">
+      <c r="C18" s="152" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="151"/>
+      <c r="D18" s="152"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -5563,7 +5566,7 @@
   <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="I1" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5631,24 +5634,24 @@
       </c>
     </row>
     <row r="5" spans="1:21" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="140"/>
-      <c r="D5" s="140"/>
-      <c r="E5" s="140"/>
-      <c r="F5" s="140"/>
-      <c r="G5" s="140"/>
+      <c r="C5" s="141"/>
+      <c r="D5" s="141"/>
+      <c r="E5" s="141"/>
+      <c r="F5" s="141"/>
+      <c r="G5" s="141"/>
       <c r="H5" s="46"/>
-      <c r="I5" s="140"/>
-      <c r="J5" s="140"/>
-      <c r="K5" s="140"/>
-      <c r="L5" s="140"/>
-      <c r="M5" s="140"/>
-      <c r="N5" s="140"/>
+      <c r="I5" s="141"/>
+      <c r="J5" s="141"/>
+      <c r="K5" s="141"/>
+      <c r="L5" s="141"/>
+      <c r="M5" s="141"/>
+      <c r="N5" s="141"/>
       <c r="O5" s="46"/>
       <c r="P5" s="134"/>
       <c r="Q5" s="134"/>
-      <c r="R5" s="140"/>
-      <c r="S5" s="140"/>
-      <c r="T5" s="140"/>
+      <c r="R5" s="141"/>
+      <c r="S5" s="141"/>
+      <c r="T5" s="141"/>
     </row>
     <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I6" s="25"/>
@@ -5665,21 +5668,21 @@
       <c r="F7" s="6"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="145" t="s">
+      <c r="I7" s="146" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="146"/>
-      <c r="K7" s="146"/>
-      <c r="L7" s="146"/>
-      <c r="M7" s="146"/>
-      <c r="N7" s="147"/>
-      <c r="O7" s="145"/>
-      <c r="P7" s="146"/>
-      <c r="Q7" s="146"/>
-      <c r="R7" s="146"/>
-      <c r="S7" s="146"/>
-      <c r="T7" s="146"/>
-      <c r="U7" s="147"/>
+      <c r="J7" s="147"/>
+      <c r="K7" s="147"/>
+      <c r="L7" s="147"/>
+      <c r="M7" s="147"/>
+      <c r="N7" s="148"/>
+      <c r="O7" s="146"/>
+      <c r="P7" s="147"/>
+      <c r="Q7" s="147"/>
+      <c r="R7" s="147"/>
+      <c r="S7" s="147"/>
+      <c r="T7" s="147"/>
+      <c r="U7" s="148"/>
     </row>
     <row r="8" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -5835,20 +5838,20 @@
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
-      <c r="H13" s="145"/>
-      <c r="I13" s="146"/>
-      <c r="J13" s="146"/>
-      <c r="K13" s="146"/>
-      <c r="L13" s="146"/>
-      <c r="M13" s="146"/>
-      <c r="N13" s="147"/>
-      <c r="O13" s="145"/>
-      <c r="P13" s="146"/>
-      <c r="Q13" s="146"/>
-      <c r="R13" s="146"/>
-      <c r="S13" s="146"/>
-      <c r="T13" s="146"/>
-      <c r="U13" s="147"/>
+      <c r="H13" s="146"/>
+      <c r="I13" s="147"/>
+      <c r="J13" s="147"/>
+      <c r="K13" s="147"/>
+      <c r="L13" s="147"/>
+      <c r="M13" s="147"/>
+      <c r="N13" s="148"/>
+      <c r="O13" s="146"/>
+      <c r="P13" s="147"/>
+      <c r="Q13" s="147"/>
+      <c r="R13" s="147"/>
+      <c r="S13" s="147"/>
+      <c r="T13" s="147"/>
+      <c r="U13" s="148"/>
     </row>
     <row r="14" spans="1:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14"/>
@@ -6014,22 +6017,22 @@
       </c>
       <c r="D20" s="47"/>
       <c r="E20" s="94"/>
-      <c r="F20" s="152"/>
-      <c r="G20" s="152"/>
-      <c r="H20" s="152"/>
-      <c r="I20" s="152"/>
-      <c r="J20" s="152"/>
-      <c r="K20" s="152"/>
-      <c r="L20" s="152"/>
-      <c r="M20" s="152"/>
-      <c r="N20" s="152"/>
-      <c r="O20" s="152"/>
-      <c r="P20" s="152"/>
-      <c r="Q20" s="152"/>
-      <c r="R20" s="152"/>
-      <c r="S20" s="152"/>
-      <c r="T20" s="152"/>
-      <c r="U20" s="152"/>
+      <c r="F20" s="153"/>
+      <c r="G20" s="153"/>
+      <c r="H20" s="153"/>
+      <c r="I20" s="153"/>
+      <c r="J20" s="153"/>
+      <c r="K20" s="153"/>
+      <c r="L20" s="153"/>
+      <c r="M20" s="153"/>
+      <c r="N20" s="153"/>
+      <c r="O20" s="153"/>
+      <c r="P20" s="153"/>
+      <c r="Q20" s="153"/>
+      <c r="R20" s="153"/>
+      <c r="S20" s="153"/>
+      <c r="T20" s="153"/>
+      <c r="U20" s="153"/>
     </row>
     <row r="21" spans="1:22" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>
@@ -6058,22 +6061,22 @@
         <v>36</v>
       </c>
       <c r="D22" s="47"/>
-      <c r="F22" s="152"/>
-      <c r="G22" s="152"/>
-      <c r="H22" s="152"/>
-      <c r="I22" s="152"/>
-      <c r="J22" s="152"/>
-      <c r="K22" s="152"/>
-      <c r="L22" s="152"/>
-      <c r="M22" s="152"/>
-      <c r="N22" s="152"/>
-      <c r="O22" s="152"/>
-      <c r="P22" s="152"/>
-      <c r="Q22" s="152"/>
-      <c r="R22" s="152"/>
-      <c r="S22" s="152"/>
-      <c r="T22" s="152"/>
-      <c r="U22" s="152"/>
+      <c r="F22" s="153"/>
+      <c r="G22" s="153"/>
+      <c r="H22" s="153"/>
+      <c r="I22" s="153"/>
+      <c r="J22" s="153"/>
+      <c r="K22" s="153"/>
+      <c r="L22" s="153"/>
+      <c r="M22" s="153"/>
+      <c r="N22" s="153"/>
+      <c r="O22" s="153"/>
+      <c r="P22" s="153"/>
+      <c r="Q22" s="153"/>
+      <c r="R22" s="153"/>
+      <c r="S22" s="153"/>
+      <c r="T22" s="153"/>
+      <c r="U22" s="153"/>
       <c r="V22" s="3"/>
     </row>
     <row r="23" spans="1:22" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -6102,22 +6105,22 @@
       </c>
       <c r="D24" s="47"/>
       <c r="E24" s="94"/>
-      <c r="F24" s="152"/>
-      <c r="G24" s="152"/>
-      <c r="H24" s="152"/>
-      <c r="I24" s="152"/>
-      <c r="J24" s="152"/>
-      <c r="K24" s="152"/>
-      <c r="L24" s="152"/>
-      <c r="M24" s="152"/>
-      <c r="N24" s="152"/>
-      <c r="O24" s="152"/>
-      <c r="P24" s="152"/>
-      <c r="Q24" s="152"/>
-      <c r="R24" s="152"/>
-      <c r="S24" s="152"/>
-      <c r="T24" s="152"/>
-      <c r="U24" s="152"/>
+      <c r="F24" s="153"/>
+      <c r="G24" s="153"/>
+      <c r="H24" s="153"/>
+      <c r="I24" s="153"/>
+      <c r="J24" s="153"/>
+      <c r="K24" s="153"/>
+      <c r="L24" s="153"/>
+      <c r="M24" s="153"/>
+      <c r="N24" s="153"/>
+      <c r="O24" s="153"/>
+      <c r="P24" s="153"/>
+      <c r="Q24" s="153"/>
+      <c r="R24" s="153"/>
+      <c r="S24" s="153"/>
+      <c r="T24" s="153"/>
+      <c r="U24" s="153"/>
     </row>
     <row r="25" spans="1:22" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="1"/>
@@ -6146,22 +6149,22 @@
         <v>48</v>
       </c>
       <c r="D26" s="47"/>
-      <c r="F26" s="143"/>
-      <c r="G26" s="143"/>
-      <c r="H26" s="143"/>
-      <c r="I26" s="143"/>
-      <c r="J26" s="143"/>
-      <c r="K26" s="143"/>
-      <c r="L26" s="143"/>
-      <c r="M26" s="143"/>
-      <c r="N26" s="143"/>
-      <c r="O26" s="143"/>
-      <c r="P26" s="143"/>
-      <c r="Q26" s="143"/>
-      <c r="R26" s="143"/>
-      <c r="S26" s="143"/>
-      <c r="T26" s="143"/>
-      <c r="U26" s="143"/>
+      <c r="F26" s="144"/>
+      <c r="G26" s="144"/>
+      <c r="H26" s="144"/>
+      <c r="I26" s="144"/>
+      <c r="J26" s="144"/>
+      <c r="K26" s="144"/>
+      <c r="L26" s="144"/>
+      <c r="M26" s="144"/>
+      <c r="N26" s="144"/>
+      <c r="O26" s="144"/>
+      <c r="P26" s="144"/>
+      <c r="Q26" s="144"/>
+      <c r="R26" s="144"/>
+      <c r="S26" s="144"/>
+      <c r="T26" s="144"/>
+      <c r="U26" s="144"/>
       <c r="V26" s="3"/>
     </row>
     <row r="27" spans="1:22" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -6189,25 +6192,32 @@
         <v>49</v>
       </c>
       <c r="D28" s="47"/>
-      <c r="F28" s="142"/>
-      <c r="G28" s="142"/>
-      <c r="H28" s="142"/>
-      <c r="I28" s="142"/>
-      <c r="J28" s="142"/>
-      <c r="K28" s="142"/>
-      <c r="L28" s="142"/>
-      <c r="M28" s="142"/>
-      <c r="N28" s="142"/>
-      <c r="O28" s="142"/>
-      <c r="P28" s="142"/>
-      <c r="Q28" s="142"/>
-      <c r="R28" s="142"/>
-      <c r="S28" s="142"/>
-      <c r="T28" s="142"/>
-      <c r="U28" s="142"/>
+      <c r="F28" s="143"/>
+      <c r="G28" s="143"/>
+      <c r="H28" s="143"/>
+      <c r="I28" s="143"/>
+      <c r="J28" s="143"/>
+      <c r="K28" s="143"/>
+      <c r="L28" s="143"/>
+      <c r="M28" s="143"/>
+      <c r="N28" s="143"/>
+      <c r="O28" s="143"/>
+      <c r="P28" s="143"/>
+      <c r="Q28" s="143"/>
+      <c r="R28" s="143"/>
+      <c r="S28" s="143"/>
+      <c r="T28" s="143"/>
+      <c r="U28" s="143"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="I7:N7"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
     <mergeCell ref="F28:U28"/>
     <mergeCell ref="F20:U20"/>
     <mergeCell ref="H13:N13"/>
@@ -6216,13 +6226,6 @@
     <mergeCell ref="F24:U24"/>
     <mergeCell ref="F26:U26"/>
     <mergeCell ref="O13:U13"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I7:N7"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:U3 C5 C4:N4 Q4:U4 U5 C6:U1048576">
     <cfRule type="expression" dxfId="2" priority="3">
@@ -6267,18 +6270,18 @@
     <row r="1" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="133"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="146"/>
-      <c r="I2" s="146"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="145"/>
-      <c r="L2" s="146"/>
-      <c r="M2" s="146"/>
-      <c r="N2" s="147"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="147"/>
+      <c r="H2" s="147"/>
+      <c r="I2" s="147"/>
+      <c r="J2" s="148"/>
+      <c r="K2" s="146"/>
+      <c r="L2" s="147"/>
+      <c r="M2" s="147"/>
+      <c r="N2" s="148"/>
       <c r="O2" s="25"/>
     </row>
     <row r="3" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6413,35 +6416,35 @@
       <c r="B10" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="153"/>
-      <c r="D10" s="154"/>
-      <c r="E10" s="154"/>
-      <c r="F10" s="155"/>
-      <c r="G10" s="153"/>
-      <c r="H10" s="154"/>
-      <c r="I10" s="154"/>
-      <c r="J10" s="155"/>
-      <c r="K10" s="153"/>
-      <c r="L10" s="154"/>
-      <c r="M10" s="154"/>
-      <c r="N10" s="155"/>
+      <c r="C10" s="154"/>
+      <c r="D10" s="155"/>
+      <c r="E10" s="155"/>
+      <c r="F10" s="156"/>
+      <c r="G10" s="154"/>
+      <c r="H10" s="155"/>
+      <c r="I10" s="155"/>
+      <c r="J10" s="156"/>
+      <c r="K10" s="154"/>
+      <c r="L10" s="155"/>
+      <c r="M10" s="155"/>
+      <c r="N10" s="156"/>
       <c r="O10" s="135"/>
     </row>
     <row r="12" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="133"/>
-      <c r="C12" s="145"/>
-      <c r="D12" s="146"/>
-      <c r="E12" s="146"/>
-      <c r="F12" s="146"/>
-      <c r="G12" s="147"/>
-      <c r="H12" s="146"/>
-      <c r="I12" s="146"/>
-      <c r="J12" s="146"/>
-      <c r="K12" s="147"/>
-      <c r="L12" s="145"/>
-      <c r="M12" s="146"/>
-      <c r="N12" s="146"/>
-      <c r="O12" s="147"/>
+      <c r="C12" s="146"/>
+      <c r="D12" s="147"/>
+      <c r="E12" s="147"/>
+      <c r="F12" s="147"/>
+      <c r="G12" s="148"/>
+      <c r="H12" s="147"/>
+      <c r="I12" s="147"/>
+      <c r="J12" s="147"/>
+      <c r="K12" s="148"/>
+      <c r="L12" s="146"/>
+      <c r="M12" s="147"/>
+      <c r="N12" s="147"/>
+      <c r="O12" s="148"/>
       <c r="P12" s="25"/>
     </row>
     <row r="13" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6583,36 +6586,36 @@
       <c r="B20" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="153"/>
-      <c r="D20" s="154"/>
-      <c r="E20" s="154"/>
-      <c r="F20" s="154"/>
-      <c r="G20" s="155"/>
-      <c r="H20" s="153"/>
-      <c r="I20" s="154"/>
-      <c r="J20" s="154"/>
-      <c r="K20" s="155"/>
-      <c r="L20" s="156"/>
-      <c r="M20" s="157"/>
-      <c r="N20" s="157"/>
-      <c r="O20" s="158"/>
+      <c r="C20" s="154"/>
+      <c r="D20" s="155"/>
+      <c r="E20" s="155"/>
+      <c r="F20" s="155"/>
+      <c r="G20" s="156"/>
+      <c r="H20" s="154"/>
+      <c r="I20" s="155"/>
+      <c r="J20" s="155"/>
+      <c r="K20" s="156"/>
+      <c r="L20" s="157"/>
+      <c r="M20" s="158"/>
+      <c r="N20" s="158"/>
+      <c r="O20" s="159"/>
       <c r="P20" s="132"/>
     </row>
     <row r="22" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="133"/>
-      <c r="C22" s="145"/>
-      <c r="D22" s="146"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="147"/>
-      <c r="G22" s="146"/>
-      <c r="H22" s="146"/>
-      <c r="I22" s="146"/>
-      <c r="J22" s="146"/>
-      <c r="K22" s="147"/>
-      <c r="L22" s="145"/>
-      <c r="M22" s="146"/>
-      <c r="N22" s="146"/>
-      <c r="O22" s="147"/>
+      <c r="C22" s="146"/>
+      <c r="D22" s="147"/>
+      <c r="E22" s="147"/>
+      <c r="F22" s="148"/>
+      <c r="G22" s="147"/>
+      <c r="H22" s="147"/>
+      <c r="I22" s="147"/>
+      <c r="J22" s="147"/>
+      <c r="K22" s="148"/>
+      <c r="L22" s="146"/>
+      <c r="M22" s="147"/>
+      <c r="N22" s="147"/>
+      <c r="O22" s="148"/>
       <c r="P22" s="25"/>
     </row>
     <row r="23" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6754,36 +6757,36 @@
       <c r="B30" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="153"/>
-      <c r="D30" s="154"/>
-      <c r="E30" s="154"/>
-      <c r="F30" s="155"/>
-      <c r="G30" s="153"/>
-      <c r="H30" s="154"/>
-      <c r="I30" s="154"/>
-      <c r="J30" s="154"/>
-      <c r="K30" s="155"/>
-      <c r="L30" s="153"/>
-      <c r="M30" s="154"/>
-      <c r="N30" s="154"/>
-      <c r="O30" s="155"/>
+      <c r="C30" s="154"/>
+      <c r="D30" s="155"/>
+      <c r="E30" s="155"/>
+      <c r="F30" s="156"/>
+      <c r="G30" s="154"/>
+      <c r="H30" s="155"/>
+      <c r="I30" s="155"/>
+      <c r="J30" s="155"/>
+      <c r="K30" s="156"/>
+      <c r="L30" s="154"/>
+      <c r="M30" s="155"/>
+      <c r="N30" s="155"/>
+      <c r="O30" s="156"/>
       <c r="P30" s="135"/>
     </row>
     <row r="32" spans="2:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="133"/>
-      <c r="C32" s="145"/>
-      <c r="D32" s="146"/>
-      <c r="E32" s="146"/>
-      <c r="F32" s="147"/>
-      <c r="G32" s="146"/>
-      <c r="H32" s="146"/>
-      <c r="I32" s="146"/>
-      <c r="J32" s="147"/>
-      <c r="K32" s="145"/>
-      <c r="L32" s="146"/>
-      <c r="M32" s="146"/>
-      <c r="N32" s="146"/>
-      <c r="O32" s="147"/>
+      <c r="C32" s="146"/>
+      <c r="D32" s="147"/>
+      <c r="E32" s="147"/>
+      <c r="F32" s="148"/>
+      <c r="G32" s="147"/>
+      <c r="H32" s="147"/>
+      <c r="I32" s="147"/>
+      <c r="J32" s="148"/>
+      <c r="K32" s="146"/>
+      <c r="L32" s="147"/>
+      <c r="M32" s="147"/>
+      <c r="N32" s="147"/>
+      <c r="O32" s="148"/>
       <c r="P32" s="25"/>
     </row>
     <row r="33" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -6925,37 +6928,37 @@
       <c r="B40" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="153"/>
-      <c r="D40" s="154"/>
-      <c r="E40" s="154"/>
-      <c r="F40" s="155"/>
-      <c r="G40" s="153"/>
-      <c r="H40" s="154"/>
-      <c r="I40" s="154"/>
-      <c r="J40" s="155"/>
-      <c r="K40" s="153"/>
-      <c r="L40" s="154"/>
-      <c r="M40" s="154"/>
-      <c r="N40" s="154"/>
-      <c r="O40" s="155"/>
+      <c r="C40" s="154"/>
+      <c r="D40" s="155"/>
+      <c r="E40" s="155"/>
+      <c r="F40" s="156"/>
+      <c r="G40" s="154"/>
+      <c r="H40" s="155"/>
+      <c r="I40" s="155"/>
+      <c r="J40" s="156"/>
+      <c r="K40" s="154"/>
+      <c r="L40" s="155"/>
+      <c r="M40" s="155"/>
+      <c r="N40" s="155"/>
+      <c r="O40" s="156"/>
       <c r="P40" s="135"/>
     </row>
     <row r="42" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="133"/>
-      <c r="C42" s="145"/>
-      <c r="D42" s="146"/>
-      <c r="E42" s="146"/>
-      <c r="F42" s="146"/>
-      <c r="G42" s="147"/>
-      <c r="H42" s="146"/>
-      <c r="I42" s="146"/>
-      <c r="J42" s="146"/>
-      <c r="K42" s="146"/>
-      <c r="L42" s="147"/>
-      <c r="M42" s="145"/>
-      <c r="N42" s="146"/>
-      <c r="O42" s="146"/>
-      <c r="P42" s="147"/>
+      <c r="C42" s="146"/>
+      <c r="D42" s="147"/>
+      <c r="E42" s="147"/>
+      <c r="F42" s="147"/>
+      <c r="G42" s="148"/>
+      <c r="H42" s="147"/>
+      <c r="I42" s="147"/>
+      <c r="J42" s="147"/>
+      <c r="K42" s="147"/>
+      <c r="L42" s="148"/>
+      <c r="M42" s="146"/>
+      <c r="N42" s="147"/>
+      <c r="O42" s="147"/>
+      <c r="P42" s="148"/>
       <c r="Q42" s="25"/>
     </row>
     <row r="43" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7104,38 +7107,38 @@
       <c r="B50" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="C50" s="153"/>
-      <c r="D50" s="154"/>
-      <c r="E50" s="154"/>
-      <c r="F50" s="154"/>
-      <c r="G50" s="155"/>
-      <c r="H50" s="153"/>
-      <c r="I50" s="154"/>
-      <c r="J50" s="154"/>
-      <c r="K50" s="154"/>
-      <c r="L50" s="155"/>
-      <c r="M50" s="153"/>
-      <c r="N50" s="154"/>
-      <c r="O50" s="154"/>
-      <c r="P50" s="155"/>
+      <c r="C50" s="154"/>
+      <c r="D50" s="155"/>
+      <c r="E50" s="155"/>
+      <c r="F50" s="155"/>
+      <c r="G50" s="156"/>
+      <c r="H50" s="154"/>
+      <c r="I50" s="155"/>
+      <c r="J50" s="155"/>
+      <c r="K50" s="155"/>
+      <c r="L50" s="156"/>
+      <c r="M50" s="154"/>
+      <c r="N50" s="155"/>
+      <c r="O50" s="155"/>
+      <c r="P50" s="156"/>
       <c r="Q50" s="135"/>
     </row>
     <row r="52" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="133"/>
-      <c r="C52" s="145"/>
-      <c r="D52" s="146"/>
-      <c r="E52" s="146"/>
-      <c r="F52" s="146"/>
-      <c r="G52" s="147"/>
-      <c r="H52" s="146"/>
-      <c r="I52" s="146"/>
-      <c r="J52" s="146"/>
-      <c r="K52" s="147"/>
-      <c r="L52" s="145"/>
-      <c r="M52" s="146"/>
-      <c r="N52" s="146"/>
-      <c r="O52" s="146"/>
-      <c r="P52" s="147"/>
+      <c r="C52" s="146"/>
+      <c r="D52" s="147"/>
+      <c r="E52" s="147"/>
+      <c r="F52" s="147"/>
+      <c r="G52" s="148"/>
+      <c r="H52" s="147"/>
+      <c r="I52" s="147"/>
+      <c r="J52" s="147"/>
+      <c r="K52" s="148"/>
+      <c r="L52" s="146"/>
+      <c r="M52" s="147"/>
+      <c r="N52" s="147"/>
+      <c r="O52" s="147"/>
+      <c r="P52" s="148"/>
       <c r="Q52" s="25"/>
     </row>
     <row r="53" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7284,38 +7287,38 @@
       <c r="B60" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="C60" s="153"/>
-      <c r="D60" s="154"/>
-      <c r="E60" s="154"/>
-      <c r="F60" s="154"/>
-      <c r="G60" s="155"/>
-      <c r="H60" s="153"/>
-      <c r="I60" s="154"/>
-      <c r="J60" s="154"/>
-      <c r="K60" s="155"/>
-      <c r="L60" s="153"/>
-      <c r="M60" s="154"/>
-      <c r="N60" s="154"/>
-      <c r="O60" s="154"/>
-      <c r="P60" s="155"/>
+      <c r="C60" s="154"/>
+      <c r="D60" s="155"/>
+      <c r="E60" s="155"/>
+      <c r="F60" s="155"/>
+      <c r="G60" s="156"/>
+      <c r="H60" s="154"/>
+      <c r="I60" s="155"/>
+      <c r="J60" s="155"/>
+      <c r="K60" s="156"/>
+      <c r="L60" s="154"/>
+      <c r="M60" s="155"/>
+      <c r="N60" s="155"/>
+      <c r="O60" s="155"/>
+      <c r="P60" s="156"/>
       <c r="Q60" s="135"/>
     </row>
     <row r="62" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="133"/>
-      <c r="C62" s="145"/>
-      <c r="D62" s="146"/>
-      <c r="E62" s="146"/>
-      <c r="F62" s="147"/>
-      <c r="G62" s="146"/>
-      <c r="H62" s="146"/>
-      <c r="I62" s="146"/>
-      <c r="J62" s="146"/>
-      <c r="K62" s="147"/>
-      <c r="L62" s="145"/>
-      <c r="M62" s="146"/>
-      <c r="N62" s="146"/>
-      <c r="O62" s="146"/>
-      <c r="P62" s="147"/>
+      <c r="C62" s="146"/>
+      <c r="D62" s="147"/>
+      <c r="E62" s="147"/>
+      <c r="F62" s="148"/>
+      <c r="G62" s="147"/>
+      <c r="H62" s="147"/>
+      <c r="I62" s="147"/>
+      <c r="J62" s="147"/>
+      <c r="K62" s="148"/>
+      <c r="L62" s="146"/>
+      <c r="M62" s="147"/>
+      <c r="N62" s="147"/>
+      <c r="O62" s="147"/>
+      <c r="P62" s="148"/>
       <c r="Q62" s="25"/>
     </row>
     <row r="63" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -7464,50 +7467,24 @@
       <c r="B70" s="115" t="s">
         <v>90</v>
       </c>
-      <c r="C70" s="153"/>
-      <c r="D70" s="154"/>
-      <c r="E70" s="154"/>
-      <c r="F70" s="155"/>
-      <c r="G70" s="153"/>
-      <c r="H70" s="154"/>
-      <c r="I70" s="154"/>
-      <c r="J70" s="154"/>
-      <c r="K70" s="155"/>
-      <c r="L70" s="153"/>
-      <c r="M70" s="154"/>
-      <c r="N70" s="154"/>
-      <c r="O70" s="154"/>
-      <c r="P70" s="155"/>
+      <c r="C70" s="154"/>
+      <c r="D70" s="155"/>
+      <c r="E70" s="155"/>
+      <c r="F70" s="156"/>
+      <c r="G70" s="154"/>
+      <c r="H70" s="155"/>
+      <c r="I70" s="155"/>
+      <c r="J70" s="155"/>
+      <c r="K70" s="156"/>
+      <c r="L70" s="154"/>
+      <c r="M70" s="155"/>
+      <c r="N70" s="155"/>
+      <c r="O70" s="155"/>
+      <c r="P70" s="156"/>
       <c r="Q70" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="L12:O12"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="K32:O32"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="G62:K62"/>
-    <mergeCell ref="L62:P62"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="M42:P42"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="L52:P52"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="L20:O20"/>
@@ -7524,6 +7501,32 @@
     <mergeCell ref="G40:J40"/>
     <mergeCell ref="K40:O40"/>
     <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="G62:K62"/>
+    <mergeCell ref="L62:P62"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="M42:P42"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="L52:P52"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="L22:O22"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="K32:O32"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="L12:O12"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:N10"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="L20 M50 K10 K40 L60 L70 C10 G10 C20 H20 C70 G70 C60 H60 C50 H50 C40 G40 C30 G30 L30" xr:uid="{C8C03E04-8C1F-4330-BDED-96AC21F8FF6E}"/>
@@ -7534,21 +7537,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000192CE90DA120240A67EE82BE1FBFF43" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="623d129459d6fae29ac2c5d491c3782f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e2beb7e-37df-4602-aab8-4f6673c75e9a" xmlns:ns4="eaec1813-26bf-4c98-9021-907af21e1945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bfd2e6b22ac1ad737273b5b960116aad" ns3:_="" ns4:_="">
     <xsd:import namespace="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
@@ -7771,32 +7759,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53520415-44BC-4FFA-B7D1-C1B985B55107}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7813,4 +7791,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB68F43B-E0EF-42BE-BAC3-92E4E861A7D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B10A51B4-5AFB-478C-ADEC-6221B89FD95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0e2beb7e-37df-4602-aab8-4f6673c75e9a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="eaec1813-26bf-4c98-9021-907af21e1945"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>